<commit_message>
small changes to grouping and closer example to WF1
</commit_message>
<xml_diff>
--- a/HC_LBL_SpecificationInterface.xlsx
+++ b/HC_LBL_SpecificationInterface.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27417"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaeltynes/repos/ESCALATE_Capture/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ipendleton/Dropbox/Desktop/ESCALATE/ESCALATE_Capture/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCC709FE-7832-8242-99C1-6BBBF21974C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25660" yWindow="40" windowWidth="38400" windowHeight="21600" tabRatio="500"/>
+    <workbookView xWindow="12800" yWindow="460" windowWidth="38400" windowHeight="21600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User Interface" sheetId="4" r:id="rId1"/>
@@ -24,7 +25,7 @@
     <definedName name="wellcount" localSheetId="0">'User Interface'!$E$6</definedName>
     <definedName name="wellcount">'WF1'!$D$7</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="275">
   <si>
     <t>Comment</t>
   </si>
@@ -149,7 +150,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="1"/>
+        <family val="2"/>
       </rPr>
       <t>)</t>
     </r>
@@ -174,7 +175,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="1"/>
+        <family val="2"/>
       </rPr>
       <t>2_molarmin</t>
     </r>
@@ -196,7 +197,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="1"/>
+        <family val="2"/>
       </rPr>
       <t>2_molarmax</t>
     </r>
@@ -210,7 +211,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="1"/>
+        <family val="2"/>
       </rPr>
       <t>Reagent1_</t>
     </r>
@@ -230,7 +231,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="1"/>
+        <family val="2"/>
       </rPr>
       <t>_list</t>
     </r>
@@ -244,7 +245,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="1"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">ECL model ID.  </t>
     </r>
@@ -269,7 +270,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="1"/>
+        <family val="2"/>
       </rPr>
       <t>Reagent2_</t>
     </r>
@@ -289,7 +290,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="1"/>
+        <family val="2"/>
       </rPr>
       <t>_list</t>
     </r>
@@ -330,7 +331,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="1"/>
+        <family val="2"/>
       </rPr>
       <t>Reagent3_</t>
     </r>
@@ -350,7 +351,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="1"/>
+        <family val="2"/>
       </rPr>
       <t>_list</t>
     </r>
@@ -376,7 +377,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="1"/>
+        <family val="2"/>
       </rPr>
       <t>Reagent4_</t>
     </r>
@@ -396,7 +397,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="1"/>
+        <family val="2"/>
       </rPr>
       <t>_list</t>
     </r>
@@ -425,7 +426,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="1"/>
+        <family val="2"/>
       </rPr>
       <t>Reagent5_</t>
     </r>
@@ -445,7 +446,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="1"/>
+        <family val="2"/>
       </rPr>
       <t>_list</t>
     </r>
@@ -547,9 +548,6 @@
     <t>reagents_prep_temperature</t>
   </si>
   <si>
-    <t xml:space="preserve"> Temperature of reagent during preparation ( °C ) </t>
-  </si>
-  <si>
     <t>reagents_prep_stirrate</t>
   </si>
   <si>
@@ -619,28 +617,7 @@
     <t>['PbI2','DMSO','DMF']</t>
   </si>
   <si>
-    <t>Spincoating Speed</t>
-  </si>
-  <si>
-    <t>Spincoating Duration (s)</t>
-  </si>
-  <si>
-    <t>Spincoating Temperature ( C )</t>
-  </si>
-  <si>
-    <t>Spincoating Duration 2 (s)</t>
-  </si>
-  <si>
-    <t>Annealing Temperature ( C )</t>
-  </si>
-  <si>
-    <t>Annealing Duration (s)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Experimental Reaction Vessel</t>
   </si>
   <si>
     <t>Actions (Experiments - Manual and Random)</t>
@@ -650,12 +627,6 @@
   </si>
   <si>
     <t>Reagent3_item3_formulaconc</t>
-  </si>
-  <si>
-    <t>['CBz']</t>
-  </si>
-  <si>
-    <t>[[215,215]]</t>
   </si>
   <si>
     <t>Total Precursor Volume (ul)</t>
@@ -680,9 +651,6 @@
   </si>
   <si>
     <t>[[215, 215]]</t>
-  </si>
-  <si>
-    <t>random_exp1</t>
   </si>
   <si>
     <t>random_exp2</t>
@@ -731,7 +699,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="1"/>
+        <family val="2"/>
       </rPr>
       <t>_list</t>
     </r>
@@ -804,7 +772,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <charset val="1"/>
+        <family val="2"/>
       </rPr>
       <t>_list</t>
     </r>
@@ -892,9 +860,6 @@
   </si>
   <si>
     <t>Reagent  BX3 (1) Preparation Duration</t>
-  </si>
-  <si>
-    <t>Reagent Extra Volume</t>
   </si>
   <si>
     <t>Reagent Preheat Temperature</t>
@@ -1145,11 +1110,35 @@
   <si>
     <t>Click here to open HC/LBL chemical data sheet</t>
   </si>
+  <si>
+    <t>[[2,3,1,7]]</t>
+  </si>
+  <si>
+    <t>[[500,500]]</t>
+  </si>
+  <si>
+    <t>Crank 0038 Testing</t>
+  </si>
+  <si>
+    <t>['GBL]</t>
+  </si>
+  <si>
+    <t>['PbI2','EtNH3I','GBL']</t>
+  </si>
+  <si>
+    <t>['EtNH3I','GBL']</t>
+  </si>
+  <si>
+    <t>['FAH']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperature of reagent during preparation ( °C ) </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1422,7 +1411,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="162">
+  <cellXfs count="163">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1905,6 +1894,10 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2287,11 +2280,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMK1024"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="92" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="G94" sqref="G94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -2315,14 +2308,14 @@
       </c>
       <c r="B1" s="145"/>
       <c r="C1" s="146" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="D1" s="147"/>
       <c r="E1" s="146" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="F1" s="148" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="G1" s="149" t="s">
         <v>5</v>
@@ -2383,7 +2376,7 @@
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="62" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D3" s="63" t="s">
         <v>2</v>
@@ -2395,7 +2388,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="G3" s="128" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H3" s="5"/>
       <c r="I3" s="6"/>
@@ -2427,14 +2420,14 @@
         <v>2</v>
       </c>
       <c r="E4" s="113" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="140" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="H4" s="154" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -2489,18 +2482,17 @@
       <c r="A6" s="14"/>
       <c r="B6" s="14"/>
       <c r="C6" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>2</v>
       </c>
       <c r="E6" s="126">
-        <f>SUM(E10,E15,fixed_wells)</f>
-        <v>3</v>
+        <v>96</v>
       </c>
       <c r="F6" s="11"/>
       <c r="G6" s="141" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="H6" s="13"/>
       <c r="I6" s="6"/>
@@ -2524,7 +2516,7 @@
     </row>
     <row r="7" spans="1:26" s="20" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="79" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="B7" s="15"/>
       <c r="C7" s="16"/>
@@ -2532,7 +2524,7 @@
       <c r="E7" s="115"/>
       <c r="F7" s="16"/>
       <c r="G7" s="130" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="H7" s="18"/>
       <c r="I7" s="19"/>
@@ -2558,19 +2550,19 @@
       <c r="A8" s="21"/>
       <c r="B8" s="21"/>
       <c r="C8" s="22" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="D8" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="116" t="s">
-        <v>115</v>
+      <c r="E8" s="117" t="s">
+        <v>267</v>
       </c>
       <c r="F8" s="22" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G8" s="142" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="H8" s="24"/>
       <c r="I8" s="25"/>
@@ -2596,19 +2588,19 @@
       <c r="A9" s="21"/>
       <c r="B9" s="21"/>
       <c r="C9" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D9" s="23" t="s">
         <v>2</v>
       </c>
       <c r="E9" s="117" t="s">
-        <v>130</v>
+        <v>268</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G9" s="142" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="H9" s="24"/>
       <c r="I9" s="25"/>
@@ -2634,13 +2626,13 @@
       <c r="A10" s="21"/>
       <c r="B10" s="21"/>
       <c r="C10" s="22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D10" s="23" t="s">
         <v>2</v>
       </c>
       <c r="E10" s="116">
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="F10" s="22">
         <v>12</v>
@@ -2672,13 +2664,13 @@
       <c r="A11" s="21"/>
       <c r="B11" s="21"/>
       <c r="C11" s="22" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="D11" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="116" t="s">
-        <v>139</v>
+      <c r="E11" s="117" t="s">
+        <v>269</v>
       </c>
       <c r="F11" s="22"/>
       <c r="G11" s="153"/>
@@ -2734,19 +2726,19 @@
       <c r="A13" s="77"/>
       <c r="B13" s="21"/>
       <c r="C13" s="22" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="D13" s="23" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="116" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G13" s="131" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="H13" s="24"/>
       <c r="I13" s="6"/>
@@ -2772,19 +2764,19 @@
       <c r="A14" s="77"/>
       <c r="B14" s="21"/>
       <c r="C14" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D14" s="23" t="s">
         <v>2</v>
       </c>
       <c r="E14" s="116" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="F14" s="22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G14" s="142" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="H14" s="24"/>
       <c r="I14" s="6"/>
@@ -2810,7 +2802,7 @@
       <c r="A15" s="77"/>
       <c r="B15" s="21"/>
       <c r="C15" s="22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D15" s="23" t="s">
         <v>2</v>
@@ -2848,13 +2840,13 @@
       <c r="A16" s="77"/>
       <c r="B16" s="21"/>
       <c r="C16" s="22" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="D16" s="23" t="s">
         <v>2</v>
       </c>
       <c r="E16" s="116" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="F16" s="26"/>
       <c r="G16" s="131"/>
@@ -2880,7 +2872,7 @@
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17" s="78" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="B17" s="28"/>
       <c r="C17" s="29"/>
@@ -2900,7 +2892,7 @@
         <v>2</v>
       </c>
       <c r="E18" s="119">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F18" s="32">
         <v>12</v>
@@ -2945,17 +2937,17 @@
         <v>29</v>
       </c>
       <c r="B20" s="70" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="C20" s="34"/>
       <c r="D20" s="35"/>
       <c r="E20" s="120"/>
       <c r="F20" s="34"/>
       <c r="G20" s="136" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="H20" s="143" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
@@ -2982,22 +2974,22 @@
         <v>1</v>
       </c>
       <c r="C21" s="72" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="D21" s="35" t="s">
         <v>2</v>
       </c>
       <c r="E21" s="121" t="s">
-        <v>129</v>
+        <v>270</v>
       </c>
       <c r="F21" s="75" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="G21" s="136" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="H21" s="144" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
@@ -3018,13 +3010,13 @@
       <c r="Y21" s="6"/>
       <c r="Z21" s="6"/>
     </row>
-    <row r="22" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A22" s="111" t="s">
         <v>29</v>
       </c>
       <c r="B22" s="68"/>
       <c r="C22" s="72" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="D22" s="35" t="s">
         <v>2</v>
@@ -3052,13 +3044,13 @@
       <c r="Y22" s="6"/>
       <c r="Z22" s="6"/>
     </row>
-    <row r="23" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A23" s="111" t="s">
         <v>29</v>
       </c>
       <c r="B23" s="68"/>
       <c r="C23" s="104" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="D23" s="35" t="s">
         <v>2</v>
@@ -3090,13 +3082,13 @@
       <c r="Y23" s="6"/>
       <c r="Z23" s="6"/>
     </row>
-    <row r="24" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A24" s="111" t="s">
         <v>29</v>
       </c>
       <c r="B24" s="68"/>
       <c r="C24" s="104" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="D24" s="35" t="s">
         <v>2</v>
@@ -3128,13 +3120,13 @@
       <c r="Y24" s="6"/>
       <c r="Z24" s="6"/>
     </row>
-    <row r="25" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A25" s="111" t="s">
         <v>29</v>
       </c>
       <c r="B25" s="68"/>
       <c r="C25" s="104" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="D25" s="105" t="s">
         <v>2</v>
@@ -3164,13 +3156,13 @@
       <c r="Y25" s="6"/>
       <c r="Z25" s="6"/>
     </row>
-    <row r="26" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A26" s="112" t="s">
         <v>29</v>
       </c>
       <c r="B26" s="68"/>
       <c r="C26" s="72" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="D26" s="35" t="s">
         <v>2</v>
@@ -3200,13 +3192,13 @@
       <c r="Y26" s="6"/>
       <c r="Z26" s="6"/>
     </row>
-    <row r="27" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A27" s="112" t="s">
         <v>29</v>
       </c>
       <c r="B27" s="68"/>
       <c r="C27" s="72" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="D27" s="35" t="s">
         <v>2</v>
@@ -3236,13 +3228,13 @@
       <c r="Y27" s="6"/>
       <c r="Z27" s="6"/>
     </row>
-    <row r="28" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A28" s="112" t="s">
         <v>29</v>
       </c>
       <c r="B28" s="68"/>
       <c r="C28" s="72" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="D28" s="35" t="s">
         <v>2</v>
@@ -3272,7 +3264,7 @@
       <c r="Y28" s="6"/>
       <c r="Z28" s="6"/>
     </row>
-    <row r="29" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:26" ht="18.75" customHeight="1" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A29" s="112"/>
       <c r="B29" s="68"/>
       <c r="C29" s="34"/>
@@ -3306,22 +3298,22 @@
         <v>2</v>
       </c>
       <c r="C30" s="127" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="D30" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="E30" s="123" t="s">
-        <v>117</v>
+      <c r="E30" s="162" t="s">
+        <v>271</v>
       </c>
       <c r="F30" s="104" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="G30" s="136" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="H30" s="108" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
@@ -3346,7 +3338,7 @@
       <c r="A31" s="110"/>
       <c r="B31" s="68"/>
       <c r="C31" s="104" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="D31" s="35" t="s">
         <v>2</v>
@@ -3358,7 +3350,7 @@
         <v>1.234</v>
       </c>
       <c r="G31" s="136" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="H31" s="36"/>
       <c r="I31" s="6"/>
@@ -3384,19 +3376,19 @@
       <c r="A32" s="110"/>
       <c r="B32" s="68"/>
       <c r="C32" s="104" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="D32" s="35" t="s">
         <v>2</v>
       </c>
       <c r="E32" s="123">
-        <v>1.2</v>
+        <v>3</v>
       </c>
       <c r="F32" s="34">
         <v>5.6779999999999999</v>
       </c>
       <c r="G32" s="136" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="H32" s="36"/>
       <c r="I32" s="6"/>
@@ -3418,13 +3410,13 @@
       <c r="Y32" s="6"/>
       <c r="Z32" s="6"/>
     </row>
-    <row r="33" spans="1:26" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:26" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A33" s="111" t="s">
         <v>29</v>
       </c>
       <c r="B33" s="68"/>
       <c r="C33" s="104" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="D33" s="105" t="s">
         <v>2</v>
@@ -3454,13 +3446,13 @@
       <c r="Y33" s="6"/>
       <c r="Z33" s="6"/>
     </row>
-    <row r="34" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A34" s="110" t="s">
         <v>29</v>
       </c>
       <c r="B34" s="69"/>
       <c r="C34" s="34" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="D34" s="43" t="s">
         <v>2</v>
@@ -3471,7 +3463,7 @@
         <v>35</v>
       </c>
       <c r="H34" s="144" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="I34" s="6"/>
       <c r="J34" s="6"/>
@@ -3492,13 +3484,13 @@
       <c r="Y34" s="6"/>
       <c r="Z34" s="6"/>
     </row>
-    <row r="35" spans="1:26" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:26" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A35" s="112" t="s">
         <v>29</v>
       </c>
       <c r="B35" s="68"/>
       <c r="C35" s="34" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="D35" s="35" t="s">
         <v>2</v>
@@ -3508,7 +3500,7 @@
         <v>75</v>
       </c>
       <c r="G35" s="136" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="H35" s="36" t="s">
         <v>43</v>
@@ -3532,13 +3524,13 @@
       <c r="Y35" s="6"/>
       <c r="Z35" s="6"/>
     </row>
-    <row r="36" spans="1:26" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:26" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A36" s="112" t="s">
         <v>29</v>
       </c>
       <c r="B36" s="68"/>
       <c r="C36" s="34" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="D36" s="35" t="s">
         <v>2</v>
@@ -3548,7 +3540,7 @@
         <v>450</v>
       </c>
       <c r="G36" s="136" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H36" s="36" t="s">
         <v>43</v>
@@ -3572,13 +3564,13 @@
       <c r="Y36" s="6"/>
       <c r="Z36" s="6"/>
     </row>
-    <row r="37" spans="1:26" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:26" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A37" s="112" t="s">
         <v>29</v>
       </c>
       <c r="B37" s="68"/>
       <c r="C37" s="34" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="D37" s="35" t="s">
         <v>2</v>
@@ -3588,7 +3580,7 @@
         <v>3600</v>
       </c>
       <c r="G37" s="136" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="H37" s="36" t="s">
         <v>43</v>
@@ -3612,7 +3604,7 @@
       <c r="Y37" s="6"/>
       <c r="Z37" s="6"/>
     </row>
-    <row r="38" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:26" ht="18" customHeight="1" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A38" s="112"/>
       <c r="B38" s="68"/>
       <c r="C38" s="34"/>
@@ -3646,19 +3638,19 @@
         <v>3</v>
       </c>
       <c r="C39" s="72" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="D39" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="E39" s="123" t="s">
-        <v>108</v>
+      <c r="E39" s="162" t="s">
+        <v>272</v>
       </c>
       <c r="F39" s="104" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="G39" s="136" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="H39" s="36"/>
       <c r="I39" s="6"/>
@@ -3684,19 +3676,19 @@
       <c r="A40" s="111"/>
       <c r="B40" s="68"/>
       <c r="C40" s="34" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="D40" s="35" t="s">
         <v>2</v>
       </c>
       <c r="E40" s="120">
-        <v>1.22</v>
+        <v>6</v>
       </c>
       <c r="F40" s="106">
         <v>1.234</v>
       </c>
       <c r="G40" s="136" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="H40" s="36"/>
       <c r="I40" s="6"/>
@@ -3718,11 +3710,13 @@
       <c r="Y40" s="6"/>
       <c r="Z40" s="6"/>
     </row>
-    <row r="41" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="111"/>
+    <row r="41" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="111" t="s">
+        <v>29</v>
+      </c>
       <c r="B41" s="68"/>
       <c r="C41" s="34" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="D41" s="35" t="s">
         <v>2</v>
@@ -3734,7 +3728,7 @@
         <v>5.6779999999999999</v>
       </c>
       <c r="G41" s="136" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="H41" s="36"/>
       <c r="I41" s="6"/>
@@ -3756,11 +3750,13 @@
       <c r="Y41" s="6"/>
       <c r="Z41" s="6"/>
     </row>
-    <row r="42" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="111"/>
+    <row r="42" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="111" t="s">
+        <v>29</v>
+      </c>
       <c r="B42" s="68"/>
       <c r="C42" s="34" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="D42" s="35" t="s">
         <v>2</v>
@@ -3772,7 +3768,7 @@
         <v>9.0120000000000005</v>
       </c>
       <c r="G42" s="136" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="H42" s="36"/>
       <c r="I42" s="6"/>
@@ -3794,13 +3790,13 @@
       <c r="Y42" s="6"/>
       <c r="Z42" s="6"/>
     </row>
-    <row r="43" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A43" s="110" t="s">
         <v>29</v>
       </c>
       <c r="B43" s="69"/>
       <c r="C43" s="72" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="D43" s="43" t="s">
         <v>2</v>
@@ -3832,13 +3828,13 @@
       <c r="Y43" s="6"/>
       <c r="Z43" s="6"/>
     </row>
-    <row r="44" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A44" s="110" t="s">
         <v>29</v>
       </c>
       <c r="B44" s="68"/>
       <c r="C44" s="34" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="D44" s="35" t="s">
         <v>2</v>
@@ -3872,13 +3868,13 @@
       <c r="Y44" s="6"/>
       <c r="Z44" s="6"/>
     </row>
-    <row r="45" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A45" s="110" t="s">
         <v>29</v>
       </c>
       <c r="B45" s="68"/>
       <c r="C45" s="34" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="D45" s="35" t="s">
         <v>2</v>
@@ -3912,13 +3908,13 @@
       <c r="Y45" s="6"/>
       <c r="Z45" s="6"/>
     </row>
-    <row r="46" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A46" s="110" t="s">
         <v>29</v>
       </c>
       <c r="B46" s="68"/>
       <c r="C46" s="34" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="D46" s="35" t="s">
         <v>2</v>
@@ -3952,7 +3948,7 @@
       <c r="Y46" s="6"/>
       <c r="Z46" s="6"/>
     </row>
-    <row r="47" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:26" ht="18.75" customHeight="1" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A47" s="112"/>
       <c r="B47" s="68"/>
       <c r="C47" s="34"/>
@@ -3988,19 +3984,19 @@
         <v>4</v>
       </c>
       <c r="C48" s="72" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="D48" s="35" t="s">
         <v>2</v>
       </c>
       <c r="E48" s="123" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F48" s="104" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="G48" s="136" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="H48" s="39"/>
       <c r="I48" s="6"/>
@@ -4028,7 +4024,7 @@
       </c>
       <c r="B49" s="68"/>
       <c r="C49" s="72" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="D49" s="43" t="s">
         <v>2</v>
@@ -4040,7 +4036,7 @@
         <v>1.234</v>
       </c>
       <c r="G49" s="136" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="H49" s="36"/>
       <c r="I49" s="6"/>
@@ -4068,7 +4064,7 @@
       </c>
       <c r="B50" s="68"/>
       <c r="C50" s="34" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="D50" s="43" t="s">
         <v>2</v>
@@ -4080,7 +4076,7 @@
         <v>5.6779999999999999</v>
       </c>
       <c r="G50" s="136" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="H50" s="36"/>
       <c r="I50" s="6"/>
@@ -4102,13 +4098,13 @@
       <c r="Y50" s="6"/>
       <c r="Z50" s="6"/>
     </row>
-    <row r="51" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A51" s="110" t="s">
         <v>29</v>
       </c>
       <c r="B51" s="68"/>
       <c r="C51" s="72" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="D51" s="43" t="s">
         <v>2</v>
@@ -4138,13 +4134,13 @@
       <c r="Y51" s="6"/>
       <c r="Z51" s="6"/>
     </row>
-    <row r="52" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A52" s="110" t="s">
         <v>29</v>
       </c>
       <c r="B52" s="69"/>
       <c r="C52" s="72" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="D52" s="43" t="s">
         <v>2</v>
@@ -4176,13 +4172,13 @@
       <c r="Y52" s="6"/>
       <c r="Z52" s="6"/>
     </row>
-    <row r="53" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A53" s="110" t="s">
         <v>29</v>
       </c>
       <c r="B53" s="68"/>
       <c r="C53" s="34" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="D53" s="43" t="s">
         <v>2</v>
@@ -4216,13 +4212,13 @@
       <c r="Y53" s="6"/>
       <c r="Z53" s="6"/>
     </row>
-    <row r="54" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A54" s="110" t="s">
         <v>29</v>
       </c>
       <c r="B54" s="68"/>
       <c r="C54" s="72" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="D54" s="43" t="s">
         <v>2</v>
@@ -4256,13 +4252,13 @@
       <c r="Y54" s="6"/>
       <c r="Z54" s="6"/>
     </row>
-    <row r="55" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A55" s="110" t="s">
         <v>29</v>
       </c>
       <c r="B55" s="68"/>
       <c r="C55" s="72" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="D55" s="43" t="s">
         <v>2</v>
@@ -4296,7 +4292,7 @@
       <c r="Y55" s="6"/>
       <c r="Z55" s="6"/>
     </row>
-    <row r="56" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:26" ht="18.75" customHeight="1" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A56" s="112"/>
       <c r="B56" s="68"/>
       <c r="C56" s="34"/>
@@ -4332,22 +4328,22 @@
         <v>5</v>
       </c>
       <c r="C57" s="72" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="D57" s="35" t="s">
         <v>2</v>
       </c>
       <c r="E57" s="123" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F57" s="104" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="G57" s="136" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="H57" s="108" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="I57" s="6"/>
       <c r="J57" s="6"/>
@@ -4374,7 +4370,7 @@
       </c>
       <c r="B58" s="69"/>
       <c r="C58" s="72" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="D58" s="35" t="s">
         <v>2</v>
@@ -4386,7 +4382,7 @@
         <v>1.234</v>
       </c>
       <c r="G58" s="136" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="H58" s="44"/>
       <c r="I58" s="6"/>
@@ -4408,13 +4404,13 @@
       <c r="Y58" s="6"/>
       <c r="Z58" s="6"/>
     </row>
-    <row r="59" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A59" s="111" t="s">
         <v>29</v>
       </c>
       <c r="B59" s="69"/>
       <c r="C59" s="34" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="D59" s="35" t="s">
         <v>2</v>
@@ -4426,7 +4422,7 @@
         <v>5.6779999999999999</v>
       </c>
       <c r="G59" s="136" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="H59" s="44"/>
       <c r="I59" s="6"/>
@@ -4448,13 +4444,13 @@
       <c r="Y59" s="6"/>
       <c r="Z59" s="6"/>
     </row>
-    <row r="60" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A60" s="111" t="s">
         <v>29</v>
       </c>
       <c r="B60" s="69"/>
       <c r="C60" s="34" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="D60" s="35" t="s">
         <v>2</v>
@@ -4466,7 +4462,7 @@
         <v>9.0120000000000005</v>
       </c>
       <c r="G60" s="136" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="H60" s="39"/>
       <c r="I60" s="6"/>
@@ -4488,13 +4484,13 @@
       <c r="Y60" s="6"/>
       <c r="Z60" s="6"/>
     </row>
-    <row r="61" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A61" s="110" t="s">
         <v>29</v>
       </c>
       <c r="B61" s="69"/>
       <c r="C61" s="75" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="D61" s="43" t="s">
         <v>2</v>
@@ -4526,13 +4522,13 @@
       <c r="Y61" s="6"/>
       <c r="Z61" s="6"/>
     </row>
-    <row r="62" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A62" s="110" t="s">
         <v>29</v>
       </c>
       <c r="B62" s="69"/>
       <c r="C62" s="34" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="D62" s="35" t="s">
         <v>2</v>
@@ -4566,13 +4562,13 @@
       <c r="Y62" s="6"/>
       <c r="Z62" s="6"/>
     </row>
-    <row r="63" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A63" s="110" t="s">
         <v>29</v>
       </c>
       <c r="B63" s="69"/>
       <c r="C63" s="72" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
       <c r="D63" s="35" t="s">
         <v>2</v>
@@ -4606,13 +4602,13 @@
       <c r="Y63" s="6"/>
       <c r="Z63" s="6"/>
     </row>
-    <row r="64" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A64" s="110" t="s">
         <v>29</v>
       </c>
       <c r="B64" s="69"/>
       <c r="C64" s="72" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="D64" s="35" t="s">
         <v>2</v>
@@ -4646,7 +4642,7 @@
       <c r="Y64" s="6"/>
       <c r="Z64" s="6"/>
     </row>
-    <row r="65" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:26" ht="18.75" customHeight="1" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A65" s="112"/>
       <c r="B65" s="68"/>
       <c r="C65" s="34"/>
@@ -4682,19 +4678,19 @@
         <v>6</v>
       </c>
       <c r="C66" s="72" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="D66" s="35" t="s">
         <v>2</v>
       </c>
       <c r="E66" s="123" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F66" s="104" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="G66" s="136" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="H66" s="36"/>
       <c r="I66" s="6"/>
@@ -4722,7 +4718,7 @@
       </c>
       <c r="B67" s="68"/>
       <c r="C67" s="34" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="D67" s="35" t="s">
         <v>2</v>
@@ -4734,7 +4730,7 @@
         <v>1.234</v>
       </c>
       <c r="G67" s="136" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
       <c r="H67" s="36"/>
       <c r="I67" s="6"/>
@@ -4762,7 +4758,7 @@
       </c>
       <c r="B68" s="68"/>
       <c r="C68" s="72" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
       <c r="D68" s="35" t="s">
         <v>2</v>
@@ -4774,7 +4770,7 @@
         <v>5.6779999999999999</v>
       </c>
       <c r="G68" s="136" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="H68" s="36"/>
       <c r="I68" s="6"/>
@@ -4796,13 +4792,13 @@
       <c r="Y68" s="6"/>
       <c r="Z68" s="6"/>
     </row>
-    <row r="69" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A69" s="109" t="s">
         <v>29</v>
       </c>
       <c r="B69" s="68"/>
       <c r="C69" s="72" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="D69" s="35" t="s">
         <v>2</v>
@@ -4832,13 +4828,13 @@
       <c r="Y69" s="6"/>
       <c r="Z69" s="6"/>
     </row>
-    <row r="70" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A70" s="112" t="s">
         <v>29</v>
       </c>
       <c r="B70" s="68"/>
       <c r="C70" s="75" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
       <c r="D70" s="35" t="s">
         <v>2</v>
@@ -4868,13 +4864,13 @@
       <c r="Y70" s="6"/>
       <c r="Z70" s="6"/>
     </row>
-    <row r="71" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A71" s="109" t="s">
         <v>29</v>
       </c>
       <c r="B71" s="68"/>
       <c r="C71" s="72" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
       <c r="D71" s="35" t="s">
         <v>2</v>
@@ -4906,13 +4902,13 @@
       <c r="Y71" s="6"/>
       <c r="Z71" s="6"/>
     </row>
-    <row r="72" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A72" s="109" t="s">
         <v>29</v>
       </c>
       <c r="B72" s="68"/>
       <c r="C72" s="72" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
       <c r="D72" s="35" t="s">
         <v>2</v>
@@ -4944,13 +4940,13 @@
       <c r="Y72" s="6"/>
       <c r="Z72" s="6"/>
     </row>
-    <row r="73" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A73" s="109" t="s">
         <v>29</v>
       </c>
       <c r="B73" s="68"/>
       <c r="C73" s="72" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
       <c r="D73" s="35" t="s">
         <v>2</v>
@@ -4982,7 +4978,7 @@
       <c r="Y73" s="6"/>
       <c r="Z73" s="6"/>
     </row>
-    <row r="74" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:26" ht="18.75" customHeight="1" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A74" s="112"/>
       <c r="B74" s="68"/>
       <c r="C74" s="34"/>
@@ -5011,26 +5007,24 @@
       <c r="Z74" s="6"/>
     </row>
     <row r="75" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="109" t="s">
-        <v>29</v>
-      </c>
+      <c r="A75" s="109"/>
       <c r="B75" s="68">
         <v>7</v>
       </c>
       <c r="C75" s="72" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="D75" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="E75" s="123" t="s">
-        <v>117</v>
+      <c r="E75" s="162" t="s">
+        <v>273</v>
       </c>
       <c r="F75" s="104" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="G75" s="136" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
       <c r="H75" s="36"/>
       <c r="I75" s="6"/>
@@ -5052,13 +5046,13 @@
       <c r="Y75" s="6"/>
       <c r="Z75" s="6"/>
     </row>
-    <row r="76" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A76" s="109" t="s">
         <v>29</v>
       </c>
       <c r="B76" s="68"/>
       <c r="C76" s="34" t="s">
-        <v>266</v>
+        <v>254</v>
       </c>
       <c r="D76" s="66" t="s">
         <v>2</v>
@@ -5070,7 +5064,7 @@
         <v>1.234</v>
       </c>
       <c r="G76" s="136" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="H76" s="36"/>
       <c r="I76" s="6"/>
@@ -5092,13 +5086,13 @@
       <c r="Y76" s="6"/>
       <c r="Z76" s="6"/>
     </row>
-    <row r="77" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A77" s="109" t="s">
         <v>29</v>
       </c>
       <c r="B77" s="68"/>
       <c r="C77" s="72" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="D77" s="66" t="s">
         <v>2</v>
@@ -5110,7 +5104,7 @@
         <v>5.6779999999999999</v>
       </c>
       <c r="G77" s="136" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
       <c r="H77" s="36"/>
       <c r="I77" s="6"/>
@@ -5132,14 +5126,14 @@
       <c r="Y77" s="6"/>
       <c r="Z77" s="6"/>
     </row>
-    <row r="78" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A78" s="112" t="str">
         <f t="shared" ref="A78" si="0">A77</f>
         <v>#</v>
       </c>
       <c r="B78" s="68"/>
       <c r="C78" s="72" t="s">
-        <v>270</v>
+        <v>258</v>
       </c>
       <c r="D78" s="66" t="s">
         <v>2</v>
@@ -5169,13 +5163,13 @@
       <c r="Y78" s="6"/>
       <c r="Z78" s="6"/>
     </row>
-    <row r="79" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A79" s="109" t="s">
         <v>29</v>
       </c>
       <c r="B79" s="68"/>
       <c r="C79" s="72" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
       <c r="D79" s="66" t="s">
         <v>2</v>
@@ -5205,13 +5199,13 @@
       <c r="Y79" s="6"/>
       <c r="Z79" s="6"/>
     </row>
-    <row r="80" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A80" s="109" t="s">
         <v>29</v>
       </c>
       <c r="B80" s="68"/>
       <c r="C80" s="72" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="D80" s="66" t="s">
         <v>2</v>
@@ -5243,13 +5237,13 @@
       <c r="Y80" s="6"/>
       <c r="Z80" s="6"/>
     </row>
-    <row r="81" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A81" s="109" t="s">
         <v>29</v>
       </c>
       <c r="B81" s="68"/>
       <c r="C81" s="72" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="D81" s="66" t="s">
         <v>2</v>
@@ -5281,13 +5275,13 @@
       <c r="Y81" s="6"/>
       <c r="Z81" s="6"/>
     </row>
-    <row r="82" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A82" s="109" t="s">
         <v>29</v>
       </c>
       <c r="B82" s="68"/>
       <c r="C82" s="72" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="D82" s="66" t="s">
         <v>2</v>
@@ -5319,9 +5313,9 @@
       <c r="Y82" s="6"/>
       <c r="Z82" s="6"/>
     </row>
-    <row r="83" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:26" ht="18.75" customHeight="1" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A83" s="67" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B83" s="67"/>
       <c r="C83" s="47"/>
@@ -5353,7 +5347,7 @@
       <c r="A84" s="50"/>
       <c r="B84" s="50"/>
       <c r="C84" s="47" t="s">
-        <v>118</v>
+        <v>70</v>
       </c>
       <c r="D84" s="48" t="s">
         <v>2</v>
@@ -5391,7 +5385,7 @@
       <c r="A85" s="50"/>
       <c r="B85" s="50"/>
       <c r="C85" s="47" t="s">
-        <v>120</v>
+        <v>72</v>
       </c>
       <c r="D85" s="48" t="s">
         <v>2</v>
@@ -5429,7 +5423,7 @@
       <c r="A86" s="50"/>
       <c r="B86" s="50"/>
       <c r="C86" s="47" t="s">
-        <v>119</v>
+        <v>74</v>
       </c>
       <c r="D86" s="48" t="s">
         <v>2</v>
@@ -5467,7 +5461,7 @@
       <c r="A87" s="50"/>
       <c r="B87" s="50"/>
       <c r="C87" s="47" t="s">
-        <v>121</v>
+        <v>76</v>
       </c>
       <c r="D87" s="48" t="s">
         <v>2</v>
@@ -5505,7 +5499,7 @@
       <c r="A88" s="50"/>
       <c r="B88" s="50"/>
       <c r="C88" s="47" t="s">
-        <v>122</v>
+        <v>78</v>
       </c>
       <c r="D88" s="48" t="s">
         <v>2</v>
@@ -5545,7 +5539,7 @@
       <c r="A89" s="50"/>
       <c r="B89" s="50"/>
       <c r="C89" s="47" t="s">
-        <v>123</v>
+        <v>81</v>
       </c>
       <c r="D89" s="48" t="s">
         <v>2</v>
@@ -5585,7 +5579,7 @@
       <c r="A90" s="50"/>
       <c r="B90" s="50"/>
       <c r="C90" s="47" t="s">
-        <v>195</v>
+        <v>84</v>
       </c>
       <c r="D90" s="48" t="s">
         <v>2</v>
@@ -5623,17 +5617,17 @@
     </row>
     <row r="91" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="51" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="B91" s="51"/>
       <c r="C91" s="52" t="s">
-        <v>125</v>
+        <v>87</v>
       </c>
       <c r="D91" s="53" t="s">
         <v>2</v>
       </c>
       <c r="E91" s="125" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
       <c r="F91" s="52"/>
       <c r="G91" s="138" t="s">
@@ -5663,7 +5657,7 @@
     </row>
     <row r="92" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="67" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
       <c r="B92" s="67"/>
       <c r="C92" s="47"/>
@@ -5695,7 +5689,7 @@
       <c r="A93" s="50"/>
       <c r="B93" s="50"/>
       <c r="C93" s="74" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="D93" s="48" t="s">
         <v>2</v>
@@ -5707,7 +5701,7 @@
         <v>45</v>
       </c>
       <c r="G93" s="139" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="H93" s="49" t="s">
         <v>92</v>
@@ -5735,7 +5729,7 @@
       <c r="A94" s="50"/>
       <c r="B94" s="50"/>
       <c r="C94" s="47" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="D94" s="48" t="s">
         <v>2</v>
@@ -5746,8 +5740,8 @@
       <c r="F94" s="47">
         <v>75</v>
       </c>
-      <c r="G94" s="137" t="s">
-        <v>94</v>
+      <c r="G94" s="139" t="s">
+        <v>274</v>
       </c>
       <c r="H94" s="49" t="s">
         <v>92</v>
@@ -5775,7 +5769,7 @@
       <c r="A95" s="50"/>
       <c r="B95" s="50"/>
       <c r="C95" s="47" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="D95" s="48" t="s">
         <v>2</v>
@@ -5787,7 +5781,7 @@
         <v>450</v>
       </c>
       <c r="G95" s="137" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H95" s="49" t="s">
         <v>92</v>
@@ -5815,7 +5809,7 @@
       <c r="A96" s="51"/>
       <c r="B96" s="51"/>
       <c r="C96" s="52" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="D96" s="53" t="s">
         <v>2</v>
@@ -5827,7 +5821,7 @@
         <v>3600</v>
       </c>
       <c r="G96" s="138" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H96" s="54" t="s">
         <v>92</v>
@@ -15052,20 +15046,20 @@
     <row r="1024" spans="1:8" x14ac:dyDescent="0.2"/>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation allowBlank="1" errorTitle="WellCountError" error="Global wellcount should be sum of random_wellcount and fixed_wells" sqref="E6"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4">
+    <dataValidation allowBlank="1" errorTitle="WellCountError" error="Global wellcount should be sum of random_wellcount and fixed_wells" sqref="E6" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"MIT_PVLab, HC, LBL, dev"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Please Check" prompt="Ensure that `ID` AND specify `Chemical list` for the same precursor, reagent, or dopant." sqref="A22"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Activated vs Deactivated" prompt="Rows WITH `#` are &quot;deactivated&quot; and won't be read.  All other rows will be read by ESCALATE." sqref="A20"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Please Check" prompt="Ensure that `ID` AND specify `Chemical list` for the same precursor, reagent, or dopant." sqref="A22" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Activated vs Deactivated" prompt="Rows WITH `#` are &quot;deactivated&quot; and won't be read.  All other rows will be read by ESCALATE." sqref="A20" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="C18" location="'Manual Experiment Interface'!B2" display="Manual Experiments"/>
-    <hyperlink ref="H20" r:id="rId1"/>
-    <hyperlink ref="H21" r:id="rId2"/>
-    <hyperlink ref="H34" r:id="rId3"/>
-    <hyperlink ref="H43" r:id="rId4"/>
-    <hyperlink ref="H52" r:id="rId5"/>
+    <hyperlink ref="C18" location="'Manual Experiment Interface'!B2" display="Manual Experiments" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="H20" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="H21" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="H34" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="H43" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="H52" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
@@ -15073,7 +15067,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:XFC500"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15094,46 +15088,46 @@
   <sheetData>
     <row r="1" spans="1:11" s="80" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="155" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="155" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" s="155" t="s">
         <v>99</v>
       </c>
-      <c r="B1" s="155" t="s">
-        <v>132</v>
-      </c>
-      <c r="C1" s="155" t="s">
+      <c r="D1" s="155" t="s">
         <v>100</v>
       </c>
-      <c r="D1" s="155" t="s">
+      <c r="E1" s="155" t="s">
         <v>101</v>
       </c>
-      <c r="E1" s="155" t="s">
+      <c r="F1" s="155" t="s">
         <v>102</v>
       </c>
-      <c r="F1" s="155" t="s">
+      <c r="G1" s="155" t="s">
         <v>103</v>
       </c>
-      <c r="G1" s="155" t="s">
+      <c r="H1" s="155" t="s">
         <v>104</v>
       </c>
-      <c r="H1" s="155" t="s">
+      <c r="I1" s="155" t="s">
         <v>105</v>
       </c>
-      <c r="I1" s="155" t="s">
-        <v>106</v>
-      </c>
       <c r="J1" s="156" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="K1" s="157" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="158">
+      <c r="A2" s="158" t="str">
         <f>IF(manual_wells &gt; 0, 1, "")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="B2" s="159" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="C2" s="156">
         <v>150</v>
@@ -15159,18 +15153,18 @@
       <c r="J2" s="156">
         <v>0</v>
       </c>
-      <c r="K2" s="157">
+      <c r="K2" s="157" t="str">
         <f>IF(NOT(A2=""), SUM(C2:J2), "")</f>
-        <v>210</v>
+        <v/>
       </c>
     </row>
     <row r="3" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="158">
+      <c r="A3" s="158" t="str">
         <f>IF(A2 &lt; fixed_wells, A2 + 1, "")</f>
-        <v>2</v>
+        <v/>
       </c>
       <c r="B3" s="159" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="C3" s="156">
         <v>150</v>
@@ -15196,18 +15190,18 @@
       <c r="J3" s="156">
         <v>0</v>
       </c>
-      <c r="K3" s="157">
+      <c r="K3" s="157" t="str">
         <f t="shared" ref="K3:K66" si="0">IF(NOT(A3=""), SUM(C3:J3), "")</f>
-        <v>215</v>
+        <v/>
       </c>
     </row>
     <row r="4" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="158">
+      <c r="A4" s="158" t="str">
         <f t="shared" ref="A4:A34" si="1">IF(A3 &lt; fixed_wells, A3 + 1, "")</f>
-        <v>3</v>
+        <v/>
       </c>
       <c r="B4" s="159" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="C4" s="156">
         <v>150</v>
@@ -15233,9 +15227,9 @@
       <c r="J4" s="156">
         <v>0</v>
       </c>
-      <c r="K4" s="157">
+      <c r="K4" s="157" t="str">
         <f t="shared" si="0"/>
-        <v>215</v>
+        <v/>
       </c>
     </row>
     <row r="5" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.2">
@@ -22232,7 +22226,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K98"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -22246,43 +22240,43 @@
   <sheetData>
     <row r="1" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="60" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="60" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1" s="60" t="s">
         <v>99</v>
       </c>
-      <c r="B1" s="60" t="s">
-        <v>132</v>
-      </c>
-      <c r="C1" s="60" t="s">
+      <c r="D1" s="60" t="s">
         <v>100</v>
       </c>
-      <c r="D1" s="60" t="s">
+      <c r="E1" s="60" t="s">
         <v>101</v>
       </c>
-      <c r="E1" s="60" t="s">
+      <c r="F1" s="60" t="s">
         <v>102</v>
       </c>
-      <c r="F1" s="60" t="s">
+      <c r="G1" s="60" t="s">
         <v>103</v>
       </c>
-      <c r="G1" s="60" t="s">
+      <c r="H1" s="60" t="s">
         <v>104</v>
       </c>
-      <c r="H1" s="60" t="s">
+      <c r="I1" s="60" t="s">
         <v>105</v>
       </c>
-      <c r="I1" s="60" t="s">
-        <v>106</v>
-      </c>
       <c r="J1" s="60" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="K1" s="61" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="A2" t="str">
         <f>IF(NOT('Manual Experiment Interface'!A2=""),'Manual Experiment Interface'!A2,"")</f>
-        <v>1</v>
+        <v/>
       </c>
       <c r="B2" t="str">
         <f>IF(NOT('Manual Experiment Interface'!B2=""),'Manual Experiment Interface'!B2,"")</f>
@@ -22320,15 +22314,15 @@
         <f>IF(NOT('Manual Experiment Interface'!J2=""),'Manual Experiment Interface'!J2,"")</f>
         <v>0</v>
       </c>
-      <c r="K2">
+      <c r="K2" t="str">
         <f>IF(NOT('Manual Experiment Interface'!K2=""),'Manual Experiment Interface'!K2,"")</f>
-        <v>210</v>
+        <v/>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="A3" t="str">
         <f>IF(NOT('Manual Experiment Interface'!A3=""),'Manual Experiment Interface'!A3,"")</f>
-        <v>2</v>
+        <v/>
       </c>
       <c r="B3" t="str">
         <f>IF(NOT('Manual Experiment Interface'!B3=""),'Manual Experiment Interface'!B3,"")</f>
@@ -22366,15 +22360,15 @@
         <f>IF(NOT('Manual Experiment Interface'!J3=""),'Manual Experiment Interface'!J3,"")</f>
         <v>0</v>
       </c>
-      <c r="K3">
+      <c r="K3" t="str">
         <f>IF(NOT('Manual Experiment Interface'!K3=""),'Manual Experiment Interface'!K3,"")</f>
-        <v>215</v>
+        <v/>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="A4" t="str">
         <f>IF(NOT('Manual Experiment Interface'!A4=""),'Manual Experiment Interface'!A4,"")</f>
-        <v>3</v>
+        <v/>
       </c>
       <c r="B4" t="str">
         <f>IF(NOT('Manual Experiment Interface'!B4=""),'Manual Experiment Interface'!B4,"")</f>
@@ -22412,9 +22406,9 @@
         <f>IF(NOT('Manual Experiment Interface'!J4=""),'Manual Experiment Interface'!J4,"")</f>
         <v>0</v>
       </c>
-      <c r="K4">
+      <c r="K4" t="str">
         <f>IF(NOT('Manual Experiment Interface'!K4=""),'Manual Experiment Interface'!K4,"")</f>
-        <v>215</v>
+        <v/>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -26747,11 +26741,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:W1021"/>
   <sheetViews>
-    <sheetView topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="B97" sqref="B97"/>
+    <sheetView topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="B90" sqref="B90:B97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -26965,7 +26959,7 @@
       </c>
       <c r="D7" s="11">
         <f>'User Interface'!wellcount</f>
-        <v>3</v>
+        <v>96</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>11</v>
@@ -27029,7 +27023,7 @@
       </c>
       <c r="D9" s="95" t="str">
         <f>'User Interface'!E8</f>
-        <v>[[2,3,1]]</v>
+        <v>[[2,3,1,7]]</v>
       </c>
       <c r="E9" s="95" t="s">
         <v>18</v>
@@ -27066,7 +27060,7 @@
       </c>
       <c r="D10" s="95" t="str">
         <f>'User Interface'!E9</f>
-        <v>[[215,215]]</v>
+        <v>[[500,500]]</v>
       </c>
       <c r="E10" s="95" t="s">
         <v>18</v>
@@ -27103,7 +27097,7 @@
       </c>
       <c r="D11" s="95">
         <f>'User Interface'!E10</f>
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="E11" s="95" t="s">
         <v>11</v>
@@ -27133,14 +27127,14 @@
         <v>0</v>
       </c>
       <c r="B12" s="95" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="C12" s="96" t="s">
         <v>2</v>
       </c>
       <c r="D12" s="95" t="str">
         <f>'User Interface'!E11</f>
-        <v>random_exp1</v>
+        <v>Crank 0038 Testing</v>
       </c>
       <c r="E12" s="95"/>
       <c r="F12" s="92"/>
@@ -27279,7 +27273,7 @@
         <v>0</v>
       </c>
       <c r="B16" s="95" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="C16" s="96" t="s">
         <v>2</v>
@@ -27325,7 +27319,7 @@
       <c r="C18" s="98"/>
       <c r="D18" s="95">
         <f>'User Interface'!E18</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E18" s="98" t="s">
         <v>11</v>
@@ -27543,7 +27537,7 @@
       </c>
       <c r="D26" s="40" t="str">
         <f>'User Interface'!E21</f>
-        <v>['CBz']</v>
+        <v>['GBL]</v>
       </c>
       <c r="E26" s="34" t="s">
         <v>18</v>
@@ -27610,7 +27604,7 @@
         <v>#</v>
       </c>
       <c r="B28" s="72" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="C28" s="35" t="s">
         <v>2</v>
@@ -27647,7 +27641,7 @@
         <v>#</v>
       </c>
       <c r="B29" s="72" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="C29" s="35" t="s">
         <v>2</v>
@@ -27684,7 +27678,7 @@
         <v>#</v>
       </c>
       <c r="B30" s="72" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="C30" s="35" t="s">
         <v>2</v>
@@ -27721,7 +27715,7 @@
         <v>#</v>
       </c>
       <c r="B31" s="72" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="C31" s="35" t="s">
         <v>2</v>
@@ -27758,7 +27752,7 @@
         <v>#</v>
       </c>
       <c r="B32" s="72" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="C32" s="35" t="s">
         <v>2</v>
@@ -27795,7 +27789,7 @@
         <v>#</v>
       </c>
       <c r="B33" s="72" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="C33" s="35" t="s">
         <v>2</v>
@@ -27864,7 +27858,7 @@
       </c>
       <c r="D35" s="34" t="str">
         <f>'User Interface'!E30</f>
-        <v>['PbI2','DMSO','DMF']</v>
+        <v>['PbI2','EtNH3I','GBL']</v>
       </c>
       <c r="E35" s="34" t="s">
         <v>18</v>
@@ -27975,7 +27969,7 @@
       </c>
       <c r="D38" s="40">
         <f>'User Interface'!E32</f>
-        <v>1.2</v>
+        <v>3</v>
       </c>
       <c r="E38" s="34" t="s">
         <v>9</v>
@@ -28005,7 +27999,7 @@
         <v>#</v>
       </c>
       <c r="B39" s="72" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C39" s="35" t="s">
         <v>2</v>
@@ -28185,7 +28179,7 @@
       </c>
       <c r="D44" s="34" t="str">
         <f>'User Interface'!E39</f>
-        <v>['MeNH3I','PbI2','DMSO', 'DMF']</v>
+        <v>['EtNH3I','GBL']</v>
       </c>
       <c r="E44" s="34" t="s">
         <v>18</v>
@@ -28259,7 +28253,7 @@
       </c>
       <c r="D46" s="34">
         <f>'User Interface'!E40</f>
-        <v>1.22</v>
+        <v>6</v>
       </c>
       <c r="E46" s="34" t="s">
         <v>9</v>
@@ -28284,12 +28278,12 @@
       <c r="W46" s="85"/>
     </row>
     <row r="47" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="37">
+      <c r="A47" s="37" t="str">
         <f>'User Interface'!A41</f>
-        <v>0</v>
+        <v>#</v>
       </c>
       <c r="B47" s="72" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="C47" s="35" t="s">
         <v>2</v>
@@ -28321,12 +28315,12 @@
       <c r="W47" s="85"/>
     </row>
     <row r="48" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="37">
+      <c r="A48" s="37" t="str">
         <f>'User Interface'!A42</f>
-        <v>0</v>
+        <v>#</v>
       </c>
       <c r="B48" s="72" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C48" s="35" t="s">
         <v>2</v>
@@ -28647,7 +28641,7 @@
         <v>#</v>
       </c>
       <c r="B57" s="72" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="C57" s="35" t="s">
         <v>2</v>
@@ -28931,7 +28925,7 @@
         <v>#</v>
       </c>
       <c r="B65" s="107" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="C65" s="35" t="s">
         <v>2</v>
@@ -28968,7 +28962,7 @@
         <v>#</v>
       </c>
       <c r="B66" s="72" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="C66" s="35" t="s">
         <v>2</v>
@@ -29141,7 +29135,7 @@
         <v>#</v>
       </c>
       <c r="B71" s="72" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="C71" s="35" t="s">
         <v>2</v>
@@ -29215,7 +29209,7 @@
         <v>#</v>
       </c>
       <c r="B73" s="107" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="C73" s="35" t="s">
         <v>2</v>
@@ -29252,7 +29246,7 @@
         <v>#</v>
       </c>
       <c r="B74" s="107" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="C74" s="35" t="s">
         <v>2</v>
@@ -29289,7 +29283,7 @@
         <v>#</v>
       </c>
       <c r="B75" s="72" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="C75" s="35" t="s">
         <v>2</v>
@@ -29326,7 +29320,7 @@
         <v>#</v>
       </c>
       <c r="B76" s="72" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="C76" s="35" t="s">
         <v>2</v>
@@ -29363,7 +29357,7 @@
         <v>#</v>
       </c>
       <c r="B77" s="72" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="C77" s="35" t="s">
         <v>2</v>
@@ -29400,7 +29394,7 @@
         <v>#</v>
       </c>
       <c r="B78" s="72" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="C78" s="35" t="s">
         <v>2</v>
@@ -29457,19 +29451,19 @@
       <c r="W79" s="85"/>
     </row>
     <row r="80" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="37" t="str">
+      <c r="A80" s="37">
         <f>'User Interface'!A75</f>
-        <v>#</v>
+        <v>0</v>
       </c>
       <c r="B80" s="72" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="C80" s="35" t="s">
         <v>2</v>
       </c>
       <c r="D80" s="34" t="str">
         <f>'User Interface'!E75</f>
-        <v>['PbI2','DMSO','DMF']</v>
+        <v>['FAH']</v>
       </c>
       <c r="E80" s="34" t="s">
         <v>18</v>
@@ -29536,7 +29530,7 @@
         <v>#</v>
       </c>
       <c r="B82" s="107" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="C82" s="35" t="s">
         <v>2</v>
@@ -29573,7 +29567,7 @@
         <v>#</v>
       </c>
       <c r="B83" s="107" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="C83" s="35" t="s">
         <v>2</v>
@@ -29610,7 +29604,7 @@
         <v>#</v>
       </c>
       <c r="B84" s="72" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="C84" s="35" t="s">
         <v>2</v>
@@ -29647,7 +29641,7 @@
         <v>#</v>
       </c>
       <c r="B85" s="72" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="C85" s="35" t="s">
         <v>2</v>
@@ -29684,7 +29678,7 @@
         <v>#</v>
       </c>
       <c r="B86" s="72" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="C86" s="35" t="s">
         <v>2</v>
@@ -29721,7 +29715,7 @@
         <v>#</v>
       </c>
       <c r="B87" s="72" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="C87" s="35" t="s">
         <v>2</v>
@@ -30174,7 +30168,7 @@
     <row r="101" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="50"/>
       <c r="B101" s="47" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C101" s="48" t="s">
         <v>2</v>
@@ -30208,7 +30202,7 @@
     <row r="102" spans="1:23" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="50"/>
       <c r="B102" s="99" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C102" s="100" t="s">
         <v>2</v>
@@ -36674,7 +36668,7 @@
     </row>
   </sheetData>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" errorTitle="WellCountError" error="Global wellcount should be sum of random_wellcount and fixed_wells" promptTitle="wellcount" prompt="MUST be sum of random_wellcount and fixed_wells" sqref="D7">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" errorTitle="WellCountError" error="Global wellcount should be sum of random_wellcount and fixed_wells" promptTitle="wellcount" prompt="MUST be sum of random_wellcount and fixed_wells" sqref="D7" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>SUM(#REF!,D18)</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
final small tweaks to interface
</commit_message>
<xml_diff>
--- a/HC_LBL_SpecificationInterface.xlsx
+++ b/HC_LBL_SpecificationInterface.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ipendleton/Dropbox/Desktop/ESCALATE/ESCALATE_Capture/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCC709FE-7832-8242-99C1-6BBBF21974C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F982A7-E8DF-014E-90D4-8D7723F0302D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12800" yWindow="460" windowWidth="38400" windowHeight="21600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -829,9 +829,6 @@
     <t>Min and Max volume for expeirment 1</t>
   </si>
   <si>
-    <t>HC</t>
-  </si>
-  <si>
     <t xml:space="preserve">Combination of Reagents in experiment. </t>
   </si>
   <si>
@@ -1120,9 +1117,6 @@
     <t>Crank 0038 Testing</t>
   </si>
   <si>
-    <t>['GBL]</t>
-  </si>
-  <si>
     <t>['PbI2','EtNH3I','GBL']</t>
   </si>
   <si>
@@ -1133,6 +1127,12 @@
   </si>
   <si>
     <t xml:space="preserve">Temperature of reagent during preparation ( °C ) </t>
+  </si>
+  <si>
+    <t>LBL</t>
+  </si>
+  <si>
+    <t>['GBL']</t>
   </si>
 </sst>
 </file>
@@ -2283,8 +2283,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMK1024"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="92" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="G94" sqref="G94"/>
+    <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -2420,7 +2420,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="113" t="s">
-        <v>173</v>
+        <v>273</v>
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="140" t="s">
@@ -2524,7 +2524,7 @@
       <c r="E7" s="115"/>
       <c r="F7" s="16"/>
       <c r="G7" s="130" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H7" s="18"/>
       <c r="I7" s="19"/>
@@ -2550,19 +2550,19 @@
       <c r="A8" s="21"/>
       <c r="B8" s="21"/>
       <c r="C8" s="22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D8" s="23" t="s">
         <v>2</v>
       </c>
       <c r="E8" s="117" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F8" s="22" t="s">
         <v>114</v>
       </c>
       <c r="G8" s="142" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H8" s="24"/>
       <c r="I8" s="25"/>
@@ -2594,7 +2594,7 @@
         <v>2</v>
       </c>
       <c r="E9" s="117" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F9" s="22" t="s">
         <v>113</v>
@@ -2670,7 +2670,7 @@
         <v>2</v>
       </c>
       <c r="E11" s="117" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F11" s="22"/>
       <c r="G11" s="153"/>
@@ -2726,7 +2726,7 @@
       <c r="A13" s="77"/>
       <c r="B13" s="21"/>
       <c r="C13" s="22" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D13" s="23" t="s">
         <v>2</v>
@@ -2738,7 +2738,7 @@
         <v>114</v>
       </c>
       <c r="G13" s="131" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H13" s="24"/>
       <c r="I13" s="6"/>
@@ -2937,17 +2937,17 @@
         <v>29</v>
       </c>
       <c r="B20" s="70" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C20" s="34"/>
       <c r="D20" s="35"/>
       <c r="E20" s="120"/>
       <c r="F20" s="34"/>
       <c r="G20" s="136" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H20" s="143" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
@@ -2974,13 +2974,13 @@
         <v>1</v>
       </c>
       <c r="C21" s="72" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D21" s="35" t="s">
         <v>2</v>
       </c>
       <c r="E21" s="121" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="F21" s="75" t="s">
         <v>134</v>
@@ -3016,7 +3016,7 @@
       </c>
       <c r="B22" s="68"/>
       <c r="C22" s="72" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D22" s="35" t="s">
         <v>2</v>
@@ -3050,7 +3050,7 @@
       </c>
       <c r="B23" s="68"/>
       <c r="C23" s="104" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D23" s="35" t="s">
         <v>2</v>
@@ -3088,7 +3088,7 @@
       </c>
       <c r="B24" s="68"/>
       <c r="C24" s="104" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D24" s="35" t="s">
         <v>2</v>
@@ -3126,7 +3126,7 @@
       </c>
       <c r="B25" s="68"/>
       <c r="C25" s="104" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D25" s="105" t="s">
         <v>2</v>
@@ -3162,7 +3162,7 @@
       </c>
       <c r="B26" s="68"/>
       <c r="C26" s="72" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D26" s="35" t="s">
         <v>2</v>
@@ -3198,7 +3198,7 @@
       </c>
       <c r="B27" s="68"/>
       <c r="C27" s="72" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D27" s="35" t="s">
         <v>2</v>
@@ -3234,7 +3234,7 @@
       </c>
       <c r="B28" s="68"/>
       <c r="C28" s="72" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D28" s="35" t="s">
         <v>2</v>
@@ -3298,19 +3298,19 @@
         <v>2</v>
       </c>
       <c r="C30" s="127" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D30" s="35" t="s">
         <v>2</v>
       </c>
       <c r="E30" s="162" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F30" s="104" t="s">
         <v>162</v>
       </c>
       <c r="G30" s="136" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H30" s="108" t="s">
         <v>169</v>
@@ -3338,7 +3338,7 @@
       <c r="A31" s="110"/>
       <c r="B31" s="68"/>
       <c r="C31" s="104" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D31" s="35" t="s">
         <v>2</v>
@@ -3350,7 +3350,7 @@
         <v>1.234</v>
       </c>
       <c r="G31" s="136" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H31" s="36"/>
       <c r="I31" s="6"/>
@@ -3376,7 +3376,7 @@
       <c r="A32" s="110"/>
       <c r="B32" s="68"/>
       <c r="C32" s="104" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D32" s="35" t="s">
         <v>2</v>
@@ -3388,7 +3388,7 @@
         <v>5.6779999999999999</v>
       </c>
       <c r="G32" s="136" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H32" s="36"/>
       <c r="I32" s="6"/>
@@ -3416,7 +3416,7 @@
       </c>
       <c r="B33" s="68"/>
       <c r="C33" s="104" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D33" s="105" t="s">
         <v>2</v>
@@ -3452,7 +3452,7 @@
       </c>
       <c r="B34" s="69"/>
       <c r="C34" s="34" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D34" s="43" t="s">
         <v>2</v>
@@ -3490,7 +3490,7 @@
       </c>
       <c r="B35" s="68"/>
       <c r="C35" s="34" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D35" s="35" t="s">
         <v>2</v>
@@ -3500,7 +3500,7 @@
         <v>75</v>
       </c>
       <c r="G35" s="136" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H35" s="36" t="s">
         <v>43</v>
@@ -3530,7 +3530,7 @@
       </c>
       <c r="B36" s="68"/>
       <c r="C36" s="34" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D36" s="35" t="s">
         <v>2</v>
@@ -3570,7 +3570,7 @@
       </c>
       <c r="B37" s="68"/>
       <c r="C37" s="34" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D37" s="35" t="s">
         <v>2</v>
@@ -3580,7 +3580,7 @@
         <v>3600</v>
       </c>
       <c r="G37" s="136" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H37" s="36" t="s">
         <v>43</v>
@@ -3638,19 +3638,19 @@
         <v>3</v>
       </c>
       <c r="C39" s="72" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D39" s="35" t="s">
         <v>2</v>
       </c>
       <c r="E39" s="162" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F39" s="104" t="s">
         <v>133</v>
       </c>
       <c r="G39" s="136" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H39" s="36"/>
       <c r="I39" s="6"/>
@@ -3676,7 +3676,7 @@
       <c r="A40" s="111"/>
       <c r="B40" s="68"/>
       <c r="C40" s="34" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D40" s="35" t="s">
         <v>2</v>
@@ -3688,7 +3688,7 @@
         <v>1.234</v>
       </c>
       <c r="G40" s="136" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H40" s="36"/>
       <c r="I40" s="6"/>
@@ -3716,7 +3716,7 @@
       </c>
       <c r="B41" s="68"/>
       <c r="C41" s="34" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D41" s="35" t="s">
         <v>2</v>
@@ -3728,7 +3728,7 @@
         <v>5.6779999999999999</v>
       </c>
       <c r="G41" s="136" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H41" s="36"/>
       <c r="I41" s="6"/>
@@ -3756,7 +3756,7 @@
       </c>
       <c r="B42" s="68"/>
       <c r="C42" s="34" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D42" s="35" t="s">
         <v>2</v>
@@ -3768,7 +3768,7 @@
         <v>9.0120000000000005</v>
       </c>
       <c r="G42" s="136" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="H42" s="36"/>
       <c r="I42" s="6"/>
@@ -3796,7 +3796,7 @@
       </c>
       <c r="B43" s="69"/>
       <c r="C43" s="72" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D43" s="43" t="s">
         <v>2</v>
@@ -3834,7 +3834,7 @@
       </c>
       <c r="B44" s="68"/>
       <c r="C44" s="34" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D44" s="35" t="s">
         <v>2</v>
@@ -3874,7 +3874,7 @@
       </c>
       <c r="B45" s="68"/>
       <c r="C45" s="34" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D45" s="35" t="s">
         <v>2</v>
@@ -3914,7 +3914,7 @@
       </c>
       <c r="B46" s="68"/>
       <c r="C46" s="34" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D46" s="35" t="s">
         <v>2</v>
@@ -3984,7 +3984,7 @@
         <v>4</v>
       </c>
       <c r="C48" s="72" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D48" s="35" t="s">
         <v>2</v>
@@ -3996,7 +3996,7 @@
         <v>162</v>
       </c>
       <c r="G48" s="136" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H48" s="39"/>
       <c r="I48" s="6"/>
@@ -4024,7 +4024,7 @@
       </c>
       <c r="B49" s="68"/>
       <c r="C49" s="72" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D49" s="43" t="s">
         <v>2</v>
@@ -4036,7 +4036,7 @@
         <v>1.234</v>
       </c>
       <c r="G49" s="136" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H49" s="36"/>
       <c r="I49" s="6"/>
@@ -4064,7 +4064,7 @@
       </c>
       <c r="B50" s="68"/>
       <c r="C50" s="34" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D50" s="43" t="s">
         <v>2</v>
@@ -4076,7 +4076,7 @@
         <v>5.6779999999999999</v>
       </c>
       <c r="G50" s="136" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H50" s="36"/>
       <c r="I50" s="6"/>
@@ -4104,7 +4104,7 @@
       </c>
       <c r="B51" s="68"/>
       <c r="C51" s="72" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D51" s="43" t="s">
         <v>2</v>
@@ -4140,7 +4140,7 @@
       </c>
       <c r="B52" s="69"/>
       <c r="C52" s="72" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D52" s="43" t="s">
         <v>2</v>
@@ -4178,7 +4178,7 @@
       </c>
       <c r="B53" s="68"/>
       <c r="C53" s="34" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D53" s="43" t="s">
         <v>2</v>
@@ -4218,7 +4218,7 @@
       </c>
       <c r="B54" s="68"/>
       <c r="C54" s="72" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D54" s="43" t="s">
         <v>2</v>
@@ -4258,7 +4258,7 @@
       </c>
       <c r="B55" s="68"/>
       <c r="C55" s="72" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D55" s="43" t="s">
         <v>2</v>
@@ -4328,7 +4328,7 @@
         <v>5</v>
       </c>
       <c r="C57" s="72" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D57" s="35" t="s">
         <v>2</v>
@@ -4340,7 +4340,7 @@
         <v>133</v>
       </c>
       <c r="G57" s="136" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="H57" s="108" t="s">
         <v>117</v>
@@ -4370,7 +4370,7 @@
       </c>
       <c r="B58" s="69"/>
       <c r="C58" s="72" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D58" s="35" t="s">
         <v>2</v>
@@ -4382,7 +4382,7 @@
         <v>1.234</v>
       </c>
       <c r="G58" s="136" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H58" s="44"/>
       <c r="I58" s="6"/>
@@ -4410,7 +4410,7 @@
       </c>
       <c r="B59" s="69"/>
       <c r="C59" s="34" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D59" s="35" t="s">
         <v>2</v>
@@ -4422,7 +4422,7 @@
         <v>5.6779999999999999</v>
       </c>
       <c r="G59" s="136" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H59" s="44"/>
       <c r="I59" s="6"/>
@@ -4450,7 +4450,7 @@
       </c>
       <c r="B60" s="69"/>
       <c r="C60" s="34" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D60" s="35" t="s">
         <v>2</v>
@@ -4462,7 +4462,7 @@
         <v>9.0120000000000005</v>
       </c>
       <c r="G60" s="136" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H60" s="39"/>
       <c r="I60" s="6"/>
@@ -4490,7 +4490,7 @@
       </c>
       <c r="B61" s="69"/>
       <c r="C61" s="75" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D61" s="43" t="s">
         <v>2</v>
@@ -4528,7 +4528,7 @@
       </c>
       <c r="B62" s="69"/>
       <c r="C62" s="34" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D62" s="35" t="s">
         <v>2</v>
@@ -4568,7 +4568,7 @@
       </c>
       <c r="B63" s="69"/>
       <c r="C63" s="72" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D63" s="35" t="s">
         <v>2</v>
@@ -4608,7 +4608,7 @@
       </c>
       <c r="B64" s="69"/>
       <c r="C64" s="72" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D64" s="35" t="s">
         <v>2</v>
@@ -4678,7 +4678,7 @@
         <v>6</v>
       </c>
       <c r="C66" s="72" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D66" s="35" t="s">
         <v>2</v>
@@ -4690,7 +4690,7 @@
         <v>162</v>
       </c>
       <c r="G66" s="136" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H66" s="36"/>
       <c r="I66" s="6"/>
@@ -4718,7 +4718,7 @@
       </c>
       <c r="B67" s="68"/>
       <c r="C67" s="34" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D67" s="35" t="s">
         <v>2</v>
@@ -4730,7 +4730,7 @@
         <v>1.234</v>
       </c>
       <c r="G67" s="136" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H67" s="36"/>
       <c r="I67" s="6"/>
@@ -4758,7 +4758,7 @@
       </c>
       <c r="B68" s="68"/>
       <c r="C68" s="72" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D68" s="35" t="s">
         <v>2</v>
@@ -4770,7 +4770,7 @@
         <v>5.6779999999999999</v>
       </c>
       <c r="G68" s="136" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H68" s="36"/>
       <c r="I68" s="6"/>
@@ -4798,7 +4798,7 @@
       </c>
       <c r="B69" s="68"/>
       <c r="C69" s="72" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D69" s="35" t="s">
         <v>2</v>
@@ -4834,7 +4834,7 @@
       </c>
       <c r="B70" s="68"/>
       <c r="C70" s="75" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D70" s="35" t="s">
         <v>2</v>
@@ -4870,7 +4870,7 @@
       </c>
       <c r="B71" s="68"/>
       <c r="C71" s="72" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D71" s="35" t="s">
         <v>2</v>
@@ -4908,7 +4908,7 @@
       </c>
       <c r="B72" s="68"/>
       <c r="C72" s="72" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D72" s="35" t="s">
         <v>2</v>
@@ -4946,7 +4946,7 @@
       </c>
       <c r="B73" s="68"/>
       <c r="C73" s="72" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D73" s="35" t="s">
         <v>2</v>
@@ -5012,19 +5012,19 @@
         <v>7</v>
       </c>
       <c r="C75" s="72" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D75" s="66" t="s">
         <v>2</v>
       </c>
       <c r="E75" s="162" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F75" s="104" t="s">
         <v>162</v>
       </c>
       <c r="G75" s="136" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H75" s="36"/>
       <c r="I75" s="6"/>
@@ -5052,7 +5052,7 @@
       </c>
       <c r="B76" s="68"/>
       <c r="C76" s="34" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D76" s="66" t="s">
         <v>2</v>
@@ -5064,7 +5064,7 @@
         <v>1.234</v>
       </c>
       <c r="G76" s="136" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H76" s="36"/>
       <c r="I76" s="6"/>
@@ -5092,7 +5092,7 @@
       </c>
       <c r="B77" s="68"/>
       <c r="C77" s="72" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D77" s="66" t="s">
         <v>2</v>
@@ -5104,7 +5104,7 @@
         <v>5.6779999999999999</v>
       </c>
       <c r="G77" s="136" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H77" s="36"/>
       <c r="I77" s="6"/>
@@ -5133,7 +5133,7 @@
       </c>
       <c r="B78" s="68"/>
       <c r="C78" s="72" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D78" s="66" t="s">
         <v>2</v>
@@ -5169,7 +5169,7 @@
       </c>
       <c r="B79" s="68"/>
       <c r="C79" s="72" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D79" s="66" t="s">
         <v>2</v>
@@ -5205,7 +5205,7 @@
       </c>
       <c r="B80" s="68"/>
       <c r="C80" s="72" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D80" s="66" t="s">
         <v>2</v>
@@ -5243,7 +5243,7 @@
       </c>
       <c r="B81" s="68"/>
       <c r="C81" s="72" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D81" s="66" t="s">
         <v>2</v>
@@ -5281,7 +5281,7 @@
       </c>
       <c r="B82" s="68"/>
       <c r="C82" s="72" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D82" s="66" t="s">
         <v>2</v>
@@ -5627,7 +5627,7 @@
         <v>2</v>
       </c>
       <c r="E91" s="125" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F91" s="52"/>
       <c r="G91" s="138" t="s">
@@ -5657,7 +5657,7 @@
     </row>
     <row r="92" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="67" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B92" s="67"/>
       <c r="C92" s="47"/>
@@ -5689,7 +5689,7 @@
       <c r="A93" s="50"/>
       <c r="B93" s="50"/>
       <c r="C93" s="74" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D93" s="48" t="s">
         <v>2</v>
@@ -5701,7 +5701,7 @@
         <v>45</v>
       </c>
       <c r="G93" s="139" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H93" s="49" t="s">
         <v>92</v>
@@ -5729,7 +5729,7 @@
       <c r="A94" s="50"/>
       <c r="B94" s="50"/>
       <c r="C94" s="47" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D94" s="48" t="s">
         <v>2</v>
@@ -5741,7 +5741,7 @@
         <v>75</v>
       </c>
       <c r="G94" s="139" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="H94" s="49" t="s">
         <v>92</v>
@@ -5769,7 +5769,7 @@
       <c r="A95" s="50"/>
       <c r="B95" s="50"/>
       <c r="C95" s="47" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D95" s="48" t="s">
         <v>2</v>
@@ -5809,7 +5809,7 @@
       <c r="A96" s="51"/>
       <c r="B96" s="51"/>
       <c r="C96" s="52" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D96" s="53" t="s">
         <v>2</v>
@@ -15118,7 +15118,7 @@
         <v>123</v>
       </c>
       <c r="K1" s="157" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.2">
@@ -26898,7 +26898,7 @@
       </c>
       <c r="D5" s="87" t="str">
         <f>'User Interface'!E4</f>
-        <v>HC</v>
+        <v>LBL</v>
       </c>
       <c r="E5" s="87" t="s">
         <v>13</v>
@@ -27537,7 +27537,7 @@
       </c>
       <c r="D26" s="40" t="str">
         <f>'User Interface'!E21</f>
-        <v>['GBL]</v>
+        <v>['GBL']</v>
       </c>
       <c r="E26" s="34" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Altering defaults on templates, fixing bug with V1 and HC/LBL
</commit_message>
<xml_diff>
--- a/HC_LBL_SpecificationInterface.xlsx
+++ b/HC_LBL_SpecificationInterface.xlsx
@@ -10,8 +10,8 @@
   <sheets>
     <sheet name="User Interface" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Manual Experiment Interface" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="ManualExps" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="WF1" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="ManualExps" sheetId="3" state="hidden" r:id="rId4"/>
+    <sheet name="WF1" sheetId="4" state="hidden" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="fixed_wells" vbProcedure="false">WF1!$D$19</definedName>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="279">
   <si>
     <t xml:space="preserve">Comment</t>
   </si>
@@ -65,7 +65,7 @@
     <t xml:space="preserve">lab</t>
   </si>
   <si>
-    <t xml:space="preserve">LBL</t>
+    <t xml:space="preserve">HC</t>
   </si>
   <si>
     <t xml:space="preserve">Select from dropdown menu</t>
@@ -131,7 +131,7 @@
     <t xml:space="preserve">Experiment 1 Group Name</t>
   </si>
   <si>
-    <t xml:space="preserve">Crank 0038 Testing</t>
+    <t xml:space="preserve">MyExampleID</t>
   </si>
   <si>
     <t xml:space="preserve">#</t>
@@ -155,7 +155,7 @@
     <t xml:space="preserve">Experiment 2 Group Name</t>
   </si>
   <si>
-    <t xml:space="preserve">random_exp2</t>
+    <t xml:space="preserve">MyExampleID-2</t>
   </si>
   <si>
     <t xml:space="preserve">Manually Specified Experiments</t>
@@ -620,7 +620,7 @@
     <t xml:space="preserve">Total Reagent Volume (ul)</t>
   </si>
   <si>
-    <t xml:space="preserve">20190306-JT-10</t>
+    <t xml:space="preserve">my example ID</t>
   </si>
   <si>
     <t xml:space="preserve">20190514-JT-15</t>
@@ -2182,22 +2182,22 @@
   </sheetPr>
   <dimension ref="A1:Z1017"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A33" colorId="64" zoomScale="92" zoomScaleNormal="92" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="92" zoomScaleNormal="92" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="true" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="44.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="91.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="92.17"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="26" min="9" style="0" width="8.83"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1025" min="27" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="44.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="91.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="92.14"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="26" min="9" style="0" width="8.85"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1025" min="27" style="0" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" s="8" customFormat="true" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2306,7 +2306,7 @@
       <c r="Y3" s="14"/>
       <c r="Z3" s="14"/>
     </row>
-    <row r="4" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="18.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="19"/>
       <c r="B4" s="19"/>
       <c r="C4" s="20" t="s">
@@ -2374,7 +2374,7 @@
       <c r="Y5" s="14"/>
       <c r="Z5" s="14"/>
     </row>
-    <row r="6" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="18.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="32"/>
       <c r="B6" s="32"/>
       <c r="C6" s="27" t="s">
@@ -2384,7 +2384,8 @@
         <v>8</v>
       </c>
       <c r="E6" s="33" t="n">
-        <v>96</v>
+        <f aca="false">SUM(E11,E16,E19)</f>
+        <v>6</v>
       </c>
       <c r="F6" s="27"/>
       <c r="G6" s="34" t="s">
@@ -2410,7 +2411,7 @@
       <c r="Y6" s="14"/>
       <c r="Z6" s="14"/>
     </row>
-    <row r="7" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="18.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="32"/>
       <c r="B7" s="32"/>
       <c r="C7" s="27" t="s">
@@ -2566,7 +2567,7 @@
         <v>8</v>
       </c>
       <c r="E11" s="51" t="n">
-        <v>96</v>
+        <v>3</v>
       </c>
       <c r="F11" s="45" t="n">
         <v>12</v>
@@ -2603,10 +2604,10 @@
       <c r="D12" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="47" t="s">
+      <c r="E12" s="47"/>
+      <c r="F12" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="45"/>
       <c r="G12" s="53"/>
       <c r="H12" s="49"/>
       <c r="I12" s="50"/>
@@ -2628,7 +2629,7 @@
       <c r="Y12" s="50"/>
       <c r="Z12" s="50"/>
     </row>
-    <row r="13" s="8" customFormat="true" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" s="8" customFormat="true" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="54"/>
       <c r="B13" s="44"/>
       <c r="C13" s="45"/>
@@ -2787,10 +2788,10 @@
       <c r="D17" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="51" t="s">
+      <c r="E17" s="51"/>
+      <c r="F17" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="F17" s="56"/>
       <c r="G17" s="52"/>
       <c r="H17" s="57"/>
       <c r="I17" s="14"/>
@@ -2825,9 +2826,7 @@
       <c r="H18" s="60"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="64" t="s">
-        <v>34</v>
-      </c>
+      <c r="A19" s="64"/>
       <c r="B19" s="65"/>
       <c r="C19" s="66" t="s">
         <v>43</v>
@@ -2836,7 +2835,7 @@
         <v>8</v>
       </c>
       <c r="E19" s="67" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F19" s="68" t="n">
         <v>12</v>
@@ -2846,7 +2845,7 @@
       </c>
       <c r="H19" s="65"/>
     </row>
-    <row r="20" customFormat="false" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="18.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="70" t="s">
         <v>45</v>
       </c>
@@ -15037,23 +15036,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T500"/>
+  <dimension ref="A1:K500"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
+      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="true" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="124" width="19.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="124" width="20.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="124" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="125" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="126" width="22"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1025" min="12" style="0" width="14.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="124" width="19.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="124" width="20.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="3" style="124" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="10" min="10" style="125" width="12.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="126" width="24.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="8.57"/>
   </cols>
   <sheetData>
-    <row r="1" s="128" customFormat="true" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="128" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="127" t="s">
         <v>178</v>
       </c>
@@ -15089,21 +15088,21 @@
       </c>
     </row>
     <row r="2" s="131" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="129" t="str">
+      <c r="A2" s="129" t="n">
         <f aca="false">IF(manual_wells &gt; 0, 1, "")</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="B2" s="130" t="s">
         <v>189</v>
       </c>
       <c r="C2" s="125" t="n">
-        <v>150</v>
+        <v>1</v>
       </c>
       <c r="D2" s="125" t="n">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="E2" s="125" t="n">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="F2" s="125" t="n">
         <v>0</v>
@@ -15115,20 +15114,20 @@
         <v>0</v>
       </c>
       <c r="I2" s="125" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J2" s="125" t="n">
         <v>0</v>
       </c>
-      <c r="K2" s="126" t="str">
+      <c r="K2" s="126" t="n">
         <f aca="false">IF(NOT(A2=""), SUM(C2:J2), "")</f>
-        <v/>
+        <v>13</v>
       </c>
     </row>
     <row r="3" s="131" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="129" t="str">
+      <c r="A3" s="129" t="n">
         <f aca="false">IF(A2 &lt; fixed_wells, A2 + 1, "")</f>
-        <v/>
+        <v>2</v>
       </c>
       <c r="B3" s="130" t="s">
         <v>190</v>
@@ -15157,15 +15156,15 @@
       <c r="J3" s="125" t="n">
         <v>0</v>
       </c>
-      <c r="K3" s="126" t="str">
+      <c r="K3" s="126" t="n">
         <f aca="false">IF(NOT(A3=""), SUM(C3:J3), "")</f>
-        <v/>
+        <v>215</v>
       </c>
     </row>
     <row r="4" s="131" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="129" t="str">
+      <c r="A4" s="129" t="n">
         <f aca="false">IF(A3 &lt; fixed_wells, A3 + 1, "")</f>
-        <v/>
+        <v>3</v>
       </c>
       <c r="B4" s="130" t="s">
         <v>191</v>
@@ -15194,9 +15193,9 @@
       <c r="J4" s="125" t="n">
         <v>0</v>
       </c>
-      <c r="K4" s="126" t="str">
+      <c r="K4" s="126" t="n">
         <f aca="false">IF(NOT(A4=""), SUM(C4:J4), "")</f>
-        <v/>
+        <v>215</v>
       </c>
     </row>
     <row r="5" s="131" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15426,10 +15425,6 @@
       <c r="J18" s="125"/>
       <c r="K18" s="126" t="str">
         <f aca="false">IF(NOT(A18=""), SUM(C18:J18), "")</f>
-        <v/>
-      </c>
-      <c r="T18" s="131" t="str">
-        <f aca="false">IF(NOT(A18=""), SUM(C18:S18), "")</f>
         <v/>
       </c>
     </row>
@@ -22183,6 +22178,7 @@
       <c r="K500" s="126"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="true" objects="true" scenarios="true" selectLockedCells="true"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -22201,18 +22197,18 @@
   <dimension ref="A1:K98"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="19.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="19.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="3" style="0" width="13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="14.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="10.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="14.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="10.57"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="132" t="s">
         <v>178</v>
       </c>
@@ -22248,25 +22244,25 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="str">
+      <c r="A2" s="0" t="n">
         <f aca="false">IF(NOT('Manual Experiment Interface'!A2=""),'Manual Experiment Interface'!A2,"")</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="B2" s="0" t="str">
         <f aca="false">IF(NOT('Manual Experiment Interface'!B2=""),'Manual Experiment Interface'!B2,"")</f>
-        <v>20190306-JT-10</v>
+        <v>my example ID</v>
       </c>
       <c r="C2" s="0" t="n">
         <f aca="false">IF(NOT('Manual Experiment Interface'!C2=""),'Manual Experiment Interface'!C2,"")</f>
-        <v>150</v>
+        <v>1</v>
       </c>
       <c r="D2" s="0" t="n">
         <f aca="false">IF(NOT('Manual Experiment Interface'!D2=""),'Manual Experiment Interface'!D2,"")</f>
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="E2" s="0" t="n">
         <f aca="false">IF(NOT('Manual Experiment Interface'!E2=""),'Manual Experiment Interface'!E2,"")</f>
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="F2" s="0" t="n">
         <f aca="false">IF(NOT('Manual Experiment Interface'!F2=""),'Manual Experiment Interface'!F2,"")</f>
@@ -22282,21 +22278,21 @@
       </c>
       <c r="I2" s="0" t="n">
         <f aca="false">IF(NOT('Manual Experiment Interface'!I2=""),'Manual Experiment Interface'!I2,"")</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J2" s="0" t="n">
         <f aca="false">IF(NOT('Manual Experiment Interface'!J2=""),'Manual Experiment Interface'!J2,"")</f>
         <v>0</v>
       </c>
-      <c r="K2" s="0" t="str">
+      <c r="K2" s="0" t="n">
         <f aca="false">IF(NOT('Manual Experiment Interface'!K2=""),'Manual Experiment Interface'!K2,"")</f>
-        <v/>
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="str">
+      <c r="A3" s="0" t="n">
         <f aca="false">IF(NOT('Manual Experiment Interface'!A3=""),'Manual Experiment Interface'!A3,"")</f>
-        <v/>
+        <v>2</v>
       </c>
       <c r="B3" s="0" t="str">
         <f aca="false">IF(NOT('Manual Experiment Interface'!B3=""),'Manual Experiment Interface'!B3,"")</f>
@@ -22334,15 +22330,15 @@
         <f aca="false">IF(NOT('Manual Experiment Interface'!J3=""),'Manual Experiment Interface'!J3,"")</f>
         <v>0</v>
       </c>
-      <c r="K3" s="0" t="str">
+      <c r="K3" s="0" t="n">
         <f aca="false">IF(NOT('Manual Experiment Interface'!K3=""),'Manual Experiment Interface'!K3,"")</f>
-        <v/>
+        <v>215</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="str">
+      <c r="A4" s="0" t="n">
         <f aca="false">IF(NOT('Manual Experiment Interface'!A4=""),'Manual Experiment Interface'!A4,"")</f>
-        <v/>
+        <v>3</v>
       </c>
       <c r="B4" s="0" t="str">
         <f aca="false">IF(NOT('Manual Experiment Interface'!B4=""),'Manual Experiment Interface'!B4,"")</f>
@@ -22380,9 +22376,9 @@
         <f aca="false">IF(NOT('Manual Experiment Interface'!J4=""),'Manual Experiment Interface'!J4,"")</f>
         <v>0</v>
       </c>
-      <c r="K4" s="0" t="str">
+      <c r="K4" s="0" t="n">
         <f aca="false">IF(NOT('Manual Experiment Interface'!K4=""),'Manual Experiment Interface'!K4,"")</f>
-        <v/>
+        <v>215</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26727,20 +26723,20 @@
   </sheetPr>
   <dimension ref="A1:W1022"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K10" activeCellId="0" sqref="K10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D113" activeCellId="0" sqref="D113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="133" width="25.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="133" width="28.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="133" width="25.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="133" width="28.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="133" width="2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="133" width="48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="133" width="18.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="6" style="133" width="8.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="24" style="133" width="14.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1023" style="133" width="8.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="133" width="18.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="6" style="133" width="8.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="24" style="133" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1023" style="133" width="8.85"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -26882,7 +26878,7 @@
       </c>
       <c r="D5" s="139" t="str">
         <f aca="false">'User Interface'!E4</f>
-        <v>LBL</v>
+        <v>HC</v>
       </c>
       <c r="E5" s="139" t="s">
         <v>200</v>
@@ -26943,7 +26939,7 @@
       </c>
       <c r="D7" s="27" t="n">
         <f aca="false">'User Interface'!wellcount</f>
-        <v>96</v>
+        <v>6</v>
       </c>
       <c r="E7" s="27" t="s">
         <v>199</v>
@@ -27102,7 +27098,7 @@
       <c r="V11" s="144"/>
       <c r="W11" s="144"/>
     </row>
-    <row r="12" s="145" customFormat="true" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" s="145" customFormat="true" ht="18.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="146" t="n">
         <f aca="false">'User Interface'!A11</f>
         <v>0</v>
@@ -27115,7 +27111,7 @@
       </c>
       <c r="D12" s="147" t="n">
         <f aca="false">'User Interface'!E11</f>
-        <v>96</v>
+        <v>3</v>
       </c>
       <c r="E12" s="147" t="s">
         <v>199</v>
@@ -27139,7 +27135,7 @@
       <c r="V12" s="144"/>
       <c r="W12" s="144"/>
     </row>
-    <row r="13" s="145" customFormat="true" ht="19" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" s="145" customFormat="true" ht="18.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="146" t="n">
         <f aca="false">'User Interface'!A12</f>
         <v>0</v>
@@ -27150,9 +27146,9 @@
       <c r="C13" s="148" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="147" t="str">
+      <c r="D13" s="147" t="n">
         <f aca="false">'User Interface'!E12</f>
-        <v>Crank 0038 Testing</v>
+        <v>0</v>
       </c>
       <c r="E13" s="147"/>
       <c r="F13" s="144"/>
@@ -27296,9 +27292,9 @@
       <c r="C17" s="148" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="147" t="str">
+      <c r="D17" s="147" t="n">
         <f aca="false">'User Interface'!E17</f>
-        <v>random_exp2</v>
+        <v>0</v>
       </c>
       <c r="E17" s="147"/>
       <c r="F17" s="138"/>
@@ -27337,7 +27333,7 @@
       <c r="C19" s="150"/>
       <c r="D19" s="147" t="n">
         <f aca="false">'User Interface'!E19</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E19" s="150" t="s">
         <v>199</v>

</xml_diff>

<commit_message>
Updated defaults to fit with current WF, small fix to new folders list
</commit_message>
<xml_diff>
--- a/HC_LBL_SpecificationInterface.xlsx
+++ b/HC_LBL_SpecificationInterface.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="User Interface" sheetId="1" state="visible" r:id="rId2"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="278">
   <si>
     <t xml:space="preserve">Comment</t>
   </si>
@@ -65,7 +65,7 @@
     <t xml:space="preserve">lab</t>
   </si>
   <si>
-    <t xml:space="preserve">HC</t>
+    <t xml:space="preserve">LBL</t>
   </si>
   <si>
     <t xml:space="preserve">Select from dropdown menu</t>
@@ -131,6 +131,9 @@
     <t xml:space="preserve">Experiment 1 Group Name</t>
   </si>
   <si>
+    <t xml:space="preserve">My Example Run</t>
+  </si>
+  <si>
     <t xml:space="preserve">MyExampleID</t>
   </si>
   <si>
@@ -182,7 +185,7 @@
     <t xml:space="preserve">Reagent 1 Chemical List</t>
   </si>
   <si>
-    <t xml:space="preserve">['GBL']</t>
+    <t xml:space="preserve">['DMF']</t>
   </si>
   <si>
     <t xml:space="preserve">['Chemical 1']</t>
@@ -218,7 +221,7 @@
     <t xml:space="preserve">Reagent 2 Chemical List</t>
   </si>
   <si>
-    <t xml:space="preserve">['PbI2','EtNH3I','GBL']</t>
+    <t xml:space="preserve">['PbI2','tButylammoniumIodide','DMF']</t>
   </si>
   <si>
     <t xml:space="preserve">['Chemical 1','Chemical 2']</t>
@@ -296,7 +299,7 @@
     <t xml:space="preserve">Reagent 3 Chemical List</t>
   </si>
   <si>
-    <t xml:space="preserve">['EtNH3I','GBL']</t>
+    <t xml:space="preserve">['tButylammoniumIodide','DMF']</t>
   </si>
   <si>
     <t xml:space="preserve">['Chemical 1','Chemical 2', 'Chemical 3']</t>
@@ -621,12 +624,6 @@
   </si>
   <si>
     <t xml:space="preserve">my example ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20190514-JT-15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20190306-JT-11</t>
   </si>
   <si>
     <t xml:space="preserve">Total Precursor Volume (ul)</t>
@@ -2180,15 +2177,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z1017"/>
+  <dimension ref="A1:Z1028"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="92" zoomScaleNormal="92" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A33" colorId="64" zoomScale="92" zoomScaleNormal="92" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E32" activeCellId="0" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="true" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="2"/>
@@ -2385,7 +2382,7 @@
       </c>
       <c r="E6" s="33" t="n">
         <f aca="false">SUM(E11,E16,E19)</f>
-        <v>6</v>
+        <v>96</v>
       </c>
       <c r="F6" s="27"/>
       <c r="G6" s="34" t="s">
@@ -2567,7 +2564,7 @@
         <v>8</v>
       </c>
       <c r="E11" s="51" t="n">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="F11" s="45" t="n">
         <v>12</v>
@@ -2604,9 +2601,11 @@
       <c r="D12" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="47"/>
+      <c r="E12" s="47" t="s">
+        <v>33</v>
+      </c>
       <c r="F12" s="45" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G12" s="53"/>
       <c r="H12" s="49"/>
@@ -2659,11 +2658,11 @@
     </row>
     <row r="14" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="55" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B14" s="44"/>
       <c r="C14" s="45" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D14" s="46" t="s">
         <v>8</v>
@@ -2699,23 +2698,23 @@
     </row>
     <row r="15" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="55" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B15" s="44"/>
       <c r="C15" s="45" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D15" s="46" t="s">
         <v>8</v>
       </c>
       <c r="E15" s="51" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F15" s="45" t="s">
         <v>28</v>
       </c>
       <c r="G15" s="48" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H15" s="49"/>
       <c r="I15" s="14"/>
@@ -2739,11 +2738,11 @@
     </row>
     <row r="16" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="55" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B16" s="44"/>
       <c r="C16" s="45" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D16" s="46" t="s">
         <v>8</v>
@@ -2779,18 +2778,18 @@
     </row>
     <row r="17" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="55" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B17" s="44"/>
       <c r="C17" s="45" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D17" s="46" t="s">
         <v>8</v>
       </c>
       <c r="E17" s="51"/>
       <c r="F17" s="56" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G17" s="52"/>
       <c r="H17" s="57"/>
@@ -2815,7 +2814,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="58" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B18" s="59"/>
       <c r="C18" s="60"/>
@@ -2829,25 +2828,25 @@
       <c r="A19" s="64"/>
       <c r="B19" s="65"/>
       <c r="C19" s="66" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D19" s="65" t="s">
         <v>8</v>
       </c>
       <c r="E19" s="67" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F19" s="68" t="n">
         <v>12</v>
       </c>
       <c r="G19" s="69" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H19" s="65"/>
     </row>
     <row r="20" customFormat="false" ht="18.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="70" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B20" s="70"/>
       <c r="C20" s="71"/>
@@ -2877,20 +2876,20 @@
     </row>
     <row r="21" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="76" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B21" s="77" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C21" s="71"/>
       <c r="D21" s="72"/>
       <c r="E21" s="73"/>
       <c r="F21" s="71"/>
       <c r="G21" s="78" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H21" s="79" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I21" s="14"/>
       <c r="J21" s="14"/>
@@ -2917,22 +2916,22 @@
         <v>1</v>
       </c>
       <c r="C22" s="82" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D22" s="72" t="s">
         <v>8</v>
       </c>
       <c r="E22" s="83" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F22" s="84" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G22" s="78" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H22" s="85" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I22" s="14"/>
       <c r="J22" s="14"/>
@@ -2955,11 +2954,11 @@
     </row>
     <row r="23" customFormat="false" ht="18.75" hidden="true" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A23" s="86" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B23" s="81"/>
       <c r="C23" s="82" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D23" s="72" t="s">
         <v>8</v>
@@ -2989,11 +2988,11 @@
     </row>
     <row r="24" customFormat="false" ht="18.75" hidden="true" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A24" s="86" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B24" s="81"/>
       <c r="C24" s="90" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D24" s="72" t="s">
         <v>8</v>
@@ -3027,11 +3026,11 @@
     </row>
     <row r="25" customFormat="false" ht="18.75" hidden="true" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A25" s="86" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B25" s="81"/>
       <c r="C25" s="90" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D25" s="72" t="s">
         <v>8</v>
@@ -3065,11 +3064,11 @@
     </row>
     <row r="26" customFormat="false" ht="18.75" hidden="true" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A26" s="86" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B26" s="81"/>
       <c r="C26" s="90" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D26" s="92" t="s">
         <v>8</v>
@@ -3101,11 +3100,11 @@
     </row>
     <row r="27" customFormat="false" ht="18.75" hidden="true" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A27" s="93" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B27" s="81"/>
       <c r="C27" s="82" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D27" s="72" t="s">
         <v>8</v>
@@ -3137,11 +3136,11 @@
     </row>
     <row r="28" customFormat="false" ht="18.75" hidden="true" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A28" s="93" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B28" s="81"/>
       <c r="C28" s="82" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D28" s="72" t="s">
         <v>8</v>
@@ -3173,11 +3172,11 @@
     </row>
     <row r="29" customFormat="false" ht="18.75" hidden="true" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A29" s="93" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B29" s="81"/>
       <c r="C29" s="82" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D29" s="72" t="s">
         <v>8</v>
@@ -3241,22 +3240,22 @@
         <v>2</v>
       </c>
       <c r="C31" s="94" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D31" s="72" t="s">
         <v>8</v>
       </c>
       <c r="E31" s="95" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F31" s="90" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G31" s="78" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H31" s="96" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I31" s="14"/>
       <c r="J31" s="14"/>
@@ -3281,19 +3280,19 @@
       <c r="A32" s="80"/>
       <c r="B32" s="81"/>
       <c r="C32" s="90" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D32" s="72" t="s">
         <v>8</v>
       </c>
       <c r="E32" s="91" t="n">
-        <v>1.5</v>
+        <v>2.52</v>
       </c>
       <c r="F32" s="71" t="n">
         <v>1.234</v>
       </c>
       <c r="G32" s="78" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H32" s="75"/>
       <c r="I32" s="14"/>
@@ -3319,19 +3318,19 @@
       <c r="A33" s="80"/>
       <c r="B33" s="81"/>
       <c r="C33" s="90" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D33" s="72" t="s">
         <v>8</v>
       </c>
       <c r="E33" s="91" t="n">
-        <v>3</v>
+        <v>2.52</v>
       </c>
       <c r="F33" s="71" t="n">
         <v>5.678</v>
       </c>
       <c r="G33" s="78" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H33" s="75"/>
       <c r="I33" s="14"/>
@@ -3355,11 +3354,11 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A34" s="86" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B34" s="81"/>
       <c r="C34" s="90" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D34" s="92" t="s">
         <v>8</v>
@@ -3391,11 +3390,11 @@
     </row>
     <row r="35" customFormat="false" ht="18.75" hidden="true" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A35" s="80" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B35" s="97"/>
       <c r="C35" s="71" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D35" s="98" t="s">
         <v>8</v>
@@ -3403,10 +3402,10 @@
       <c r="E35" s="87"/>
       <c r="F35" s="88"/>
       <c r="G35" s="99" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H35" s="85" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I35" s="14"/>
       <c r="J35" s="14"/>
@@ -3429,11 +3428,11 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A36" s="93" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B36" s="81"/>
       <c r="C36" s="71" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D36" s="72" t="s">
         <v>8</v>
@@ -3443,10 +3442,10 @@
         <v>75</v>
       </c>
       <c r="G36" s="78" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H36" s="75" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I36" s="14"/>
       <c r="J36" s="14"/>
@@ -3469,11 +3468,11 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A37" s="93" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B37" s="81"/>
       <c r="C37" s="71" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D37" s="72" t="s">
         <v>8</v>
@@ -3483,10 +3482,10 @@
         <v>450</v>
       </c>
       <c r="G37" s="78" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H37" s="75" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I37" s="14"/>
       <c r="J37" s="14"/>
@@ -3509,11 +3508,11 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A38" s="93" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B38" s="81"/>
       <c r="C38" s="71" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D38" s="72" t="s">
         <v>8</v>
@@ -3523,10 +3522,10 @@
         <v>3600</v>
       </c>
       <c r="G38" s="78" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H38" s="75" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I38" s="14"/>
       <c r="J38" s="14"/>
@@ -3581,19 +3580,19 @@
         <v>3</v>
       </c>
       <c r="C40" s="82" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D40" s="72" t="s">
         <v>8</v>
       </c>
       <c r="E40" s="95" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F40" s="90" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G40" s="78" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H40" s="75"/>
       <c r="I40" s="14"/>
@@ -3619,19 +3618,19 @@
       <c r="A41" s="86"/>
       <c r="B41" s="81"/>
       <c r="C41" s="71" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D41" s="72" t="s">
         <v>8</v>
       </c>
       <c r="E41" s="73" t="n">
-        <v>6</v>
+        <v>2.36</v>
       </c>
       <c r="F41" s="101" t="n">
         <v>1.234</v>
       </c>
       <c r="G41" s="78" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H41" s="75"/>
       <c r="I41" s="14"/>
@@ -3655,11 +3654,11 @@
     </row>
     <row r="42" customFormat="false" ht="18.75" hidden="true" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A42" s="86" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B42" s="81"/>
       <c r="C42" s="71" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D42" s="72" t="s">
         <v>8</v>
@@ -3671,7 +3670,7 @@
         <v>5.678</v>
       </c>
       <c r="G42" s="78" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H42" s="75"/>
       <c r="I42" s="14"/>
@@ -3695,11 +3694,11 @@
     </row>
     <row r="43" customFormat="false" ht="18.75" hidden="true" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A43" s="86" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B43" s="81"/>
       <c r="C43" s="71" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D43" s="72" t="s">
         <v>8</v>
@@ -3711,7 +3710,7 @@
         <v>9.012</v>
       </c>
       <c r="G43" s="78" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H43" s="75"/>
       <c r="I43" s="14"/>
@@ -3735,11 +3734,11 @@
     </row>
     <row r="44" customFormat="false" ht="18.75" hidden="true" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A44" s="80" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B44" s="97"/>
       <c r="C44" s="82" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D44" s="98" t="s">
         <v>8</v>
@@ -3747,10 +3746,10 @@
       <c r="E44" s="87"/>
       <c r="F44" s="84"/>
       <c r="G44" s="99" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H44" s="102" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I44" s="14"/>
       <c r="J44" s="14"/>
@@ -3773,11 +3772,11 @@
     </row>
     <row r="45" customFormat="false" ht="18.75" hidden="true" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A45" s="80" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B45" s="81"/>
       <c r="C45" s="71" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D45" s="72" t="s">
         <v>8</v>
@@ -3787,10 +3786,10 @@
         <v>75</v>
       </c>
       <c r="G45" s="74" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H45" s="75" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I45" s="14"/>
       <c r="J45" s="14"/>
@@ -3813,11 +3812,11 @@
     </row>
     <row r="46" customFormat="false" ht="18.75" hidden="true" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A46" s="80" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B46" s="81"/>
       <c r="C46" s="71" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D46" s="72" t="s">
         <v>8</v>
@@ -3827,10 +3826,10 @@
         <v>450</v>
       </c>
       <c r="G46" s="74" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H46" s="75" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I46" s="14"/>
       <c r="J46" s="14"/>
@@ -3853,11 +3852,11 @@
     </row>
     <row r="47" customFormat="false" ht="18.75" hidden="true" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A47" s="80" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B47" s="81"/>
       <c r="C47" s="71" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D47" s="72" t="s">
         <v>8</v>
@@ -3867,10 +3866,10 @@
         <v>3600</v>
       </c>
       <c r="G47" s="74" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H47" s="75" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I47" s="14"/>
       <c r="J47" s="14"/>
@@ -3921,25 +3920,25 @@
     </row>
     <row r="49" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="86" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B49" s="81" t="n">
         <v>4</v>
       </c>
       <c r="C49" s="82" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D49" s="72" t="s">
         <v>8</v>
       </c>
       <c r="E49" s="91" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F49" s="90" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G49" s="78" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H49" s="100"/>
       <c r="I49" s="14"/>
@@ -3963,11 +3962,11 @@
     </row>
     <row r="50" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="86" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B50" s="81"/>
       <c r="C50" s="82" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D50" s="98" t="s">
         <v>8</v>
@@ -3979,7 +3978,7 @@
         <v>1.234</v>
       </c>
       <c r="G50" s="78" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H50" s="75"/>
       <c r="I50" s="14"/>
@@ -4003,11 +4002,11 @@
     </row>
     <row r="51" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="86" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B51" s="81"/>
       <c r="C51" s="71" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D51" s="98" t="s">
         <v>8</v>
@@ -4019,7 +4018,7 @@
         <v>5.678</v>
       </c>
       <c r="G51" s="78" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H51" s="75"/>
       <c r="I51" s="14"/>
@@ -4043,11 +4042,11 @@
     </row>
     <row r="52" customFormat="false" ht="18.75" hidden="true" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A52" s="80" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B52" s="81"/>
       <c r="C52" s="82" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D52" s="98" t="s">
         <v>8</v>
@@ -4079,11 +4078,11 @@
     </row>
     <row r="53" customFormat="false" ht="18.75" hidden="true" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A53" s="80" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B53" s="97"/>
       <c r="C53" s="82" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D53" s="98" t="s">
         <v>8</v>
@@ -4091,10 +4090,10 @@
       <c r="E53" s="87"/>
       <c r="F53" s="88"/>
       <c r="G53" s="99" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H53" s="102" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I53" s="14"/>
       <c r="J53" s="14"/>
@@ -4117,11 +4116,11 @@
     </row>
     <row r="54" customFormat="false" ht="18.75" hidden="true" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A54" s="80" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B54" s="81"/>
       <c r="C54" s="71" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D54" s="98" t="s">
         <v>8</v>
@@ -4131,10 +4130,10 @@
         <v>75</v>
       </c>
       <c r="G54" s="74" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H54" s="75" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I54" s="14"/>
       <c r="J54" s="14"/>
@@ -4157,11 +4156,11 @@
     </row>
     <row r="55" customFormat="false" ht="18.75" hidden="true" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A55" s="80" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B55" s="81"/>
       <c r="C55" s="82" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D55" s="98" t="s">
         <v>8</v>
@@ -4171,10 +4170,10 @@
         <v>450</v>
       </c>
       <c r="G55" s="74" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H55" s="75" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I55" s="14"/>
       <c r="J55" s="14"/>
@@ -4197,11 +4196,11 @@
     </row>
     <row r="56" customFormat="false" ht="18.75" hidden="true" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A56" s="80" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B56" s="81"/>
       <c r="C56" s="82" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D56" s="98" t="s">
         <v>8</v>
@@ -4211,10 +4210,10 @@
         <v>3600</v>
       </c>
       <c r="G56" s="74" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H56" s="75" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I56" s="14"/>
       <c r="J56" s="14"/>
@@ -4265,28 +4264,28 @@
     </row>
     <row r="58" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="76" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B58" s="81" t="n">
         <v>5</v>
       </c>
       <c r="C58" s="82" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D58" s="72" t="s">
         <v>8</v>
       </c>
       <c r="E58" s="91" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F58" s="90" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G58" s="78" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H58" s="96" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="I58" s="14"/>
       <c r="J58" s="14"/>
@@ -4309,11 +4308,11 @@
     </row>
     <row r="59" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="86" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B59" s="97"/>
       <c r="C59" s="82" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D59" s="72" t="s">
         <v>8</v>
@@ -4325,7 +4324,7 @@
         <v>1.234</v>
       </c>
       <c r="G59" s="78" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H59" s="103"/>
       <c r="I59" s="14"/>
@@ -4349,11 +4348,11 @@
     </row>
     <row r="60" customFormat="false" ht="18.75" hidden="true" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A60" s="86" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B60" s="97"/>
       <c r="C60" s="71" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D60" s="72" t="s">
         <v>8</v>
@@ -4365,7 +4364,7 @@
         <v>5.678</v>
       </c>
       <c r="G60" s="78" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H60" s="103"/>
       <c r="I60" s="14"/>
@@ -4389,11 +4388,11 @@
     </row>
     <row r="61" customFormat="false" ht="18.75" hidden="true" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A61" s="86" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B61" s="97"/>
       <c r="C61" s="71" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D61" s="72" t="s">
         <v>8</v>
@@ -4405,7 +4404,7 @@
         <v>9.012</v>
       </c>
       <c r="G61" s="78" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H61" s="100"/>
       <c r="I61" s="14"/>
@@ -4429,11 +4428,11 @@
     </row>
     <row r="62" customFormat="false" ht="18.75" hidden="true" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A62" s="80" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B62" s="97"/>
       <c r="C62" s="84" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D62" s="98" t="s">
         <v>8</v>
@@ -4441,10 +4440,10 @@
       <c r="E62" s="87"/>
       <c r="F62" s="88"/>
       <c r="G62" s="99" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H62" s="103" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I62" s="14"/>
       <c r="J62" s="14"/>
@@ -4467,11 +4466,11 @@
     </row>
     <row r="63" customFormat="false" ht="18.75" hidden="true" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A63" s="80" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B63" s="97"/>
       <c r="C63" s="71" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D63" s="72" t="s">
         <v>8</v>
@@ -4481,10 +4480,10 @@
         <v>75</v>
       </c>
       <c r="G63" s="74" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H63" s="75" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I63" s="14"/>
       <c r="J63" s="14"/>
@@ -4507,11 +4506,11 @@
     </row>
     <row r="64" customFormat="false" ht="18.75" hidden="true" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A64" s="80" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B64" s="97"/>
       <c r="C64" s="82" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D64" s="72" t="s">
         <v>8</v>
@@ -4521,10 +4520,10 @@
         <v>450</v>
       </c>
       <c r="G64" s="74" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H64" s="75" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I64" s="14"/>
       <c r="J64" s="14"/>
@@ -4547,11 +4546,11 @@
     </row>
     <row r="65" customFormat="false" ht="18.75" hidden="true" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A65" s="80" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B65" s="97"/>
       <c r="C65" s="82" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D65" s="72" t="s">
         <v>8</v>
@@ -4561,10 +4560,10 @@
         <v>3600</v>
       </c>
       <c r="G65" s="74" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H65" s="75" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I65" s="14"/>
       <c r="J65" s="14"/>
@@ -4615,25 +4614,25 @@
     </row>
     <row r="67" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="76" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B67" s="81" t="n">
         <v>6</v>
       </c>
       <c r="C67" s="82" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D67" s="72" t="s">
         <v>8</v>
       </c>
       <c r="E67" s="91" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F67" s="90" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G67" s="78" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H67" s="75"/>
       <c r="I67" s="14"/>
@@ -4657,11 +4656,11 @@
     </row>
     <row r="68" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="76" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B68" s="81"/>
       <c r="C68" s="71" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D68" s="72" t="s">
         <v>8</v>
@@ -4673,7 +4672,7 @@
         <v>1.234</v>
       </c>
       <c r="G68" s="78" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H68" s="75"/>
       <c r="I68" s="14"/>
@@ -4697,11 +4696,11 @@
     </row>
     <row r="69" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="76" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B69" s="81"/>
       <c r="C69" s="82" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D69" s="72" t="s">
         <v>8</v>
@@ -4713,7 +4712,7 @@
         <v>5.678</v>
       </c>
       <c r="G69" s="78" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H69" s="75"/>
       <c r="I69" s="14"/>
@@ -4737,11 +4736,11 @@
     </row>
     <row r="70" customFormat="false" ht="18.75" hidden="true" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A70" s="76" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B70" s="81"/>
       <c r="C70" s="82" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D70" s="72" t="s">
         <v>8</v>
@@ -4773,11 +4772,11 @@
     </row>
     <row r="71" customFormat="false" ht="18.75" hidden="true" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A71" s="93" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B71" s="81"/>
       <c r="C71" s="84" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D71" s="72" t="s">
         <v>8</v>
@@ -4786,7 +4785,7 @@
       <c r="F71" s="71"/>
       <c r="G71" s="74"/>
       <c r="H71" s="103" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I71" s="14"/>
       <c r="J71" s="14"/>
@@ -4809,11 +4808,11 @@
     </row>
     <row r="72" customFormat="false" ht="18.75" hidden="true" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A72" s="76" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B72" s="81"/>
       <c r="C72" s="82" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D72" s="72" t="s">
         <v>8</v>
@@ -4824,7 +4823,7 @@
       </c>
       <c r="G72" s="74"/>
       <c r="H72" s="75" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I72" s="14"/>
       <c r="J72" s="14"/>
@@ -4847,11 +4846,11 @@
     </row>
     <row r="73" customFormat="false" ht="18.75" hidden="true" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A73" s="76" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B73" s="81"/>
       <c r="C73" s="82" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D73" s="72" t="s">
         <v>8</v>
@@ -4862,7 +4861,7 @@
       </c>
       <c r="G73" s="74"/>
       <c r="H73" s="75" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I73" s="14"/>
       <c r="J73" s="14"/>
@@ -4885,11 +4884,11 @@
     </row>
     <row r="74" customFormat="false" ht="18.75" hidden="true" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A74" s="76" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B74" s="81"/>
       <c r="C74" s="82" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D74" s="72" t="s">
         <v>8</v>
@@ -4900,7 +4899,7 @@
       </c>
       <c r="G74" s="74"/>
       <c r="H74" s="75" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I74" s="14"/>
       <c r="J74" s="14"/>
@@ -4955,19 +4954,19 @@
         <v>7</v>
       </c>
       <c r="C76" s="82" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D76" s="72" t="s">
         <v>8</v>
       </c>
       <c r="E76" s="95" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F76" s="90" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G76" s="78" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H76" s="75"/>
       <c r="I76" s="14"/>
@@ -4991,11 +4990,11 @@
     </row>
     <row r="77" customFormat="false" ht="18.75" hidden="true" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A77" s="76" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B77" s="81"/>
       <c r="C77" s="71" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D77" s="72" t="s">
         <v>8</v>
@@ -5007,7 +5006,7 @@
         <v>1.234</v>
       </c>
       <c r="G77" s="78" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H77" s="75"/>
       <c r="I77" s="14"/>
@@ -5031,11 +5030,11 @@
     </row>
     <row r="78" customFormat="false" ht="18.75" hidden="true" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A78" s="76" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B78" s="81"/>
       <c r="C78" s="82" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D78" s="72" t="s">
         <v>8</v>
@@ -5047,7 +5046,7 @@
         <v>5.678</v>
       </c>
       <c r="G78" s="78" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H78" s="75"/>
       <c r="I78" s="14"/>
@@ -5076,7 +5075,7 @@
       </c>
       <c r="B79" s="81"/>
       <c r="C79" s="82" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D79" s="72" t="s">
         <v>8</v>
@@ -5108,11 +5107,11 @@
     </row>
     <row r="80" customFormat="false" ht="18.75" hidden="true" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A80" s="76" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B80" s="81"/>
       <c r="C80" s="82" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D80" s="72" t="s">
         <v>8</v>
@@ -5121,7 +5120,7 @@
       <c r="F80" s="90"/>
       <c r="G80" s="74"/>
       <c r="H80" s="103" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I80" s="14"/>
       <c r="J80" s="14"/>
@@ -5144,11 +5143,11 @@
     </row>
     <row r="81" customFormat="false" ht="18.75" hidden="true" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A81" s="76" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B81" s="81"/>
       <c r="C81" s="82" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D81" s="72" t="s">
         <v>8</v>
@@ -5159,7 +5158,7 @@
       </c>
       <c r="G81" s="74"/>
       <c r="H81" s="75" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I81" s="14"/>
       <c r="J81" s="14"/>
@@ -5182,11 +5181,11 @@
     </row>
     <row r="82" customFormat="false" ht="18.75" hidden="true" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A82" s="76" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B82" s="81"/>
       <c r="C82" s="82" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D82" s="72" t="s">
         <v>8</v>
@@ -5197,7 +5196,7 @@
       </c>
       <c r="G82" s="74"/>
       <c r="H82" s="75" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I82" s="14"/>
       <c r="J82" s="14"/>
@@ -5220,11 +5219,11 @@
     </row>
     <row r="83" customFormat="false" ht="18.75" hidden="true" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A83" s="76" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B83" s="81"/>
       <c r="C83" s="82" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D83" s="72" t="s">
         <v>8</v>
@@ -5235,7 +5234,7 @@
       </c>
       <c r="G83" s="74"/>
       <c r="H83" s="75" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I83" s="14"/>
       <c r="J83" s="14"/>
@@ -5258,7 +5257,7 @@
     </row>
     <row r="84" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="104" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B84" s="104"/>
       <c r="C84" s="105"/>
@@ -5290,7 +5289,7 @@
       <c r="A85" s="110"/>
       <c r="B85" s="110"/>
       <c r="C85" s="105" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D85" s="106" t="s">
         <v>8</v>
@@ -5302,7 +5301,7 @@
         <v>750</v>
       </c>
       <c r="G85" s="108" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H85" s="109"/>
       <c r="I85" s="14"/>
@@ -5328,7 +5327,7 @@
       <c r="A86" s="110"/>
       <c r="B86" s="110"/>
       <c r="C86" s="105" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D86" s="106" t="s">
         <v>8</v>
@@ -5340,7 +5339,7 @@
         <v>80</v>
       </c>
       <c r="G86" s="108" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H86" s="109"/>
       <c r="I86" s="14"/>
@@ -5366,7 +5365,7 @@
       <c r="A87" s="110"/>
       <c r="B87" s="110"/>
       <c r="C87" s="105" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D87" s="106" t="s">
         <v>8</v>
@@ -5378,7 +5377,7 @@
         <v>900</v>
       </c>
       <c r="G87" s="108" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H87" s="109"/>
       <c r="I87" s="14"/>
@@ -5404,7 +5403,7 @@
       <c r="A88" s="110"/>
       <c r="B88" s="110"/>
       <c r="C88" s="105" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D88" s="106" t="s">
         <v>8</v>
@@ -5416,7 +5415,7 @@
         <v>1200</v>
       </c>
       <c r="G88" s="108" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H88" s="109"/>
       <c r="I88" s="14"/>
@@ -5442,7 +5441,7 @@
       <c r="A89" s="110"/>
       <c r="B89" s="110"/>
       <c r="C89" s="105" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D89" s="106" t="s">
         <v>8</v>
@@ -5454,10 +5453,10 @@
         <v>105</v>
       </c>
       <c r="G89" s="108" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H89" s="109" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="I89" s="14"/>
       <c r="J89" s="14"/>
@@ -5482,7 +5481,7 @@
       <c r="A90" s="110"/>
       <c r="B90" s="110"/>
       <c r="C90" s="105" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D90" s="106" t="s">
         <v>8</v>
@@ -5494,10 +5493,10 @@
         <v>12600</v>
       </c>
       <c r="G90" s="108" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H90" s="109" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="I90" s="14"/>
       <c r="J90" s="14"/>
@@ -5522,22 +5521,22 @@
       <c r="A91" s="110"/>
       <c r="B91" s="110"/>
       <c r="C91" s="105" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D91" s="106" t="s">
         <v>8</v>
       </c>
       <c r="E91" s="107" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F91" s="105" t="n">
         <v>3</v>
       </c>
       <c r="G91" s="108" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H91" s="109" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="I91" s="14"/>
       <c r="J91" s="14"/>
@@ -5560,24 +5559,24 @@
     </row>
     <row r="92" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="111" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B92" s="111"/>
       <c r="C92" s="112" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D92" s="113" t="s">
         <v>8</v>
       </c>
       <c r="E92" s="114" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F92" s="112"/>
       <c r="G92" s="115" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H92" s="116" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="I92" s="25"/>
       <c r="J92" s="25"/>
@@ -5600,7 +5599,7 @@
     </row>
     <row r="93" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="104" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B93" s="104"/>
       <c r="C93" s="105"/>
@@ -5632,7 +5631,7 @@
       <c r="A94" s="110"/>
       <c r="B94" s="110"/>
       <c r="C94" s="117" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D94" s="106" t="s">
         <v>8</v>
@@ -5644,10 +5643,10 @@
         <v>45</v>
       </c>
       <c r="G94" s="118" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H94" s="109" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="I94" s="14"/>
       <c r="J94" s="14"/>
@@ -5672,22 +5671,22 @@
       <c r="A95" s="110"/>
       <c r="B95" s="110"/>
       <c r="C95" s="105" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D95" s="106" t="s">
         <v>8</v>
       </c>
       <c r="E95" s="107" t="n">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="F95" s="105" t="n">
         <v>75</v>
       </c>
       <c r="G95" s="118" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H95" s="109" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="I95" s="14"/>
       <c r="J95" s="14"/>
@@ -5712,7 +5711,7 @@
       <c r="A96" s="110"/>
       <c r="B96" s="110"/>
       <c r="C96" s="105" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D96" s="106" t="s">
         <v>8</v>
@@ -5724,10 +5723,10 @@
         <v>450</v>
       </c>
       <c r="G96" s="108" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H96" s="109" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="I96" s="14"/>
       <c r="J96" s="14"/>
@@ -5752,7 +5751,7 @@
       <c r="A97" s="111"/>
       <c r="B97" s="111"/>
       <c r="C97" s="112" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D97" s="113" t="s">
         <v>8</v>
@@ -5764,10 +5763,10 @@
         <v>3600</v>
       </c>
       <c r="G97" s="115" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H97" s="116" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="I97" s="25"/>
       <c r="J97" s="25"/>
@@ -15038,8 +15037,8 @@
   </sheetPr>
   <dimension ref="A1:K500"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="true" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15054,37 +15053,37 @@
   <sheetData>
     <row r="1" s="128" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="127" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B1" s="127" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C1" s="127" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D1" s="127" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E1" s="127" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F1" s="127" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G1" s="127" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H1" s="127" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="I1" s="127" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J1" s="125" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="K1" s="126" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2" s="131" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15093,7 +15092,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="130" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C2" s="125" t="n">
         <v>1</v>
@@ -15124,78 +15123,46 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" s="131" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="129" t="n">
+    <row r="3" s="131" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="129" t="str">
         <f aca="false">IF(A2 &lt; fixed_wells, A2 + 1, "")</f>
-        <v>2</v>
-      </c>
-      <c r="B3" s="130" t="s">
-        <v>190</v>
-      </c>
-      <c r="C3" s="125" t="n">
-        <v>150</v>
-      </c>
-      <c r="D3" s="125" t="n">
-        <v>30</v>
-      </c>
-      <c r="E3" s="125" t="n">
-        <v>35</v>
-      </c>
-      <c r="F3" s="125" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" s="125" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" s="125" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" s="125" t="n">
-        <v>0</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B3" s="130"/>
+      <c r="C3" s="125"/>
+      <c r="D3" s="125"/>
+      <c r="E3" s="125"/>
+      <c r="F3" s="125"/>
+      <c r="G3" s="125"/>
+      <c r="H3" s="125"/>
+      <c r="I3" s="125"/>
       <c r="J3" s="125" t="n">
         <v>0</v>
       </c>
-      <c r="K3" s="126" t="n">
+      <c r="K3" s="126" t="str">
         <f aca="false">IF(NOT(A3=""), SUM(C3:J3), "")</f>
-        <v>215</v>
-      </c>
-    </row>
-    <row r="4" s="131" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="129" t="n">
+        <v/>
+      </c>
+    </row>
+    <row r="4" s="131" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="129" t="str">
         <f aca="false">IF(A3 &lt; fixed_wells, A3 + 1, "")</f>
-        <v>3</v>
-      </c>
-      <c r="B4" s="130" t="s">
-        <v>191</v>
-      </c>
-      <c r="C4" s="125" t="n">
-        <v>150</v>
-      </c>
-      <c r="D4" s="125" t="n">
-        <v>30</v>
-      </c>
-      <c r="E4" s="125" t="n">
-        <v>35</v>
-      </c>
-      <c r="F4" s="125" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" s="125" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" s="125" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" s="125" t="n">
-        <v>0</v>
-      </c>
+        <v/>
+      </c>
+      <c r="B4" s="130"/>
+      <c r="C4" s="125"/>
+      <c r="D4" s="125"/>
+      <c r="E4" s="125"/>
+      <c r="F4" s="125"/>
+      <c r="G4" s="125"/>
+      <c r="H4" s="125"/>
+      <c r="I4" s="125"/>
       <c r="J4" s="125" t="n">
         <v>0</v>
       </c>
-      <c r="K4" s="126" t="n">
+      <c r="K4" s="126" t="str">
         <f aca="false">IF(NOT(A4=""), SUM(C4:J4), "")</f>
-        <v>215</v>
+        <v/>
       </c>
     </row>
     <row r="5" s="131" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22210,37 +22177,37 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="132" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B1" s="132" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C1" s="132" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D1" s="132" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E1" s="132" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F1" s="132" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G1" s="132" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H1" s="132" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="I1" s="132" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="J1" s="132" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="K1" s="131" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22290,95 +22257,95 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="0" t="str">
         <f aca="false">IF(NOT('Manual Experiment Interface'!A3=""),'Manual Experiment Interface'!A3,"")</f>
-        <v>2</v>
+        <v/>
       </c>
       <c r="B3" s="0" t="str">
         <f aca="false">IF(NOT('Manual Experiment Interface'!B3=""),'Manual Experiment Interface'!B3,"")</f>
-        <v>20190514-JT-15</v>
-      </c>
-      <c r="C3" s="0" t="n">
+        <v/>
+      </c>
+      <c r="C3" s="0" t="str">
         <f aca="false">IF(NOT('Manual Experiment Interface'!C3=""),'Manual Experiment Interface'!C3,"")</f>
-        <v>150</v>
-      </c>
-      <c r="D3" s="0" t="n">
+        <v/>
+      </c>
+      <c r="D3" s="0" t="str">
         <f aca="false">IF(NOT('Manual Experiment Interface'!D3=""),'Manual Experiment Interface'!D3,"")</f>
-        <v>30</v>
-      </c>
-      <c r="E3" s="0" t="n">
+        <v/>
+      </c>
+      <c r="E3" s="0" t="str">
         <f aca="false">IF(NOT('Manual Experiment Interface'!E3=""),'Manual Experiment Interface'!E3,"")</f>
-        <v>35</v>
-      </c>
-      <c r="F3" s="0" t="n">
+        <v/>
+      </c>
+      <c r="F3" s="0" t="str">
         <f aca="false">IF(NOT('Manual Experiment Interface'!F3=""),'Manual Experiment Interface'!F3,"")</f>
-        <v>0</v>
-      </c>
-      <c r="G3" s="0" t="n">
+        <v/>
+      </c>
+      <c r="G3" s="0" t="str">
         <f aca="false">IF(NOT('Manual Experiment Interface'!G3=""),'Manual Experiment Interface'!G3,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H3" s="0" t="n">
+        <v/>
+      </c>
+      <c r="H3" s="0" t="str">
         <f aca="false">IF(NOT('Manual Experiment Interface'!H3=""),'Manual Experiment Interface'!H3,"")</f>
-        <v>0</v>
-      </c>
-      <c r="I3" s="0" t="n">
+        <v/>
+      </c>
+      <c r="I3" s="0" t="str">
         <f aca="false">IF(NOT('Manual Experiment Interface'!I3=""),'Manual Experiment Interface'!I3,"")</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="J3" s="0" t="n">
         <f aca="false">IF(NOT('Manual Experiment Interface'!J3=""),'Manual Experiment Interface'!J3,"")</f>
         <v>0</v>
       </c>
-      <c r="K3" s="0" t="n">
+      <c r="K3" s="0" t="str">
         <f aca="false">IF(NOT('Manual Experiment Interface'!K3=""),'Manual Experiment Interface'!K3,"")</f>
-        <v>215</v>
+        <v/>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="0" t="str">
         <f aca="false">IF(NOT('Manual Experiment Interface'!A4=""),'Manual Experiment Interface'!A4,"")</f>
-        <v>3</v>
+        <v/>
       </c>
       <c r="B4" s="0" t="str">
         <f aca="false">IF(NOT('Manual Experiment Interface'!B4=""),'Manual Experiment Interface'!B4,"")</f>
-        <v>20190306-JT-11</v>
-      </c>
-      <c r="C4" s="0" t="n">
+        <v/>
+      </c>
+      <c r="C4" s="0" t="str">
         <f aca="false">IF(NOT('Manual Experiment Interface'!C4=""),'Manual Experiment Interface'!C4,"")</f>
-        <v>150</v>
-      </c>
-      <c r="D4" s="0" t="n">
+        <v/>
+      </c>
+      <c r="D4" s="0" t="str">
         <f aca="false">IF(NOT('Manual Experiment Interface'!D4=""),'Manual Experiment Interface'!D4,"")</f>
-        <v>30</v>
-      </c>
-      <c r="E4" s="0" t="n">
+        <v/>
+      </c>
+      <c r="E4" s="0" t="str">
         <f aca="false">IF(NOT('Manual Experiment Interface'!E4=""),'Manual Experiment Interface'!E4,"")</f>
-        <v>35</v>
-      </c>
-      <c r="F4" s="0" t="n">
+        <v/>
+      </c>
+      <c r="F4" s="0" t="str">
         <f aca="false">IF(NOT('Manual Experiment Interface'!F4=""),'Manual Experiment Interface'!F4,"")</f>
-        <v>0</v>
-      </c>
-      <c r="G4" s="0" t="n">
+        <v/>
+      </c>
+      <c r="G4" s="0" t="str">
         <f aca="false">IF(NOT('Manual Experiment Interface'!G4=""),'Manual Experiment Interface'!G4,"")</f>
-        <v>0</v>
-      </c>
-      <c r="H4" s="0" t="n">
+        <v/>
+      </c>
+      <c r="H4" s="0" t="str">
         <f aca="false">IF(NOT('Manual Experiment Interface'!H4=""),'Manual Experiment Interface'!H4,"")</f>
-        <v>0</v>
-      </c>
-      <c r="I4" s="0" t="n">
+        <v/>
+      </c>
+      <c r="I4" s="0" t="str">
         <f aca="false">IF(NOT('Manual Experiment Interface'!I4=""),'Manual Experiment Interface'!I4,"")</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="J4" s="0" t="n">
         <f aca="false">IF(NOT('Manual Experiment Interface'!J4=""),'Manual Experiment Interface'!J4,"")</f>
         <v>0</v>
       </c>
-      <c r="K4" s="0" t="n">
+      <c r="K4" s="0" t="str">
         <f aca="false">IF(NOT('Manual Experiment Interface'!K4=""),'Manual Experiment Interface'!K4,"")</f>
-        <v>215</v>
+        <v/>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26744,16 +26711,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="135" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C1" s="136" t="s">
         <v>8</v>
       </c>
       <c r="D1" s="135" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1" s="137" t="s">
         <v>194</v>
-      </c>
-      <c r="E1" s="137" t="s">
-        <v>195</v>
       </c>
       <c r="F1" s="138"/>
       <c r="G1" s="138"/>
@@ -26804,7 +26771,7 @@
     <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="15"/>
       <c r="B3" s="10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>8</v>
@@ -26814,7 +26781,7 @@
         <v>1.1</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F3" s="138"/>
       <c r="G3" s="138"/>
@@ -26838,7 +26805,7 @@
     <row r="4" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="15"/>
       <c r="B4" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>8</v>
@@ -26847,7 +26814,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F4" s="138"/>
       <c r="G4" s="138"/>
@@ -26878,10 +26845,10 @@
       </c>
       <c r="D5" s="139" t="str">
         <f aca="false">'User Interface'!E4</f>
-        <v>HC</v>
+        <v>LBL</v>
       </c>
       <c r="E5" s="139" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F5" s="138"/>
       <c r="G5" s="138"/>
@@ -26932,17 +26899,17 @@
     <row r="7" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="32"/>
       <c r="B7" s="27" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C7" s="28" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="27" t="n">
         <f aca="false">'User Interface'!wellcount</f>
-        <v>6</v>
+        <v>96</v>
       </c>
       <c r="E7" s="27" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F7" s="138"/>
       <c r="G7" s="138"/>
@@ -26966,7 +26933,7 @@
     <row r="8" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="32"/>
       <c r="B8" s="27" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C8" s="28" t="s">
         <v>8</v>
@@ -26976,7 +26943,7 @@
         <v>[7]</v>
       </c>
       <c r="E8" s="27" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F8" s="138"/>
       <c r="G8" s="138"/>
@@ -26999,7 +26966,7 @@
     </row>
     <row r="9" s="145" customFormat="true" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="141" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B9" s="142"/>
       <c r="C9" s="143"/>
@@ -27030,7 +26997,7 @@
         <v>0</v>
       </c>
       <c r="B10" s="147" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C10" s="148" t="s">
         <v>8</v>
@@ -27040,7 +27007,7 @@
         <v>[[2,3,1,7]]</v>
       </c>
       <c r="E10" s="147" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F10" s="144"/>
       <c r="G10" s="144"/>
@@ -27067,7 +27034,7 @@
         <v>0</v>
       </c>
       <c r="B11" s="147" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C11" s="148" t="s">
         <v>8</v>
@@ -27077,7 +27044,7 @@
         <v>[[500,500]]</v>
       </c>
       <c r="E11" s="147" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F11" s="144"/>
       <c r="G11" s="144"/>
@@ -27104,17 +27071,17 @@
         <v>0</v>
       </c>
       <c r="B12" s="147" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C12" s="148" t="s">
         <v>8</v>
       </c>
       <c r="D12" s="147" t="n">
         <f aca="false">'User Interface'!E11</f>
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="E12" s="147" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F12" s="144"/>
       <c r="G12" s="144"/>
@@ -27141,14 +27108,14 @@
         <v>0</v>
       </c>
       <c r="B13" s="147" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C13" s="148" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="147" t="n">
+      <c r="D13" s="147" t="str">
         <f aca="false">'User Interface'!E12</f>
-        <v>0</v>
+        <v>My Example Run</v>
       </c>
       <c r="E13" s="147"/>
       <c r="F13" s="144"/>
@@ -27176,7 +27143,7 @@
         <v>#</v>
       </c>
       <c r="B14" s="147" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C14" s="148" t="s">
         <v>8</v>
@@ -27186,7 +27153,7 @@
         <v>[[2,3,1]]</v>
       </c>
       <c r="E14" s="147" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F14" s="138"/>
       <c r="G14" s="138"/>
@@ -27213,7 +27180,7 @@
         <v>#</v>
       </c>
       <c r="B15" s="147" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C15" s="148" t="s">
         <v>8</v>
@@ -27223,7 +27190,7 @@
         <v>[[215, 215]]</v>
       </c>
       <c r="E15" s="147" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F15" s="138"/>
       <c r="G15" s="138"/>
@@ -27250,7 +27217,7 @@
         <v>#</v>
       </c>
       <c r="B16" s="147" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C16" s="148" t="s">
         <v>8</v>
@@ -27260,7 +27227,7 @@
         <v>0</v>
       </c>
       <c r="E16" s="147" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F16" s="138"/>
       <c r="G16" s="138"/>
@@ -27287,7 +27254,7 @@
         <v>#</v>
       </c>
       <c r="B17" s="147" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C17" s="148" t="s">
         <v>8</v>
@@ -27318,7 +27285,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="149" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B18" s="150"/>
       <c r="C18" s="150"/>
@@ -27328,20 +27295,20 @@
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="150"/>
       <c r="B19" s="150" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C19" s="150"/>
       <c r="D19" s="147" t="n">
         <f aca="false">'User Interface'!E19</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E19" s="150" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="70" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B20" s="71"/>
       <c r="C20" s="72"/>
@@ -27393,10 +27360,10 @@
     </row>
     <row r="22" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="151" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B22" s="152" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C22" s="72" t="s">
         <v>8</v>
@@ -27405,7 +27372,7 @@
         <v>0.2</v>
       </c>
       <c r="E22" s="71" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F22" s="138"/>
       <c r="G22" s="138"/>
@@ -27428,10 +27395,10 @@
     </row>
     <row r="23" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="153" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B23" s="152" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C23" s="72" t="s">
         <v>8</v>
@@ -27440,7 +27407,7 @@
         <v>1.5</v>
       </c>
       <c r="E23" s="71" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F23" s="138"/>
       <c r="G23" s="138"/>
@@ -27488,7 +27455,7 @@
     </row>
     <row r="25" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="70" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B25" s="71"/>
       <c r="C25" s="72"/>
@@ -27544,17 +27511,17 @@
         <v>0</v>
       </c>
       <c r="B27" s="71" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C27" s="72" t="s">
         <v>8</v>
       </c>
       <c r="D27" s="88" t="str">
         <f aca="false">'User Interface'!E22</f>
-        <v>['GBL']</v>
+        <v>['DMF']</v>
       </c>
       <c r="E27" s="71" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F27" s="138"/>
       <c r="G27" s="138"/>
@@ -27581,7 +27548,7 @@
         <v>#</v>
       </c>
       <c r="B28" s="88" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C28" s="98" t="s">
         <v>8</v>
@@ -27591,7 +27558,7 @@
         <v>0</v>
       </c>
       <c r="E28" s="88" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F28" s="138"/>
       <c r="G28" s="138"/>
@@ -27618,7 +27585,7 @@
         <v>#</v>
       </c>
       <c r="B29" s="82" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C29" s="72" t="s">
         <v>8</v>
@@ -27628,7 +27595,7 @@
         <v>1.5</v>
       </c>
       <c r="E29" s="71" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F29" s="138"/>
       <c r="G29" s="138"/>
@@ -27655,7 +27622,7 @@
         <v>#</v>
       </c>
       <c r="B30" s="82" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C30" s="72" t="s">
         <v>8</v>
@@ -27665,7 +27632,7 @@
         <v>7.63</v>
       </c>
       <c r="E30" s="71" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F30" s="138"/>
       <c r="G30" s="138"/>
@@ -27692,7 +27659,7 @@
         <v>#</v>
       </c>
       <c r="B31" s="82" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C31" s="72" t="s">
         <v>8</v>
@@ -27702,7 +27669,7 @@
         <v>0</v>
       </c>
       <c r="E31" s="71" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F31" s="138"/>
       <c r="G31" s="138"/>
@@ -27729,7 +27696,7 @@
         <v>#</v>
       </c>
       <c r="B32" s="82" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C32" s="72" t="s">
         <v>8</v>
@@ -27739,7 +27706,7 @@
         <v>0</v>
       </c>
       <c r="E32" s="71" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F32" s="138"/>
       <c r="G32" s="138"/>
@@ -27766,7 +27733,7 @@
         <v>#</v>
       </c>
       <c r="B33" s="82" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C33" s="72" t="s">
         <v>8</v>
@@ -27776,7 +27743,7 @@
         <v>0</v>
       </c>
       <c r="E33" s="71" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F33" s="138"/>
       <c r="G33" s="138"/>
@@ -27803,7 +27770,7 @@
         <v>#</v>
       </c>
       <c r="B34" s="82" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C34" s="72" t="s">
         <v>8</v>
@@ -27813,7 +27780,7 @@
         <v>0</v>
       </c>
       <c r="E34" s="71" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F34" s="138"/>
       <c r="G34" s="138"/>
@@ -27865,17 +27832,17 @@
         <v>0</v>
       </c>
       <c r="B36" s="71" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C36" s="72" t="s">
         <v>8</v>
       </c>
       <c r="D36" s="71" t="str">
         <f aca="false">'User Interface'!E31</f>
-        <v>['PbI2','EtNH3I','GBL']</v>
+        <v>['PbI2','tButylammoniumIodide','DMF']</v>
       </c>
       <c r="E36" s="71" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F36" s="138"/>
       <c r="G36" s="138"/>
@@ -27902,7 +27869,7 @@
         <v>#</v>
       </c>
       <c r="B37" s="88" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C37" s="98" t="s">
         <v>8</v>
@@ -27912,7 +27879,7 @@
         <v>0</v>
       </c>
       <c r="E37" s="88" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F37" s="138"/>
       <c r="G37" s="138"/>
@@ -27939,17 +27906,17 @@
         <v>0</v>
       </c>
       <c r="B38" s="71" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C38" s="72" t="s">
         <v>8</v>
       </c>
       <c r="D38" s="88" t="n">
         <f aca="false">'User Interface'!E32</f>
-        <v>1.5</v>
+        <v>2.52</v>
       </c>
       <c r="E38" s="71" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F38" s="138"/>
       <c r="G38" s="138"/>
@@ -27976,17 +27943,17 @@
         <v>0</v>
       </c>
       <c r="B39" s="71" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C39" s="72" t="s">
         <v>8</v>
       </c>
       <c r="D39" s="88" t="n">
         <f aca="false">'User Interface'!E33</f>
-        <v>3</v>
+        <v>2.52</v>
       </c>
       <c r="E39" s="71" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F39" s="138"/>
       <c r="G39" s="138"/>
@@ -28013,7 +27980,7 @@
         <v>#</v>
       </c>
       <c r="B40" s="82" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C40" s="72" t="s">
         <v>8</v>
@@ -28023,7 +27990,7 @@
         <v>0</v>
       </c>
       <c r="E40" s="71" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F40" s="138"/>
       <c r="G40" s="138"/>
@@ -28050,7 +28017,7 @@
         <v>#</v>
       </c>
       <c r="B41" s="71" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C41" s="72" t="s">
         <v>8</v>
@@ -28060,7 +28027,7 @@
         <v>0</v>
       </c>
       <c r="E41" s="71" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F41" s="138"/>
       <c r="G41" s="138"/>
@@ -28087,7 +28054,7 @@
         <v>#</v>
       </c>
       <c r="B42" s="71" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C42" s="72" t="s">
         <v>8</v>
@@ -28097,7 +28064,7 @@
         <v>0</v>
       </c>
       <c r="E42" s="71" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F42" s="138"/>
       <c r="G42" s="138"/>
@@ -28124,7 +28091,7 @@
         <v>#</v>
       </c>
       <c r="B43" s="71" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C43" s="72" t="s">
         <v>8</v>
@@ -28134,7 +28101,7 @@
         <v>0</v>
       </c>
       <c r="E43" s="71" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F43" s="138"/>
       <c r="G43" s="138"/>
@@ -28186,17 +28153,17 @@
         <v>0</v>
       </c>
       <c r="B45" s="71" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C45" s="72" t="s">
         <v>8</v>
       </c>
       <c r="D45" s="71" t="str">
         <f aca="false">'User Interface'!E40</f>
-        <v>['EtNH3I','GBL']</v>
+        <v>['tButylammoniumIodide','DMF']</v>
       </c>
       <c r="E45" s="71" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F45" s="138"/>
       <c r="G45" s="138"/>
@@ -28223,7 +28190,7 @@
         <v>#</v>
       </c>
       <c r="B46" s="88" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C46" s="98" t="s">
         <v>8</v>
@@ -28233,7 +28200,7 @@
         <v>0</v>
       </c>
       <c r="E46" s="88" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F46" s="138"/>
       <c r="G46" s="138"/>
@@ -28260,17 +28227,17 @@
         <v>0</v>
       </c>
       <c r="B47" s="154" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C47" s="72" t="s">
         <v>8</v>
       </c>
       <c r="D47" s="71" t="n">
         <f aca="false">'User Interface'!E41</f>
-        <v>6</v>
+        <v>2.36</v>
       </c>
       <c r="E47" s="71" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F47" s="138"/>
       <c r="G47" s="138"/>
@@ -28297,7 +28264,7 @@
         <v>#</v>
       </c>
       <c r="B48" s="82" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C48" s="72" t="s">
         <v>8</v>
@@ -28307,7 +28274,7 @@
         <v>1.33</v>
       </c>
       <c r="E48" s="71" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F48" s="138"/>
       <c r="G48" s="138"/>
@@ -28334,7 +28301,7 @@
         <v>#</v>
       </c>
       <c r="B49" s="82" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C49" s="72" t="s">
         <v>8</v>
@@ -28344,7 +28311,7 @@
         <v>1.2</v>
       </c>
       <c r="E49" s="71" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F49" s="138"/>
       <c r="G49" s="138"/>
@@ -28371,7 +28338,7 @@
         <v>#</v>
       </c>
       <c r="B50" s="71" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C50" s="72" t="s">
         <v>8</v>
@@ -28381,7 +28348,7 @@
         <v>0</v>
       </c>
       <c r="E50" s="71" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F50" s="138"/>
       <c r="G50" s="138"/>
@@ -28408,7 +28375,7 @@
         <v>#</v>
       </c>
       <c r="B51" s="71" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C51" s="72" t="s">
         <v>8</v>
@@ -28418,7 +28385,7 @@
         <v>0</v>
       </c>
       <c r="E51" s="71" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F51" s="138"/>
       <c r="G51" s="138"/>
@@ -28445,7 +28412,7 @@
         <v>#</v>
       </c>
       <c r="B52" s="71" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C52" s="72" t="s">
         <v>8</v>
@@ -28455,7 +28422,7 @@
         <v>0</v>
       </c>
       <c r="E52" s="71" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F52" s="138"/>
       <c r="G52" s="138"/>
@@ -28507,7 +28474,7 @@
         <v>#</v>
       </c>
       <c r="B54" s="71" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C54" s="72" t="s">
         <v>8</v>
@@ -28517,7 +28484,7 @@
         <v>['PbI2','DMSO','DMF']</v>
       </c>
       <c r="E54" s="71" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F54" s="138"/>
       <c r="G54" s="138"/>
@@ -28544,7 +28511,7 @@
         <v>#</v>
       </c>
       <c r="B55" s="88" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C55" s="98" t="s">
         <v>8</v>
@@ -28554,7 +28521,7 @@
         <v>0</v>
       </c>
       <c r="E55" s="88" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F55" s="138"/>
       <c r="G55" s="138"/>
@@ -28581,7 +28548,7 @@
         <v>#</v>
       </c>
       <c r="B56" s="154" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C56" s="72" t="s">
         <v>8</v>
@@ -28591,7 +28558,7 @@
         <v>1.5</v>
       </c>
       <c r="E56" s="71" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F56" s="138"/>
       <c r="G56" s="138"/>
@@ -28618,7 +28585,7 @@
         <v>#</v>
       </c>
       <c r="B57" s="154" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C57" s="72" t="s">
         <v>8</v>
@@ -28628,7 +28595,7 @@
         <v>7.63</v>
       </c>
       <c r="E57" s="71" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F57" s="138"/>
       <c r="G57" s="138"/>
@@ -28655,7 +28622,7 @@
         <v>#</v>
       </c>
       <c r="B58" s="82" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C58" s="72" t="s">
         <v>8</v>
@@ -28665,7 +28632,7 @@
         <v>0</v>
       </c>
       <c r="E58" s="71" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F58" s="138"/>
       <c r="G58" s="138"/>
@@ -28692,7 +28659,7 @@
         <v>#</v>
       </c>
       <c r="B59" s="71" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C59" s="72" t="s">
         <v>8</v>
@@ -28702,7 +28669,7 @@
         <v>0</v>
       </c>
       <c r="E59" s="71" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F59" s="138"/>
       <c r="G59" s="138"/>
@@ -28729,7 +28696,7 @@
         <v>#</v>
       </c>
       <c r="B60" s="71" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C60" s="72" t="s">
         <v>8</v>
@@ -28739,7 +28706,7 @@
         <v>0</v>
       </c>
       <c r="E60" s="71" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F60" s="138"/>
       <c r="G60" s="138"/>
@@ -28766,7 +28733,7 @@
         <v>#</v>
       </c>
       <c r="B61" s="71" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C61" s="72" t="s">
         <v>8</v>
@@ -28776,7 +28743,7 @@
         <v>0</v>
       </c>
       <c r="E61" s="71" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F61" s="138"/>
       <c r="G61" s="138"/>
@@ -28828,7 +28795,7 @@
         <v>#</v>
       </c>
       <c r="B63" s="71" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C63" s="72" t="s">
         <v>8</v>
@@ -28838,7 +28805,7 @@
         <v>['MeNH3I','PbI2','DMSO', 'DMF']</v>
       </c>
       <c r="E63" s="71" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F63" s="138"/>
       <c r="G63" s="138"/>
@@ -28865,7 +28832,7 @@
         <v>#</v>
       </c>
       <c r="B64" s="88" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C64" s="98" t="s">
         <v>8</v>
@@ -28875,7 +28842,7 @@
         <v>0</v>
       </c>
       <c r="E64" s="88" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F64" s="138"/>
       <c r="G64" s="138"/>
@@ -28902,7 +28869,7 @@
         <v>#</v>
       </c>
       <c r="B65" s="154" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C65" s="72" t="s">
         <v>8</v>
@@ -28912,7 +28879,7 @@
         <v>1.22</v>
       </c>
       <c r="E65" s="71" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F65" s="138"/>
       <c r="G65" s="138"/>
@@ -28939,7 +28906,7 @@
         <v>#</v>
       </c>
       <c r="B66" s="155" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C66" s="72" t="s">
         <v>8</v>
@@ -28949,7 +28916,7 @@
         <v>1.33</v>
       </c>
       <c r="E66" s="71" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F66" s="138"/>
       <c r="G66" s="138"/>
@@ -28976,7 +28943,7 @@
         <v>#</v>
       </c>
       <c r="B67" s="82" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C67" s="72" t="s">
         <v>8</v>
@@ -28986,7 +28953,7 @@
         <v>7</v>
       </c>
       <c r="E67" s="71" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F67" s="138"/>
       <c r="G67" s="138"/>
@@ -29013,7 +28980,7 @@
         <v>#</v>
       </c>
       <c r="B68" s="71" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C68" s="72" t="s">
         <v>8</v>
@@ -29023,7 +28990,7 @@
         <v>0</v>
       </c>
       <c r="E68" s="71" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F68" s="138"/>
       <c r="G68" s="138"/>
@@ -29050,7 +29017,7 @@
         <v>#</v>
       </c>
       <c r="B69" s="71" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C69" s="72" t="s">
         <v>8</v>
@@ -29060,7 +29027,7 @@
         <v>0</v>
       </c>
       <c r="E69" s="71" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F69" s="138"/>
       <c r="G69" s="138"/>
@@ -29087,7 +29054,7 @@
         <v>#</v>
       </c>
       <c r="B70" s="71" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C70" s="72" t="s">
         <v>8</v>
@@ -29097,7 +29064,7 @@
         <v>0</v>
       </c>
       <c r="E70" s="71" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F70" s="138"/>
       <c r="G70" s="138"/>
@@ -29149,7 +29116,7 @@
         <v>#</v>
       </c>
       <c r="B72" s="82" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C72" s="72" t="s">
         <v>8</v>
@@ -29159,7 +29126,7 @@
         <v>['PbI2','DMSO','DMF']</v>
       </c>
       <c r="E72" s="71" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F72" s="138"/>
       <c r="G72" s="138"/>
@@ -29186,7 +29153,7 @@
         <v>#</v>
       </c>
       <c r="B73" s="84" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C73" s="98" t="s">
         <v>8</v>
@@ -29196,7 +29163,7 @@
         <v>0</v>
       </c>
       <c r="E73" s="88" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F73" s="138"/>
       <c r="G73" s="138"/>
@@ -29223,7 +29190,7 @@
         <v>#</v>
       </c>
       <c r="B74" s="155" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C74" s="72" t="s">
         <v>8</v>
@@ -29233,7 +29200,7 @@
         <v>1.5</v>
       </c>
       <c r="E74" s="71" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F74" s="138"/>
       <c r="G74" s="138"/>
@@ -29260,7 +29227,7 @@
         <v>#</v>
       </c>
       <c r="B75" s="155" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C75" s="72" t="s">
         <v>8</v>
@@ -29270,7 +29237,7 @@
         <v>7.63</v>
       </c>
       <c r="E75" s="71" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F75" s="138"/>
       <c r="G75" s="138"/>
@@ -29297,7 +29264,7 @@
         <v>#</v>
       </c>
       <c r="B76" s="82" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C76" s="72" t="s">
         <v>8</v>
@@ -29307,7 +29274,7 @@
         <v>0</v>
       </c>
       <c r="E76" s="71" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F76" s="138"/>
       <c r="G76" s="138"/>
@@ -29334,7 +29301,7 @@
         <v>#</v>
       </c>
       <c r="B77" s="82" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C77" s="72" t="s">
         <v>8</v>
@@ -29344,7 +29311,7 @@
         <v>0</v>
       </c>
       <c r="E77" s="71" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F77" s="138"/>
       <c r="G77" s="138"/>
@@ -29371,7 +29338,7 @@
         <v>#</v>
       </c>
       <c r="B78" s="82" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C78" s="72" t="s">
         <v>8</v>
@@ -29381,7 +29348,7 @@
         <v>0</v>
       </c>
       <c r="E78" s="71" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F78" s="138"/>
       <c r="G78" s="138"/>
@@ -29408,7 +29375,7 @@
         <v>#</v>
       </c>
       <c r="B79" s="82" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C79" s="72" t="s">
         <v>8</v>
@@ -29418,7 +29385,7 @@
         <v>0</v>
       </c>
       <c r="E79" s="71" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F79" s="138"/>
       <c r="G79" s="138"/>
@@ -29470,7 +29437,7 @@
         <v>0</v>
       </c>
       <c r="B81" s="82" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C81" s="72" t="s">
         <v>8</v>
@@ -29480,7 +29447,7 @@
         <v>['FAH']</v>
       </c>
       <c r="E81" s="71" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F81" s="138"/>
       <c r="G81" s="138"/>
@@ -29507,7 +29474,7 @@
         <v>#</v>
       </c>
       <c r="B82" s="84" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C82" s="98" t="s">
         <v>8</v>
@@ -29517,7 +29484,7 @@
         <v>0</v>
       </c>
       <c r="E82" s="88" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F82" s="138"/>
       <c r="G82" s="138"/>
@@ -29544,7 +29511,7 @@
         <v>#</v>
       </c>
       <c r="B83" s="155" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C83" s="72" t="s">
         <v>8</v>
@@ -29554,7 +29521,7 @@
         <v>1.5</v>
       </c>
       <c r="E83" s="71" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F83" s="138"/>
       <c r="G83" s="138"/>
@@ -29581,7 +29548,7 @@
         <v>#</v>
       </c>
       <c r="B84" s="155" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C84" s="72" t="s">
         <v>8</v>
@@ -29591,7 +29558,7 @@
         <v>7.63</v>
       </c>
       <c r="E84" s="71" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F84" s="138"/>
       <c r="G84" s="138"/>
@@ -29618,7 +29585,7 @@
         <v>#</v>
       </c>
       <c r="B85" s="82" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C85" s="72" t="s">
         <v>8</v>
@@ -29628,7 +29595,7 @@
         <v>0</v>
       </c>
       <c r="E85" s="71" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F85" s="138"/>
       <c r="G85" s="138"/>
@@ -29655,7 +29622,7 @@
         <v>#</v>
       </c>
       <c r="B86" s="82" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C86" s="72" t="s">
         <v>8</v>
@@ -29665,7 +29632,7 @@
         <v>0</v>
       </c>
       <c r="E86" s="71" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F86" s="138"/>
       <c r="G86" s="138"/>
@@ -29692,7 +29659,7 @@
         <v>#</v>
       </c>
       <c r="B87" s="82" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C87" s="72" t="s">
         <v>8</v>
@@ -29702,7 +29669,7 @@
         <v>0</v>
       </c>
       <c r="E87" s="71" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F87" s="138"/>
       <c r="G87" s="138"/>
@@ -29729,7 +29696,7 @@
         <v>#</v>
       </c>
       <c r="B88" s="82" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C88" s="72" t="s">
         <v>8</v>
@@ -29739,7 +29706,7 @@
         <v>0</v>
       </c>
       <c r="E88" s="71" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F88" s="138"/>
       <c r="G88" s="138"/>
@@ -29787,7 +29754,7 @@
     </row>
     <row r="90" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="157" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B90" s="105"/>
       <c r="C90" s="106"/>
@@ -29815,7 +29782,7 @@
     <row r="91" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="110"/>
       <c r="B91" s="105" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C91" s="106" t="s">
         <v>8</v>
@@ -29825,7 +29792,7 @@
         <v>750</v>
       </c>
       <c r="E91" s="105" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F91" s="138"/>
       <c r="G91" s="138"/>
@@ -29849,7 +29816,7 @@
     <row r="92" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="110"/>
       <c r="B92" s="105" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C92" s="106" t="s">
         <v>8</v>
@@ -29859,7 +29826,7 @@
         <v>80</v>
       </c>
       <c r="E92" s="105" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F92" s="138"/>
       <c r="G92" s="138"/>
@@ -29883,7 +29850,7 @@
     <row r="93" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="110"/>
       <c r="B93" s="105" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C93" s="106" t="s">
         <v>8</v>
@@ -29893,7 +29860,7 @@
         <v>900</v>
       </c>
       <c r="E93" s="105" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F93" s="138"/>
       <c r="G93" s="138"/>
@@ -29917,7 +29884,7 @@
     <row r="94" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="110"/>
       <c r="B94" s="105" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C94" s="106" t="s">
         <v>8</v>
@@ -29927,7 +29894,7 @@
         <v>1200</v>
       </c>
       <c r="E94" s="105" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F94" s="138"/>
       <c r="G94" s="138"/>
@@ -29951,7 +29918,7 @@
     <row r="95" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="110"/>
       <c r="B95" s="105" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C95" s="106" t="s">
         <v>8</v>
@@ -29961,7 +29928,7 @@
         <v>105</v>
       </c>
       <c r="E95" s="105" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F95" s="138"/>
       <c r="G95" s="138"/>
@@ -29985,7 +29952,7 @@
     <row r="96" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="110"/>
       <c r="B96" s="105" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C96" s="106" t="s">
         <v>8</v>
@@ -29995,7 +29962,7 @@
         <v>12600</v>
       </c>
       <c r="E96" s="105" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F96" s="138"/>
       <c r="G96" s="138"/>
@@ -30019,17 +29986,17 @@
     <row r="97" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="110"/>
       <c r="B97" s="105" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C97" s="106" t="s">
         <v>8</v>
       </c>
       <c r="D97" s="105" t="n">
         <f aca="false">'User Interface'!E91</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E97" s="105" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F97" s="138"/>
       <c r="G97" s="138"/>
@@ -30053,7 +30020,7 @@
     <row r="98" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="110"/>
       <c r="B98" s="158" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C98" s="159" t="s">
         <v>8</v>
@@ -30063,7 +30030,7 @@
         <v>Symyx_96_well_0003</v>
       </c>
       <c r="E98" s="158" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F98" s="138"/>
       <c r="G98" s="138"/>
@@ -30086,7 +30053,7 @@
     </row>
     <row r="99" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="157" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B99" s="105"/>
       <c r="C99" s="106"/>
@@ -30114,7 +30081,7 @@
     <row r="100" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="110"/>
       <c r="B100" s="105" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C100" s="106" t="s">
         <v>8</v>
@@ -30124,7 +30091,7 @@
         <v>45</v>
       </c>
       <c r="E100" s="105" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F100" s="138"/>
       <c r="G100" s="138"/>
@@ -30148,17 +30115,17 @@
     <row r="101" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="110"/>
       <c r="B101" s="105" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C101" s="106" t="s">
         <v>8</v>
       </c>
       <c r="D101" s="105" t="n">
         <f aca="false">'User Interface'!E95</f>
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="E101" s="105" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F101" s="138"/>
       <c r="G101" s="138"/>
@@ -30182,7 +30149,7 @@
     <row r="102" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="110"/>
       <c r="B102" s="105" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C102" s="106" t="s">
         <v>8</v>
@@ -30192,7 +30159,7 @@
         <v>450</v>
       </c>
       <c r="E102" s="105" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F102" s="138"/>
       <c r="G102" s="138"/>
@@ -30216,7 +30183,7 @@
     <row r="103" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="110"/>
       <c r="B103" s="158" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C103" s="159" t="s">
         <v>8</v>
@@ -30226,7 +30193,7 @@
         <v>3600</v>
       </c>
       <c r="E103" s="158" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F103" s="138"/>
       <c r="G103" s="138"/>

</xml_diff>

<commit_message>
Hide backend sheet in HC/LBL interface
</commit_message>
<xml_diff>
--- a/HC_LBL_SpecificationInterface.xlsx
+++ b/HC_LBL_SpecificationInterface.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="-16600" windowWidth="38400" windowHeight="21600"/>
+    <workbookView xWindow="25600" yWindow="-16600" windowWidth="38400" windowHeight="21600" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="User Interface" sheetId="1" r:id="rId1"/>
     <sheet name="Manual Experiment Interface" sheetId="2" r:id="rId2"/>
     <sheet name="ManualExps" sheetId="3" state="hidden" r:id="rId3"/>
-    <sheet name="WF1" sheetId="4" r:id="rId4"/>
+    <sheet name="WF1" sheetId="4" state="hidden" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="fixed_wells" localSheetId="0">'User Interface'!$E$19</definedName>
@@ -2082,8 +2082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="109" zoomScaleNormal="109" zoomScalePageLayoutView="109" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView topLeftCell="A9" zoomScale="109" zoomScaleNormal="109" zoomScalePageLayoutView="109" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -8413,7 +8413,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix bug: frontend/backend cell ordering mismatch
</commit_message>
<xml_diff>
--- a/HC_LBL_SpecificationInterface.xlsx
+++ b/HC_LBL_SpecificationInterface.xlsx
@@ -20,8 +20,9 @@
   </sheets>
   <definedNames>
     <definedName name="fixed_wells" localSheetId="0">'User Interface'!$E$20</definedName>
-    <definedName name="fixed_wells">'WF1'!$D$19</definedName>
+    <definedName name="fixed_wells">'WF1'!$D$20</definedName>
     <definedName name="manual_wells">'User Interface'!$E$20</definedName>
+    <definedName name="multi_stock_sampling">'User Interface'!$E$8</definedName>
     <definedName name="wellcount" localSheetId="0">'User Interface'!$E$6</definedName>
     <definedName name="wellcount">'WF1'!$D$7</definedName>
   </definedNames>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="342">
   <si>
     <t>Manual Well Number</t>
   </si>
@@ -1323,9 +1324,6 @@
     <t>OldReagent3_chemical_list</t>
   </si>
   <si>
-    <t>OldReagent3_ID</t>
-  </si>
-  <si>
     <t>OldReagent3_item1_formulaconc</t>
   </si>
   <si>
@@ -1395,9 +1393,6 @@
     <t>OldReagent6_chemical_list</t>
   </si>
   <si>
-    <t>OldReagent6_ID</t>
-  </si>
-  <si>
     <t>OldReagent6_item1_formulaconc</t>
   </si>
   <si>
@@ -1450,6 +1445,12 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>multi_stock_sampling</t>
+  </si>
+  <si>
+    <t>Oldreagent3_ID</t>
   </si>
 </sst>
 </file>
@@ -2396,7 +2397,7 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView zoomScale="109" zoomScaleNormal="109" zoomScalePageLayoutView="109" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -2665,13 +2666,13 @@
       <c r="A8" s="32"/>
       <c r="B8" s="32"/>
       <c r="C8" s="126" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D8" s="29" t="s">
         <v>20</v>
       </c>
       <c r="E8" s="109" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="F8" s="28"/>
       <c r="G8" s="124"/>
@@ -29895,8 +29896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -30140,7 +30141,7 @@
         <v>75</v>
       </c>
       <c r="H16" s="123" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -30160,7 +30161,7 @@
         <v>450</v>
       </c>
       <c r="H17" s="123" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -36628,10 +36629,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1062"/>
+  <dimension ref="A1:Z1063"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D104" sqref="D104"/>
+    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
+      <selection activeCell="B149" sqref="B149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -36927,54 +36928,48 @@
       <c r="Y8" s="4"/>
       <c r="Z8" s="4"/>
     </row>
-    <row r="9" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="40" t="s">
+    <row r="9" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="32"/>
+      <c r="B9" s="28" t="s">
+        <v>340</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="28">
+        <f>IF(multi_stock_sampling="Yes", 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="28" t="s">
+        <v>192</v>
+      </c>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="19"/>
+      <c r="O9" s="19"/>
+      <c r="P9" s="19"/>
+      <c r="Q9" s="19"/>
+      <c r="R9" s="19"/>
+      <c r="S9" s="19"/>
+      <c r="T9" s="19"/>
+      <c r="U9" s="19"/>
+      <c r="V9" s="19"/>
+      <c r="W9" s="19"/>
+    </row>
+    <row r="10" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="40" t="s">
         <v>197</v>
       </c>
-      <c r="B9" s="41"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="45"/>
-      <c r="G9" s="45"/>
-      <c r="H9" s="45"/>
-      <c r="I9" s="45"/>
-      <c r="J9" s="45"/>
-      <c r="K9" s="45"/>
-      <c r="L9" s="45"/>
-      <c r="M9" s="45"/>
-      <c r="N9" s="45"/>
-      <c r="O9" s="45"/>
-      <c r="P9" s="45"/>
-      <c r="Q9" s="45"/>
-      <c r="R9" s="45"/>
-      <c r="S9" s="45"/>
-      <c r="T9" s="45"/>
-      <c r="U9" s="45"/>
-      <c r="V9" s="45"/>
-      <c r="W9" s="45"/>
-      <c r="X9" s="97"/>
-      <c r="Y9" s="97"/>
-      <c r="Z9" s="97"/>
-    </row>
-    <row r="10" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="40">
-        <f>'User Interface'!A10</f>
-        <v>0</v>
-      </c>
-      <c r="B10" s="41" t="s">
-        <v>198</v>
-      </c>
-      <c r="C10" s="42" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="41" t="str">
-        <f>'User Interface'!E10</f>
-        <v>[[2,3,4,5,1,7]]</v>
-      </c>
-      <c r="E10" s="41" t="s">
-        <v>196</v>
-      </c>
+      <c r="B10" s="41"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
       <c r="F10" s="45"/>
       <c r="G10" s="45"/>
       <c r="H10" s="45"/>
@@ -36999,18 +36994,18 @@
     </row>
     <row r="11" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="40">
-        <f>'User Interface'!A11</f>
+        <f>'User Interface'!A10</f>
         <v>0</v>
       </c>
       <c r="B11" s="41" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C11" s="42" t="s">
         <v>20</v>
       </c>
       <c r="D11" s="41" t="str">
-        <f>'User Interface'!E11</f>
-        <v>[[500,500]]</v>
+        <f>'User Interface'!E10</f>
+        <v>[[2,3,4,5,1,7]]</v>
       </c>
       <c r="E11" s="41" t="s">
         <v>196</v>
@@ -37039,21 +37034,21 @@
     </row>
     <row r="12" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="40">
-        <f>'User Interface'!A12</f>
+        <f>'User Interface'!A11</f>
         <v>0</v>
       </c>
       <c r="B12" s="41" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C12" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="41">
-        <f>'User Interface'!E12</f>
-        <v>96</v>
+      <c r="D12" s="41" t="str">
+        <f>'User Interface'!E11</f>
+        <v>[[500,500]]</v>
       </c>
       <c r="E12" s="41" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="F12" s="45"/>
       <c r="G12" s="45"/>
@@ -37079,20 +37074,22 @@
     </row>
     <row r="13" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="40">
-        <f>'User Interface'!A13</f>
+        <f>'User Interface'!A12</f>
         <v>0</v>
       </c>
       <c r="B13" s="41" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C13" s="42" t="s">
         <v>20</v>
       </c>
       <c r="D13" s="41">
-        <f>'User Interface'!E13</f>
-        <v>0</v>
-      </c>
-      <c r="E13" s="41"/>
+        <f>'User Interface'!E12</f>
+        <v>96</v>
+      </c>
+      <c r="E13" s="41" t="s">
+        <v>192</v>
+      </c>
       <c r="F13" s="45"/>
       <c r="G13" s="45"/>
       <c r="H13" s="45"/>
@@ -37116,59 +37113,57 @@
       <c r="Z13" s="97"/>
     </row>
     <row r="14" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="40" t="str">
+      <c r="A14" s="40">
+        <f>'User Interface'!A13</f>
+        <v>0</v>
+      </c>
+      <c r="B14" s="41" t="s">
+        <v>201</v>
+      </c>
+      <c r="C14" s="42" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="41">
+        <f>'User Interface'!E13</f>
+        <v>0</v>
+      </c>
+      <c r="E14" s="41"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="45"/>
+      <c r="J14" s="45"/>
+      <c r="K14" s="45"/>
+      <c r="L14" s="45"/>
+      <c r="M14" s="45"/>
+      <c r="N14" s="45"/>
+      <c r="O14" s="45"/>
+      <c r="P14" s="45"/>
+      <c r="Q14" s="45"/>
+      <c r="R14" s="45"/>
+      <c r="S14" s="45"/>
+      <c r="T14" s="45"/>
+      <c r="U14" s="45"/>
+      <c r="V14" s="45"/>
+      <c r="W14" s="45"/>
+      <c r="X14" s="97"/>
+      <c r="Y14" s="97"/>
+      <c r="Z14" s="97"/>
+    </row>
+    <row r="15" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="40" t="str">
         <f>'User Interface'!A15</f>
         <v>#</v>
       </c>
-      <c r="B14" s="41" t="s">
+      <c r="B15" s="41" t="s">
         <v>202</v>
       </c>
-      <c r="C14" s="42" t="s">
+      <c r="C15" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="41" t="str">
+      <c r="D15" s="41" t="str">
         <f>'User Interface'!E15</f>
         <v>[[2,3,1]]</v>
-      </c>
-      <c r="E14" s="41" t="s">
-        <v>196</v>
-      </c>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="19"/>
-      <c r="K14" s="19"/>
-      <c r="L14" s="19"/>
-      <c r="M14" s="19"/>
-      <c r="N14" s="19"/>
-      <c r="O14" s="19"/>
-      <c r="P14" s="19"/>
-      <c r="Q14" s="19"/>
-      <c r="R14" s="19"/>
-      <c r="S14" s="19"/>
-      <c r="T14" s="19"/>
-      <c r="U14" s="19"/>
-      <c r="V14" s="19"/>
-      <c r="W14" s="19"/>
-      <c r="X14" s="4"/>
-      <c r="Y14" s="4"/>
-      <c r="Z14" s="4"/>
-    </row>
-    <row r="15" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="40" t="str">
-        <f>'User Interface'!A16</f>
-        <v>#</v>
-      </c>
-      <c r="B15" s="41" t="s">
-        <v>203</v>
-      </c>
-      <c r="C15" s="42" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="41" t="str">
-        <f>'User Interface'!E16</f>
-        <v>[[215, 215]]</v>
       </c>
       <c r="E15" s="41" t="s">
         <v>196</v>
@@ -37197,21 +37192,21 @@
     </row>
     <row r="16" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="40" t="str">
-        <f>'User Interface'!A17</f>
+        <f>'User Interface'!A16</f>
         <v>#</v>
       </c>
       <c r="B16" s="41" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C16" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="41">
-        <f>'User Interface'!E17</f>
-        <v>0</v>
+      <c r="D16" s="41" t="str">
+        <f>'User Interface'!E16</f>
+        <v>[[215, 215]]</v>
       </c>
       <c r="E16" s="41" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="F16" s="19"/>
       <c r="G16" s="19"/>
@@ -37237,20 +37232,22 @@
     </row>
     <row r="17" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="40" t="str">
-        <f>'User Interface'!A18</f>
+        <f>'User Interface'!A17</f>
         <v>#</v>
       </c>
       <c r="B17" s="41" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C17" s="42" t="s">
         <v>20</v>
       </c>
       <c r="D17" s="41">
-        <f>'User Interface'!E18</f>
+        <f>'User Interface'!E17</f>
         <v>0</v>
       </c>
-      <c r="E17" s="41"/>
+      <c r="E17" s="41" t="s">
+        <v>192</v>
+      </c>
       <c r="F17" s="19"/>
       <c r="G17" s="19"/>
       <c r="H17" s="19"/>
@@ -37273,49 +37270,52 @@
       <c r="Y17" s="4"/>
       <c r="Z17" s="4"/>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A18" s="50" t="s">
-        <v>53</v>
-      </c>
-      <c r="B18" s="51"/>
-      <c r="C18" s="51"/>
-      <c r="D18" s="51"/>
-      <c r="E18" s="51"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
-      <c r="P18" s="4"/>
-      <c r="Q18" s="4"/>
-      <c r="R18" s="4"/>
-      <c r="S18" s="4"/>
-      <c r="T18" s="4"/>
-      <c r="U18" s="4"/>
-      <c r="V18" s="4"/>
-      <c r="W18" s="4"/>
+    <row r="18" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="40" t="str">
+        <f>'User Interface'!A18</f>
+        <v>#</v>
+      </c>
+      <c r="B18" s="41" t="s">
+        <v>205</v>
+      </c>
+      <c r="C18" s="42" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="41">
+        <f>'User Interface'!E18</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="41"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="19"/>
+      <c r="N18" s="19"/>
+      <c r="O18" s="19"/>
+      <c r="P18" s="19"/>
+      <c r="Q18" s="19"/>
+      <c r="R18" s="19"/>
+      <c r="S18" s="19"/>
+      <c r="T18" s="19"/>
+      <c r="U18" s="19"/>
+      <c r="V18" s="19"/>
+      <c r="W18" s="19"/>
       <c r="X18" s="4"/>
       <c r="Y18" s="4"/>
       <c r="Z18" s="4"/>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A19" s="51"/>
-      <c r="B19" s="51" t="s">
-        <v>206</v>
-      </c>
+      <c r="A19" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="51"/>
       <c r="C19" s="51"/>
-      <c r="D19" s="41">
-        <f>'User Interface'!E20</f>
-        <v>0</v>
-      </c>
-      <c r="E19" s="51" t="s">
-        <v>192</v>
-      </c>
+      <c r="D19" s="51"/>
+      <c r="E19" s="51"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
@@ -37338,38 +37338,45 @@
       <c r="Y19" s="4"/>
       <c r="Z19" s="4"/>
     </row>
-    <row r="20" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="59" t="s">
-        <v>207</v>
-      </c>
-      <c r="B20" s="60"/>
-      <c r="C20" s="61"/>
-      <c r="D20" s="60"/>
-      <c r="E20" s="60"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
-      <c r="L20" s="19"/>
-      <c r="M20" s="19"/>
-      <c r="N20" s="19"/>
-      <c r="O20" s="19"/>
-      <c r="P20" s="19"/>
-      <c r="Q20" s="19"/>
-      <c r="R20" s="19"/>
-      <c r="S20" s="19"/>
-      <c r="T20" s="19"/>
-      <c r="U20" s="19"/>
-      <c r="V20" s="19"/>
-      <c r="W20" s="19"/>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A20" s="51"/>
+      <c r="B20" s="51" t="s">
+        <v>206</v>
+      </c>
+      <c r="C20" s="51"/>
+      <c r="D20" s="41">
+        <f>'User Interface'!E20</f>
+        <v>0</v>
+      </c>
+      <c r="E20" s="51" t="s">
+        <v>192</v>
+      </c>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="4"/>
+      <c r="R20" s="4"/>
+      <c r="S20" s="4"/>
+      <c r="T20" s="4"/>
+      <c r="U20" s="4"/>
+      <c r="V20" s="4"/>
+      <c r="W20" s="4"/>
       <c r="X20" s="4"/>
       <c r="Y20" s="4"/>
       <c r="Z20" s="4"/>
     </row>
     <row r="21" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="64"/>
+      <c r="A21" s="59" t="s">
+        <v>207</v>
+      </c>
       <c r="B21" s="60"/>
       <c r="C21" s="61"/>
       <c r="D21" s="60"/>
@@ -37397,21 +37404,11 @@
       <c r="Z21" s="4"/>
     </row>
     <row r="22" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="64" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" s="98" t="s">
-        <v>208</v>
-      </c>
-      <c r="C22" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="D22" s="60">
-        <v>0.2</v>
-      </c>
-      <c r="E22" s="60" t="s">
-        <v>190</v>
-      </c>
+      <c r="A22" s="64"/>
+      <c r="B22" s="60"/>
+      <c r="C22" s="61"/>
+      <c r="D22" s="60"/>
+      <c r="E22" s="60"/>
       <c r="F22" s="19"/>
       <c r="G22" s="19"/>
       <c r="H22" s="19"/>
@@ -37439,13 +37436,13 @@
         <v>44</v>
       </c>
       <c r="B23" s="98" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C23" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D23" s="60">
-        <v>1.5</v>
+        <v>0.2</v>
       </c>
       <c r="E23" s="60" t="s">
         <v>190</v>
@@ -37473,11 +37470,21 @@
       <c r="Z23" s="4"/>
     </row>
     <row r="24" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="64"/>
-      <c r="B24" s="60"/>
-      <c r="C24" s="61"/>
-      <c r="D24" s="60"/>
-      <c r="E24" s="60"/>
+      <c r="A24" s="64" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="98" t="s">
+        <v>209</v>
+      </c>
+      <c r="C24" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" s="60">
+        <v>1.5</v>
+      </c>
+      <c r="E24" s="60" t="s">
+        <v>190</v>
+      </c>
       <c r="F24" s="19"/>
       <c r="G24" s="19"/>
       <c r="H24" s="19"/>
@@ -37501,9 +37508,7 @@
       <c r="Z24" s="4"/>
     </row>
     <row r="25" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="59" t="s">
-        <v>55</v>
-      </c>
+      <c r="A25" s="64"/>
       <c r="B25" s="60"/>
       <c r="C25" s="61"/>
       <c r="D25" s="60"/>
@@ -37531,7 +37536,9 @@
       <c r="Z25" s="4"/>
     </row>
     <row r="26" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="64"/>
+      <c r="A26" s="59" t="s">
+        <v>55</v>
+      </c>
       <c r="B26" s="60"/>
       <c r="C26" s="61"/>
       <c r="D26" s="60"/>
@@ -37559,23 +37566,11 @@
       <c r="Z26" s="4"/>
     </row>
     <row r="27" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="64">
-        <f>'User Interface'!A23</f>
-        <v>0</v>
-      </c>
-      <c r="B27" s="60" t="s">
-        <v>210</v>
-      </c>
-      <c r="C27" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="D27" s="69" t="str">
-        <f>'User Interface'!E23</f>
-        <v>['DMSO']</v>
-      </c>
-      <c r="E27" s="60" t="s">
-        <v>196</v>
-      </c>
+      <c r="A27" s="64"/>
+      <c r="B27" s="60"/>
+      <c r="C27" s="61"/>
+      <c r="D27" s="60"/>
+      <c r="E27" s="60"/>
       <c r="F27" s="19"/>
       <c r="G27" s="19"/>
       <c r="H27" s="19"/>
@@ -37599,22 +37594,22 @@
       <c r="Z27" s="4"/>
     </row>
     <row r="28" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="64" t="str">
-        <f>'User Interface'!A24</f>
-        <v>#</v>
-      </c>
-      <c r="B28" s="69" t="s">
-        <v>211</v>
-      </c>
-      <c r="C28" s="73" t="s">
+      <c r="A28" s="64">
+        <f>'User Interface'!A23</f>
+        <v>0</v>
+      </c>
+      <c r="B28" s="60" t="s">
+        <v>210</v>
+      </c>
+      <c r="C28" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="D28" s="69">
-        <f>'User Interface'!E24</f>
-        <v>0</v>
-      </c>
-      <c r="E28" s="69" t="s">
-        <v>193</v>
+      <c r="D28" s="69" t="str">
+        <f>'User Interface'!E23</f>
+        <v>['DMSO']</v>
+      </c>
+      <c r="E28" s="60" t="s">
+        <v>196</v>
       </c>
       <c r="F28" s="19"/>
       <c r="G28" s="19"/>
@@ -37640,21 +37635,21 @@
     </row>
     <row r="29" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="64" t="str">
-        <f>'User Interface'!A25</f>
+        <f>'User Interface'!A24</f>
         <v>#</v>
       </c>
-      <c r="B29" s="60" t="s">
-        <v>212</v>
-      </c>
-      <c r="C29" s="61" t="s">
+      <c r="B29" s="69" t="s">
+        <v>211</v>
+      </c>
+      <c r="C29" s="73" t="s">
         <v>20</v>
       </c>
       <c r="D29" s="69">
-        <f>'User Interface'!E25</f>
-        <v>1.5</v>
-      </c>
-      <c r="E29" s="60" t="s">
-        <v>190</v>
+        <f>'User Interface'!E24</f>
+        <v>0</v>
+      </c>
+      <c r="E29" s="69" t="s">
+        <v>193</v>
       </c>
       <c r="F29" s="19"/>
       <c r="G29" s="19"/>
@@ -37680,18 +37675,18 @@
     </row>
     <row r="30" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="64" t="str">
-        <f>'User Interface'!A26</f>
+        <f>'User Interface'!A25</f>
         <v>#</v>
       </c>
       <c r="B30" s="60" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C30" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D30" s="69">
-        <f>'User Interface'!E26</f>
-        <v>7.63</v>
+        <f>'User Interface'!E25</f>
+        <v>1.5</v>
       </c>
       <c r="E30" s="60" t="s">
         <v>190</v>
@@ -37720,18 +37715,18 @@
     </row>
     <row r="31" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="64" t="str">
-        <f>'User Interface'!A27</f>
+        <f>'User Interface'!A26</f>
         <v>#</v>
       </c>
       <c r="B31" s="60" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C31" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D31" s="69">
-        <f>'User Interface'!E27</f>
-        <v>0</v>
+        <f>'User Interface'!E26</f>
+        <v>7.63</v>
       </c>
       <c r="E31" s="60" t="s">
         <v>190</v>
@@ -37760,21 +37755,21 @@
     </row>
     <row r="32" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="64" t="str">
-        <f>'User Interface'!A28</f>
+        <f>'User Interface'!A27</f>
         <v>#</v>
       </c>
       <c r="B32" s="60" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C32" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D32" s="69">
-        <f>'User Interface'!E28</f>
+        <f>'User Interface'!E27</f>
         <v>0</v>
       </c>
       <c r="E32" s="60" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F32" s="19"/>
       <c r="G32" s="19"/>
@@ -37800,17 +37795,17 @@
     </row>
     <row r="33" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="64" t="str">
-        <f>'User Interface'!A29</f>
+        <f>'User Interface'!A28</f>
         <v>#</v>
       </c>
       <c r="B33" s="60" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C33" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D33" s="69">
-        <f>'User Interface'!E29</f>
+        <f>'User Interface'!E28</f>
         <v>0</v>
       </c>
       <c r="E33" s="60" t="s">
@@ -37840,17 +37835,17 @@
     </row>
     <row r="34" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="64" t="str">
-        <f>'User Interface'!A30</f>
+        <f>'User Interface'!A29</f>
         <v>#</v>
       </c>
       <c r="B34" s="60" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C34" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D34" s="69">
-        <f>'User Interface'!E30</f>
+        <f>'User Interface'!E29</f>
         <v>0</v>
       </c>
       <c r="E34" s="60" t="s">
@@ -37879,11 +37874,23 @@
       <c r="Z34" s="4"/>
     </row>
     <row r="35" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="64"/>
-      <c r="B35" s="69"/>
-      <c r="C35" s="73"/>
-      <c r="D35" s="69"/>
-      <c r="E35" s="69"/>
+      <c r="A35" s="64" t="str">
+        <f>'User Interface'!A30</f>
+        <v>#</v>
+      </c>
+      <c r="B35" s="60" t="s">
+        <v>217</v>
+      </c>
+      <c r="C35" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="D35" s="69">
+        <f>'User Interface'!E30</f>
+        <v>0</v>
+      </c>
+      <c r="E35" s="60" t="s">
+        <v>192</v>
+      </c>
       <c r="F35" s="19"/>
       <c r="G35" s="19"/>
       <c r="H35" s="19"/>
@@ -37907,23 +37914,11 @@
       <c r="Z35" s="4"/>
     </row>
     <row r="36" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="64">
-        <f>'User Interface'!A32</f>
-        <v>0</v>
-      </c>
-      <c r="B36" s="60" t="s">
-        <v>218</v>
-      </c>
-      <c r="C36" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="D36" s="60" t="str">
-        <f>'User Interface'!E32</f>
-        <v>['PbI2','PyrrolidiniumIodide','DMSO']</v>
-      </c>
-      <c r="E36" s="60" t="s">
-        <v>196</v>
-      </c>
+      <c r="A36" s="64"/>
+      <c r="B36" s="69"/>
+      <c r="C36" s="73"/>
+      <c r="D36" s="69"/>
+      <c r="E36" s="69"/>
       <c r="F36" s="19"/>
       <c r="G36" s="19"/>
       <c r="H36" s="19"/>
@@ -37947,22 +37942,22 @@
       <c r="Z36" s="4"/>
     </row>
     <row r="37" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="64" t="str">
-        <f>'User Interface'!A36</f>
-        <v>#</v>
-      </c>
-      <c r="B37" s="69" t="s">
-        <v>219</v>
-      </c>
-      <c r="C37" s="73" t="s">
+      <c r="A37" s="64">
+        <f>'User Interface'!A32</f>
+        <v>0</v>
+      </c>
+      <c r="B37" s="60" t="s">
+        <v>218</v>
+      </c>
+      <c r="C37" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="D37" s="69">
-        <f>'User Interface'!E36</f>
-        <v>0</v>
-      </c>
-      <c r="E37" s="69" t="s">
-        <v>193</v>
+      <c r="D37" s="60" t="str">
+        <f>'User Interface'!E32</f>
+        <v>['PbI2','PyrrolidiniumIodide','DMSO']</v>
+      </c>
+      <c r="E37" s="60" t="s">
+        <v>196</v>
       </c>
       <c r="F37" s="19"/>
       <c r="G37" s="19"/>
@@ -37987,22 +37982,22 @@
       <c r="Z37" s="4"/>
     </row>
     <row r="38" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="64">
-        <f>'User Interface'!A33</f>
+      <c r="A38" s="64" t="str">
+        <f>'User Interface'!A36</f>
+        <v>#</v>
+      </c>
+      <c r="B38" s="69" t="s">
+        <v>219</v>
+      </c>
+      <c r="C38" s="73" t="s">
+        <v>20</v>
+      </c>
+      <c r="D38" s="69">
+        <f>'User Interface'!E36</f>
         <v>0</v>
       </c>
-      <c r="B38" s="60" t="s">
-        <v>220</v>
-      </c>
-      <c r="C38" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="D38" s="69">
-        <f>'User Interface'!E33</f>
-        <v>1.55</v>
-      </c>
-      <c r="E38" s="60" t="s">
-        <v>190</v>
+      <c r="E38" s="69" t="s">
+        <v>193</v>
       </c>
       <c r="F38" s="19"/>
       <c r="G38" s="19"/>
@@ -38028,18 +38023,18 @@
     </row>
     <row r="39" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="64">
-        <f>'User Interface'!A34</f>
+        <f>'User Interface'!A33</f>
         <v>0</v>
       </c>
       <c r="B39" s="60" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C39" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D39" s="69">
-        <f>'User Interface'!E34</f>
-        <v>1.93</v>
+        <f>'User Interface'!E33</f>
+        <v>1.55</v>
       </c>
       <c r="E39" s="60" t="s">
         <v>190</v>
@@ -38067,19 +38062,19 @@
       <c r="Z39" s="4"/>
     </row>
     <row r="40" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="64" t="str">
-        <f>'User Interface'!A35</f>
-        <v>#</v>
+      <c r="A40" s="64">
+        <f>'User Interface'!A34</f>
+        <v>0</v>
       </c>
       <c r="B40" s="60" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C40" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="D40" s="60">
-        <f>'User Interface'!E35</f>
-        <v>0</v>
+      <c r="D40" s="69">
+        <f>'User Interface'!E34</f>
+        <v>1.93</v>
       </c>
       <c r="E40" s="60" t="s">
         <v>190</v>
@@ -38108,21 +38103,21 @@
     </row>
     <row r="41" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="64" t="str">
-        <f>'User Interface'!A37</f>
+        <f>'User Interface'!A35</f>
         <v>#</v>
       </c>
       <c r="B41" s="60" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C41" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="D41" s="69">
-        <f>'User Interface'!E37</f>
+      <c r="D41" s="60">
+        <f>'User Interface'!E35</f>
         <v>0</v>
       </c>
       <c r="E41" s="60" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F41" s="19"/>
       <c r="G41" s="19"/>
@@ -38148,17 +38143,17 @@
     </row>
     <row r="42" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="64" t="str">
-        <f>'User Interface'!A38</f>
+        <f>'User Interface'!A37</f>
         <v>#</v>
       </c>
       <c r="B42" s="60" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C42" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D42" s="69">
-        <f>'User Interface'!E38</f>
+        <f>'User Interface'!E37</f>
         <v>0</v>
       </c>
       <c r="E42" s="60" t="s">
@@ -38188,17 +38183,17 @@
     </row>
     <row r="43" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="64" t="str">
-        <f>'User Interface'!A39</f>
+        <f>'User Interface'!A38</f>
         <v>#</v>
       </c>
       <c r="B43" s="60" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C43" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D43" s="69">
-        <f>'User Interface'!E39</f>
+        <f>'User Interface'!E38</f>
         <v>0</v>
       </c>
       <c r="E43" s="60" t="s">
@@ -38227,11 +38222,23 @@
       <c r="Z43" s="4"/>
     </row>
     <row r="44" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="64"/>
-      <c r="B44" s="60"/>
-      <c r="C44" s="61"/>
-      <c r="D44" s="60"/>
-      <c r="E44" s="60"/>
+      <c r="A44" s="64" t="str">
+        <f>'User Interface'!A39</f>
+        <v>#</v>
+      </c>
+      <c r="B44" s="60" t="s">
+        <v>225</v>
+      </c>
+      <c r="C44" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="D44" s="69">
+        <f>'User Interface'!E39</f>
+        <v>0</v>
+      </c>
+      <c r="E44" s="60" t="s">
+        <v>192</v>
+      </c>
       <c r="F44" s="19"/>
       <c r="G44" s="19"/>
       <c r="H44" s="19"/>
@@ -38255,23 +38262,11 @@
       <c r="Z44" s="4"/>
     </row>
     <row r="45" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="64">
-        <f>'User Interface'!A41</f>
-        <v>0</v>
-      </c>
-      <c r="B45" s="60" t="s">
-        <v>226</v>
-      </c>
-      <c r="C45" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="D45" s="60" t="str">
-        <f>'User Interface'!E41</f>
-        <v>['PyrrolidiniumIodide','DMSO']</v>
-      </c>
-      <c r="E45" s="60" t="s">
-        <v>196</v>
-      </c>
+      <c r="A45" s="64"/>
+      <c r="B45" s="60"/>
+      <c r="C45" s="61"/>
+      <c r="D45" s="60"/>
+      <c r="E45" s="60"/>
       <c r="F45" s="19"/>
       <c r="G45" s="19"/>
       <c r="H45" s="19"/>
@@ -38295,22 +38290,22 @@
       <c r="Z45" s="4"/>
     </row>
     <row r="46" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="64" t="str">
-        <f>'User Interface'!A45</f>
-        <v>#</v>
-      </c>
-      <c r="B46" s="69" t="s">
-        <v>227</v>
-      </c>
-      <c r="C46" s="73" t="s">
+      <c r="A46" s="64">
+        <f>'User Interface'!A41</f>
+        <v>0</v>
+      </c>
+      <c r="B46" s="60" t="s">
+        <v>226</v>
+      </c>
+      <c r="C46" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="D46" s="60">
-        <f>'User Interface'!E45</f>
-        <v>0</v>
-      </c>
-      <c r="E46" s="69" t="s">
-        <v>193</v>
+      <c r="D46" s="60" t="str">
+        <f>'User Interface'!E41</f>
+        <v>['PyrrolidiniumIodide','DMSO']</v>
+      </c>
+      <c r="E46" s="60" t="s">
+        <v>196</v>
       </c>
       <c r="F46" s="19"/>
       <c r="G46" s="19"/>
@@ -38335,22 +38330,22 @@
       <c r="Z46" s="4"/>
     </row>
     <row r="47" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="64">
-        <f>'User Interface'!A42</f>
+      <c r="A47" s="64" t="str">
+        <f>'User Interface'!A45</f>
+        <v>#</v>
+      </c>
+      <c r="B47" s="69" t="s">
+        <v>227</v>
+      </c>
+      <c r="C47" s="73" t="s">
+        <v>20</v>
+      </c>
+      <c r="D47" s="60">
+        <f>'User Interface'!E45</f>
         <v>0</v>
       </c>
-      <c r="B47" s="99" t="s">
-        <v>228</v>
-      </c>
-      <c r="C47" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="D47" s="60">
-        <f>'User Interface'!E42</f>
-        <v>2.06</v>
-      </c>
-      <c r="E47" s="60" t="s">
-        <v>190</v>
+      <c r="E47" s="69" t="s">
+        <v>193</v>
       </c>
       <c r="F47" s="19"/>
       <c r="G47" s="19"/>
@@ -38375,19 +38370,19 @@
       <c r="Z47" s="4"/>
     </row>
     <row r="48" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="64" t="str">
-        <f>'User Interface'!A43</f>
-        <v>#</v>
-      </c>
-      <c r="B48" s="60" t="s">
-        <v>229</v>
+      <c r="A48" s="64">
+        <f>'User Interface'!A42</f>
+        <v>0</v>
+      </c>
+      <c r="B48" s="99" t="s">
+        <v>228</v>
       </c>
       <c r="C48" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D48" s="60">
-        <f>'User Interface'!E43</f>
-        <v>1.33</v>
+        <f>'User Interface'!E42</f>
+        <v>2.06</v>
       </c>
       <c r="E48" s="60" t="s">
         <v>190</v>
@@ -38416,18 +38411,18 @@
     </row>
     <row r="49" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="64" t="str">
-        <f>'User Interface'!A44</f>
+        <f>'User Interface'!A43</f>
         <v>#</v>
       </c>
       <c r="B49" s="60" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C49" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D49" s="60">
-        <f>'User Interface'!E44</f>
-        <v>1.2</v>
+        <f>'User Interface'!E43</f>
+        <v>1.33</v>
       </c>
       <c r="E49" s="60" t="s">
         <v>190</v>
@@ -38456,21 +38451,21 @@
     </row>
     <row r="50" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="64" t="str">
-        <f>'User Interface'!A46</f>
+        <f>'User Interface'!A44</f>
         <v>#</v>
       </c>
       <c r="B50" s="60" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C50" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D50" s="60">
-        <f>'User Interface'!E46</f>
-        <v>0</v>
+        <f>'User Interface'!E44</f>
+        <v>1.2</v>
       </c>
       <c r="E50" s="60" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F50" s="19"/>
       <c r="G50" s="19"/>
@@ -38496,17 +38491,17 @@
     </row>
     <row r="51" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="64" t="str">
-        <f>'User Interface'!A47</f>
+        <f>'User Interface'!A46</f>
         <v>#</v>
       </c>
       <c r="B51" s="60" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C51" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D51" s="60">
-        <f>'User Interface'!E47</f>
+        <f>'User Interface'!E46</f>
         <v>0</v>
       </c>
       <c r="E51" s="60" t="s">
@@ -38536,17 +38531,17 @@
     </row>
     <row r="52" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="64" t="str">
-        <f>'User Interface'!A48</f>
+        <f>'User Interface'!A47</f>
         <v>#</v>
       </c>
       <c r="B52" s="60" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C52" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D52" s="60">
-        <f>'User Interface'!E48</f>
+        <f>'User Interface'!E47</f>
         <v>0</v>
       </c>
       <c r="E52" s="60" t="s">
@@ -38575,11 +38570,23 @@
       <c r="Z52" s="4"/>
     </row>
     <row r="53" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="64"/>
-      <c r="B53" s="60"/>
-      <c r="C53" s="61"/>
-      <c r="D53" s="60"/>
-      <c r="E53" s="60"/>
+      <c r="A53" s="64" t="str">
+        <f>'User Interface'!A48</f>
+        <v>#</v>
+      </c>
+      <c r="B53" s="60" t="s">
+        <v>233</v>
+      </c>
+      <c r="C53" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="D53" s="60">
+        <f>'User Interface'!E48</f>
+        <v>0</v>
+      </c>
+      <c r="E53" s="60" t="s">
+        <v>192</v>
+      </c>
       <c r="F53" s="19"/>
       <c r="G53" s="19"/>
       <c r="H53" s="19"/>
@@ -38603,23 +38610,11 @@
       <c r="Z53" s="4"/>
     </row>
     <row r="54" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="64">
-        <f>'User Interface'!A50</f>
-        <v>0</v>
-      </c>
-      <c r="B54" s="60" t="s">
-        <v>234</v>
-      </c>
-      <c r="C54" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="D54" s="60" t="str">
-        <f>'User Interface'!E50</f>
-        <v>['PbI2','PyrrolidiniumIodide','DMSO']</v>
-      </c>
-      <c r="E54" s="60" t="s">
-        <v>196</v>
-      </c>
+      <c r="A54" s="64"/>
+      <c r="B54" s="60"/>
+      <c r="C54" s="61"/>
+      <c r="D54" s="60"/>
+      <c r="E54" s="60"/>
       <c r="F54" s="19"/>
       <c r="G54" s="19"/>
       <c r="H54" s="19"/>
@@ -38643,22 +38638,22 @@
       <c r="Z54" s="4"/>
     </row>
     <row r="55" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="64" t="str">
-        <f>'User Interface'!A54</f>
-        <v>#</v>
-      </c>
-      <c r="B55" s="69" t="s">
-        <v>235</v>
-      </c>
-      <c r="C55" s="73" t="s">
+      <c r="A55" s="64">
+        <f>'User Interface'!A50</f>
+        <v>0</v>
+      </c>
+      <c r="B55" s="60" t="s">
+        <v>234</v>
+      </c>
+      <c r="C55" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="D55" s="60">
-        <f>'User Interface'!E54</f>
-        <v>0</v>
-      </c>
-      <c r="E55" s="69" t="s">
-        <v>193</v>
+      <c r="D55" s="60" t="str">
+        <f>'User Interface'!E50</f>
+        <v>['PbI2','PyrrolidiniumIodide','DMSO']</v>
+      </c>
+      <c r="E55" s="60" t="s">
+        <v>196</v>
       </c>
       <c r="F55" s="19"/>
       <c r="G55" s="19"/>
@@ -38683,22 +38678,22 @@
       <c r="Z55" s="4"/>
     </row>
     <row r="56" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="64">
-        <f>'User Interface'!A51</f>
+      <c r="A56" s="64" t="str">
+        <f>'User Interface'!A54</f>
+        <v>#</v>
+      </c>
+      <c r="B56" s="69" t="s">
+        <v>235</v>
+      </c>
+      <c r="C56" s="73" t="s">
+        <v>20</v>
+      </c>
+      <c r="D56" s="60">
+        <f>'User Interface'!E54</f>
         <v>0</v>
       </c>
-      <c r="B56" s="99" t="s">
-        <v>236</v>
-      </c>
-      <c r="C56" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="D56" s="60">
-        <f>'User Interface'!E51</f>
-        <v>1.18</v>
-      </c>
-      <c r="E56" s="60" t="s">
-        <v>190</v>
+      <c r="E56" s="69" t="s">
+        <v>193</v>
       </c>
       <c r="F56" s="19"/>
       <c r="G56" s="19"/>
@@ -38724,18 +38719,18 @@
     </row>
     <row r="57" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="64">
-        <f>'User Interface'!A52</f>
+        <f>'User Interface'!A51</f>
         <v>0</v>
       </c>
       <c r="B57" s="99" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C57" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D57" s="60">
-        <f>'User Interface'!E52</f>
-        <v>0.74</v>
+        <f>'User Interface'!E51</f>
+        <v>1.18</v>
       </c>
       <c r="E57" s="60" t="s">
         <v>190</v>
@@ -38763,19 +38758,19 @@
       <c r="Z57" s="4"/>
     </row>
     <row r="58" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="64" t="str">
-        <f>'User Interface'!A53</f>
-        <v>#</v>
-      </c>
-      <c r="B58" s="60" t="s">
-        <v>238</v>
+      <c r="A58" s="64">
+        <f>'User Interface'!A52</f>
+        <v>0</v>
+      </c>
+      <c r="B58" s="99" t="s">
+        <v>237</v>
       </c>
       <c r="C58" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D58" s="60">
-        <f>'User Interface'!E53</f>
-        <v>0</v>
+        <f>'User Interface'!E52</f>
+        <v>0.74</v>
       </c>
       <c r="E58" s="60" t="s">
         <v>190</v>
@@ -38804,21 +38799,21 @@
     </row>
     <row r="59" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="64" t="str">
-        <f>'User Interface'!A55</f>
+        <f>'User Interface'!A53</f>
         <v>#</v>
       </c>
       <c r="B59" s="60" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C59" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D59" s="60">
-        <f>'User Interface'!E55</f>
+        <f>'User Interface'!E53</f>
         <v>0</v>
       </c>
       <c r="E59" s="60" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F59" s="19"/>
       <c r="G59" s="19"/>
@@ -38844,17 +38839,17 @@
     </row>
     <row r="60" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="64" t="str">
-        <f>'User Interface'!A56</f>
+        <f>'User Interface'!A55</f>
         <v>#</v>
       </c>
       <c r="B60" s="60" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C60" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D60" s="60">
-        <f>'User Interface'!E56</f>
+        <f>'User Interface'!E55</f>
         <v>0</v>
       </c>
       <c r="E60" s="60" t="s">
@@ -38884,17 +38879,17 @@
     </row>
     <row r="61" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="64" t="str">
-        <f>'User Interface'!A57</f>
+        <f>'User Interface'!A56</f>
         <v>#</v>
       </c>
       <c r="B61" s="60" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C61" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D61" s="60">
-        <f>'User Interface'!E57</f>
+        <f>'User Interface'!E56</f>
         <v>0</v>
       </c>
       <c r="E61" s="60" t="s">
@@ -38923,11 +38918,23 @@
       <c r="Z61" s="4"/>
     </row>
     <row r="62" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="64"/>
-      <c r="B62" s="60"/>
-      <c r="C62" s="61"/>
-      <c r="D62" s="60"/>
-      <c r="E62" s="60"/>
+      <c r="A62" s="64" t="str">
+        <f>'User Interface'!A57</f>
+        <v>#</v>
+      </c>
+      <c r="B62" s="60" t="s">
+        <v>241</v>
+      </c>
+      <c r="C62" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="D62" s="60">
+        <f>'User Interface'!E57</f>
+        <v>0</v>
+      </c>
+      <c r="E62" s="60" t="s">
+        <v>192</v>
+      </c>
       <c r="F62" s="19"/>
       <c r="G62" s="19"/>
       <c r="H62" s="19"/>
@@ -38951,23 +38958,11 @@
       <c r="Z62" s="4"/>
     </row>
     <row r="63" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="64">
-        <f>'User Interface'!A59</f>
-        <v>0</v>
-      </c>
-      <c r="B63" s="60" t="s">
-        <v>242</v>
-      </c>
-      <c r="C63" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="D63" s="60" t="str">
-        <f>'User Interface'!E59</f>
-        <v>['PbI2','PyrrolidiniumIodide','DMSO']</v>
-      </c>
-      <c r="E63" s="60" t="s">
-        <v>196</v>
-      </c>
+      <c r="A63" s="64"/>
+      <c r="B63" s="60"/>
+      <c r="C63" s="61"/>
+      <c r="D63" s="60"/>
+      <c r="E63" s="60"/>
       <c r="F63" s="19"/>
       <c r="G63" s="19"/>
       <c r="H63" s="19"/>
@@ -38991,22 +38986,22 @@
       <c r="Z63" s="4"/>
     </row>
     <row r="64" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="64" t="str">
-        <f>'User Interface'!A63</f>
-        <v>#</v>
-      </c>
-      <c r="B64" s="69" t="s">
-        <v>243</v>
-      </c>
-      <c r="C64" s="73" t="s">
+      <c r="A64" s="64">
+        <f>'User Interface'!A59</f>
+        <v>0</v>
+      </c>
+      <c r="B64" s="60" t="s">
+        <v>242</v>
+      </c>
+      <c r="C64" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="D64" s="60">
-        <f>'User Interface'!E63</f>
-        <v>1.42</v>
-      </c>
-      <c r="E64" s="69" t="s">
-        <v>193</v>
+      <c r="D64" s="60" t="str">
+        <f>'User Interface'!E59</f>
+        <v>['PbI2','PyrrolidiniumIodide','DMSO']</v>
+      </c>
+      <c r="E64" s="60" t="s">
+        <v>196</v>
       </c>
       <c r="F64" s="19"/>
       <c r="G64" s="19"/>
@@ -39031,22 +39026,22 @@
       <c r="Z64" s="4"/>
     </row>
     <row r="65" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="64">
-        <f>'User Interface'!A60</f>
-        <v>0</v>
-      </c>
-      <c r="B65" s="99" t="s">
-        <v>244</v>
-      </c>
-      <c r="C65" s="61" t="s">
+      <c r="A65" s="64" t="str">
+        <f>'User Interface'!A63</f>
+        <v>#</v>
+      </c>
+      <c r="B65" s="69" t="s">
+        <v>243</v>
+      </c>
+      <c r="C65" s="73" t="s">
         <v>20</v>
       </c>
       <c r="D65" s="60">
-        <f>'User Interface'!E60</f>
+        <f>'User Interface'!E63</f>
         <v>1.42</v>
       </c>
-      <c r="E65" s="60" t="s">
-        <v>190</v>
+      <c r="E65" s="69" t="s">
+        <v>193</v>
       </c>
       <c r="F65" s="19"/>
       <c r="G65" s="19"/>
@@ -39072,18 +39067,18 @@
     </row>
     <row r="66" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="64">
-        <f>'User Interface'!A61</f>
+        <f>'User Interface'!A60</f>
         <v>0</v>
       </c>
       <c r="B66" s="99" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C66" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D66" s="60">
-        <f>'User Interface'!E61</f>
-        <v>1.06</v>
+        <f>'User Interface'!E60</f>
+        <v>1.42</v>
       </c>
       <c r="E66" s="60" t="s">
         <v>190</v>
@@ -39111,19 +39106,19 @@
       <c r="Z66" s="4"/>
     </row>
     <row r="67" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="64" t="str">
-        <f>'User Interface'!A62</f>
-        <v>#</v>
-      </c>
-      <c r="B67" s="60" t="s">
-        <v>246</v>
+      <c r="A67" s="64">
+        <f>'User Interface'!A61</f>
+        <v>0</v>
+      </c>
+      <c r="B67" s="99" t="s">
+        <v>245</v>
       </c>
       <c r="C67" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="D67" s="60" t="str">
-        <f>'User Interface'!E62</f>
-        <v>['PbI2','PyrrolidiniumIodide','DMSO']</v>
+      <c r="D67" s="60">
+        <f>'User Interface'!E61</f>
+        <v>1.06</v>
       </c>
       <c r="E67" s="60" t="s">
         <v>190</v>
@@ -39152,21 +39147,21 @@
     </row>
     <row r="68" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="64" t="str">
-        <f>'User Interface'!A64</f>
+        <f>'User Interface'!A62</f>
         <v>#</v>
       </c>
       <c r="B68" s="60" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C68" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="D68" s="60">
-        <f>'User Interface'!E64</f>
-        <v>1.06</v>
+      <c r="D68" s="60" t="str">
+        <f>'User Interface'!E62</f>
+        <v>['PbI2','PyrrolidiniumIodide','DMSO']</v>
       </c>
       <c r="E68" s="60" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F68" s="19"/>
       <c r="G68" s="19"/>
@@ -39192,18 +39187,18 @@
     </row>
     <row r="69" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="64" t="str">
-        <f>'User Interface'!A65</f>
+        <f>'User Interface'!A64</f>
         <v>#</v>
       </c>
       <c r="B69" s="60" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C69" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="D69" s="60" t="str">
-        <f>'User Interface'!E65</f>
-        <v>['PbI2','PyrrolidiniumIodide','DMSO']</v>
+      <c r="D69" s="60">
+        <f>'User Interface'!E64</f>
+        <v>1.06</v>
       </c>
       <c r="E69" s="60" t="s">
         <v>192</v>
@@ -39232,18 +39227,18 @@
     </row>
     <row r="70" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="64" t="str">
-        <f>'User Interface'!A66</f>
+        <f>'User Interface'!A65</f>
         <v>#</v>
       </c>
       <c r="B70" s="60" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C70" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="D70" s="60">
-        <f>'User Interface'!E66</f>
-        <v>1.42</v>
+      <c r="D70" s="60" t="str">
+        <f>'User Interface'!E65</f>
+        <v>['PbI2','PyrrolidiniumIodide','DMSO']</v>
       </c>
       <c r="E70" s="60" t="s">
         <v>192</v>
@@ -39271,11 +39266,23 @@
       <c r="Z70" s="4"/>
     </row>
     <row r="71" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="64"/>
-      <c r="B71" s="60"/>
-      <c r="C71" s="61"/>
-      <c r="D71" s="60"/>
-      <c r="E71" s="60"/>
+      <c r="A71" s="64" t="str">
+        <f>'User Interface'!A66</f>
+        <v>#</v>
+      </c>
+      <c r="B71" s="60" t="s">
+        <v>249</v>
+      </c>
+      <c r="C71" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="D71" s="60">
+        <f>'User Interface'!E66</f>
+        <v>1.42</v>
+      </c>
+      <c r="E71" s="60" t="s">
+        <v>192</v>
+      </c>
       <c r="F71" s="19"/>
       <c r="G71" s="19"/>
       <c r="H71" s="19"/>
@@ -39299,23 +39306,11 @@
       <c r="Z71" s="4"/>
     </row>
     <row r="72" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="64" t="str">
-        <f>'User Interface'!A68</f>
-        <v>#</v>
-      </c>
-      <c r="B72" s="60" t="s">
-        <v>250</v>
-      </c>
-      <c r="C72" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="D72" s="60" t="str">
-        <f>'User Interface'!E68</f>
-        <v>['PbI2','PyrrolidiniumIodide','DMSO']</v>
-      </c>
-      <c r="E72" s="60" t="s">
-        <v>196</v>
-      </c>
+      <c r="A72" s="64"/>
+      <c r="B72" s="60"/>
+      <c r="C72" s="61"/>
+      <c r="D72" s="60"/>
+      <c r="E72" s="60"/>
       <c r="F72" s="19"/>
       <c r="G72" s="19"/>
       <c r="H72" s="19"/>
@@ -39340,21 +39335,21 @@
     </row>
     <row r="73" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="64" t="str">
-        <f>'User Interface'!A72</f>
+        <f>'User Interface'!A68</f>
         <v>#</v>
       </c>
-      <c r="B73" s="69" t="s">
-        <v>251</v>
-      </c>
-      <c r="C73" s="73" t="s">
+      <c r="B73" s="60" t="s">
+        <v>250</v>
+      </c>
+      <c r="C73" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="D73" s="60">
-        <f>'User Interface'!E72</f>
-        <v>0</v>
-      </c>
-      <c r="E73" s="69" t="s">
-        <v>193</v>
+      <c r="D73" s="60" t="str">
+        <f>'User Interface'!E68</f>
+        <v>['PbI2','PyrrolidiniumIodide','DMSO']</v>
+      </c>
+      <c r="E73" s="60" t="s">
+        <v>196</v>
       </c>
       <c r="F73" s="19"/>
       <c r="G73" s="19"/>
@@ -39380,21 +39375,21 @@
     </row>
     <row r="74" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="64" t="str">
-        <f>'User Interface'!A69</f>
+        <f>'User Interface'!A72</f>
         <v>#</v>
       </c>
-      <c r="B74" s="99" t="s">
-        <v>252</v>
-      </c>
-      <c r="C74" s="61" t="s">
+      <c r="B74" s="69" t="s">
+        <v>251</v>
+      </c>
+      <c r="C74" s="73" t="s">
         <v>20</v>
       </c>
       <c r="D74" s="60">
-        <f>'User Interface'!E69</f>
-        <v>1.42</v>
-      </c>
-      <c r="E74" s="60" t="s">
-        <v>190</v>
+        <f>'User Interface'!E72</f>
+        <v>0</v>
+      </c>
+      <c r="E74" s="69" t="s">
+        <v>193</v>
       </c>
       <c r="F74" s="19"/>
       <c r="G74" s="19"/>
@@ -39420,18 +39415,18 @@
     </row>
     <row r="75" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="64" t="str">
-        <f>'User Interface'!A70</f>
+        <f>'User Interface'!A69</f>
         <v>#</v>
       </c>
       <c r="B75" s="99" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C75" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D75" s="60">
-        <f>'User Interface'!E70</f>
-        <v>1.06</v>
+        <f>'User Interface'!E69</f>
+        <v>1.42</v>
       </c>
       <c r="E75" s="60" t="s">
         <v>190</v>
@@ -39460,18 +39455,18 @@
     </row>
     <row r="76" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="64" t="str">
-        <f>'User Interface'!A71</f>
+        <f>'User Interface'!A70</f>
         <v>#</v>
       </c>
-      <c r="B76" s="60" t="s">
-        <v>254</v>
+      <c r="B76" s="99" t="s">
+        <v>253</v>
       </c>
       <c r="C76" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D76" s="60">
-        <f>'User Interface'!E71</f>
-        <v>0</v>
+        <f>'User Interface'!E70</f>
+        <v>1.06</v>
       </c>
       <c r="E76" s="60" t="s">
         <v>190</v>
@@ -39500,21 +39495,21 @@
     </row>
     <row r="77" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="64" t="str">
-        <f>'User Interface'!A73</f>
+        <f>'User Interface'!A71</f>
         <v>#</v>
       </c>
       <c r="B77" s="60" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C77" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D77" s="60">
-        <f>'User Interface'!E73</f>
+        <f>'User Interface'!E71</f>
         <v>0</v>
       </c>
       <c r="E77" s="60" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F77" s="19"/>
       <c r="G77" s="19"/>
@@ -39540,17 +39535,17 @@
     </row>
     <row r="78" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="64" t="str">
-        <f>'User Interface'!A74</f>
+        <f>'User Interface'!A73</f>
         <v>#</v>
       </c>
       <c r="B78" s="60" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C78" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D78" s="60">
-        <f>'User Interface'!E74</f>
+        <f>'User Interface'!E73</f>
         <v>0</v>
       </c>
       <c r="E78" s="60" t="s">
@@ -39580,17 +39575,17 @@
     </row>
     <row r="79" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="64" t="str">
-        <f>'User Interface'!A75</f>
+        <f>'User Interface'!A74</f>
         <v>#</v>
       </c>
       <c r="B79" s="60" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C79" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D79" s="60">
-        <f>'User Interface'!E75</f>
+        <f>'User Interface'!E74</f>
         <v>0</v>
       </c>
       <c r="E79" s="60" t="s">
@@ -39619,11 +39614,23 @@
       <c r="Z79" s="4"/>
     </row>
     <row r="80" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="67"/>
-      <c r="B80" s="60"/>
-      <c r="C80" s="73"/>
-      <c r="D80" s="69"/>
-      <c r="E80" s="69"/>
+      <c r="A80" s="64" t="str">
+        <f>'User Interface'!A75</f>
+        <v>#</v>
+      </c>
+      <c r="B80" s="60" t="s">
+        <v>257</v>
+      </c>
+      <c r="C80" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="D80" s="60">
+        <f>'User Interface'!E75</f>
+        <v>0</v>
+      </c>
+      <c r="E80" s="60" t="s">
+        <v>192</v>
+      </c>
       <c r="F80" s="19"/>
       <c r="G80" s="19"/>
       <c r="H80" s="19"/>
@@ -39647,23 +39654,11 @@
       <c r="Z80" s="4"/>
     </row>
     <row r="81" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="64">
-        <f>'User Interface'!A77</f>
-        <v>0</v>
-      </c>
-      <c r="B81" s="60" t="s">
-        <v>258</v>
-      </c>
-      <c r="C81" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="D81" s="60" t="str">
-        <f>'User Interface'!E77</f>
-        <v>['FAH']</v>
-      </c>
-      <c r="E81" s="60" t="s">
-        <v>196</v>
-      </c>
+      <c r="A81" s="67"/>
+      <c r="B81" s="60"/>
+      <c r="C81" s="73"/>
+      <c r="D81" s="69"/>
+      <c r="E81" s="69"/>
       <c r="F81" s="19"/>
       <c r="G81" s="19"/>
       <c r="H81" s="19"/>
@@ -39687,22 +39682,22 @@
       <c r="Z81" s="4"/>
     </row>
     <row r="82" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="64" t="str">
-        <f>'User Interface'!A81</f>
-        <v>#</v>
-      </c>
-      <c r="B82" s="69" t="s">
-        <v>259</v>
-      </c>
-      <c r="C82" s="73" t="s">
+      <c r="A82" s="64">
+        <f>'User Interface'!A77</f>
+        <v>0</v>
+      </c>
+      <c r="B82" s="60" t="s">
+        <v>258</v>
+      </c>
+      <c r="C82" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="D82" s="60">
-        <f>'User Interface'!E81</f>
-        <v>0</v>
-      </c>
-      <c r="E82" s="69" t="s">
-        <v>193</v>
+      <c r="D82" s="60" t="str">
+        <f>'User Interface'!E77</f>
+        <v>['FAH']</v>
+      </c>
+      <c r="E82" s="60" t="s">
+        <v>196</v>
       </c>
       <c r="F82" s="19"/>
       <c r="G82" s="19"/>
@@ -39728,21 +39723,21 @@
     </row>
     <row r="83" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="64" t="str">
-        <f>'User Interface'!A78</f>
+        <f>'User Interface'!A81</f>
         <v>#</v>
       </c>
-      <c r="B83" s="99" t="s">
-        <v>260</v>
-      </c>
-      <c r="C83" s="61" t="s">
+      <c r="B83" s="69" t="s">
+        <v>259</v>
+      </c>
+      <c r="C83" s="73" t="s">
         <v>20</v>
       </c>
       <c r="D83" s="60">
-        <f>'User Interface'!E78</f>
-        <v>1.5</v>
-      </c>
-      <c r="E83" s="60" t="s">
-        <v>190</v>
+        <f>'User Interface'!E81</f>
+        <v>0</v>
+      </c>
+      <c r="E83" s="69" t="s">
+        <v>193</v>
       </c>
       <c r="F83" s="19"/>
       <c r="G83" s="19"/>
@@ -39768,18 +39763,18 @@
     </row>
     <row r="84" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="64" t="str">
-        <f>'User Interface'!A79</f>
+        <f>'User Interface'!A78</f>
         <v>#</v>
       </c>
       <c r="B84" s="99" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C84" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D84" s="60">
-        <f>'User Interface'!E79</f>
-        <v>7.63</v>
+        <f>'User Interface'!E78</f>
+        <v>1.5</v>
       </c>
       <c r="E84" s="60" t="s">
         <v>190</v>
@@ -39808,18 +39803,18 @@
     </row>
     <row r="85" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="64" t="str">
-        <f>'User Interface'!A80</f>
+        <f>'User Interface'!A79</f>
         <v>#</v>
       </c>
-      <c r="B85" s="60" t="s">
-        <v>262</v>
+      <c r="B85" s="99" t="s">
+        <v>261</v>
       </c>
       <c r="C85" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D85" s="60">
-        <f>'User Interface'!E80</f>
-        <v>0</v>
+        <f>'User Interface'!E79</f>
+        <v>7.63</v>
       </c>
       <c r="E85" s="60" t="s">
         <v>190</v>
@@ -39848,21 +39843,21 @@
     </row>
     <row r="86" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="64" t="str">
-        <f>'User Interface'!A82</f>
+        <f>'User Interface'!A80</f>
         <v>#</v>
       </c>
       <c r="B86" s="60" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C86" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D86" s="60">
-        <f>'User Interface'!E82</f>
+        <f>'User Interface'!E80</f>
         <v>0</v>
       </c>
       <c r="E86" s="60" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F86" s="19"/>
       <c r="G86" s="19"/>
@@ -39888,17 +39883,17 @@
     </row>
     <row r="87" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="64" t="str">
-        <f>'User Interface'!A83</f>
+        <f>'User Interface'!A82</f>
         <v>#</v>
       </c>
       <c r="B87" s="60" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C87" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D87" s="60">
-        <f>'User Interface'!E83</f>
+        <f>'User Interface'!E82</f>
         <v>0</v>
       </c>
       <c r="E87" s="60" t="s">
@@ -39928,17 +39923,17 @@
     </row>
     <row r="88" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="64" t="str">
-        <f>'User Interface'!A84</f>
+        <f>'User Interface'!A83</f>
         <v>#</v>
       </c>
       <c r="B88" s="60" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C88" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D88" s="60">
-        <f>'User Interface'!E84</f>
+        <f>'User Interface'!E83</f>
         <v>0</v>
       </c>
       <c r="E88" s="60" t="s">
@@ -39967,11 +39962,23 @@
       <c r="Z88" s="4"/>
     </row>
     <row r="89" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="67"/>
-      <c r="B89" s="69"/>
-      <c r="C89" s="73"/>
-      <c r="D89" s="69"/>
-      <c r="E89" s="69"/>
+      <c r="A89" s="64" t="str">
+        <f>'User Interface'!A84</f>
+        <v>#</v>
+      </c>
+      <c r="B89" s="60" t="s">
+        <v>265</v>
+      </c>
+      <c r="C89" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="D89" s="60">
+        <f>'User Interface'!E84</f>
+        <v>0</v>
+      </c>
+      <c r="E89" s="60" t="s">
+        <v>192</v>
+      </c>
       <c r="F89" s="19"/>
       <c r="G89" s="19"/>
       <c r="H89" s="19"/>
@@ -39995,23 +40002,11 @@
       <c r="Z89" s="4"/>
     </row>
     <row r="90" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="64">
-        <f>'Old Reagents'!B11</f>
-        <v>0</v>
-      </c>
-      <c r="B90" s="60" t="s">
-        <v>282</v>
-      </c>
-      <c r="C90" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="D90" s="69" t="str">
-        <f>'Old Reagents'!F11</f>
-        <v>['DMSO']</v>
-      </c>
-      <c r="E90" s="60" t="s">
-        <v>196</v>
-      </c>
+      <c r="A90" s="67"/>
+      <c r="B90" s="69"/>
+      <c r="C90" s="73"/>
+      <c r="D90" s="69"/>
+      <c r="E90" s="69"/>
       <c r="F90" s="19"/>
       <c r="G90" s="19"/>
       <c r="H90" s="19"/>
@@ -40035,22 +40030,22 @@
       <c r="Z90" s="4"/>
     </row>
     <row r="91" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="64" t="str">
-        <f>'Old Reagents'!B12</f>
-        <v>#</v>
-      </c>
-      <c r="B91" s="69" t="s">
-        <v>283</v>
-      </c>
-      <c r="C91" s="73" t="s">
+      <c r="A91" s="64">
+        <f>'Old Reagents'!B11</f>
+        <v>0</v>
+      </c>
+      <c r="B91" s="60" t="s">
+        <v>282</v>
+      </c>
+      <c r="C91" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="D91" s="69">
-        <f>'Old Reagents'!F12</f>
-        <v>0</v>
-      </c>
-      <c r="E91" s="69" t="s">
-        <v>193</v>
+      <c r="D91" s="69" t="str">
+        <f>'Old Reagents'!F11</f>
+        <v>['DMSO']</v>
+      </c>
+      <c r="E91" s="60" t="s">
+        <v>196</v>
       </c>
       <c r="F91" s="19"/>
       <c r="G91" s="19"/>
@@ -40076,21 +40071,21 @@
     </row>
     <row r="92" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="64" t="str">
-        <f>'Old Reagents'!B13</f>
+        <f>'Old Reagents'!B12</f>
         <v>#</v>
       </c>
       <c r="B92" s="60" t="s">
         <v>284</v>
       </c>
-      <c r="C92" s="61" t="s">
+      <c r="C92" s="73" t="s">
         <v>20</v>
       </c>
       <c r="D92" s="69">
-        <f>'Old Reagents'!F13</f>
-        <v>1.5</v>
-      </c>
-      <c r="E92" s="60" t="s">
-        <v>190</v>
+        <f>'Old Reagents'!F12</f>
+        <v>0</v>
+      </c>
+      <c r="E92" s="69" t="s">
+        <v>193</v>
       </c>
       <c r="F92" s="19"/>
       <c r="G92" s="19"/>
@@ -40116,7 +40111,7 @@
     </row>
     <row r="93" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="64" t="str">
-        <f>'Old Reagents'!B14</f>
+        <f>'Old Reagents'!B13</f>
         <v>#</v>
       </c>
       <c r="B93" s="60" t="s">
@@ -40126,8 +40121,8 @@
         <v>20</v>
       </c>
       <c r="D93" s="69">
-        <f>'Old Reagents'!F14</f>
-        <v>7.63</v>
+        <f>'Old Reagents'!F13</f>
+        <v>1.5</v>
       </c>
       <c r="E93" s="60" t="s">
         <v>190</v>
@@ -40156,7 +40151,7 @@
     </row>
     <row r="94" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="64" t="str">
-        <f>'Old Reagents'!B15</f>
+        <f>'Old Reagents'!B14</f>
         <v>#</v>
       </c>
       <c r="B94" s="60" t="s">
@@ -40166,8 +40161,8 @@
         <v>20</v>
       </c>
       <c r="D94" s="69">
-        <f>'Old Reagents'!F15</f>
-        <v>0</v>
+        <f>'Old Reagents'!F14</f>
+        <v>7.63</v>
       </c>
       <c r="E94" s="60" t="s">
         <v>190</v>
@@ -40196,21 +40191,21 @@
     </row>
     <row r="95" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="64" t="str">
-        <f>'Old Reagents'!B16</f>
+        <f>'Old Reagents'!B15</f>
         <v>#</v>
       </c>
       <c r="B95" s="60" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="C95" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D95" s="69">
-        <f>'Old Reagents'!F16</f>
+        <f>'Old Reagents'!F15</f>
         <v>0</v>
       </c>
       <c r="E95" s="60" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F95" s="19"/>
       <c r="G95" s="19"/>
@@ -40236,17 +40231,17 @@
     </row>
     <row r="96" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="64" t="str">
-        <f>'Old Reagents'!B17</f>
+        <f>'Old Reagents'!B16</f>
         <v>#</v>
       </c>
       <c r="B96" s="60" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C96" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D96" s="69">
-        <f>'Old Reagents'!F17</f>
+        <f>'Old Reagents'!F16</f>
         <v>0</v>
       </c>
       <c r="E96" s="60" t="s">
@@ -40276,17 +40271,17 @@
     </row>
     <row r="97" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="64" t="str">
-        <f>'Old Reagents'!B18</f>
+        <f>'Old Reagents'!B17</f>
         <v>#</v>
       </c>
       <c r="B97" s="60" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C97" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D97" s="69">
-        <f>'Old Reagents'!F18</f>
+        <f>'Old Reagents'!F17</f>
         <v>0</v>
       </c>
       <c r="E97" s="60" t="s">
@@ -40315,11 +40310,23 @@
       <c r="Z97" s="4"/>
     </row>
     <row r="98" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="64"/>
-      <c r="B98" s="69"/>
-      <c r="C98" s="73"/>
-      <c r="D98" s="69"/>
-      <c r="E98" s="69"/>
+      <c r="A98" s="64" t="str">
+        <f>'Old Reagents'!B18</f>
+        <v>#</v>
+      </c>
+      <c r="B98" s="60" t="s">
+        <v>289</v>
+      </c>
+      <c r="C98" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="D98" s="69">
+        <f>'Old Reagents'!F18</f>
+        <v>0</v>
+      </c>
+      <c r="E98" s="60" t="s">
+        <v>192</v>
+      </c>
       <c r="F98" s="19"/>
       <c r="G98" s="19"/>
       <c r="H98" s="19"/>
@@ -40343,23 +40350,11 @@
       <c r="Z98" s="4"/>
     </row>
     <row r="99" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="64">
-        <f>'Old Reagents'!B20</f>
-        <v>0</v>
-      </c>
-      <c r="B99" s="60" t="s">
-        <v>290</v>
-      </c>
-      <c r="C99" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="D99" s="69" t="str">
-        <f>'Old Reagents'!F20</f>
-        <v>['PbI2','PyrrolidiniumIodide','DMSO']</v>
-      </c>
-      <c r="E99" s="60" t="s">
-        <v>196</v>
-      </c>
+      <c r="A99" s="64"/>
+      <c r="B99" s="69"/>
+      <c r="C99" s="73"/>
+      <c r="D99" s="69"/>
+      <c r="E99" s="69"/>
       <c r="F99" s="19"/>
       <c r="G99" s="19"/>
       <c r="H99" s="19"/>
@@ -40384,21 +40379,21 @@
     </row>
     <row r="100" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="64">
-        <f>'Old Reagents'!B21</f>
+        <f>'Old Reagents'!B20</f>
         <v>0</v>
       </c>
-      <c r="B100" s="69" t="s">
-        <v>291</v>
-      </c>
-      <c r="C100" s="73" t="s">
+      <c r="B100" s="60" t="s">
+        <v>290</v>
+      </c>
+      <c r="C100" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="D100" s="69">
-        <f>'Old Reagents'!F21</f>
-        <v>1.55</v>
-      </c>
-      <c r="E100" s="69" t="s">
-        <v>193</v>
+      <c r="D100" s="69" t="str">
+        <f>'Old Reagents'!F20</f>
+        <v>['PbI2','PyrrolidiniumIodide','DMSO']</v>
+      </c>
+      <c r="E100" s="60" t="s">
+        <v>196</v>
       </c>
       <c r="F100" s="19"/>
       <c r="G100" s="19"/>
@@ -40424,21 +40419,21 @@
     </row>
     <row r="101" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="64">
-        <f>'Old Reagents'!B22</f>
+        <f>'Old Reagents'!B21</f>
         <v>0</v>
       </c>
       <c r="B101" s="60" t="s">
         <v>292</v>
       </c>
-      <c r="C101" s="61" t="s">
+      <c r="C101" s="73" t="s">
         <v>20</v>
       </c>
       <c r="D101" s="69">
-        <f>'Old Reagents'!F22</f>
-        <v>1.93</v>
-      </c>
-      <c r="E101" s="60" t="s">
-        <v>190</v>
+        <f>'Old Reagents'!F21</f>
+        <v>1.55</v>
+      </c>
+      <c r="E101" s="69" t="s">
+        <v>193</v>
       </c>
       <c r="F101" s="19"/>
       <c r="G101" s="19"/>
@@ -40463,9 +40458,9 @@
       <c r="Z101" s="4"/>
     </row>
     <row r="102" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="64" t="str">
-        <f>'Old Reagents'!B23</f>
-        <v>#</v>
+      <c r="A102" s="64">
+        <f>'Old Reagents'!B22</f>
+        <v>0</v>
       </c>
       <c r="B102" s="60" t="s">
         <v>293</v>
@@ -40474,8 +40469,8 @@
         <v>20</v>
       </c>
       <c r="D102" s="69">
-        <f>'Old Reagents'!F23</f>
-        <v>0</v>
+        <f>'Old Reagents'!F22</f>
+        <v>1.93</v>
       </c>
       <c r="E102" s="60" t="s">
         <v>190</v>
@@ -40504,7 +40499,7 @@
     </row>
     <row r="103" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="64" t="str">
-        <f>'Old Reagents'!B24</f>
+        <f>'Old Reagents'!B23</f>
         <v>#</v>
       </c>
       <c r="B103" s="60" t="s">
@@ -40514,7 +40509,7 @@
         <v>20</v>
       </c>
       <c r="D103" s="69">
-        <f>'Old Reagents'!F24</f>
+        <f>'Old Reagents'!F23</f>
         <v>0</v>
       </c>
       <c r="E103" s="60" t="s">
@@ -40544,57 +40539,57 @@
     </row>
     <row r="104" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="64" t="str">
-        <f>'Old Reagents'!B25</f>
+        <f>'Old Reagents'!B24</f>
         <v>#</v>
       </c>
       <c r="B104" s="60" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C104" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D104" s="69">
-        <f>'Old Reagents'!F25</f>
+        <f>'Old Reagents'!F24</f>
         <v>0</v>
       </c>
       <c r="E104" s="60" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F104" s="19"/>
-      <c r="G104" s="4"/>
-      <c r="H104" s="4"/>
-      <c r="I104" s="4"/>
-      <c r="J104" s="4"/>
-      <c r="K104" s="4"/>
-      <c r="L104" s="4"/>
-      <c r="M104" s="4"/>
-      <c r="N104" s="4"/>
-      <c r="O104" s="4"/>
-      <c r="P104" s="4"/>
-      <c r="Q104" s="4"/>
-      <c r="R104" s="4"/>
-      <c r="S104" s="4"/>
-      <c r="T104" s="4"/>
-      <c r="U104" s="4"/>
-      <c r="V104" s="4"/>
-      <c r="W104" s="4"/>
+      <c r="G104" s="19"/>
+      <c r="H104" s="19"/>
+      <c r="I104" s="19"/>
+      <c r="J104" s="19"/>
+      <c r="K104" s="19"/>
+      <c r="L104" s="19"/>
+      <c r="M104" s="19"/>
+      <c r="N104" s="19"/>
+      <c r="O104" s="19"/>
+      <c r="P104" s="19"/>
+      <c r="Q104" s="19"/>
+      <c r="R104" s="19"/>
+      <c r="S104" s="19"/>
+      <c r="T104" s="19"/>
+      <c r="U104" s="19"/>
+      <c r="V104" s="19"/>
+      <c r="W104" s="19"/>
       <c r="X104" s="4"/>
       <c r="Y104" s="4"/>
       <c r="Z104" s="4"/>
     </row>
-    <row r="105" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="64" t="str">
-        <f>'Old Reagents'!B26</f>
+        <f>'Old Reagents'!B25</f>
         <v>#</v>
       </c>
       <c r="B105" s="60" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C105" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D105" s="69">
-        <f>'Old Reagents'!F26</f>
+        <f>'Old Reagents'!F25</f>
         <v>0</v>
       </c>
       <c r="E105" s="60" t="s">
@@ -40624,17 +40619,17 @@
     </row>
     <row r="106" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="64" t="str">
-        <f>'Old Reagents'!B27</f>
+        <f>'Old Reagents'!B26</f>
         <v>#</v>
       </c>
       <c r="B106" s="60" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C106" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D106" s="69">
-        <f>'Old Reagents'!F27</f>
+        <f>'Old Reagents'!F26</f>
         <v>0</v>
       </c>
       <c r="E106" s="60" t="s">
@@ -40663,14 +40658,23 @@
       <c r="Z106" s="4"/>
     </row>
     <row r="107" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="64"/>
-      <c r="B107" s="60"/>
-      <c r="C107" s="61"/>
+      <c r="A107" s="64" t="str">
+        <f>'Old Reagents'!B27</f>
+        <v>#</v>
+      </c>
+      <c r="B107" s="60" t="s">
+        <v>297</v>
+      </c>
+      <c r="C107" s="61" t="s">
+        <v>20</v>
+      </c>
       <c r="D107" s="69">
-        <f>'Old Reagents'!F28</f>
+        <f>'Old Reagents'!F27</f>
         <v>0</v>
       </c>
-      <c r="E107" s="60"/>
+      <c r="E107" s="60" t="s">
+        <v>192</v>
+      </c>
       <c r="F107" s="19"/>
       <c r="G107" s="4"/>
       <c r="H107" s="4"/>
@@ -40694,23 +40698,14 @@
       <c r="Z107" s="4"/>
     </row>
     <row r="108" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="64">
-        <f>'Old Reagents'!B29</f>
+      <c r="A108" s="64"/>
+      <c r="B108" s="60"/>
+      <c r="C108" s="61"/>
+      <c r="D108" s="69">
+        <f>'Old Reagents'!F28</f>
         <v>0</v>
       </c>
-      <c r="B108" s="60" t="s">
-        <v>298</v>
-      </c>
-      <c r="C108" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="D108" s="69" t="str">
-        <f>'Old Reagents'!F29</f>
-        <v>['PyrrolidiniumIodide','DMSO']</v>
-      </c>
-      <c r="E108" s="60" t="s">
-        <v>196</v>
-      </c>
+      <c r="E108" s="60"/>
       <c r="F108" s="19"/>
       <c r="G108" s="4"/>
       <c r="H108" s="4"/>
@@ -40735,21 +40730,21 @@
     </row>
     <row r="109" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="64">
-        <f>'Old Reagents'!B30</f>
+        <f>'Old Reagents'!B29</f>
         <v>0</v>
       </c>
-      <c r="B109" s="69" t="s">
-        <v>299</v>
-      </c>
-      <c r="C109" s="73" t="s">
+      <c r="B109" s="60" t="s">
+        <v>298</v>
+      </c>
+      <c r="C109" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="D109" s="69">
-        <f>'Old Reagents'!F30</f>
-        <v>2.06</v>
-      </c>
-      <c r="E109" s="69" t="s">
-        <v>193</v>
+      <c r="D109" s="69" t="str">
+        <f>'Old Reagents'!F29</f>
+        <v>['PyrrolidiniumIodide','DMSO']</v>
+      </c>
+      <c r="E109" s="60" t="s">
+        <v>196</v>
       </c>
       <c r="F109" s="19"/>
       <c r="G109" s="4"/>
@@ -40774,22 +40769,22 @@
       <c r="Z109" s="4"/>
     </row>
     <row r="110" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="64" t="str">
-        <f>'Old Reagents'!B31</f>
-        <v>#</v>
+      <c r="A110" s="64">
+        <f>'Old Reagents'!B30</f>
+        <v>0</v>
       </c>
       <c r="B110" s="99" t="s">
-        <v>300</v>
-      </c>
-      <c r="C110" s="61" t="s">
+        <v>299</v>
+      </c>
+      <c r="C110" s="73" t="s">
         <v>20</v>
       </c>
       <c r="D110" s="69">
-        <f>'Old Reagents'!F31</f>
-        <v>1.33</v>
-      </c>
-      <c r="E110" s="60" t="s">
-        <v>190</v>
+        <f>'Old Reagents'!F30</f>
+        <v>2.06</v>
+      </c>
+      <c r="E110" s="69" t="s">
+        <v>193</v>
       </c>
       <c r="F110" s="19"/>
       <c r="G110" s="4"/>
@@ -40815,18 +40810,18 @@
     </row>
     <row r="111" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="64" t="str">
-        <f>'Old Reagents'!B32</f>
+        <f>'Old Reagents'!B31</f>
         <v>#</v>
       </c>
       <c r="B111" s="60" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C111" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D111" s="69">
-        <f>'Old Reagents'!F32</f>
-        <v>1.2</v>
+        <f>'Old Reagents'!F31</f>
+        <v>1.33</v>
       </c>
       <c r="E111" s="60" t="s">
         <v>190</v>
@@ -40855,18 +40850,18 @@
     </row>
     <row r="112" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="64" t="str">
-        <f>'Old Reagents'!B33</f>
+        <f>'Old Reagents'!B32</f>
         <v>#</v>
       </c>
       <c r="B112" s="60" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C112" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D112" s="69">
-        <f>'Old Reagents'!F33</f>
-        <v>0</v>
+        <f>'Old Reagents'!F32</f>
+        <v>1.2</v>
       </c>
       <c r="E112" s="60" t="s">
         <v>190</v>
@@ -40895,21 +40890,21 @@
     </row>
     <row r="113" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="64" t="str">
-        <f>'Old Reagents'!B34</f>
+        <f>'Old Reagents'!B33</f>
         <v>#</v>
       </c>
       <c r="B113" s="60" t="s">
-        <v>303</v>
+        <v>341</v>
       </c>
       <c r="C113" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D113" s="69">
-        <f>'Old Reagents'!F34</f>
+        <f>'Old Reagents'!F33</f>
         <v>0</v>
       </c>
       <c r="E113" s="60" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F113" s="19"/>
       <c r="G113" s="4"/>
@@ -40935,17 +40930,17 @@
     </row>
     <row r="114" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="64" t="str">
-        <f>'Old Reagents'!B35</f>
+        <f>'Old Reagents'!B34</f>
         <v>#</v>
       </c>
       <c r="B114" s="60" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C114" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D114" s="69">
-        <f>'Old Reagents'!F35</f>
+        <f>'Old Reagents'!F34</f>
         <v>0</v>
       </c>
       <c r="E114" s="60" t="s">
@@ -40975,17 +40970,17 @@
     </row>
     <row r="115" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="64" t="str">
-        <f>'Old Reagents'!B36</f>
+        <f>'Old Reagents'!B35</f>
         <v>#</v>
       </c>
       <c r="B115" s="60" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C115" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D115" s="69">
-        <f>'Old Reagents'!F36</f>
+        <f>'Old Reagents'!F35</f>
         <v>0</v>
       </c>
       <c r="E115" s="60" t="s">
@@ -41014,11 +41009,23 @@
       <c r="Z115" s="4"/>
     </row>
     <row r="116" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="64"/>
-      <c r="B116" s="60"/>
-      <c r="C116" s="61"/>
-      <c r="D116" s="69"/>
-      <c r="E116" s="60"/>
+      <c r="A116" s="64" t="str">
+        <f>'Old Reagents'!B36</f>
+        <v>#</v>
+      </c>
+      <c r="B116" s="60" t="s">
+        <v>304</v>
+      </c>
+      <c r="C116" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="D116" s="69">
+        <f>'Old Reagents'!F36</f>
+        <v>0</v>
+      </c>
+      <c r="E116" s="60" t="s">
+        <v>192</v>
+      </c>
       <c r="F116" s="19"/>
       <c r="G116" s="4"/>
       <c r="H116" s="4"/>
@@ -41042,23 +41049,11 @@
       <c r="Z116" s="4"/>
     </row>
     <row r="117" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="64">
-        <f>'Old Reagents'!B38</f>
-        <v>0</v>
-      </c>
-      <c r="B117" s="60" t="s">
-        <v>306</v>
-      </c>
-      <c r="C117" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="D117" s="69" t="str">
-        <f>'Old Reagents'!F38</f>
-        <v>['PbI2','PyrrolidiniumIodide','DMSO']</v>
-      </c>
-      <c r="E117" s="60" t="s">
-        <v>196</v>
-      </c>
+      <c r="A117" s="64"/>
+      <c r="B117" s="60"/>
+      <c r="C117" s="61"/>
+      <c r="D117" s="69"/>
+      <c r="E117" s="60"/>
       <c r="F117" s="19"/>
       <c r="G117" s="4"/>
       <c r="H117" s="4"/>
@@ -41083,21 +41078,21 @@
     </row>
     <row r="118" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="64">
-        <f>'Old Reagents'!B39</f>
+        <f>'Old Reagents'!B38</f>
         <v>0</v>
       </c>
-      <c r="B118" s="69" t="s">
-        <v>307</v>
-      </c>
-      <c r="C118" s="73" t="s">
+      <c r="B118" s="60" t="s">
+        <v>305</v>
+      </c>
+      <c r="C118" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="D118" s="69">
-        <f>'Old Reagents'!F39</f>
-        <v>1.18</v>
-      </c>
-      <c r="E118" s="69" t="s">
-        <v>193</v>
+      <c r="D118" s="69" t="str">
+        <f>'Old Reagents'!F38</f>
+        <v>['PbI2','PyrrolidiniumIodide','DMSO']</v>
+      </c>
+      <c r="E118" s="60" t="s">
+        <v>196</v>
       </c>
       <c r="F118" s="19"/>
       <c r="G118" s="4"/>
@@ -41123,21 +41118,21 @@
     </row>
     <row r="119" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="64">
-        <f>'Old Reagents'!B40</f>
+        <f>'Old Reagents'!B39</f>
         <v>0</v>
       </c>
       <c r="B119" s="99" t="s">
-        <v>308</v>
-      </c>
-      <c r="C119" s="61" t="s">
+        <v>307</v>
+      </c>
+      <c r="C119" s="73" t="s">
         <v>20</v>
       </c>
       <c r="D119" s="69">
-        <f>'Old Reagents'!F40</f>
-        <v>0.74</v>
-      </c>
-      <c r="E119" s="60" t="s">
-        <v>190</v>
+        <f>'Old Reagents'!F39</f>
+        <v>1.18</v>
+      </c>
+      <c r="E119" s="69" t="s">
+        <v>193</v>
       </c>
       <c r="F119" s="19"/>
       <c r="G119" s="4"/>
@@ -41162,19 +41157,19 @@
       <c r="Z119" s="4"/>
     </row>
     <row r="120" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="64" t="str">
-        <f>'Old Reagents'!B41</f>
-        <v>#</v>
+      <c r="A120" s="64">
+        <f>'Old Reagents'!B40</f>
+        <v>0</v>
       </c>
       <c r="B120" s="99" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C120" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D120" s="69">
-        <f>'Old Reagents'!F41</f>
-        <v>0</v>
+        <f>'Old Reagents'!F40</f>
+        <v>0.74</v>
       </c>
       <c r="E120" s="60" t="s">
         <v>190</v>
@@ -41203,17 +41198,17 @@
     </row>
     <row r="121" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="64" t="str">
-        <f>'Old Reagents'!B42</f>
+        <f>'Old Reagents'!B41</f>
         <v>#</v>
       </c>
       <c r="B121" s="60" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C121" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D121" s="69">
-        <f>'Old Reagents'!F42</f>
+        <f>'Old Reagents'!F41</f>
         <v>0</v>
       </c>
       <c r="E121" s="60" t="s">
@@ -41243,21 +41238,21 @@
     </row>
     <row r="122" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="64" t="str">
-        <f>'Old Reagents'!B43</f>
+        <f>'Old Reagents'!B42</f>
         <v>#</v>
       </c>
       <c r="B122" s="60" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="C122" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D122" s="69">
-        <f>'Old Reagents'!F43</f>
+        <f>'Old Reagents'!F42</f>
         <v>0</v>
       </c>
       <c r="E122" s="60" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F122" s="19"/>
       <c r="G122" s="4"/>
@@ -41283,17 +41278,17 @@
     </row>
     <row r="123" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="64" t="str">
-        <f>'Old Reagents'!B44</f>
+        <f>'Old Reagents'!B43</f>
         <v>#</v>
       </c>
       <c r="B123" s="60" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C123" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D123" s="69">
-        <f>'Old Reagents'!F44</f>
+        <f>'Old Reagents'!F43</f>
         <v>0</v>
       </c>
       <c r="E123" s="60" t="s">
@@ -41323,17 +41318,17 @@
     </row>
     <row r="124" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="64" t="str">
-        <f>'Old Reagents'!B45</f>
+        <f>'Old Reagents'!B44</f>
         <v>#</v>
       </c>
       <c r="B124" s="60" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C124" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D124" s="69">
-        <f>'Old Reagents'!F45</f>
+        <f>'Old Reagents'!F44</f>
         <v>0</v>
       </c>
       <c r="E124" s="60" t="s">
@@ -41362,11 +41357,23 @@
       <c r="Z124" s="4"/>
     </row>
     <row r="125" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A125" s="64"/>
-      <c r="B125" s="60"/>
-      <c r="C125" s="61"/>
-      <c r="D125" s="69"/>
-      <c r="E125" s="60"/>
+      <c r="A125" s="64" t="str">
+        <f>'Old Reagents'!B45</f>
+        <v>#</v>
+      </c>
+      <c r="B125" s="60" t="s">
+        <v>312</v>
+      </c>
+      <c r="C125" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="D125" s="69">
+        <f>'Old Reagents'!F45</f>
+        <v>0</v>
+      </c>
+      <c r="E125" s="60" t="s">
+        <v>192</v>
+      </c>
       <c r="F125" s="19"/>
       <c r="G125" s="4"/>
       <c r="H125" s="4"/>
@@ -41390,23 +41397,11 @@
       <c r="Z125" s="4"/>
     </row>
     <row r="126" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="64">
-        <f>'Old Reagents'!B47</f>
-        <v>0</v>
-      </c>
-      <c r="B126" s="60" t="s">
-        <v>314</v>
-      </c>
-      <c r="C126" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="D126" s="69" t="str">
-        <f>'Old Reagents'!F47</f>
-        <v>['PbI2','PyrrolidiniumIodide','DMSO']</v>
-      </c>
-      <c r="E126" s="60" t="s">
-        <v>196</v>
-      </c>
+      <c r="A126" s="64"/>
+      <c r="B126" s="60"/>
+      <c r="C126" s="61"/>
+      <c r="D126" s="69"/>
+      <c r="E126" s="60"/>
       <c r="F126" s="19"/>
       <c r="G126" s="4"/>
       <c r="H126" s="4"/>
@@ -41431,21 +41426,21 @@
     </row>
     <row r="127" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="64">
-        <f>'Old Reagents'!B48</f>
+        <f>'Old Reagents'!B47</f>
         <v>0</v>
       </c>
-      <c r="B127" s="69" t="s">
-        <v>315</v>
-      </c>
-      <c r="C127" s="73" t="s">
+      <c r="B127" s="60" t="s">
+        <v>313</v>
+      </c>
+      <c r="C127" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="D127" s="69">
-        <f>'Old Reagents'!F48</f>
-        <v>1.42</v>
-      </c>
-      <c r="E127" s="69" t="s">
-        <v>193</v>
+      <c r="D127" s="69" t="str">
+        <f>'Old Reagents'!F47</f>
+        <v>['PbI2','PyrrolidiniumIodide','DMSO']</v>
+      </c>
+      <c r="E127" s="60" t="s">
+        <v>196</v>
       </c>
       <c r="F127" s="19"/>
       <c r="G127" s="4"/>
@@ -41471,21 +41466,21 @@
     </row>
     <row r="128" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="64">
-        <f>'Old Reagents'!B49</f>
+        <f>'Old Reagents'!B48</f>
         <v>0</v>
       </c>
       <c r="B128" s="99" t="s">
-        <v>316</v>
-      </c>
-      <c r="C128" s="61" t="s">
+        <v>315</v>
+      </c>
+      <c r="C128" s="73" t="s">
         <v>20</v>
       </c>
       <c r="D128" s="69">
-        <f>'Old Reagents'!F49</f>
-        <v>1.06</v>
-      </c>
-      <c r="E128" s="60" t="s">
-        <v>190</v>
+        <f>'Old Reagents'!F48</f>
+        <v>1.42</v>
+      </c>
+      <c r="E128" s="69" t="s">
+        <v>193</v>
       </c>
       <c r="F128" s="19"/>
       <c r="G128" s="4"/>
@@ -41510,19 +41505,19 @@
       <c r="Z128" s="4"/>
     </row>
     <row r="129" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A129" s="64" t="str">
-        <f>'Old Reagents'!B50</f>
-        <v>#</v>
+      <c r="A129" s="64">
+        <f>'Old Reagents'!B49</f>
+        <v>0</v>
       </c>
       <c r="B129" s="99" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C129" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="D129" s="69" t="str">
-        <f>'Old Reagents'!F50</f>
-        <v>['PbI2','PyrrolidiniumIodide','DMSO']</v>
+      <c r="D129" s="69">
+        <f>'Old Reagents'!F49</f>
+        <v>1.06</v>
       </c>
       <c r="E129" s="60" t="s">
         <v>190</v>
@@ -41551,18 +41546,18 @@
     </row>
     <row r="130" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="64" t="str">
-        <f>'Old Reagents'!B51</f>
+        <f>'Old Reagents'!B50</f>
         <v>#</v>
       </c>
       <c r="B130" s="60" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C130" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="D130" s="69">
-        <f>'Old Reagents'!F51</f>
-        <v>1.42</v>
+      <c r="D130" s="69" t="str">
+        <f>'Old Reagents'!F50</f>
+        <v>['PbI2','PyrrolidiniumIodide','DMSO']</v>
       </c>
       <c r="E130" s="60" t="s">
         <v>190</v>
@@ -41591,21 +41586,21 @@
     </row>
     <row r="131" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="64" t="str">
-        <f>'Old Reagents'!B52</f>
+        <f>'Old Reagents'!B51</f>
         <v>#</v>
       </c>
       <c r="B131" s="60" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="C131" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D131" s="69">
-        <f>'Old Reagents'!F52</f>
-        <v>1.06</v>
+        <f>'Old Reagents'!F51</f>
+        <v>1.42</v>
       </c>
       <c r="E131" s="60" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F131" s="19"/>
       <c r="G131" s="4"/>
@@ -41631,18 +41626,18 @@
     </row>
     <row r="132" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="64" t="str">
-        <f>'Old Reagents'!B53</f>
+        <f>'Old Reagents'!B52</f>
         <v>#</v>
       </c>
       <c r="B132" s="60" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C132" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="D132" s="69" t="str">
-        <f>'Old Reagents'!F53</f>
-        <v>['PbI2','PyrrolidiniumIodide','DMSO']</v>
+      <c r="D132" s="69">
+        <f>'Old Reagents'!F52</f>
+        <v>1.06</v>
       </c>
       <c r="E132" s="60" t="s">
         <v>192</v>
@@ -41671,18 +41666,18 @@
     </row>
     <row r="133" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="64" t="str">
-        <f>'Old Reagents'!B54</f>
+        <f>'Old Reagents'!B53</f>
         <v>#</v>
       </c>
       <c r="B133" s="60" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C133" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="D133" s="69">
-        <f>'Old Reagents'!F54</f>
-        <v>1.42</v>
+      <c r="D133" s="69" t="str">
+        <f>'Old Reagents'!F53</f>
+        <v>['PbI2','PyrrolidiniumIodide','DMSO']</v>
       </c>
       <c r="E133" s="60" t="s">
         <v>192</v>
@@ -41710,11 +41705,23 @@
       <c r="Z133" s="4"/>
     </row>
     <row r="134" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A134" s="64"/>
-      <c r="B134" s="60"/>
-      <c r="C134" s="61"/>
-      <c r="D134" s="69"/>
-      <c r="E134" s="60"/>
+      <c r="A134" s="64" t="str">
+        <f>'Old Reagents'!B54</f>
+        <v>#</v>
+      </c>
+      <c r="B134" s="60" t="s">
+        <v>320</v>
+      </c>
+      <c r="C134" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="D134" s="69">
+        <f>'Old Reagents'!F54</f>
+        <v>1.42</v>
+      </c>
+      <c r="E134" s="60" t="s">
+        <v>192</v>
+      </c>
       <c r="F134" s="19"/>
       <c r="G134" s="4"/>
       <c r="H134" s="4"/>
@@ -41738,23 +41745,11 @@
       <c r="Z134" s="4"/>
     </row>
     <row r="135" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A135" s="64" t="str">
-        <f>'Old Reagents'!B56</f>
-        <v>#</v>
-      </c>
-      <c r="B135" s="60" t="s">
-        <v>322</v>
-      </c>
-      <c r="C135" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="D135" s="69" t="str">
-        <f>'Old Reagents'!F56</f>
-        <v>['PbI2','PyrrolidiniumIodide','DMSO']</v>
-      </c>
-      <c r="E135" s="60" t="s">
-        <v>196</v>
-      </c>
+      <c r="A135" s="64"/>
+      <c r="B135" s="60"/>
+      <c r="C135" s="61"/>
+      <c r="D135" s="69"/>
+      <c r="E135" s="60"/>
       <c r="F135" s="19"/>
       <c r="G135" s="4"/>
       <c r="H135" s="4"/>
@@ -41779,21 +41774,21 @@
     </row>
     <row r="136" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="64" t="str">
-        <f>'Old Reagents'!B57</f>
+        <f>'Old Reagents'!B56</f>
         <v>#</v>
       </c>
-      <c r="B136" s="69" t="s">
-        <v>323</v>
-      </c>
-      <c r="C136" s="73" t="s">
+      <c r="B136" s="60" t="s">
+        <v>321</v>
+      </c>
+      <c r="C136" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="D136" s="69">
-        <f>'Old Reagents'!F57</f>
-        <v>1.42</v>
-      </c>
-      <c r="E136" s="69" t="s">
-        <v>193</v>
+      <c r="D136" s="69" t="str">
+        <f>'Old Reagents'!F56</f>
+        <v>['PbI2','PyrrolidiniumIodide','DMSO']</v>
+      </c>
+      <c r="E136" s="60" t="s">
+        <v>196</v>
       </c>
       <c r="F136" s="19"/>
       <c r="G136" s="4"/>
@@ -41819,21 +41814,21 @@
     </row>
     <row r="137" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="64" t="str">
-        <f>'Old Reagents'!B58</f>
+        <f>'Old Reagents'!B57</f>
         <v>#</v>
       </c>
       <c r="B137" s="99" t="s">
-        <v>324</v>
-      </c>
-      <c r="C137" s="61" t="s">
+        <v>322</v>
+      </c>
+      <c r="C137" s="73" t="s">
         <v>20</v>
       </c>
       <c r="D137" s="69">
-        <f>'Old Reagents'!F58</f>
-        <v>1.06</v>
-      </c>
-      <c r="E137" s="60" t="s">
-        <v>190</v>
+        <f>'Old Reagents'!F57</f>
+        <v>1.42</v>
+      </c>
+      <c r="E137" s="69" t="s">
+        <v>193</v>
       </c>
       <c r="F137" s="19"/>
       <c r="G137" s="4"/>
@@ -41859,18 +41854,18 @@
     </row>
     <row r="138" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="64" t="str">
-        <f>'Old Reagents'!B59</f>
+        <f>'Old Reagents'!B58</f>
         <v>#</v>
       </c>
       <c r="B138" s="99" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C138" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D138" s="69">
-        <f>'Old Reagents'!F59</f>
-        <v>0</v>
+        <f>'Old Reagents'!F58</f>
+        <v>1.06</v>
       </c>
       <c r="E138" s="60" t="s">
         <v>190</v>
@@ -41899,17 +41894,17 @@
     </row>
     <row r="139" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="64" t="str">
-        <f>'Old Reagents'!B60</f>
+        <f>'Old Reagents'!B59</f>
         <v>#</v>
       </c>
       <c r="B139" s="60" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C139" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D139" s="69">
-        <f>'Old Reagents'!F60</f>
+        <f>'Old Reagents'!F59</f>
         <v>0</v>
       </c>
       <c r="E139" s="60" t="s">
@@ -41939,21 +41934,21 @@
     </row>
     <row r="140" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="64" t="str">
-        <f>'Old Reagents'!B61</f>
+        <f>'Old Reagents'!B60</f>
         <v>#</v>
       </c>
       <c r="B140" s="60" t="s">
-        <v>327</v>
+        <v>314</v>
       </c>
       <c r="C140" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D140" s="69">
-        <f>'Old Reagents'!F61</f>
+        <f>'Old Reagents'!F60</f>
         <v>0</v>
       </c>
       <c r="E140" s="60" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F140" s="19"/>
       <c r="G140" s="4"/>
@@ -41979,17 +41974,17 @@
     </row>
     <row r="141" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="64" t="str">
-        <f>'Old Reagents'!B62</f>
+        <f>'Old Reagents'!B61</f>
         <v>#</v>
       </c>
       <c r="B141" s="60" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C141" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D141" s="69">
-        <f>'Old Reagents'!F62</f>
+        <f>'Old Reagents'!F61</f>
         <v>0</v>
       </c>
       <c r="E141" s="60" t="s">
@@ -42019,17 +42014,17 @@
     </row>
     <row r="142" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="64" t="str">
-        <f>'Old Reagents'!B63</f>
+        <f>'Old Reagents'!B62</f>
         <v>#</v>
       </c>
       <c r="B142" s="60" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C142" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D142" s="69">
-        <f>'Old Reagents'!F63</f>
+        <f>'Old Reagents'!F62</f>
         <v>0</v>
       </c>
       <c r="E142" s="60" t="s">
@@ -42058,11 +42053,23 @@
       <c r="Z142" s="4"/>
     </row>
     <row r="143" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A143" s="64"/>
-      <c r="B143" s="60"/>
-      <c r="C143" s="73"/>
-      <c r="D143" s="69"/>
-      <c r="E143" s="69"/>
+      <c r="A143" s="64" t="str">
+        <f>'Old Reagents'!B63</f>
+        <v>#</v>
+      </c>
+      <c r="B143" s="60" t="s">
+        <v>327</v>
+      </c>
+      <c r="C143" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="D143" s="69">
+        <f>'Old Reagents'!F63</f>
+        <v>0</v>
+      </c>
+      <c r="E143" s="60" t="s">
+        <v>192</v>
+      </c>
       <c r="F143" s="19"/>
       <c r="G143" s="4"/>
       <c r="H143" s="4"/>
@@ -42086,23 +42093,11 @@
       <c r="Z143" s="4"/>
     </row>
     <row r="144" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A144" s="64">
-        <f>'Old Reagents'!B65</f>
-        <v>0</v>
-      </c>
-      <c r="B144" s="60" t="s">
-        <v>330</v>
-      </c>
-      <c r="C144" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="D144" s="69" t="str">
-        <f>'Old Reagents'!F65</f>
-        <v>['FAH']</v>
-      </c>
-      <c r="E144" s="60" t="s">
-        <v>196</v>
-      </c>
+      <c r="A144" s="64"/>
+      <c r="B144" s="60"/>
+      <c r="C144" s="73"/>
+      <c r="D144" s="69"/>
+      <c r="E144" s="69"/>
       <c r="F144" s="19"/>
       <c r="G144" s="4"/>
       <c r="H144" s="4"/>
@@ -42126,22 +42121,22 @@
       <c r="Z144" s="4"/>
     </row>
     <row r="145" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A145" s="64" t="str">
-        <f>'Old Reagents'!B66</f>
-        <v>#</v>
-      </c>
-      <c r="B145" s="69" t="s">
-        <v>331</v>
-      </c>
-      <c r="C145" s="73" t="s">
+      <c r="A145" s="64">
+        <f>'Old Reagents'!B65</f>
+        <v>0</v>
+      </c>
+      <c r="B145" s="60" t="s">
+        <v>328</v>
+      </c>
+      <c r="C145" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="D145" s="69">
-        <f>'Old Reagents'!F66</f>
-        <v>1.5</v>
-      </c>
-      <c r="E145" s="69" t="s">
-        <v>193</v>
+      <c r="D145" s="69" t="str">
+        <f>'Old Reagents'!F65</f>
+        <v>['FAH']</v>
+      </c>
+      <c r="E145" s="60" t="s">
+        <v>196</v>
       </c>
       <c r="F145" s="19"/>
       <c r="G145" s="4"/>
@@ -42167,21 +42162,21 @@
     </row>
     <row r="146" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="64" t="str">
-        <f>'Old Reagents'!B67</f>
+        <f>'Old Reagents'!B66</f>
         <v>#</v>
       </c>
       <c r="B146" s="99" t="s">
-        <v>332</v>
-      </c>
-      <c r="C146" s="61" t="s">
+        <v>330</v>
+      </c>
+      <c r="C146" s="73" t="s">
         <v>20</v>
       </c>
       <c r="D146" s="69">
-        <f>'Old Reagents'!F67</f>
-        <v>7.63</v>
-      </c>
-      <c r="E146" s="60" t="s">
-        <v>190</v>
+        <f>'Old Reagents'!F66</f>
+        <v>1.5</v>
+      </c>
+      <c r="E146" s="69" t="s">
+        <v>193</v>
       </c>
       <c r="F146" s="19"/>
       <c r="G146" s="4"/>
@@ -42207,18 +42202,18 @@
     </row>
     <row r="147" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="64" t="str">
-        <f>'Old Reagents'!B68</f>
+        <f>'Old Reagents'!B67</f>
         <v>#</v>
       </c>
       <c r="B147" s="99" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C147" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D147" s="69">
-        <f>'Old Reagents'!F68</f>
-        <v>0</v>
+        <f>'Old Reagents'!F67</f>
+        <v>7.63</v>
       </c>
       <c r="E147" s="60" t="s">
         <v>190</v>
@@ -42247,17 +42242,17 @@
     </row>
     <row r="148" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="64" t="str">
-        <f>'Old Reagents'!B69</f>
+        <f>'Old Reagents'!B68</f>
         <v>#</v>
       </c>
       <c r="B148" s="60" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C148" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D148" s="69">
-        <f>'Old Reagents'!F69</f>
+        <f>'Old Reagents'!F68</f>
         <v>0</v>
       </c>
       <c r="E148" s="60" t="s">
@@ -42287,21 +42282,21 @@
     </row>
     <row r="149" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="64" t="str">
-        <f>'Old Reagents'!B70</f>
+        <f>'Old Reagents'!B69</f>
         <v>#</v>
       </c>
       <c r="B149" s="60" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="C149" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D149" s="69">
-        <f>'Old Reagents'!F70</f>
+        <f>'Old Reagents'!F69</f>
         <v>0</v>
       </c>
       <c r="E149" s="60" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F149" s="19"/>
       <c r="G149" s="4"/>
@@ -42327,17 +42322,17 @@
     </row>
     <row r="150" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="64" t="str">
-        <f>'Old Reagents'!B71</f>
+        <f>'Old Reagents'!B70</f>
         <v>#</v>
       </c>
       <c r="B150" s="60" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C150" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D150" s="69">
-        <f>'Old Reagents'!F71</f>
+        <f>'Old Reagents'!F70</f>
         <v>0</v>
       </c>
       <c r="E150" s="60" t="s">
@@ -42367,17 +42362,17 @@
     </row>
     <row r="151" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="64" t="str">
-        <f>'Old Reagents'!B72</f>
+        <f>'Old Reagents'!B71</f>
         <v>#</v>
       </c>
       <c r="B151" s="60" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="C151" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D151" s="69">
-        <f>'Old Reagents'!F72</f>
+        <f>'Old Reagents'!F71</f>
         <v>0</v>
       </c>
       <c r="E151" s="60" t="s">
@@ -42406,14 +42401,24 @@
       <c r="Z151" s="4"/>
     </row>
     <row r="152" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A152" s="100" t="s">
-        <v>266</v>
-      </c>
-      <c r="B152" s="78"/>
-      <c r="C152" s="79"/>
-      <c r="D152" s="78"/>
-      <c r="E152" s="78"/>
-      <c r="F152" s="4"/>
+      <c r="A152" s="64" t="str">
+        <f>'Old Reagents'!B72</f>
+        <v>#</v>
+      </c>
+      <c r="B152" s="60" t="s">
+        <v>335</v>
+      </c>
+      <c r="C152" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="D152" s="69">
+        <f>'Old Reagents'!F72</f>
+        <v>0</v>
+      </c>
+      <c r="E152" s="60" t="s">
+        <v>192</v>
+      </c>
+      <c r="F152" s="19"/>
       <c r="G152" s="4"/>
       <c r="H152" s="4"/>
       <c r="I152" s="4"/>
@@ -42436,20 +42441,13 @@
       <c r="Z152" s="4"/>
     </row>
     <row r="153" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A153" s="82"/>
-      <c r="B153" s="78" t="s">
-        <v>156</v>
-      </c>
-      <c r="C153" s="79" t="s">
-        <v>20</v>
-      </c>
-      <c r="D153" s="78">
-        <f>'User Interface'!E86</f>
-        <v>750</v>
-      </c>
-      <c r="E153" s="78" t="s">
-        <v>192</v>
-      </c>
+      <c r="A153" s="100" t="s">
+        <v>266</v>
+      </c>
+      <c r="B153" s="78"/>
+      <c r="C153" s="79"/>
+      <c r="D153" s="78"/>
+      <c r="E153" s="78"/>
       <c r="F153" s="4"/>
       <c r="G153" s="4"/>
       <c r="H153" s="4"/>
@@ -42475,14 +42473,14 @@
     <row r="154" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="82"/>
       <c r="B154" s="78" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C154" s="79" t="s">
         <v>20</v>
       </c>
       <c r="D154" s="78">
-        <f>'User Interface'!E87</f>
-        <v>80</v>
+        <f>'User Interface'!E86</f>
+        <v>750</v>
       </c>
       <c r="E154" s="78" t="s">
         <v>192</v>
@@ -42512,14 +42510,14 @@
     <row r="155" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="82"/>
       <c r="B155" s="78" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C155" s="79" t="s">
         <v>20</v>
       </c>
       <c r="D155" s="78">
-        <f>'User Interface'!E88</f>
-        <v>900</v>
+        <f>'User Interface'!E87</f>
+        <v>80</v>
       </c>
       <c r="E155" s="78" t="s">
         <v>192</v>
@@ -42549,14 +42547,14 @@
     <row r="156" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="82"/>
       <c r="B156" s="78" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C156" s="79" t="s">
         <v>20</v>
       </c>
       <c r="D156" s="78">
-        <f>'User Interface'!E89</f>
-        <v>1200</v>
+        <f>'User Interface'!E88</f>
+        <v>900</v>
       </c>
       <c r="E156" s="78" t="s">
         <v>192</v>
@@ -42586,14 +42584,14 @@
     <row r="157" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="82"/>
       <c r="B157" s="78" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C157" s="79" t="s">
         <v>20</v>
       </c>
       <c r="D157" s="78">
-        <f>'User Interface'!E90</f>
-        <v>105</v>
+        <f>'User Interface'!E89</f>
+        <v>1200</v>
       </c>
       <c r="E157" s="78" t="s">
         <v>192</v>
@@ -42623,14 +42621,14 @@
     <row r="158" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="82"/>
       <c r="B158" s="78" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C158" s="79" t="s">
         <v>20</v>
       </c>
       <c r="D158" s="78">
-        <f>'User Interface'!E91</f>
-        <v>12600</v>
+        <f>'User Interface'!E90</f>
+        <v>105</v>
       </c>
       <c r="E158" s="78" t="s">
         <v>192</v>
@@ -42660,17 +42658,17 @@
     <row r="159" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="82"/>
       <c r="B159" s="78" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C159" s="79" t="s">
         <v>20</v>
       </c>
       <c r="D159" s="78">
-        <f>'User Interface'!E92</f>
-        <v>2</v>
+        <f>'User Interface'!E91</f>
+        <v>12600</v>
       </c>
       <c r="E159" s="78" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="F159" s="4"/>
       <c r="G159" s="4"/>
@@ -42697,17 +42695,17 @@
     <row r="160" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="82"/>
       <c r="B160" s="78" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C160" s="79" t="s">
         <v>20</v>
       </c>
-      <c r="D160" s="78" t="str">
-        <f>'User Interface'!E93</f>
-        <v>Symyx_96_well_0003</v>
+      <c r="D160" s="78">
+        <f>'User Interface'!E92</f>
+        <v>2</v>
       </c>
       <c r="E160" s="78" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="F160" s="4"/>
       <c r="G160" s="4"/>
@@ -42732,13 +42730,20 @@
       <c r="Z160" s="4"/>
     </row>
     <row r="161" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A161" s="100" t="s">
-        <v>267</v>
-      </c>
-      <c r="B161" s="78"/>
-      <c r="C161" s="79"/>
-      <c r="D161" s="78"/>
-      <c r="E161" s="78"/>
+      <c r="A161" s="82"/>
+      <c r="B161" s="78" t="s">
+        <v>173</v>
+      </c>
+      <c r="C161" s="79" t="s">
+        <v>20</v>
+      </c>
+      <c r="D161" s="78" t="str">
+        <f>'User Interface'!E93</f>
+        <v>Symyx_96_well_0003</v>
+      </c>
+      <c r="E161" s="78" t="s">
+        <v>193</v>
+      </c>
       <c r="F161" s="4"/>
       <c r="G161" s="4"/>
       <c r="H161" s="4"/>
@@ -42762,20 +42767,13 @@
       <c r="Z161" s="4"/>
     </row>
     <row r="162" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A162" s="82"/>
-      <c r="B162" s="78" t="s">
-        <v>268</v>
-      </c>
-      <c r="C162" s="79" t="s">
-        <v>20</v>
-      </c>
-      <c r="D162" s="78">
-        <f>'User Interface'!E95</f>
-        <v>45</v>
-      </c>
-      <c r="E162" s="78" t="s">
-        <v>192</v>
-      </c>
+      <c r="A162" s="100" t="s">
+        <v>267</v>
+      </c>
+      <c r="B162" s="78"/>
+      <c r="C162" s="79"/>
+      <c r="D162" s="78"/>
+      <c r="E162" s="78"/>
       <c r="F162" s="4"/>
       <c r="G162" s="4"/>
       <c r="H162" s="4"/>
@@ -42801,14 +42799,14 @@
     <row r="163" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="82"/>
       <c r="B163" s="78" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C163" s="79" t="s">
         <v>20</v>
       </c>
       <c r="D163" s="78">
-        <f>'User Interface'!E96</f>
-        <v>75</v>
+        <f>'User Interface'!E95</f>
+        <v>45</v>
       </c>
       <c r="E163" s="78" t="s">
         <v>192</v>
@@ -42838,14 +42836,14 @@
     <row r="164" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="82"/>
       <c r="B164" s="78" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C164" s="79" t="s">
         <v>20</v>
       </c>
       <c r="D164" s="78">
-        <f>'User Interface'!E97</f>
-        <v>450</v>
+        <f>'User Interface'!E96</f>
+        <v>75</v>
       </c>
       <c r="E164" s="78" t="s">
         <v>192</v>
@@ -42875,14 +42873,14 @@
     <row r="165" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="82"/>
       <c r="B165" s="78" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C165" s="79" t="s">
         <v>20</v>
       </c>
       <c r="D165" s="78">
-        <f>'User Interface'!E98</f>
-        <v>3600</v>
+        <f>'User Interface'!E97</f>
+        <v>450</v>
       </c>
       <c r="E165" s="78" t="s">
         <v>192</v>
@@ -42910,11 +42908,20 @@
       <c r="Z165" s="4"/>
     </row>
     <row r="166" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A166" s="88"/>
-      <c r="B166" s="89"/>
-      <c r="C166" s="90"/>
-      <c r="D166" s="89"/>
-      <c r="E166" s="89"/>
+      <c r="A166" s="82"/>
+      <c r="B166" s="78" t="s">
+        <v>271</v>
+      </c>
+      <c r="C166" s="79" t="s">
+        <v>20</v>
+      </c>
+      <c r="D166" s="78">
+        <f>'User Interface'!E98</f>
+        <v>3600</v>
+      </c>
+      <c r="E166" s="78" t="s">
+        <v>192</v>
+      </c>
       <c r="F166" s="4"/>
       <c r="G166" s="4"/>
       <c r="H166" s="4"/>
@@ -48510,11 +48517,11 @@
       <c r="Z365" s="4"/>
     </row>
     <row r="366" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A366" s="4"/>
-      <c r="B366" s="4"/>
-      <c r="C366" s="4"/>
-      <c r="D366" s="4"/>
-      <c r="E366" s="4"/>
+      <c r="A366" s="88"/>
+      <c r="B366" s="89"/>
+      <c r="C366" s="90"/>
+      <c r="D366" s="89"/>
+      <c r="E366" s="89"/>
       <c r="F366" s="4"/>
       <c r="G366" s="4"/>
       <c r="H366" s="4"/>
@@ -66289,12 +66296,33 @@
       <c r="Y1000" s="4"/>
       <c r="Z1000" s="4"/>
     </row>
-    <row r="1001" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1001" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1001" s="4"/>
       <c r="B1001" s="4"/>
       <c r="C1001" s="4"/>
       <c r="D1001" s="4"/>
       <c r="E1001" s="4"/>
+      <c r="F1001" s="4"/>
+      <c r="G1001" s="4"/>
+      <c r="H1001" s="4"/>
+      <c r="I1001" s="4"/>
+      <c r="J1001" s="4"/>
+      <c r="K1001" s="4"/>
+      <c r="L1001" s="4"/>
+      <c r="M1001" s="4"/>
+      <c r="N1001" s="4"/>
+      <c r="O1001" s="4"/>
+      <c r="P1001" s="4"/>
+      <c r="Q1001" s="4"/>
+      <c r="R1001" s="4"/>
+      <c r="S1001" s="4"/>
+      <c r="T1001" s="4"/>
+      <c r="U1001" s="4"/>
+      <c r="V1001" s="4"/>
+      <c r="W1001" s="4"/>
+      <c r="X1001" s="4"/>
+      <c r="Y1001" s="4"/>
+      <c r="Z1001" s="4"/>
     </row>
     <row r="1002" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1002" s="4"/>
@@ -66723,6 +66751,13 @@
       <c r="D1062" s="4"/>
       <c r="E1062" s="4"/>
     </row>
+    <row r="1063" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1063" s="4"/>
+      <c r="B1063" s="4"/>
+      <c r="C1063" s="4"/>
+      <c r="D1063" s="4"/>
+      <c r="E1063" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
warn user that sampler must be wolfram for multistock
</commit_message>
<xml_diff>
--- a/HC_LBL_SpecificationInterface.xlsx
+++ b/HC_LBL_SpecificationInterface.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="User Interface" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1030" uniqueCount="341">
   <si>
     <t>Manual Well Number</t>
   </si>
@@ -1435,16 +1435,7 @@
     <t>OldReagent7_prep_duration</t>
   </si>
   <si>
-    <t xml:space="preserve">Strictly speaking, we can delete these attributes for each reagent, </t>
-  </si>
-  <si>
-    <t>although you can see why we may not want to (copy/paste)</t>
-  </si>
-  <si>
     <t>Multi Stock Sampling</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
   <si>
     <t>multi_stock_sampling</t>
@@ -1452,12 +1443,34 @@
   <si>
     <t>Oldreagent3_ID</t>
   </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>NOTE:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> multistock sampling is only supported for use with the Wolfram Mathematica sampler</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1593,6 +1606,12 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -2397,7 +2416,7 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView zoomScale="109" zoomScaleNormal="109" zoomScalePageLayoutView="109" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -2666,7 +2685,7 @@
       <c r="A8" s="32"/>
       <c r="B8" s="32"/>
       <c r="C8" s="126" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D8" s="29" t="s">
         <v>20</v>
@@ -29894,10 +29913,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H72"/>
+  <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -29990,101 +30009,87 @@
       <c r="G7" s="118"/>
       <c r="H7" s="118"/>
     </row>
-    <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="121"/>
-      <c r="B8" s="122"/>
-      <c r="C8" s="122"/>
-      <c r="D8" s="122"/>
-      <c r="E8" s="122"/>
-      <c r="F8" s="122"/>
-      <c r="G8" s="122"/>
-      <c r="H8" s="122"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="59"/>
-      <c r="B9" s="59" t="s">
+    <row r="8" spans="1:8" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="119"/>
+      <c r="B8" s="118"/>
+      <c r="C8" s="118"/>
+      <c r="D8" s="118"/>
+      <c r="E8" s="118"/>
+      <c r="F8" s="118"/>
+      <c r="G8" s="118"/>
+      <c r="H8" s="118"/>
+    </row>
+    <row r="9" spans="1:8" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="119" t="s">
+        <v>340</v>
+      </c>
+      <c r="B9" s="118"/>
+      <c r="C9" s="118"/>
+      <c r="D9" s="118"/>
+      <c r="E9" s="118"/>
+      <c r="F9" s="118"/>
+      <c r="G9" s="118"/>
+      <c r="H9" s="118"/>
+    </row>
+    <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="121"/>
+      <c r="B10" s="122"/>
+      <c r="C10" s="122"/>
+      <c r="D10" s="122"/>
+      <c r="E10" s="122"/>
+      <c r="F10" s="122"/>
+      <c r="G10" s="122"/>
+      <c r="H10" s="122"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="59"/>
+      <c r="B11" s="59" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="59"/>
-      <c r="D9" s="60"/>
-      <c r="E9" s="61"/>
-      <c r="F9" s="114"/>
-      <c r="G9" s="60"/>
-      <c r="H9" s="62"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="103"/>
-      <c r="B10" s="103" t="s">
+      <c r="C11" s="59"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="61"/>
+      <c r="F11" s="114"/>
+      <c r="G11" s="60"/>
+      <c r="H11" s="62"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="103"/>
+      <c r="B12" s="103" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="65" t="s">
+      <c r="C12" s="65" t="s">
         <v>56</v>
       </c>
-      <c r="D10" s="60"/>
-      <c r="E10" s="61"/>
-      <c r="F10" s="114"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="62" t="s">
+      <c r="D12" s="60"/>
+      <c r="E12" s="61"/>
+      <c r="F12" s="114"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="62" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="104"/>
-      <c r="B11" s="104"/>
-      <c r="C11" s="68">
-        <v>1</v>
-      </c>
-      <c r="D11" s="60" t="s">
-        <v>59</v>
-      </c>
-      <c r="E11" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="115" t="s">
-        <v>273</v>
-      </c>
-      <c r="G11" s="69" t="s">
-        <v>60</v>
-      </c>
-      <c r="H11" s="62" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="104"/>
-      <c r="B12" s="104" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="68"/>
-      <c r="D12" s="60" t="s">
-        <v>63</v>
-      </c>
-      <c r="E12" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="115"/>
-      <c r="G12" s="69"/>
-      <c r="H12" s="62"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="104"/>
-      <c r="B13" s="104" t="s">
-        <v>44</v>
-      </c>
-      <c r="C13" s="68"/>
-      <c r="D13" s="69" t="s">
-        <v>64</v>
+      <c r="B13" s="104"/>
+      <c r="C13" s="68">
+        <v>1</v>
+      </c>
+      <c r="D13" s="60" t="s">
+        <v>59</v>
       </c>
       <c r="E13" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="115">
-        <v>1.5</v>
-      </c>
-      <c r="G13" s="60">
-        <v>1.234</v>
-      </c>
-      <c r="H13" s="62"/>
+      <c r="F13" s="115" t="s">
+        <v>273</v>
+      </c>
+      <c r="G13" s="69" t="s">
+        <v>60</v>
+      </c>
+      <c r="H13" s="62" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="104"/>
@@ -30092,18 +30097,14 @@
         <v>44</v>
       </c>
       <c r="C14" s="68"/>
-      <c r="D14" s="69" t="s">
-        <v>65</v>
+      <c r="D14" s="60" t="s">
+        <v>63</v>
       </c>
       <c r="E14" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F14" s="115">
-        <v>7.63</v>
-      </c>
-      <c r="G14" s="60">
-        <v>5.6779999999999999</v>
-      </c>
+      <c r="F14" s="115"/>
+      <c r="G14" s="69"/>
       <c r="H14" s="62"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -30113,56 +30114,56 @@
       </c>
       <c r="C15" s="68"/>
       <c r="D15" s="69" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E15" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="115"/>
+      <c r="F15" s="115">
+        <v>1.5</v>
+      </c>
       <c r="G15" s="60">
-        <v>9.0120000000000005</v>
-      </c>
-      <c r="H15" s="123"/>
+        <v>1.234</v>
+      </c>
+      <c r="H15" s="62"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="103"/>
-      <c r="B16" s="103" t="s">
+      <c r="A16" s="104"/>
+      <c r="B16" s="104" t="s">
         <v>44</v>
       </c>
       <c r="C16" s="68"/>
-      <c r="D16" s="60" t="s">
-        <v>67</v>
+      <c r="D16" s="69" t="s">
+        <v>65</v>
       </c>
       <c r="E16" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F16" s="114"/>
+      <c r="F16" s="115">
+        <v>7.63</v>
+      </c>
       <c r="G16" s="60">
-        <v>75</v>
-      </c>
-      <c r="H16" s="123" t="s">
-        <v>336</v>
-      </c>
+        <v>5.6779999999999999</v>
+      </c>
+      <c r="H16" s="62"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="103"/>
-      <c r="B17" s="103" t="s">
+      <c r="A17" s="104"/>
+      <c r="B17" s="104" t="s">
         <v>44</v>
       </c>
       <c r="C17" s="68"/>
-      <c r="D17" s="60" t="s">
-        <v>68</v>
+      <c r="D17" s="69" t="s">
+        <v>66</v>
       </c>
       <c r="E17" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="114"/>
+      <c r="F17" s="115"/>
       <c r="G17" s="60">
-        <v>450</v>
-      </c>
-      <c r="H17" s="123" t="s">
-        <v>337</v>
-      </c>
+        <v>9.0120000000000005</v>
+      </c>
+      <c r="H17" s="123"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="103"/>
@@ -30171,163 +30172,159 @@
       </c>
       <c r="C18" s="68"/>
       <c r="D18" s="60" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E18" s="61" t="s">
         <v>20</v>
       </c>
       <c r="F18" s="114"/>
       <c r="G18" s="60">
-        <v>3600</v>
-      </c>
-      <c r="H18" s="62"/>
+        <v>75</v>
+      </c>
+      <c r="H18" s="123"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="103"/>
-      <c r="B19" s="103"/>
+      <c r="B19" s="103" t="s">
+        <v>44</v>
+      </c>
       <c r="C19" s="68"/>
-      <c r="D19" s="60"/>
-      <c r="E19" s="61"/>
+      <c r="D19" s="60" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" s="61" t="s">
+        <v>20</v>
+      </c>
       <c r="F19" s="114"/>
-      <c r="G19" s="60"/>
-      <c r="H19" s="62"/>
+      <c r="G19" s="60">
+        <v>450</v>
+      </c>
+      <c r="H19" s="123"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="104"/>
-      <c r="B20" s="104"/>
-      <c r="C20" s="68">
-        <v>2</v>
-      </c>
+      <c r="A20" s="103"/>
+      <c r="B20" s="103" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="68"/>
       <c r="D20" s="60" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E20" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F20" s="115" t="s">
-        <v>274</v>
-      </c>
-      <c r="G20" s="69" t="s">
-        <v>71</v>
-      </c>
-      <c r="H20" s="62" t="s">
-        <v>72</v>
-      </c>
+      <c r="F20" s="114"/>
+      <c r="G20" s="60">
+        <v>3600</v>
+      </c>
+      <c r="H20" s="62"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="104"/>
-      <c r="B21" s="104"/>
+      <c r="A21" s="103"/>
+      <c r="B21" s="103"/>
       <c r="C21" s="68"/>
-      <c r="D21" s="69" t="s">
-        <v>74</v>
-      </c>
-      <c r="E21" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F21" s="115">
-        <v>1.55</v>
-      </c>
-      <c r="G21" s="60">
-        <v>1.234</v>
-      </c>
-      <c r="H21" s="62" t="s">
-        <v>75</v>
-      </c>
+      <c r="D21" s="60"/>
+      <c r="E21" s="61"/>
+      <c r="F21" s="114"/>
+      <c r="G21" s="60"/>
+      <c r="H21" s="62"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="104"/>
       <c r="B22" s="104"/>
-      <c r="C22" s="68"/>
-      <c r="D22" s="69" t="s">
-        <v>76</v>
+      <c r="C22" s="68">
+        <v>2</v>
+      </c>
+      <c r="D22" s="60" t="s">
+        <v>70</v>
       </c>
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="115">
-        <v>1.93</v>
-      </c>
-      <c r="G22" s="60">
-        <v>5.6779999999999999</v>
+      <c r="F22" s="115" t="s">
+        <v>274</v>
+      </c>
+      <c r="G22" s="69" t="s">
+        <v>71</v>
       </c>
       <c r="H22" s="62" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="104"/>
-      <c r="B23" s="104" t="s">
-        <v>44</v>
-      </c>
+      <c r="B23" s="104"/>
       <c r="C23" s="68"/>
       <c r="D23" s="69" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E23" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="115"/>
+      <c r="F23" s="115">
+        <v>1.55</v>
+      </c>
       <c r="G23" s="60">
-        <v>9.0120000000000005</v>
-      </c>
-      <c r="H23" s="62"/>
+        <v>1.234</v>
+      </c>
+      <c r="H23" s="62" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="104"/>
-      <c r="B24" s="104" t="s">
+      <c r="B24" s="104"/>
+      <c r="C24" s="68"/>
+      <c r="D24" s="69" t="s">
+        <v>76</v>
+      </c>
+      <c r="E24" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" s="115">
+        <v>1.93</v>
+      </c>
+      <c r="G24" s="60">
+        <v>5.6779999999999999</v>
+      </c>
+      <c r="H24" s="62" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="104"/>
+      <c r="B25" s="104" t="s">
         <v>44</v>
       </c>
-      <c r="C24" s="72"/>
-      <c r="D24" s="60" t="s">
-        <v>79</v>
-      </c>
-      <c r="E24" s="73" t="s">
-        <v>20</v>
-      </c>
-      <c r="F24" s="115"/>
-      <c r="G24" s="69"/>
-      <c r="H24" s="74" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="103"/>
-      <c r="B25" s="103" t="s">
-        <v>44</v>
-      </c>
       <c r="C25" s="68"/>
-      <c r="D25" s="60" t="s">
-        <v>81</v>
+      <c r="D25" s="69" t="s">
+        <v>78</v>
       </c>
       <c r="E25" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F25" s="114"/>
+      <c r="F25" s="115"/>
       <c r="G25" s="60">
-        <v>75</v>
-      </c>
-      <c r="H25" s="62" t="s">
-        <v>82</v>
-      </c>
+        <v>9.0120000000000005</v>
+      </c>
+      <c r="H25" s="62"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="103"/>
-      <c r="B26" s="103" t="s">
+      <c r="A26" s="104"/>
+      <c r="B26" s="104" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="68"/>
+      <c r="C26" s="72"/>
       <c r="D26" s="60" t="s">
-        <v>84</v>
-      </c>
-      <c r="E26" s="61" t="s">
+        <v>79</v>
+      </c>
+      <c r="E26" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="F26" s="114"/>
-      <c r="G26" s="60">
-        <v>450</v>
-      </c>
-      <c r="H26" s="62" t="s">
-        <v>85</v>
+      <c r="F26" s="115"/>
+      <c r="G26" s="69"/>
+      <c r="H26" s="74" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
@@ -30337,113 +30334,109 @@
       </c>
       <c r="C27" s="68"/>
       <c r="D27" s="60" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E27" s="61" t="s">
         <v>20</v>
       </c>
       <c r="F27" s="114"/>
       <c r="G27" s="60">
-        <v>3600</v>
+        <v>75</v>
       </c>
       <c r="H27" s="62" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="103"/>
-      <c r="B28" s="103"/>
+      <c r="B28" s="103" t="s">
+        <v>44</v>
+      </c>
       <c r="C28" s="68"/>
-      <c r="D28" s="60"/>
-      <c r="E28" s="61"/>
+      <c r="D28" s="60" t="s">
+        <v>84</v>
+      </c>
+      <c r="E28" s="61" t="s">
+        <v>20</v>
+      </c>
       <c r="F28" s="114"/>
-      <c r="G28" s="60"/>
-      <c r="H28" s="62"/>
+      <c r="G28" s="60">
+        <v>450</v>
+      </c>
+      <c r="H28" s="62" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="104"/>
-      <c r="B29" s="104"/>
-      <c r="C29" s="68">
-        <v>3</v>
-      </c>
+      <c r="A29" s="103"/>
+      <c r="B29" s="103" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" s="68"/>
       <c r="D29" s="60" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E29" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F29" s="115" t="s">
-        <v>275</v>
-      </c>
-      <c r="G29" s="69" t="s">
-        <v>89</v>
+      <c r="F29" s="114"/>
+      <c r="G29" s="60">
+        <v>3600</v>
       </c>
       <c r="H29" s="62" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="104"/>
-      <c r="B30" s="104"/>
+      <c r="A30" s="103"/>
+      <c r="B30" s="103"/>
       <c r="C30" s="68"/>
-      <c r="D30" s="60" t="s">
-        <v>91</v>
-      </c>
-      <c r="E30" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F30" s="114">
-        <v>2.06</v>
-      </c>
-      <c r="G30" s="60">
-        <v>1.234</v>
-      </c>
-      <c r="H30" s="62" t="s">
-        <v>92</v>
-      </c>
+      <c r="D30" s="60"/>
+      <c r="E30" s="61"/>
+      <c r="F30" s="114"/>
+      <c r="G30" s="60"/>
+      <c r="H30" s="62"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="104"/>
-      <c r="B31" s="104" t="s">
-        <v>44</v>
-      </c>
-      <c r="C31" s="68"/>
+      <c r="B31" s="104"/>
+      <c r="C31" s="68">
+        <v>3</v>
+      </c>
       <c r="D31" s="60" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E31" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F31" s="114">
-        <v>1.33</v>
-      </c>
-      <c r="G31" s="60">
-        <v>5.6779999999999999</v>
+      <c r="F31" s="115" t="s">
+        <v>275</v>
+      </c>
+      <c r="G31" s="69" t="s">
+        <v>89</v>
       </c>
       <c r="H31" s="62" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="104"/>
-      <c r="B32" s="104" t="s">
-        <v>44</v>
-      </c>
+      <c r="B32" s="104"/>
       <c r="C32" s="68"/>
       <c r="D32" s="60" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E32" s="61" t="s">
         <v>20</v>
       </c>
       <c r="F32" s="114">
-        <v>1.2</v>
+        <v>2.06</v>
       </c>
       <c r="G32" s="60">
-        <v>9.0120000000000005</v>
+        <v>1.234</v>
       </c>
       <c r="H32" s="62" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
@@ -30451,17 +30444,21 @@
       <c r="B33" s="104" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="72"/>
+      <c r="C33" s="68"/>
       <c r="D33" s="60" t="s">
-        <v>97</v>
-      </c>
-      <c r="E33" s="73" t="s">
+        <v>93</v>
+      </c>
+      <c r="E33" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F33" s="115"/>
-      <c r="G33" s="69"/>
-      <c r="H33" s="74" t="s">
-        <v>80</v>
+      <c r="F33" s="114">
+        <v>1.33</v>
+      </c>
+      <c r="G33" s="60">
+        <v>5.6779999999999999</v>
+      </c>
+      <c r="H33" s="62" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
@@ -30471,17 +30468,19 @@
       </c>
       <c r="C34" s="68"/>
       <c r="D34" s="60" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E34" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F34" s="114"/>
+      <c r="F34" s="114">
+        <v>1.2</v>
+      </c>
       <c r="G34" s="60">
-        <v>75</v>
+        <v>9.0120000000000005</v>
       </c>
       <c r="H34" s="62" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -30489,19 +30488,17 @@
       <c r="B35" s="104" t="s">
         <v>44</v>
       </c>
-      <c r="C35" s="68"/>
+      <c r="C35" s="72"/>
       <c r="D35" s="60" t="s">
-        <v>102</v>
-      </c>
-      <c r="E35" s="61" t="s">
+        <v>97</v>
+      </c>
+      <c r="E35" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="F35" s="114"/>
-      <c r="G35" s="60">
-        <v>450</v>
-      </c>
-      <c r="H35" s="62" t="s">
-        <v>103</v>
+      <c r="F35" s="115"/>
+      <c r="G35" s="69"/>
+      <c r="H35" s="74" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
@@ -30511,125 +30508,129 @@
       </c>
       <c r="C36" s="68"/>
       <c r="D36" s="60" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E36" s="61" t="s">
         <v>20</v>
       </c>
       <c r="F36" s="114"/>
       <c r="G36" s="60">
-        <v>3600</v>
+        <v>75</v>
       </c>
       <c r="H36" s="62" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="103"/>
-      <c r="B37" s="103"/>
+      <c r="A37" s="104"/>
+      <c r="B37" s="104" t="s">
+        <v>44</v>
+      </c>
       <c r="C37" s="68"/>
-      <c r="D37" s="60"/>
-      <c r="E37" s="61"/>
+      <c r="D37" s="60" t="s">
+        <v>102</v>
+      </c>
+      <c r="E37" s="61" t="s">
+        <v>20</v>
+      </c>
       <c r="F37" s="114"/>
-      <c r="G37" s="60"/>
-      <c r="H37" s="62"/>
+      <c r="G37" s="60">
+        <v>450</v>
+      </c>
+      <c r="H37" s="62" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="104"/>
-      <c r="B38" s="104"/>
-      <c r="C38" s="68">
-        <v>4</v>
-      </c>
+      <c r="B38" s="104" t="s">
+        <v>44</v>
+      </c>
+      <c r="C38" s="68"/>
       <c r="D38" s="60" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E38" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F38" s="115" t="s">
-        <v>274</v>
-      </c>
-      <c r="G38" s="69" t="s">
-        <v>71</v>
+      <c r="F38" s="114"/>
+      <c r="G38" s="60">
+        <v>3600</v>
       </c>
       <c r="H38" s="62" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="104"/>
-      <c r="B39" s="104"/>
+      <c r="A39" s="103"/>
+      <c r="B39" s="103"/>
       <c r="C39" s="68"/>
-      <c r="D39" s="60" t="s">
-        <v>108</v>
-      </c>
-      <c r="E39" s="73" t="s">
-        <v>20</v>
-      </c>
-      <c r="F39" s="115">
-        <v>1.18</v>
-      </c>
-      <c r="G39" s="60">
-        <v>1.234</v>
-      </c>
-      <c r="H39" s="62" t="s">
-        <v>109</v>
-      </c>
+      <c r="D39" s="60"/>
+      <c r="E39" s="61"/>
+      <c r="F39" s="114"/>
+      <c r="G39" s="60"/>
+      <c r="H39" s="62"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="104"/>
       <c r="B40" s="104"/>
-      <c r="C40" s="68"/>
+      <c r="C40" s="68">
+        <v>4</v>
+      </c>
       <c r="D40" s="60" t="s">
-        <v>110</v>
-      </c>
-      <c r="E40" s="73" t="s">
+        <v>106</v>
+      </c>
+      <c r="E40" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F40" s="115">
-        <v>0.74</v>
-      </c>
-      <c r="G40" s="60">
-        <v>5.6779999999999999</v>
+      <c r="F40" s="115" t="s">
+        <v>274</v>
+      </c>
+      <c r="G40" s="69" t="s">
+        <v>71</v>
       </c>
       <c r="H40" s="62" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="104"/>
-      <c r="B41" s="104" t="s">
-        <v>44</v>
-      </c>
+      <c r="B41" s="104"/>
       <c r="C41" s="68"/>
       <c r="D41" s="60" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E41" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="F41" s="114"/>
+      <c r="F41" s="115">
+        <v>1.18</v>
+      </c>
       <c r="G41" s="60">
-        <v>9.0120000000000005</v>
-      </c>
-      <c r="H41" s="62"/>
+        <v>1.234</v>
+      </c>
+      <c r="H41" s="62" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="104"/>
-      <c r="B42" s="104" t="s">
-        <v>44</v>
-      </c>
-      <c r="C42" s="72"/>
+      <c r="B42" s="104"/>
+      <c r="C42" s="68"/>
       <c r="D42" s="60" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E42" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="F42" s="115"/>
-      <c r="G42" s="69"/>
-      <c r="H42" s="74" t="s">
-        <v>80</v>
+      <c r="F42" s="115">
+        <v>0.74</v>
+      </c>
+      <c r="G42" s="60">
+        <v>5.6779999999999999</v>
+      </c>
+      <c r="H42" s="62" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
@@ -30639,37 +30640,33 @@
       </c>
       <c r="C43" s="68"/>
       <c r="D43" s="60" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E43" s="73" t="s">
         <v>20</v>
       </c>
       <c r="F43" s="114"/>
       <c r="G43" s="60">
-        <v>75</v>
-      </c>
-      <c r="H43" s="62" t="s">
-        <v>101</v>
-      </c>
+        <v>9.0120000000000005</v>
+      </c>
+      <c r="H43" s="62"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="104"/>
       <c r="B44" s="104" t="s">
         <v>44</v>
       </c>
-      <c r="C44" s="68"/>
+      <c r="C44" s="72"/>
       <c r="D44" s="60" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E44" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="F44" s="114"/>
-      <c r="G44" s="60">
-        <v>450</v>
-      </c>
-      <c r="H44" s="62" t="s">
-        <v>103</v>
+      <c r="F44" s="115"/>
+      <c r="G44" s="69"/>
+      <c r="H44" s="74" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
@@ -30679,131 +30676,129 @@
       </c>
       <c r="C45" s="68"/>
       <c r="D45" s="60" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E45" s="73" t="s">
         <v>20</v>
       </c>
       <c r="F45" s="114"/>
       <c r="G45" s="60">
+        <v>75</v>
+      </c>
+      <c r="H45" s="62" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" s="104"/>
+      <c r="B46" s="104" t="s">
+        <v>44</v>
+      </c>
+      <c r="C46" s="68"/>
+      <c r="D46" s="60" t="s">
+        <v>116</v>
+      </c>
+      <c r="E46" s="73" t="s">
+        <v>20</v>
+      </c>
+      <c r="F46" s="114"/>
+      <c r="G46" s="60">
+        <v>450</v>
+      </c>
+      <c r="H46" s="62" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" s="104"/>
+      <c r="B47" s="104" t="s">
+        <v>44</v>
+      </c>
+      <c r="C47" s="68"/>
+      <c r="D47" s="60" t="s">
+        <v>117</v>
+      </c>
+      <c r="E47" s="73" t="s">
+        <v>20</v>
+      </c>
+      <c r="F47" s="114"/>
+      <c r="G47" s="60">
         <v>3600</v>
       </c>
-      <c r="H45" s="62" t="s">
+      <c r="H47" s="62" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A46" s="103"/>
-      <c r="B46" s="103"/>
-      <c r="C46" s="68"/>
-      <c r="D46" s="60"/>
-      <c r="E46" s="61"/>
-      <c r="F46" s="114"/>
-      <c r="G46" s="60"/>
-      <c r="H46" s="62"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A47" s="103"/>
-      <c r="B47" s="103"/>
-      <c r="C47" s="68">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" s="103"/>
+      <c r="B48" s="103"/>
+      <c r="C48" s="68"/>
+      <c r="D48" s="60"/>
+      <c r="E48" s="61"/>
+      <c r="F48" s="114"/>
+      <c r="G48" s="60"/>
+      <c r="H48" s="62"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" s="103"/>
+      <c r="B49" s="103"/>
+      <c r="C49" s="68">
         <v>5</v>
       </c>
-      <c r="D47" s="60" t="s">
+      <c r="D49" s="60" t="s">
         <v>118</v>
-      </c>
-      <c r="E47" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F47" s="115" t="s">
-        <v>274</v>
-      </c>
-      <c r="G47" s="69" t="s">
-        <v>89</v>
-      </c>
-      <c r="H47" s="62" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A48" s="104"/>
-      <c r="B48" s="104"/>
-      <c r="C48" s="72"/>
-      <c r="D48" s="60" t="s">
-        <v>121</v>
-      </c>
-      <c r="E48" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F48" s="115">
-        <v>1.42</v>
-      </c>
-      <c r="G48" s="60">
-        <v>1.234</v>
-      </c>
-      <c r="H48" s="62" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" s="104"/>
-      <c r="B49" s="104"/>
-      <c r="C49" s="72"/>
-      <c r="D49" s="60" t="s">
-        <v>123</v>
       </c>
       <c r="E49" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F49" s="115">
-        <v>1.06</v>
-      </c>
-      <c r="G49" s="60">
-        <v>5.6779999999999999</v>
+      <c r="F49" s="115" t="s">
+        <v>274</v>
+      </c>
+      <c r="G49" s="69" t="s">
+        <v>89</v>
       </c>
       <c r="H49" s="62" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="104"/>
-      <c r="B50" s="104" t="s">
-        <v>44</v>
-      </c>
+      <c r="B50" s="104"/>
       <c r="C50" s="72"/>
       <c r="D50" s="60" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E50" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F50" s="115" t="s">
-        <v>274</v>
+      <c r="F50" s="115">
+        <v>1.42</v>
       </c>
       <c r="G50" s="60">
-        <v>9.0120000000000005</v>
+        <v>1.234</v>
       </c>
       <c r="H50" s="62" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="104"/>
-      <c r="B51" s="104" t="s">
-        <v>44</v>
-      </c>
+      <c r="B51" s="104"/>
       <c r="C51" s="72"/>
-      <c r="D51" s="69" t="s">
-        <v>127</v>
-      </c>
-      <c r="E51" s="73" t="s">
+      <c r="D51" s="60" t="s">
+        <v>123</v>
+      </c>
+      <c r="E51" s="61" t="s">
         <v>20</v>
       </c>
       <c r="F51" s="115">
-        <v>1.42</v>
-      </c>
-      <c r="G51" s="69"/>
-      <c r="H51" s="74" t="s">
-        <v>80</v>
+        <v>1.06</v>
+      </c>
+      <c r="G51" s="60">
+        <v>5.6779999999999999</v>
+      </c>
+      <c r="H51" s="62" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
@@ -30813,19 +30808,19 @@
       </c>
       <c r="C52" s="72"/>
       <c r="D52" s="60" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E52" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F52" s="115">
-        <v>1.06</v>
+      <c r="F52" s="115" t="s">
+        <v>274</v>
       </c>
       <c r="G52" s="60">
-        <v>75</v>
+        <v>9.0120000000000005</v>
       </c>
       <c r="H52" s="62" t="s">
-        <v>101</v>
+        <v>126</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
@@ -30834,20 +30829,18 @@
         <v>44</v>
       </c>
       <c r="C53" s="72"/>
-      <c r="D53" s="60" t="s">
-        <v>130</v>
-      </c>
-      <c r="E53" s="61" t="s">
+      <c r="D53" s="69" t="s">
+        <v>127</v>
+      </c>
+      <c r="E53" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="F53" s="115" t="s">
-        <v>274</v>
-      </c>
-      <c r="G53" s="60">
-        <v>450</v>
-      </c>
-      <c r="H53" s="62" t="s">
-        <v>103</v>
+      <c r="F53" s="115">
+        <v>1.42</v>
+      </c>
+      <c r="G53" s="69"/>
+      <c r="H53" s="74" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
@@ -30857,97 +30850,97 @@
       </c>
       <c r="C54" s="72"/>
       <c r="D54" s="60" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E54" s="61" t="s">
         <v>20</v>
       </c>
       <c r="F54" s="115">
-        <v>1.42</v>
+        <v>1.06</v>
       </c>
       <c r="G54" s="60">
-        <v>3600</v>
+        <v>75</v>
       </c>
       <c r="H54" s="62" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A55" s="103"/>
-      <c r="B55" s="103"/>
-      <c r="C55" s="68"/>
-      <c r="D55" s="60"/>
-      <c r="E55" s="61"/>
-      <c r="F55" s="114"/>
-      <c r="G55" s="60"/>
-      <c r="H55" s="62"/>
+      <c r="A55" s="104"/>
+      <c r="B55" s="104" t="s">
+        <v>44</v>
+      </c>
+      <c r="C55" s="72"/>
+      <c r="D55" s="60" t="s">
+        <v>130</v>
+      </c>
+      <c r="E55" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F55" s="115" t="s">
+        <v>274</v>
+      </c>
+      <c r="G55" s="60">
+        <v>450</v>
+      </c>
+      <c r="H55" s="62" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56" s="103"/>
-      <c r="B56" s="103" t="s">
+      <c r="A56" s="104"/>
+      <c r="B56" s="104" t="s">
         <v>44</v>
       </c>
-      <c r="C56" s="68">
-        <v>6</v>
-      </c>
+      <c r="C56" s="72"/>
       <c r="D56" s="60" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E56" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F56" s="115" t="s">
-        <v>274</v>
-      </c>
-      <c r="G56" s="69" t="s">
-        <v>71</v>
+      <c r="F56" s="115">
+        <v>1.42</v>
+      </c>
+      <c r="G56" s="60">
+        <v>3600</v>
       </c>
       <c r="H56" s="62" t="s">
-        <v>133</v>
+        <v>105</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="103"/>
-      <c r="B57" s="103" t="s">
-        <v>44</v>
-      </c>
+      <c r="B57" s="103"/>
       <c r="C57" s="68"/>
-      <c r="D57" s="60" t="s">
-        <v>134</v>
-      </c>
-      <c r="E57" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F57" s="115">
-        <v>1.42</v>
-      </c>
-      <c r="G57" s="60">
-        <v>1.234</v>
-      </c>
-      <c r="H57" s="62" t="s">
-        <v>135</v>
-      </c>
+      <c r="D57" s="60"/>
+      <c r="E57" s="61"/>
+      <c r="F57" s="114"/>
+      <c r="G57" s="60"/>
+      <c r="H57" s="62"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="103"/>
       <c r="B58" s="103" t="s">
         <v>44</v>
       </c>
-      <c r="C58" s="68"/>
+      <c r="C58" s="68">
+        <v>6</v>
+      </c>
       <c r="D58" s="60" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E58" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F58" s="115">
-        <v>1.06</v>
-      </c>
-      <c r="G58" s="60">
-        <v>5.6779999999999999</v>
+      <c r="F58" s="115" t="s">
+        <v>274</v>
+      </c>
+      <c r="G58" s="69" t="s">
+        <v>71</v>
       </c>
       <c r="H58" s="62" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
@@ -30957,16 +30950,20 @@
       </c>
       <c r="C59" s="68"/>
       <c r="D59" s="60" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E59" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F59" s="114"/>
+      <c r="F59" s="115">
+        <v>1.42</v>
+      </c>
       <c r="G59" s="60">
-        <v>9.0120000000000005</v>
-      </c>
-      <c r="H59" s="62"/>
+        <v>1.234</v>
+      </c>
+      <c r="H59" s="62" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="103"/>
@@ -30974,15 +30971,21 @@
         <v>44</v>
       </c>
       <c r="C60" s="68"/>
-      <c r="D60" s="69" t="s">
-        <v>139</v>
+      <c r="D60" s="60" t="s">
+        <v>136</v>
       </c>
       <c r="E60" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F60" s="114"/>
-      <c r="G60" s="60"/>
-      <c r="H60" s="62"/>
+      <c r="F60" s="115">
+        <v>1.06</v>
+      </c>
+      <c r="G60" s="60">
+        <v>5.6779999999999999</v>
+      </c>
+      <c r="H60" s="62" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="103"/>
@@ -30991,14 +30994,14 @@
       </c>
       <c r="C61" s="68"/>
       <c r="D61" s="60" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E61" s="61" t="s">
         <v>20</v>
       </c>
       <c r="F61" s="114"/>
       <c r="G61" s="60">
-        <v>75</v>
+        <v>9.0120000000000005</v>
       </c>
       <c r="H61" s="62"/>
     </row>
@@ -31008,16 +31011,14 @@
         <v>44</v>
       </c>
       <c r="C62" s="68"/>
-      <c r="D62" s="60" t="s">
-        <v>141</v>
+      <c r="D62" s="69" t="s">
+        <v>139</v>
       </c>
       <c r="E62" s="61" t="s">
         <v>20</v>
       </c>
       <c r="F62" s="114"/>
-      <c r="G62" s="60">
-        <v>450</v>
-      </c>
+      <c r="G62" s="60"/>
       <c r="H62" s="62"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
@@ -31027,111 +31028,106 @@
       </c>
       <c r="C63" s="68"/>
       <c r="D63" s="60" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E63" s="61" t="s">
         <v>20</v>
       </c>
       <c r="F63" s="114"/>
       <c r="G63" s="60">
-        <v>3600</v>
+        <v>75</v>
       </c>
       <c r="H63" s="62"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="103"/>
-      <c r="B64" s="103"/>
+      <c r="B64" s="103" t="s">
+        <v>44</v>
+      </c>
       <c r="C64" s="68"/>
-      <c r="D64" s="60"/>
-      <c r="E64" s="61"/>
+      <c r="D64" s="60" t="s">
+        <v>141</v>
+      </c>
+      <c r="E64" s="61" t="s">
+        <v>20</v>
+      </c>
       <c r="F64" s="114"/>
-      <c r="G64" s="60"/>
+      <c r="G64" s="60">
+        <v>450</v>
+      </c>
       <c r="H64" s="62"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="103"/>
-      <c r="B65" s="103"/>
-      <c r="C65" s="68">
-        <v>7</v>
-      </c>
+      <c r="B65" s="103" t="s">
+        <v>44</v>
+      </c>
+      <c r="C65" s="68"/>
       <c r="D65" s="60" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E65" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F65" s="115" t="s">
-        <v>144</v>
-      </c>
-      <c r="G65" s="69" t="s">
-        <v>71</v>
-      </c>
-      <c r="H65" s="62" t="s">
-        <v>145</v>
-      </c>
+      <c r="F65" s="114"/>
+      <c r="G65" s="60">
+        <v>3600</v>
+      </c>
+      <c r="H65" s="62"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="103"/>
-      <c r="B66" s="103" t="s">
-        <v>44</v>
-      </c>
+      <c r="B66" s="103"/>
       <c r="C66" s="68"/>
-      <c r="D66" s="60" t="s">
-        <v>146</v>
-      </c>
-      <c r="E66" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F66" s="115">
-        <v>1.5</v>
-      </c>
-      <c r="G66" s="60">
-        <v>1.234</v>
-      </c>
-      <c r="H66" s="62" t="s">
-        <v>147</v>
-      </c>
+      <c r="D66" s="60"/>
+      <c r="E66" s="61"/>
+      <c r="F66" s="114"/>
+      <c r="G66" s="60"/>
+      <c r="H66" s="62"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="103"/>
-      <c r="B67" s="103" t="s">
-        <v>44</v>
-      </c>
-      <c r="C67" s="68"/>
+      <c r="B67" s="103"/>
+      <c r="C67" s="68">
+        <v>7</v>
+      </c>
       <c r="D67" s="60" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="E67" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F67" s="115">
-        <v>7.63</v>
-      </c>
-      <c r="G67" s="60">
-        <v>5.6779999999999999</v>
+      <c r="F67" s="115" t="s">
+        <v>144</v>
+      </c>
+      <c r="G67" s="69" t="s">
+        <v>71</v>
       </c>
       <c r="H67" s="62" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="103"/>
-      <c r="B68" s="103" t="str">
-        <f>B67</f>
-        <v>#</v>
+      <c r="B68" s="103" t="s">
+        <v>44</v>
       </c>
       <c r="C68" s="68"/>
       <c r="D68" s="60" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E68" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F68" s="114"/>
+      <c r="F68" s="115">
+        <v>1.5</v>
+      </c>
       <c r="G68" s="60">
-        <v>9.0120000000000005</v>
-      </c>
-      <c r="H68" s="62"/>
+        <v>1.234</v>
+      </c>
+      <c r="H68" s="62" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="103"/>
@@ -31140,30 +31136,37 @@
       </c>
       <c r="C69" s="68"/>
       <c r="D69" s="60" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E69" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F69" s="114"/>
-      <c r="G69" s="69"/>
-      <c r="H69" s="62"/>
+      <c r="F69" s="115">
+        <v>7.63</v>
+      </c>
+      <c r="G69" s="60">
+        <v>5.6779999999999999</v>
+      </c>
+      <c r="H69" s="62" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" s="103"/>
-      <c r="B70" s="103" t="s">
-        <v>44</v>
+      <c r="B70" s="103" t="str">
+        <f>B69</f>
+        <v>#</v>
       </c>
       <c r="C70" s="68"/>
       <c r="D70" s="60" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E70" s="61" t="s">
         <v>20</v>
       </c>
       <c r="F70" s="114"/>
       <c r="G70" s="60">
-        <v>75</v>
+        <v>9.0120000000000005</v>
       </c>
       <c r="H70" s="62"/>
     </row>
@@ -31174,15 +31177,13 @@
       </c>
       <c r="C71" s="68"/>
       <c r="D71" s="60" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E71" s="61" t="s">
         <v>20</v>
       </c>
       <c r="F71" s="114"/>
-      <c r="G71" s="60">
-        <v>450</v>
-      </c>
+      <c r="G71" s="69"/>
       <c r="H71" s="62"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
@@ -31192,16 +31193,52 @@
       </c>
       <c r="C72" s="68"/>
       <c r="D72" s="60" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E72" s="61" t="s">
         <v>20</v>
       </c>
       <c r="F72" s="114"/>
       <c r="G72" s="60">
+        <v>75</v>
+      </c>
+      <c r="H72" s="62"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A73" s="103"/>
+      <c r="B73" s="103" t="s">
+        <v>44</v>
+      </c>
+      <c r="C73" s="68"/>
+      <c r="D73" s="60" t="s">
+        <v>153</v>
+      </c>
+      <c r="E73" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F73" s="114"/>
+      <c r="G73" s="60">
+        <v>450</v>
+      </c>
+      <c r="H73" s="62"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" s="103"/>
+      <c r="B74" s="103" t="s">
+        <v>44</v>
+      </c>
+      <c r="C74" s="68"/>
+      <c r="D74" s="60" t="s">
+        <v>154</v>
+      </c>
+      <c r="E74" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F74" s="114"/>
+      <c r="G74" s="60">
         <v>3600</v>
       </c>
-      <c r="H72" s="62"/>
+      <c r="H74" s="62"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -36631,7 +36668,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1063"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B149" sqref="B149"/>
     </sheetView>
   </sheetViews>
@@ -36931,14 +36968,14 @@
     <row r="9" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="32"/>
       <c r="B9" s="28" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C9" s="29" t="s">
         <v>20</v>
       </c>
       <c r="D9" s="28">
         <f>IF(multi_stock_sampling="Yes", 1, 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="28" t="s">
         <v>192</v>
@@ -40031,7 +40068,7 @@
     </row>
     <row r="91" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="64">
-        <f>'Old Reagents'!B11</f>
+        <f>'Old Reagents'!B13</f>
         <v>0</v>
       </c>
       <c r="B91" s="60" t="s">
@@ -40041,7 +40078,7 @@
         <v>20</v>
       </c>
       <c r="D91" s="69" t="str">
-        <f>'Old Reagents'!F11</f>
+        <f>'Old Reagents'!F13</f>
         <v>['DMSO']</v>
       </c>
       <c r="E91" s="60" t="s">
@@ -40071,7 +40108,7 @@
     </row>
     <row r="92" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="64" t="str">
-        <f>'Old Reagents'!B12</f>
+        <f>'Old Reagents'!B14</f>
         <v>#</v>
       </c>
       <c r="B92" s="60" t="s">
@@ -40081,7 +40118,7 @@
         <v>20</v>
       </c>
       <c r="D92" s="69">
-        <f>'Old Reagents'!F12</f>
+        <f>'Old Reagents'!F14</f>
         <v>0</v>
       </c>
       <c r="E92" s="69" t="s">
@@ -40111,7 +40148,7 @@
     </row>
     <row r="93" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="64" t="str">
-        <f>'Old Reagents'!B13</f>
+        <f>'Old Reagents'!B15</f>
         <v>#</v>
       </c>
       <c r="B93" s="60" t="s">
@@ -40121,7 +40158,7 @@
         <v>20</v>
       </c>
       <c r="D93" s="69">
-        <f>'Old Reagents'!F13</f>
+        <f>'Old Reagents'!F15</f>
         <v>1.5</v>
       </c>
       <c r="E93" s="60" t="s">
@@ -40151,7 +40188,7 @@
     </row>
     <row r="94" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="64" t="str">
-        <f>'Old Reagents'!B14</f>
+        <f>'Old Reagents'!B16</f>
         <v>#</v>
       </c>
       <c r="B94" s="60" t="s">
@@ -40161,7 +40198,7 @@
         <v>20</v>
       </c>
       <c r="D94" s="69">
-        <f>'Old Reagents'!F14</f>
+        <f>'Old Reagents'!F16</f>
         <v>7.63</v>
       </c>
       <c r="E94" s="60" t="s">
@@ -40191,7 +40228,7 @@
     </row>
     <row r="95" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="64" t="str">
-        <f>'Old Reagents'!B15</f>
+        <f>'Old Reagents'!B17</f>
         <v>#</v>
       </c>
       <c r="B95" s="60" t="s">
@@ -40201,7 +40238,7 @@
         <v>20</v>
       </c>
       <c r="D95" s="69">
-        <f>'Old Reagents'!F15</f>
+        <f>'Old Reagents'!F17</f>
         <v>0</v>
       </c>
       <c r="E95" s="60" t="s">
@@ -40231,7 +40268,7 @@
     </row>
     <row r="96" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="64" t="str">
-        <f>'Old Reagents'!B16</f>
+        <f>'Old Reagents'!B18</f>
         <v>#</v>
       </c>
       <c r="B96" s="60" t="s">
@@ -40241,7 +40278,7 @@
         <v>20</v>
       </c>
       <c r="D96" s="69">
-        <f>'Old Reagents'!F16</f>
+        <f>'Old Reagents'!F18</f>
         <v>0</v>
       </c>
       <c r="E96" s="60" t="s">
@@ -40271,7 +40308,7 @@
     </row>
     <row r="97" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="64" t="str">
-        <f>'Old Reagents'!B17</f>
+        <f>'Old Reagents'!B19</f>
         <v>#</v>
       </c>
       <c r="B97" s="60" t="s">
@@ -40281,7 +40318,7 @@
         <v>20</v>
       </c>
       <c r="D97" s="69">
-        <f>'Old Reagents'!F17</f>
+        <f>'Old Reagents'!F19</f>
         <v>0</v>
       </c>
       <c r="E97" s="60" t="s">
@@ -40311,7 +40348,7 @@
     </row>
     <row r="98" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="64" t="str">
-        <f>'Old Reagents'!B18</f>
+        <f>'Old Reagents'!B20</f>
         <v>#</v>
       </c>
       <c r="B98" s="60" t="s">
@@ -40321,7 +40358,7 @@
         <v>20</v>
       </c>
       <c r="D98" s="69">
-        <f>'Old Reagents'!F18</f>
+        <f>'Old Reagents'!F20</f>
         <v>0</v>
       </c>
       <c r="E98" s="60" t="s">
@@ -40379,7 +40416,7 @@
     </row>
     <row r="100" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="64">
-        <f>'Old Reagents'!B20</f>
+        <f>'Old Reagents'!B22</f>
         <v>0</v>
       </c>
       <c r="B100" s="60" t="s">
@@ -40389,7 +40426,7 @@
         <v>20</v>
       </c>
       <c r="D100" s="69" t="str">
-        <f>'Old Reagents'!F20</f>
+        <f>'Old Reagents'!F22</f>
         <v>['PbI2','PyrrolidiniumIodide','DMSO']</v>
       </c>
       <c r="E100" s="60" t="s">
@@ -40419,7 +40456,7 @@
     </row>
     <row r="101" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="64">
-        <f>'Old Reagents'!B21</f>
+        <f>'Old Reagents'!B23</f>
         <v>0</v>
       </c>
       <c r="B101" s="60" t="s">
@@ -40429,7 +40466,7 @@
         <v>20</v>
       </c>
       <c r="D101" s="69">
-        <f>'Old Reagents'!F21</f>
+        <f>'Old Reagents'!F23</f>
         <v>1.55</v>
       </c>
       <c r="E101" s="69" t="s">
@@ -40459,7 +40496,7 @@
     </row>
     <row r="102" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="64">
-        <f>'Old Reagents'!B22</f>
+        <f>'Old Reagents'!B24</f>
         <v>0</v>
       </c>
       <c r="B102" s="60" t="s">
@@ -40469,7 +40506,7 @@
         <v>20</v>
       </c>
       <c r="D102" s="69">
-        <f>'Old Reagents'!F22</f>
+        <f>'Old Reagents'!F24</f>
         <v>1.93</v>
       </c>
       <c r="E102" s="60" t="s">
@@ -40499,7 +40536,7 @@
     </row>
     <row r="103" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="64" t="str">
-        <f>'Old Reagents'!B23</f>
+        <f>'Old Reagents'!B25</f>
         <v>#</v>
       </c>
       <c r="B103" s="60" t="s">
@@ -40509,7 +40546,7 @@
         <v>20</v>
       </c>
       <c r="D103" s="69">
-        <f>'Old Reagents'!F23</f>
+        <f>'Old Reagents'!F25</f>
         <v>0</v>
       </c>
       <c r="E103" s="60" t="s">
@@ -40539,7 +40576,7 @@
     </row>
     <row r="104" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="64" t="str">
-        <f>'Old Reagents'!B24</f>
+        <f>'Old Reagents'!B26</f>
         <v>#</v>
       </c>
       <c r="B104" s="60" t="s">
@@ -40549,7 +40586,7 @@
         <v>20</v>
       </c>
       <c r="D104" s="69">
-        <f>'Old Reagents'!F24</f>
+        <f>'Old Reagents'!F26</f>
         <v>0</v>
       </c>
       <c r="E104" s="60" t="s">
@@ -40579,7 +40616,7 @@
     </row>
     <row r="105" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="64" t="str">
-        <f>'Old Reagents'!B25</f>
+        <f>'Old Reagents'!B27</f>
         <v>#</v>
       </c>
       <c r="B105" s="60" t="s">
@@ -40589,7 +40626,7 @@
         <v>20</v>
       </c>
       <c r="D105" s="69">
-        <f>'Old Reagents'!F25</f>
+        <f>'Old Reagents'!F27</f>
         <v>0</v>
       </c>
       <c r="E105" s="60" t="s">
@@ -40619,7 +40656,7 @@
     </row>
     <row r="106" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="64" t="str">
-        <f>'Old Reagents'!B26</f>
+        <f>'Old Reagents'!B28</f>
         <v>#</v>
       </c>
       <c r="B106" s="60" t="s">
@@ -40629,7 +40666,7 @@
         <v>20</v>
       </c>
       <c r="D106" s="69">
-        <f>'Old Reagents'!F26</f>
+        <f>'Old Reagents'!F28</f>
         <v>0</v>
       </c>
       <c r="E106" s="60" t="s">
@@ -40659,7 +40696,7 @@
     </row>
     <row r="107" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="64" t="str">
-        <f>'Old Reagents'!B27</f>
+        <f>'Old Reagents'!B29</f>
         <v>#</v>
       </c>
       <c r="B107" s="60" t="s">
@@ -40669,7 +40706,7 @@
         <v>20</v>
       </c>
       <c r="D107" s="69">
-        <f>'Old Reagents'!F27</f>
+        <f>'Old Reagents'!F29</f>
         <v>0</v>
       </c>
       <c r="E107" s="60" t="s">
@@ -40702,7 +40739,7 @@
       <c r="B108" s="60"/>
       <c r="C108" s="61"/>
       <c r="D108" s="69">
-        <f>'Old Reagents'!F28</f>
+        <f>'Old Reagents'!F30</f>
         <v>0</v>
       </c>
       <c r="E108" s="60"/>
@@ -40730,7 +40767,7 @@
     </row>
     <row r="109" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="64">
-        <f>'Old Reagents'!B29</f>
+        <f>'Old Reagents'!B31</f>
         <v>0</v>
       </c>
       <c r="B109" s="60" t="s">
@@ -40740,7 +40777,7 @@
         <v>20</v>
       </c>
       <c r="D109" s="69" t="str">
-        <f>'Old Reagents'!F29</f>
+        <f>'Old Reagents'!F31</f>
         <v>['PyrrolidiniumIodide','DMSO']</v>
       </c>
       <c r="E109" s="60" t="s">
@@ -40770,7 +40807,7 @@
     </row>
     <row r="110" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="64">
-        <f>'Old Reagents'!B30</f>
+        <f>'Old Reagents'!B32</f>
         <v>0</v>
       </c>
       <c r="B110" s="99" t="s">
@@ -40780,7 +40817,7 @@
         <v>20</v>
       </c>
       <c r="D110" s="69">
-        <f>'Old Reagents'!F30</f>
+        <f>'Old Reagents'!F32</f>
         <v>2.06</v>
       </c>
       <c r="E110" s="69" t="s">
@@ -40810,7 +40847,7 @@
     </row>
     <row r="111" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="64" t="str">
-        <f>'Old Reagents'!B31</f>
+        <f>'Old Reagents'!B33</f>
         <v>#</v>
       </c>
       <c r="B111" s="60" t="s">
@@ -40820,7 +40857,7 @@
         <v>20</v>
       </c>
       <c r="D111" s="69">
-        <f>'Old Reagents'!F31</f>
+        <f>'Old Reagents'!F33</f>
         <v>1.33</v>
       </c>
       <c r="E111" s="60" t="s">
@@ -40850,7 +40887,7 @@
     </row>
     <row r="112" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="64" t="str">
-        <f>'Old Reagents'!B32</f>
+        <f>'Old Reagents'!B34</f>
         <v>#</v>
       </c>
       <c r="B112" s="60" t="s">
@@ -40860,7 +40897,7 @@
         <v>20</v>
       </c>
       <c r="D112" s="69">
-        <f>'Old Reagents'!F32</f>
+        <f>'Old Reagents'!F34</f>
         <v>1.2</v>
       </c>
       <c r="E112" s="60" t="s">
@@ -40890,17 +40927,17 @@
     </row>
     <row r="113" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="64" t="str">
-        <f>'Old Reagents'!B33</f>
+        <f>'Old Reagents'!B35</f>
         <v>#</v>
       </c>
       <c r="B113" s="60" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C113" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D113" s="69">
-        <f>'Old Reagents'!F33</f>
+        <f>'Old Reagents'!F35</f>
         <v>0</v>
       </c>
       <c r="E113" s="60" t="s">
@@ -40930,7 +40967,7 @@
     </row>
     <row r="114" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="64" t="str">
-        <f>'Old Reagents'!B34</f>
+        <f>'Old Reagents'!B36</f>
         <v>#</v>
       </c>
       <c r="B114" s="60" t="s">
@@ -40940,7 +40977,7 @@
         <v>20</v>
       </c>
       <c r="D114" s="69">
-        <f>'Old Reagents'!F34</f>
+        <f>'Old Reagents'!F36</f>
         <v>0</v>
       </c>
       <c r="E114" s="60" t="s">
@@ -40970,7 +41007,7 @@
     </row>
     <row r="115" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="64" t="str">
-        <f>'Old Reagents'!B35</f>
+        <f>'Old Reagents'!B37</f>
         <v>#</v>
       </c>
       <c r="B115" s="60" t="s">
@@ -40980,7 +41017,7 @@
         <v>20</v>
       </c>
       <c r="D115" s="69">
-        <f>'Old Reagents'!F35</f>
+        <f>'Old Reagents'!F37</f>
         <v>0</v>
       </c>
       <c r="E115" s="60" t="s">
@@ -41010,7 +41047,7 @@
     </row>
     <row r="116" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="64" t="str">
-        <f>'Old Reagents'!B36</f>
+        <f>'Old Reagents'!B38</f>
         <v>#</v>
       </c>
       <c r="B116" s="60" t="s">
@@ -41020,7 +41057,7 @@
         <v>20</v>
       </c>
       <c r="D116" s="69">
-        <f>'Old Reagents'!F36</f>
+        <f>'Old Reagents'!F38</f>
         <v>0</v>
       </c>
       <c r="E116" s="60" t="s">
@@ -41078,7 +41115,7 @@
     </row>
     <row r="118" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="64">
-        <f>'Old Reagents'!B38</f>
+        <f>'Old Reagents'!B40</f>
         <v>0</v>
       </c>
       <c r="B118" s="60" t="s">
@@ -41088,7 +41125,7 @@
         <v>20</v>
       </c>
       <c r="D118" s="69" t="str">
-        <f>'Old Reagents'!F38</f>
+        <f>'Old Reagents'!F40</f>
         <v>['PbI2','PyrrolidiniumIodide','DMSO']</v>
       </c>
       <c r="E118" s="60" t="s">
@@ -41118,7 +41155,7 @@
     </row>
     <row r="119" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="64">
-        <f>'Old Reagents'!B39</f>
+        <f>'Old Reagents'!B41</f>
         <v>0</v>
       </c>
       <c r="B119" s="99" t="s">
@@ -41128,7 +41165,7 @@
         <v>20</v>
       </c>
       <c r="D119" s="69">
-        <f>'Old Reagents'!F39</f>
+        <f>'Old Reagents'!F41</f>
         <v>1.18</v>
       </c>
       <c r="E119" s="69" t="s">
@@ -41158,7 +41195,7 @@
     </row>
     <row r="120" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="64">
-        <f>'Old Reagents'!B40</f>
+        <f>'Old Reagents'!B42</f>
         <v>0</v>
       </c>
       <c r="B120" s="99" t="s">
@@ -41168,7 +41205,7 @@
         <v>20</v>
       </c>
       <c r="D120" s="69">
-        <f>'Old Reagents'!F40</f>
+        <f>'Old Reagents'!F42</f>
         <v>0.74</v>
       </c>
       <c r="E120" s="60" t="s">
@@ -41198,7 +41235,7 @@
     </row>
     <row r="121" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="64" t="str">
-        <f>'Old Reagents'!B41</f>
+        <f>'Old Reagents'!B43</f>
         <v>#</v>
       </c>
       <c r="B121" s="60" t="s">
@@ -41208,7 +41245,7 @@
         <v>20</v>
       </c>
       <c r="D121" s="69">
-        <f>'Old Reagents'!F41</f>
+        <f>'Old Reagents'!F43</f>
         <v>0</v>
       </c>
       <c r="E121" s="60" t="s">
@@ -41238,7 +41275,7 @@
     </row>
     <row r="122" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="64" t="str">
-        <f>'Old Reagents'!B42</f>
+        <f>'Old Reagents'!B44</f>
         <v>#</v>
       </c>
       <c r="B122" s="60" t="s">
@@ -41248,7 +41285,7 @@
         <v>20</v>
       </c>
       <c r="D122" s="69">
-        <f>'Old Reagents'!F42</f>
+        <f>'Old Reagents'!F44</f>
         <v>0</v>
       </c>
       <c r="E122" s="60" t="s">
@@ -41278,7 +41315,7 @@
     </row>
     <row r="123" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="64" t="str">
-        <f>'Old Reagents'!B43</f>
+        <f>'Old Reagents'!B45</f>
         <v>#</v>
       </c>
       <c r="B123" s="60" t="s">
@@ -41288,7 +41325,7 @@
         <v>20</v>
       </c>
       <c r="D123" s="69">
-        <f>'Old Reagents'!F43</f>
+        <f>'Old Reagents'!F45</f>
         <v>0</v>
       </c>
       <c r="E123" s="60" t="s">
@@ -41318,7 +41355,7 @@
     </row>
     <row r="124" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="64" t="str">
-        <f>'Old Reagents'!B44</f>
+        <f>'Old Reagents'!B46</f>
         <v>#</v>
       </c>
       <c r="B124" s="60" t="s">
@@ -41328,7 +41365,7 @@
         <v>20</v>
       </c>
       <c r="D124" s="69">
-        <f>'Old Reagents'!F44</f>
+        <f>'Old Reagents'!F46</f>
         <v>0</v>
       </c>
       <c r="E124" s="60" t="s">
@@ -41358,7 +41395,7 @@
     </row>
     <row r="125" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="64" t="str">
-        <f>'Old Reagents'!B45</f>
+        <f>'Old Reagents'!B47</f>
         <v>#</v>
       </c>
       <c r="B125" s="60" t="s">
@@ -41368,7 +41405,7 @@
         <v>20</v>
       </c>
       <c r="D125" s="69">
-        <f>'Old Reagents'!F45</f>
+        <f>'Old Reagents'!F47</f>
         <v>0</v>
       </c>
       <c r="E125" s="60" t="s">
@@ -41426,7 +41463,7 @@
     </row>
     <row r="127" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="64">
-        <f>'Old Reagents'!B47</f>
+        <f>'Old Reagents'!B49</f>
         <v>0</v>
       </c>
       <c r="B127" s="60" t="s">
@@ -41436,7 +41473,7 @@
         <v>20</v>
       </c>
       <c r="D127" s="69" t="str">
-        <f>'Old Reagents'!F47</f>
+        <f>'Old Reagents'!F49</f>
         <v>['PbI2','PyrrolidiniumIodide','DMSO']</v>
       </c>
       <c r="E127" s="60" t="s">
@@ -41466,7 +41503,7 @@
     </row>
     <row r="128" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="64">
-        <f>'Old Reagents'!B48</f>
+        <f>'Old Reagents'!B50</f>
         <v>0</v>
       </c>
       <c r="B128" s="99" t="s">
@@ -41476,7 +41513,7 @@
         <v>20</v>
       </c>
       <c r="D128" s="69">
-        <f>'Old Reagents'!F48</f>
+        <f>'Old Reagents'!F50</f>
         <v>1.42</v>
       </c>
       <c r="E128" s="69" t="s">
@@ -41506,7 +41543,7 @@
     </row>
     <row r="129" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="64">
-        <f>'Old Reagents'!B49</f>
+        <f>'Old Reagents'!B51</f>
         <v>0</v>
       </c>
       <c r="B129" s="99" t="s">
@@ -41516,7 +41553,7 @@
         <v>20</v>
       </c>
       <c r="D129" s="69">
-        <f>'Old Reagents'!F49</f>
+        <f>'Old Reagents'!F51</f>
         <v>1.06</v>
       </c>
       <c r="E129" s="60" t="s">
@@ -41546,7 +41583,7 @@
     </row>
     <row r="130" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="64" t="str">
-        <f>'Old Reagents'!B50</f>
+        <f>'Old Reagents'!B52</f>
         <v>#</v>
       </c>
       <c r="B130" s="60" t="s">
@@ -41556,7 +41593,7 @@
         <v>20</v>
       </c>
       <c r="D130" s="69" t="str">
-        <f>'Old Reagents'!F50</f>
+        <f>'Old Reagents'!F52</f>
         <v>['PbI2','PyrrolidiniumIodide','DMSO']</v>
       </c>
       <c r="E130" s="60" t="s">
@@ -41586,7 +41623,7 @@
     </row>
     <row r="131" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="64" t="str">
-        <f>'Old Reagents'!B51</f>
+        <f>'Old Reagents'!B53</f>
         <v>#</v>
       </c>
       <c r="B131" s="60" t="s">
@@ -41596,7 +41633,7 @@
         <v>20</v>
       </c>
       <c r="D131" s="69">
-        <f>'Old Reagents'!F51</f>
+        <f>'Old Reagents'!F53</f>
         <v>1.42</v>
       </c>
       <c r="E131" s="60" t="s">
@@ -41626,7 +41663,7 @@
     </row>
     <row r="132" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="64" t="str">
-        <f>'Old Reagents'!B52</f>
+        <f>'Old Reagents'!B54</f>
         <v>#</v>
       </c>
       <c r="B132" s="60" t="s">
@@ -41636,7 +41673,7 @@
         <v>20</v>
       </c>
       <c r="D132" s="69">
-        <f>'Old Reagents'!F52</f>
+        <f>'Old Reagents'!F54</f>
         <v>1.06</v>
       </c>
       <c r="E132" s="60" t="s">
@@ -41666,7 +41703,7 @@
     </row>
     <row r="133" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="64" t="str">
-        <f>'Old Reagents'!B53</f>
+        <f>'Old Reagents'!B55</f>
         <v>#</v>
       </c>
       <c r="B133" s="60" t="s">
@@ -41676,7 +41713,7 @@
         <v>20</v>
       </c>
       <c r="D133" s="69" t="str">
-        <f>'Old Reagents'!F53</f>
+        <f>'Old Reagents'!F55</f>
         <v>['PbI2','PyrrolidiniumIodide','DMSO']</v>
       </c>
       <c r="E133" s="60" t="s">
@@ -41706,7 +41743,7 @@
     </row>
     <row r="134" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="64" t="str">
-        <f>'Old Reagents'!B54</f>
+        <f>'Old Reagents'!B56</f>
         <v>#</v>
       </c>
       <c r="B134" s="60" t="s">
@@ -41716,7 +41753,7 @@
         <v>20</v>
       </c>
       <c r="D134" s="69">
-        <f>'Old Reagents'!F54</f>
+        <f>'Old Reagents'!F56</f>
         <v>1.42</v>
       </c>
       <c r="E134" s="60" t="s">
@@ -41774,7 +41811,7 @@
     </row>
     <row r="136" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="64" t="str">
-        <f>'Old Reagents'!B56</f>
+        <f>'Old Reagents'!B58</f>
         <v>#</v>
       </c>
       <c r="B136" s="60" t="s">
@@ -41784,7 +41821,7 @@
         <v>20</v>
       </c>
       <c r="D136" s="69" t="str">
-        <f>'Old Reagents'!F56</f>
+        <f>'Old Reagents'!F58</f>
         <v>['PbI2','PyrrolidiniumIodide','DMSO']</v>
       </c>
       <c r="E136" s="60" t="s">
@@ -41814,7 +41851,7 @@
     </row>
     <row r="137" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="64" t="str">
-        <f>'Old Reagents'!B57</f>
+        <f>'Old Reagents'!B59</f>
         <v>#</v>
       </c>
       <c r="B137" s="99" t="s">
@@ -41824,7 +41861,7 @@
         <v>20</v>
       </c>
       <c r="D137" s="69">
-        <f>'Old Reagents'!F57</f>
+        <f>'Old Reagents'!F59</f>
         <v>1.42</v>
       </c>
       <c r="E137" s="69" t="s">
@@ -41854,7 +41891,7 @@
     </row>
     <row r="138" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="64" t="str">
-        <f>'Old Reagents'!B58</f>
+        <f>'Old Reagents'!B60</f>
         <v>#</v>
       </c>
       <c r="B138" s="99" t="s">
@@ -41864,7 +41901,7 @@
         <v>20</v>
       </c>
       <c r="D138" s="69">
-        <f>'Old Reagents'!F58</f>
+        <f>'Old Reagents'!F60</f>
         <v>1.06</v>
       </c>
       <c r="E138" s="60" t="s">
@@ -41894,7 +41931,7 @@
     </row>
     <row r="139" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="64" t="str">
-        <f>'Old Reagents'!B59</f>
+        <f>'Old Reagents'!B61</f>
         <v>#</v>
       </c>
       <c r="B139" s="60" t="s">
@@ -41904,7 +41941,7 @@
         <v>20</v>
       </c>
       <c r="D139" s="69">
-        <f>'Old Reagents'!F59</f>
+        <f>'Old Reagents'!F61</f>
         <v>0</v>
       </c>
       <c r="E139" s="60" t="s">
@@ -41934,7 +41971,7 @@
     </row>
     <row r="140" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="64" t="str">
-        <f>'Old Reagents'!B60</f>
+        <f>'Old Reagents'!B62</f>
         <v>#</v>
       </c>
       <c r="B140" s="60" t="s">
@@ -41944,7 +41981,7 @@
         <v>20</v>
       </c>
       <c r="D140" s="69">
-        <f>'Old Reagents'!F60</f>
+        <f>'Old Reagents'!F62</f>
         <v>0</v>
       </c>
       <c r="E140" s="60" t="s">
@@ -41974,7 +42011,7 @@
     </row>
     <row r="141" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="64" t="str">
-        <f>'Old Reagents'!B61</f>
+        <f>'Old Reagents'!B63</f>
         <v>#</v>
       </c>
       <c r="B141" s="60" t="s">
@@ -41984,7 +42021,7 @@
         <v>20</v>
       </c>
       <c r="D141" s="69">
-        <f>'Old Reagents'!F61</f>
+        <f>'Old Reagents'!F63</f>
         <v>0</v>
       </c>
       <c r="E141" s="60" t="s">
@@ -42014,7 +42051,7 @@
     </row>
     <row r="142" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="64" t="str">
-        <f>'Old Reagents'!B62</f>
+        <f>'Old Reagents'!B64</f>
         <v>#</v>
       </c>
       <c r="B142" s="60" t="s">
@@ -42024,7 +42061,7 @@
         <v>20</v>
       </c>
       <c r="D142" s="69">
-        <f>'Old Reagents'!F62</f>
+        <f>'Old Reagents'!F64</f>
         <v>0</v>
       </c>
       <c r="E142" s="60" t="s">
@@ -42054,7 +42091,7 @@
     </row>
     <row r="143" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="64" t="str">
-        <f>'Old Reagents'!B63</f>
+        <f>'Old Reagents'!B65</f>
         <v>#</v>
       </c>
       <c r="B143" s="60" t="s">
@@ -42064,7 +42101,7 @@
         <v>20</v>
       </c>
       <c r="D143" s="69">
-        <f>'Old Reagents'!F63</f>
+        <f>'Old Reagents'!F65</f>
         <v>0</v>
       </c>
       <c r="E143" s="60" t="s">
@@ -42122,7 +42159,7 @@
     </row>
     <row r="145" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="64">
-        <f>'Old Reagents'!B65</f>
+        <f>'Old Reagents'!B67</f>
         <v>0</v>
       </c>
       <c r="B145" s="60" t="s">
@@ -42132,7 +42169,7 @@
         <v>20</v>
       </c>
       <c r="D145" s="69" t="str">
-        <f>'Old Reagents'!F65</f>
+        <f>'Old Reagents'!F67</f>
         <v>['FAH']</v>
       </c>
       <c r="E145" s="60" t="s">
@@ -42162,7 +42199,7 @@
     </row>
     <row r="146" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="64" t="str">
-        <f>'Old Reagents'!B66</f>
+        <f>'Old Reagents'!B68</f>
         <v>#</v>
       </c>
       <c r="B146" s="99" t="s">
@@ -42172,7 +42209,7 @@
         <v>20</v>
       </c>
       <c r="D146" s="69">
-        <f>'Old Reagents'!F66</f>
+        <f>'Old Reagents'!F68</f>
         <v>1.5</v>
       </c>
       <c r="E146" s="69" t="s">
@@ -42202,7 +42239,7 @@
     </row>
     <row r="147" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="64" t="str">
-        <f>'Old Reagents'!B67</f>
+        <f>'Old Reagents'!B69</f>
         <v>#</v>
       </c>
       <c r="B147" s="99" t="s">
@@ -42212,7 +42249,7 @@
         <v>20</v>
       </c>
       <c r="D147" s="69">
-        <f>'Old Reagents'!F67</f>
+        <f>'Old Reagents'!F69</f>
         <v>7.63</v>
       </c>
       <c r="E147" s="60" t="s">
@@ -42242,7 +42279,7 @@
     </row>
     <row r="148" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="64" t="str">
-        <f>'Old Reagents'!B68</f>
+        <f>'Old Reagents'!B70</f>
         <v>#</v>
       </c>
       <c r="B148" s="60" t="s">
@@ -42252,7 +42289,7 @@
         <v>20</v>
       </c>
       <c r="D148" s="69">
-        <f>'Old Reagents'!F68</f>
+        <f>'Old Reagents'!F70</f>
         <v>0</v>
       </c>
       <c r="E148" s="60" t="s">
@@ -42282,7 +42319,7 @@
     </row>
     <row r="149" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="64" t="str">
-        <f>'Old Reagents'!B69</f>
+        <f>'Old Reagents'!B71</f>
         <v>#</v>
       </c>
       <c r="B149" s="60" t="s">
@@ -42292,7 +42329,7 @@
         <v>20</v>
       </c>
       <c r="D149" s="69">
-        <f>'Old Reagents'!F69</f>
+        <f>'Old Reagents'!F71</f>
         <v>0</v>
       </c>
       <c r="E149" s="60" t="s">
@@ -42322,7 +42359,7 @@
     </row>
     <row r="150" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="64" t="str">
-        <f>'Old Reagents'!B70</f>
+        <f>'Old Reagents'!B72</f>
         <v>#</v>
       </c>
       <c r="B150" s="60" t="s">
@@ -42332,7 +42369,7 @@
         <v>20</v>
       </c>
       <c r="D150" s="69">
-        <f>'Old Reagents'!F70</f>
+        <f>'Old Reagents'!F72</f>
         <v>0</v>
       </c>
       <c r="E150" s="60" t="s">
@@ -42362,7 +42399,7 @@
     </row>
     <row r="151" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="64" t="str">
-        <f>'Old Reagents'!B71</f>
+        <f>'Old Reagents'!B73</f>
         <v>#</v>
       </c>
       <c r="B151" s="60" t="s">
@@ -42372,7 +42409,7 @@
         <v>20</v>
       </c>
       <c r="D151" s="69">
-        <f>'Old Reagents'!F71</f>
+        <f>'Old Reagents'!F73</f>
         <v>0</v>
       </c>
       <c r="E151" s="60" t="s">
@@ -42402,7 +42439,7 @@
     </row>
     <row r="152" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="64" t="str">
-        <f>'Old Reagents'!B72</f>
+        <f>'Old Reagents'!B74</f>
         <v>#</v>
       </c>
       <c r="B152" s="60" t="s">
@@ -42412,7 +42449,7 @@
         <v>20</v>
       </c>
       <c r="D152" s="69">
-        <f>'Old Reagents'!F72</f>
+        <f>'Old Reagents'!F74</f>
         <v>0</v>
       </c>
       <c r="E152" s="60" t="s">

</xml_diff>

<commit_message>
bug in old_reagents dict construction
need ian's help.

CBz is appearing in both old_reagents and rdict, when it shouldnt
</commit_message>
<xml_diff>
--- a/HC_LBL_SpecificationInterface.xlsx
+++ b/HC_LBL_SpecificationInterface.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="User Interface" sheetId="1" r:id="rId1"/>
-    <sheet name="Manual Experiment Interface" sheetId="2" r:id="rId2"/>
-    <sheet name="Old Reagents" sheetId="5" r:id="rId3"/>
+    <sheet name="Old Reagents" sheetId="5" r:id="rId2"/>
+    <sheet name="Manual Experiment Interface" sheetId="2" r:id="rId3"/>
     <sheet name="ManualExps" sheetId="3" state="hidden" r:id="rId4"/>
     <sheet name="WF1" sheetId="4" r:id="rId5"/>
   </sheets>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1030" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1032" uniqueCount="342">
   <si>
     <t>Manual Well Number</t>
   </si>
@@ -1465,6 +1465,9 @@
       <t xml:space="preserve"> multistock sampling is only supported for use with the Wolfram Mathematica sampler</t>
     </r>
   </si>
+  <si>
+    <t>['PbI2','PyrrolidiniumIodide','CBz']</t>
+  </si>
 </sst>
 </file>
 
@@ -2415,8 +2418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView zoomScale="109" zoomScaleNormal="109" zoomScalePageLayoutView="109" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView topLeftCell="A35" zoomScale="109" zoomScaleNormal="109" zoomScalePageLayoutView="109" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -8782,6 +8785,1344 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H74"/>
+  <sheetViews>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" customWidth="1"/>
+    <col min="5" max="5" width="8" customWidth="1"/>
+    <col min="6" max="6" width="29.1640625" customWidth="1"/>
+    <col min="8" max="8" width="58.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="31" x14ac:dyDescent="0.35">
+      <c r="A1" s="120" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="F1" s="118"/>
+      <c r="G1" s="118"/>
+      <c r="H1" s="118"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="118"/>
+      <c r="B2" s="118"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="118"/>
+      <c r="F2" s="118"/>
+      <c r="G2" s="118"/>
+      <c r="H2" s="118"/>
+    </row>
+    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="119" t="s">
+        <v>277</v>
+      </c>
+      <c r="B3" s="118"/>
+      <c r="C3" s="118"/>
+      <c r="D3" s="118"/>
+      <c r="E3" s="118"/>
+      <c r="F3" s="118"/>
+      <c r="G3" s="118"/>
+      <c r="H3" s="118"/>
+    </row>
+    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="119" t="s">
+        <v>280</v>
+      </c>
+      <c r="B4" s="118"/>
+      <c r="C4" s="118"/>
+      <c r="D4" s="118"/>
+      <c r="E4" s="118"/>
+      <c r="F4" s="118"/>
+      <c r="G4" s="118"/>
+      <c r="H4" s="118"/>
+    </row>
+    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="119"/>
+      <c r="B5" s="118"/>
+      <c r="C5" s="118"/>
+      <c r="D5" s="118"/>
+      <c r="E5" s="118"/>
+      <c r="F5" s="118"/>
+      <c r="G5" s="118"/>
+      <c r="H5" s="118"/>
+    </row>
+    <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="119" t="s">
+        <v>278</v>
+      </c>
+      <c r="B6" s="118"/>
+      <c r="C6" s="118"/>
+      <c r="D6" s="118"/>
+      <c r="E6" s="118"/>
+      <c r="F6" s="118"/>
+      <c r="G6" s="118"/>
+      <c r="H6" s="118"/>
+    </row>
+    <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="119" t="s">
+        <v>281</v>
+      </c>
+      <c r="B7" s="118"/>
+      <c r="C7" s="118"/>
+      <c r="D7" s="118"/>
+      <c r="E7" s="118"/>
+      <c r="F7" s="118"/>
+      <c r="G7" s="118"/>
+      <c r="H7" s="118"/>
+    </row>
+    <row r="8" spans="1:8" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="119"/>
+      <c r="B8" s="118"/>
+      <c r="C8" s="118"/>
+      <c r="D8" s="118"/>
+      <c r="E8" s="118"/>
+      <c r="F8" s="118"/>
+      <c r="G8" s="118"/>
+      <c r="H8" s="118"/>
+    </row>
+    <row r="9" spans="1:8" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="119" t="s">
+        <v>340</v>
+      </c>
+      <c r="B9" s="118"/>
+      <c r="C9" s="118"/>
+      <c r="D9" s="118"/>
+      <c r="E9" s="118"/>
+      <c r="F9" s="118"/>
+      <c r="G9" s="118"/>
+      <c r="H9" s="118"/>
+    </row>
+    <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="121"/>
+      <c r="B10" s="122"/>
+      <c r="C10" s="122"/>
+      <c r="D10" s="122"/>
+      <c r="E10" s="122"/>
+      <c r="F10" s="122"/>
+      <c r="G10" s="122"/>
+      <c r="H10" s="122"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="59"/>
+      <c r="B11" s="59" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="59"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="61"/>
+      <c r="F11" s="114"/>
+      <c r="G11" s="60"/>
+      <c r="H11" s="62"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="103"/>
+      <c r="B12" s="103" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="65" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="60"/>
+      <c r="E12" s="61"/>
+      <c r="F12" s="114"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="62" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="104"/>
+      <c r="B13" s="104"/>
+      <c r="C13" s="68">
+        <v>1</v>
+      </c>
+      <c r="D13" s="60" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="115" t="s">
+        <v>273</v>
+      </c>
+      <c r="G13" s="69" t="s">
+        <v>60</v>
+      </c>
+      <c r="H13" s="62" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="104"/>
+      <c r="B14" s="104" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="68"/>
+      <c r="D14" s="60" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="115"/>
+      <c r="G14" s="69"/>
+      <c r="H14" s="62"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="104"/>
+      <c r="B15" s="104" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="68"/>
+      <c r="D15" s="69" t="s">
+        <v>64</v>
+      </c>
+      <c r="E15" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="115">
+        <v>1.5</v>
+      </c>
+      <c r="G15" s="60">
+        <v>1.234</v>
+      </c>
+      <c r="H15" s="62"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="104"/>
+      <c r="B16" s="104" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="68"/>
+      <c r="D16" s="69" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="115">
+        <v>7.63</v>
+      </c>
+      <c r="G16" s="60">
+        <v>5.6779999999999999</v>
+      </c>
+      <c r="H16" s="62"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="104"/>
+      <c r="B17" s="104" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="68"/>
+      <c r="D17" s="69" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="115"/>
+      <c r="G17" s="60">
+        <v>9.0120000000000005</v>
+      </c>
+      <c r="H17" s="123"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="103"/>
+      <c r="B18" s="103" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="68"/>
+      <c r="D18" s="60" t="s">
+        <v>67</v>
+      </c>
+      <c r="E18" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="114"/>
+      <c r="G18" s="60">
+        <v>75</v>
+      </c>
+      <c r="H18" s="123"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="103"/>
+      <c r="B19" s="103" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="68"/>
+      <c r="D19" s="60" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="114"/>
+      <c r="G19" s="60">
+        <v>450</v>
+      </c>
+      <c r="H19" s="123"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="103"/>
+      <c r="B20" s="103" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="68"/>
+      <c r="D20" s="60" t="s">
+        <v>69</v>
+      </c>
+      <c r="E20" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" s="114"/>
+      <c r="G20" s="60">
+        <v>3600</v>
+      </c>
+      <c r="H20" s="62"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="103"/>
+      <c r="B21" s="103"/>
+      <c r="C21" s="68"/>
+      <c r="D21" s="60"/>
+      <c r="E21" s="61"/>
+      <c r="F21" s="114"/>
+      <c r="G21" s="60"/>
+      <c r="H21" s="62"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="104"/>
+      <c r="B22" s="104"/>
+      <c r="C22" s="68">
+        <v>2</v>
+      </c>
+      <c r="D22" s="60" t="s">
+        <v>70</v>
+      </c>
+      <c r="E22" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22" s="115" t="s">
+        <v>274</v>
+      </c>
+      <c r="G22" s="69" t="s">
+        <v>71</v>
+      </c>
+      <c r="H22" s="62" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="104"/>
+      <c r="B23" s="104"/>
+      <c r="C23" s="68"/>
+      <c r="D23" s="69" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="115">
+        <v>1.55</v>
+      </c>
+      <c r="G23" s="60">
+        <v>1.234</v>
+      </c>
+      <c r="H23" s="62" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="104"/>
+      <c r="B24" s="104"/>
+      <c r="C24" s="68"/>
+      <c r="D24" s="69" t="s">
+        <v>76</v>
+      </c>
+      <c r="E24" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" s="115">
+        <v>1.93</v>
+      </c>
+      <c r="G24" s="60">
+        <v>5.6779999999999999</v>
+      </c>
+      <c r="H24" s="62" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="104"/>
+      <c r="B25" s="104" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="68"/>
+      <c r="D25" s="69" t="s">
+        <v>78</v>
+      </c>
+      <c r="E25" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" s="115"/>
+      <c r="G25" s="60">
+        <v>9.0120000000000005</v>
+      </c>
+      <c r="H25" s="62"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="104"/>
+      <c r="B26" s="104" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="72"/>
+      <c r="D26" s="60" t="s">
+        <v>79</v>
+      </c>
+      <c r="E26" s="73" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" s="115"/>
+      <c r="G26" s="69"/>
+      <c r="H26" s="74" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="103"/>
+      <c r="B27" s="103" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="68"/>
+      <c r="D27" s="60" t="s">
+        <v>81</v>
+      </c>
+      <c r="E27" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27" s="114"/>
+      <c r="G27" s="60">
+        <v>75</v>
+      </c>
+      <c r="H27" s="62" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="103"/>
+      <c r="B28" s="103" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" s="68"/>
+      <c r="D28" s="60" t="s">
+        <v>84</v>
+      </c>
+      <c r="E28" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F28" s="114"/>
+      <c r="G28" s="60">
+        <v>450</v>
+      </c>
+      <c r="H28" s="62" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="103"/>
+      <c r="B29" s="103" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" s="68"/>
+      <c r="D29" s="60" t="s">
+        <v>86</v>
+      </c>
+      <c r="E29" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F29" s="114"/>
+      <c r="G29" s="60">
+        <v>3600</v>
+      </c>
+      <c r="H29" s="62" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="103"/>
+      <c r="B30" s="103"/>
+      <c r="C30" s="68"/>
+      <c r="D30" s="60"/>
+      <c r="E30" s="61"/>
+      <c r="F30" s="114"/>
+      <c r="G30" s="60"/>
+      <c r="H30" s="62"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="104"/>
+      <c r="B31" s="104" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31" s="68">
+        <v>3</v>
+      </c>
+      <c r="D31" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="E31" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F31" s="115" t="s">
+        <v>275</v>
+      </c>
+      <c r="G31" s="69" t="s">
+        <v>89</v>
+      </c>
+      <c r="H31" s="62" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="104"/>
+      <c r="B32" s="104" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32" s="68"/>
+      <c r="D32" s="60" t="s">
+        <v>91</v>
+      </c>
+      <c r="E32" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F32" s="114">
+        <v>2.06</v>
+      </c>
+      <c r="G32" s="60">
+        <v>1.234</v>
+      </c>
+      <c r="H32" s="62" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="104"/>
+      <c r="B33" s="104" t="s">
+        <v>44</v>
+      </c>
+      <c r="C33" s="68"/>
+      <c r="D33" s="60" t="s">
+        <v>93</v>
+      </c>
+      <c r="E33" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F33" s="114">
+        <v>1.33</v>
+      </c>
+      <c r="G33" s="60">
+        <v>5.6779999999999999</v>
+      </c>
+      <c r="H33" s="62" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="104"/>
+      <c r="B34" s="104" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" s="68"/>
+      <c r="D34" s="60" t="s">
+        <v>95</v>
+      </c>
+      <c r="E34" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F34" s="114">
+        <v>1.2</v>
+      </c>
+      <c r="G34" s="60">
+        <v>9.0120000000000005</v>
+      </c>
+      <c r="H34" s="62" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="104"/>
+      <c r="B35" s="104" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35" s="72"/>
+      <c r="D35" s="60" t="s">
+        <v>97</v>
+      </c>
+      <c r="E35" s="73" t="s">
+        <v>20</v>
+      </c>
+      <c r="F35" s="115"/>
+      <c r="G35" s="69"/>
+      <c r="H35" s="74" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="104"/>
+      <c r="B36" s="104" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36" s="68"/>
+      <c r="D36" s="60" t="s">
+        <v>100</v>
+      </c>
+      <c r="E36" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F36" s="114"/>
+      <c r="G36" s="60">
+        <v>75</v>
+      </c>
+      <c r="H36" s="62" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="104"/>
+      <c r="B37" s="104" t="s">
+        <v>44</v>
+      </c>
+      <c r="C37" s="68"/>
+      <c r="D37" s="60" t="s">
+        <v>102</v>
+      </c>
+      <c r="E37" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F37" s="114"/>
+      <c r="G37" s="60">
+        <v>450</v>
+      </c>
+      <c r="H37" s="62" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="104"/>
+      <c r="B38" s="104" t="s">
+        <v>44</v>
+      </c>
+      <c r="C38" s="68"/>
+      <c r="D38" s="60" t="s">
+        <v>104</v>
+      </c>
+      <c r="E38" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F38" s="114"/>
+      <c r="G38" s="60">
+        <v>3600</v>
+      </c>
+      <c r="H38" s="62" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="103"/>
+      <c r="B39" s="103"/>
+      <c r="C39" s="68"/>
+      <c r="D39" s="60"/>
+      <c r="E39" s="61"/>
+      <c r="F39" s="114"/>
+      <c r="G39" s="60"/>
+      <c r="H39" s="62"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="104"/>
+      <c r="B40" s="104"/>
+      <c r="C40" s="68">
+        <v>4</v>
+      </c>
+      <c r="D40" s="60" t="s">
+        <v>106</v>
+      </c>
+      <c r="E40" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F40" s="115" t="s">
+        <v>341</v>
+      </c>
+      <c r="G40" s="69" t="s">
+        <v>71</v>
+      </c>
+      <c r="H40" s="62" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="104"/>
+      <c r="B41" s="104"/>
+      <c r="C41" s="68"/>
+      <c r="D41" s="60" t="s">
+        <v>108</v>
+      </c>
+      <c r="E41" s="73" t="s">
+        <v>20</v>
+      </c>
+      <c r="F41" s="115">
+        <v>1.18</v>
+      </c>
+      <c r="G41" s="60">
+        <v>1.234</v>
+      </c>
+      <c r="H41" s="62" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="104"/>
+      <c r="B42" s="104"/>
+      <c r="C42" s="68"/>
+      <c r="D42" s="60" t="s">
+        <v>110</v>
+      </c>
+      <c r="E42" s="73" t="s">
+        <v>20</v>
+      </c>
+      <c r="F42" s="115">
+        <v>0.74</v>
+      </c>
+      <c r="G42" s="60">
+        <v>5.6779999999999999</v>
+      </c>
+      <c r="H42" s="62" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="104"/>
+      <c r="B43" s="104" t="s">
+        <v>44</v>
+      </c>
+      <c r="C43" s="68"/>
+      <c r="D43" s="60" t="s">
+        <v>112</v>
+      </c>
+      <c r="E43" s="73" t="s">
+        <v>20</v>
+      </c>
+      <c r="F43" s="114"/>
+      <c r="G43" s="60">
+        <v>9.0120000000000005</v>
+      </c>
+      <c r="H43" s="62"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="104"/>
+      <c r="B44" s="104" t="s">
+        <v>44</v>
+      </c>
+      <c r="C44" s="72"/>
+      <c r="D44" s="60" t="s">
+        <v>113</v>
+      </c>
+      <c r="E44" s="73" t="s">
+        <v>20</v>
+      </c>
+      <c r="F44" s="115"/>
+      <c r="G44" s="69"/>
+      <c r="H44" s="74" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="104"/>
+      <c r="B45" s="104" t="s">
+        <v>44</v>
+      </c>
+      <c r="C45" s="68"/>
+      <c r="D45" s="60" t="s">
+        <v>115</v>
+      </c>
+      <c r="E45" s="73" t="s">
+        <v>20</v>
+      </c>
+      <c r="F45" s="114"/>
+      <c r="G45" s="60">
+        <v>75</v>
+      </c>
+      <c r="H45" s="62" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" s="104"/>
+      <c r="B46" s="104" t="s">
+        <v>44</v>
+      </c>
+      <c r="C46" s="68"/>
+      <c r="D46" s="60" t="s">
+        <v>116</v>
+      </c>
+      <c r="E46" s="73" t="s">
+        <v>20</v>
+      </c>
+      <c r="F46" s="114"/>
+      <c r="G46" s="60">
+        <v>450</v>
+      </c>
+      <c r="H46" s="62" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" s="104"/>
+      <c r="B47" s="104" t="s">
+        <v>44</v>
+      </c>
+      <c r="C47" s="68"/>
+      <c r="D47" s="60" t="s">
+        <v>117</v>
+      </c>
+      <c r="E47" s="73" t="s">
+        <v>20</v>
+      </c>
+      <c r="F47" s="114"/>
+      <c r="G47" s="60">
+        <v>3600</v>
+      </c>
+      <c r="H47" s="62" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" s="103"/>
+      <c r="B48" s="103"/>
+      <c r="C48" s="68"/>
+      <c r="D48" s="60"/>
+      <c r="E48" s="61"/>
+      <c r="F48" s="114"/>
+      <c r="G48" s="60"/>
+      <c r="H48" s="62"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" s="103"/>
+      <c r="B49" s="103"/>
+      <c r="C49" s="68">
+        <v>5</v>
+      </c>
+      <c r="D49" s="60" t="s">
+        <v>118</v>
+      </c>
+      <c r="E49" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F49" s="115" t="s">
+        <v>274</v>
+      </c>
+      <c r="G49" s="69" t="s">
+        <v>89</v>
+      </c>
+      <c r="H49" s="62" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="104"/>
+      <c r="B50" s="104"/>
+      <c r="C50" s="72"/>
+      <c r="D50" s="60" t="s">
+        <v>121</v>
+      </c>
+      <c r="E50" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F50" s="115">
+        <v>1.42</v>
+      </c>
+      <c r="G50" s="60">
+        <v>1.234</v>
+      </c>
+      <c r="H50" s="62" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="104"/>
+      <c r="B51" s="104"/>
+      <c r="C51" s="72"/>
+      <c r="D51" s="60" t="s">
+        <v>123</v>
+      </c>
+      <c r="E51" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F51" s="115">
+        <v>1.06</v>
+      </c>
+      <c r="G51" s="60">
+        <v>5.6779999999999999</v>
+      </c>
+      <c r="H51" s="62" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" s="104"/>
+      <c r="B52" s="104" t="s">
+        <v>44</v>
+      </c>
+      <c r="C52" s="72"/>
+      <c r="D52" s="60" t="s">
+        <v>125</v>
+      </c>
+      <c r="E52" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F52" s="115" t="s">
+        <v>274</v>
+      </c>
+      <c r="G52" s="60">
+        <v>9.0120000000000005</v>
+      </c>
+      <c r="H52" s="62" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" s="104"/>
+      <c r="B53" s="104" t="s">
+        <v>44</v>
+      </c>
+      <c r="C53" s="72"/>
+      <c r="D53" s="69" t="s">
+        <v>127</v>
+      </c>
+      <c r="E53" s="73" t="s">
+        <v>20</v>
+      </c>
+      <c r="F53" s="115">
+        <v>1.42</v>
+      </c>
+      <c r="G53" s="69"/>
+      <c r="H53" s="74" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" s="104"/>
+      <c r="B54" s="104" t="s">
+        <v>44</v>
+      </c>
+      <c r="C54" s="72"/>
+      <c r="D54" s="60" t="s">
+        <v>129</v>
+      </c>
+      <c r="E54" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F54" s="115">
+        <v>1.06</v>
+      </c>
+      <c r="G54" s="60">
+        <v>75</v>
+      </c>
+      <c r="H54" s="62" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" s="104"/>
+      <c r="B55" s="104" t="s">
+        <v>44</v>
+      </c>
+      <c r="C55" s="72"/>
+      <c r="D55" s="60" t="s">
+        <v>130</v>
+      </c>
+      <c r="E55" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F55" s="115" t="s">
+        <v>274</v>
+      </c>
+      <c r="G55" s="60">
+        <v>450</v>
+      </c>
+      <c r="H55" s="62" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" s="104"/>
+      <c r="B56" s="104" t="s">
+        <v>44</v>
+      </c>
+      <c r="C56" s="72"/>
+      <c r="D56" s="60" t="s">
+        <v>131</v>
+      </c>
+      <c r="E56" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F56" s="115">
+        <v>1.42</v>
+      </c>
+      <c r="G56" s="60">
+        <v>3600</v>
+      </c>
+      <c r="H56" s="62" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" s="103"/>
+      <c r="B57" s="103"/>
+      <c r="C57" s="68"/>
+      <c r="D57" s="60"/>
+      <c r="E57" s="61"/>
+      <c r="F57" s="114"/>
+      <c r="G57" s="60"/>
+      <c r="H57" s="62"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" s="103"/>
+      <c r="B58" s="103" t="s">
+        <v>44</v>
+      </c>
+      <c r="C58" s="68">
+        <v>6</v>
+      </c>
+      <c r="D58" s="60" t="s">
+        <v>132</v>
+      </c>
+      <c r="E58" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F58" s="115" t="s">
+        <v>274</v>
+      </c>
+      <c r="G58" s="69" t="s">
+        <v>71</v>
+      </c>
+      <c r="H58" s="62" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" s="103"/>
+      <c r="B59" s="103" t="s">
+        <v>44</v>
+      </c>
+      <c r="C59" s="68"/>
+      <c r="D59" s="60" t="s">
+        <v>134</v>
+      </c>
+      <c r="E59" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F59" s="115">
+        <v>1.42</v>
+      </c>
+      <c r="G59" s="60">
+        <v>1.234</v>
+      </c>
+      <c r="H59" s="62" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="103"/>
+      <c r="B60" s="103" t="s">
+        <v>44</v>
+      </c>
+      <c r="C60" s="68"/>
+      <c r="D60" s="60" t="s">
+        <v>136</v>
+      </c>
+      <c r="E60" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F60" s="115">
+        <v>1.06</v>
+      </c>
+      <c r="G60" s="60">
+        <v>5.6779999999999999</v>
+      </c>
+      <c r="H60" s="62" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" s="103"/>
+      <c r="B61" s="103" t="s">
+        <v>44</v>
+      </c>
+      <c r="C61" s="68"/>
+      <c r="D61" s="60" t="s">
+        <v>138</v>
+      </c>
+      <c r="E61" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F61" s="114"/>
+      <c r="G61" s="60">
+        <v>9.0120000000000005</v>
+      </c>
+      <c r="H61" s="62"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62" s="103"/>
+      <c r="B62" s="103" t="s">
+        <v>44</v>
+      </c>
+      <c r="C62" s="68"/>
+      <c r="D62" s="69" t="s">
+        <v>139</v>
+      </c>
+      <c r="E62" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F62" s="114"/>
+      <c r="G62" s="60"/>
+      <c r="H62" s="62"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" s="103"/>
+      <c r="B63" s="103" t="s">
+        <v>44</v>
+      </c>
+      <c r="C63" s="68"/>
+      <c r="D63" s="60" t="s">
+        <v>140</v>
+      </c>
+      <c r="E63" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F63" s="114"/>
+      <c r="G63" s="60">
+        <v>75</v>
+      </c>
+      <c r="H63" s="62"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" s="103"/>
+      <c r="B64" s="103" t="s">
+        <v>44</v>
+      </c>
+      <c r="C64" s="68"/>
+      <c r="D64" s="60" t="s">
+        <v>141</v>
+      </c>
+      <c r="E64" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F64" s="114"/>
+      <c r="G64" s="60">
+        <v>450</v>
+      </c>
+      <c r="H64" s="62"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A65" s="103"/>
+      <c r="B65" s="103" t="s">
+        <v>44</v>
+      </c>
+      <c r="C65" s="68"/>
+      <c r="D65" s="60" t="s">
+        <v>142</v>
+      </c>
+      <c r="E65" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F65" s="114"/>
+      <c r="G65" s="60">
+        <v>3600</v>
+      </c>
+      <c r="H65" s="62"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" s="103"/>
+      <c r="B66" s="103"/>
+      <c r="C66" s="68"/>
+      <c r="D66" s="60"/>
+      <c r="E66" s="61"/>
+      <c r="F66" s="114"/>
+      <c r="G66" s="60"/>
+      <c r="H66" s="62"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" s="103"/>
+      <c r="B67" s="103"/>
+      <c r="C67" s="68">
+        <v>7</v>
+      </c>
+      <c r="D67" s="60" t="s">
+        <v>143</v>
+      </c>
+      <c r="E67" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F67" s="115" t="s">
+        <v>144</v>
+      </c>
+      <c r="G67" s="69" t="s">
+        <v>71</v>
+      </c>
+      <c r="H67" s="62" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" s="103"/>
+      <c r="B68" s="103" t="s">
+        <v>44</v>
+      </c>
+      <c r="C68" s="68"/>
+      <c r="D68" s="60" t="s">
+        <v>146</v>
+      </c>
+      <c r="E68" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F68" s="115">
+        <v>1.5</v>
+      </c>
+      <c r="G68" s="60">
+        <v>1.234</v>
+      </c>
+      <c r="H68" s="62" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" s="103"/>
+      <c r="B69" s="103" t="s">
+        <v>44</v>
+      </c>
+      <c r="C69" s="68"/>
+      <c r="D69" s="60" t="s">
+        <v>148</v>
+      </c>
+      <c r="E69" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F69" s="115">
+        <v>7.63</v>
+      </c>
+      <c r="G69" s="60">
+        <v>5.6779999999999999</v>
+      </c>
+      <c r="H69" s="62" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A70" s="103"/>
+      <c r="B70" s="103" t="str">
+        <f>B69</f>
+        <v>#</v>
+      </c>
+      <c r="C70" s="68"/>
+      <c r="D70" s="60" t="s">
+        <v>150</v>
+      </c>
+      <c r="E70" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F70" s="114"/>
+      <c r="G70" s="60">
+        <v>9.0120000000000005</v>
+      </c>
+      <c r="H70" s="62"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" s="103"/>
+      <c r="B71" s="103" t="s">
+        <v>44</v>
+      </c>
+      <c r="C71" s="68"/>
+      <c r="D71" s="60" t="s">
+        <v>151</v>
+      </c>
+      <c r="E71" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F71" s="114"/>
+      <c r="G71" s="69"/>
+      <c r="H71" s="62"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A72" s="103"/>
+      <c r="B72" s="103" t="s">
+        <v>44</v>
+      </c>
+      <c r="C72" s="68"/>
+      <c r="D72" s="60" t="s">
+        <v>152</v>
+      </c>
+      <c r="E72" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F72" s="114"/>
+      <c r="G72" s="60">
+        <v>75</v>
+      </c>
+      <c r="H72" s="62"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A73" s="103"/>
+      <c r="B73" s="103" t="s">
+        <v>44</v>
+      </c>
+      <c r="C73" s="68"/>
+      <c r="D73" s="60" t="s">
+        <v>153</v>
+      </c>
+      <c r="E73" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F73" s="114"/>
+      <c r="G73" s="60">
+        <v>450</v>
+      </c>
+      <c r="H73" s="62"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" s="103"/>
+      <c r="B74" s="103" t="s">
+        <v>44</v>
+      </c>
+      <c r="C74" s="68"/>
+      <c r="D74" s="60" t="s">
+        <v>154</v>
+      </c>
+      <c r="E74" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="F74" s="114"/>
+      <c r="G74" s="60">
+        <v>3600</v>
+      </c>
+      <c r="H74" s="62"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -29908,1340 +31249,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H74"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" customWidth="1"/>
-    <col min="4" max="4" width="29.6640625" customWidth="1"/>
-    <col min="5" max="5" width="8" customWidth="1"/>
-    <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="8" max="8" width="58.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="31" x14ac:dyDescent="0.35">
-      <c r="A1" s="120" t="s">
-        <v>279</v>
-      </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
-      <c r="D1" s="118"/>
-      <c r="E1" s="118"/>
-      <c r="F1" s="118"/>
-      <c r="G1" s="118"/>
-      <c r="H1" s="118"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="118"/>
-      <c r="B2" s="118"/>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
-      <c r="F2" s="118"/>
-      <c r="G2" s="118"/>
-      <c r="H2" s="118"/>
-    </row>
-    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="119" t="s">
-        <v>277</v>
-      </c>
-      <c r="B3" s="118"/>
-      <c r="C3" s="118"/>
-      <c r="D3" s="118"/>
-      <c r="E3" s="118"/>
-      <c r="F3" s="118"/>
-      <c r="G3" s="118"/>
-      <c r="H3" s="118"/>
-    </row>
-    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="119" t="s">
-        <v>280</v>
-      </c>
-      <c r="B4" s="118"/>
-      <c r="C4" s="118"/>
-      <c r="D4" s="118"/>
-      <c r="E4" s="118"/>
-      <c r="F4" s="118"/>
-      <c r="G4" s="118"/>
-      <c r="H4" s="118"/>
-    </row>
-    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="119"/>
-      <c r="B5" s="118"/>
-      <c r="C5" s="118"/>
-      <c r="D5" s="118"/>
-      <c r="E5" s="118"/>
-      <c r="F5" s="118"/>
-      <c r="G5" s="118"/>
-      <c r="H5" s="118"/>
-    </row>
-    <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="119" t="s">
-        <v>278</v>
-      </c>
-      <c r="B6" s="118"/>
-      <c r="C6" s="118"/>
-      <c r="D6" s="118"/>
-      <c r="E6" s="118"/>
-      <c r="F6" s="118"/>
-      <c r="G6" s="118"/>
-      <c r="H6" s="118"/>
-    </row>
-    <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="119" t="s">
-        <v>281</v>
-      </c>
-      <c r="B7" s="118"/>
-      <c r="C7" s="118"/>
-      <c r="D7" s="118"/>
-      <c r="E7" s="118"/>
-      <c r="F7" s="118"/>
-      <c r="G7" s="118"/>
-      <c r="H7" s="118"/>
-    </row>
-    <row r="8" spans="1:8" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="119"/>
-      <c r="B8" s="118"/>
-      <c r="C8" s="118"/>
-      <c r="D8" s="118"/>
-      <c r="E8" s="118"/>
-      <c r="F8" s="118"/>
-      <c r="G8" s="118"/>
-      <c r="H8" s="118"/>
-    </row>
-    <row r="9" spans="1:8" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="119" t="s">
-        <v>340</v>
-      </c>
-      <c r="B9" s="118"/>
-      <c r="C9" s="118"/>
-      <c r="D9" s="118"/>
-      <c r="E9" s="118"/>
-      <c r="F9" s="118"/>
-      <c r="G9" s="118"/>
-      <c r="H9" s="118"/>
-    </row>
-    <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="121"/>
-      <c r="B10" s="122"/>
-      <c r="C10" s="122"/>
-      <c r="D10" s="122"/>
-      <c r="E10" s="122"/>
-      <c r="F10" s="122"/>
-      <c r="G10" s="122"/>
-      <c r="H10" s="122"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="59"/>
-      <c r="B11" s="59" t="s">
-        <v>55</v>
-      </c>
-      <c r="C11" s="59"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="61"/>
-      <c r="F11" s="114"/>
-      <c r="G11" s="60"/>
-      <c r="H11" s="62"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="103"/>
-      <c r="B12" s="103" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="65" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" s="60"/>
-      <c r="E12" s="61"/>
-      <c r="F12" s="114"/>
-      <c r="G12" s="60"/>
-      <c r="H12" s="62" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="104"/>
-      <c r="B13" s="104"/>
-      <c r="C13" s="68">
-        <v>1</v>
-      </c>
-      <c r="D13" s="60" t="s">
-        <v>59</v>
-      </c>
-      <c r="E13" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F13" s="115" t="s">
-        <v>273</v>
-      </c>
-      <c r="G13" s="69" t="s">
-        <v>60</v>
-      </c>
-      <c r="H13" s="62" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="104"/>
-      <c r="B14" s="104" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="68"/>
-      <c r="D14" s="60" t="s">
-        <v>63</v>
-      </c>
-      <c r="E14" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14" s="115"/>
-      <c r="G14" s="69"/>
-      <c r="H14" s="62"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="104"/>
-      <c r="B15" s="104" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" s="68"/>
-      <c r="D15" s="69" t="s">
-        <v>64</v>
-      </c>
-      <c r="E15" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" s="115">
-        <v>1.5</v>
-      </c>
-      <c r="G15" s="60">
-        <v>1.234</v>
-      </c>
-      <c r="H15" s="62"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="104"/>
-      <c r="B16" s="104" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="68"/>
-      <c r="D16" s="69" t="s">
-        <v>65</v>
-      </c>
-      <c r="E16" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F16" s="115">
-        <v>7.63</v>
-      </c>
-      <c r="G16" s="60">
-        <v>5.6779999999999999</v>
-      </c>
-      <c r="H16" s="62"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="104"/>
-      <c r="B17" s="104" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" s="68"/>
-      <c r="D17" s="69" t="s">
-        <v>66</v>
-      </c>
-      <c r="E17" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F17" s="115"/>
-      <c r="G17" s="60">
-        <v>9.0120000000000005</v>
-      </c>
-      <c r="H17" s="123"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="103"/>
-      <c r="B18" s="103" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" s="68"/>
-      <c r="D18" s="60" t="s">
-        <v>67</v>
-      </c>
-      <c r="E18" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F18" s="114"/>
-      <c r="G18" s="60">
-        <v>75</v>
-      </c>
-      <c r="H18" s="123"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="103"/>
-      <c r="B19" s="103" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="68"/>
-      <c r="D19" s="60" t="s">
-        <v>68</v>
-      </c>
-      <c r="E19" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F19" s="114"/>
-      <c r="G19" s="60">
-        <v>450</v>
-      </c>
-      <c r="H19" s="123"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="103"/>
-      <c r="B20" s="103" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" s="68"/>
-      <c r="D20" s="60" t="s">
-        <v>69</v>
-      </c>
-      <c r="E20" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F20" s="114"/>
-      <c r="G20" s="60">
-        <v>3600</v>
-      </c>
-      <c r="H20" s="62"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="103"/>
-      <c r="B21" s="103"/>
-      <c r="C21" s="68"/>
-      <c r="D21" s="60"/>
-      <c r="E21" s="61"/>
-      <c r="F21" s="114"/>
-      <c r="G21" s="60"/>
-      <c r="H21" s="62"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="104"/>
-      <c r="B22" s="104"/>
-      <c r="C22" s="68">
-        <v>2</v>
-      </c>
-      <c r="D22" s="60" t="s">
-        <v>70</v>
-      </c>
-      <c r="E22" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F22" s="115" t="s">
-        <v>274</v>
-      </c>
-      <c r="G22" s="69" t="s">
-        <v>71</v>
-      </c>
-      <c r="H22" s="62" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="104"/>
-      <c r="B23" s="104"/>
-      <c r="C23" s="68"/>
-      <c r="D23" s="69" t="s">
-        <v>74</v>
-      </c>
-      <c r="E23" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F23" s="115">
-        <v>1.55</v>
-      </c>
-      <c r="G23" s="60">
-        <v>1.234</v>
-      </c>
-      <c r="H23" s="62" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="104"/>
-      <c r="B24" s="104"/>
-      <c r="C24" s="68"/>
-      <c r="D24" s="69" t="s">
-        <v>76</v>
-      </c>
-      <c r="E24" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F24" s="115">
-        <v>1.93</v>
-      </c>
-      <c r="G24" s="60">
-        <v>5.6779999999999999</v>
-      </c>
-      <c r="H24" s="62" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="104"/>
-      <c r="B25" s="104" t="s">
-        <v>44</v>
-      </c>
-      <c r="C25" s="68"/>
-      <c r="D25" s="69" t="s">
-        <v>78</v>
-      </c>
-      <c r="E25" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F25" s="115"/>
-      <c r="G25" s="60">
-        <v>9.0120000000000005</v>
-      </c>
-      <c r="H25" s="62"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="104"/>
-      <c r="B26" s="104" t="s">
-        <v>44</v>
-      </c>
-      <c r="C26" s="72"/>
-      <c r="D26" s="60" t="s">
-        <v>79</v>
-      </c>
-      <c r="E26" s="73" t="s">
-        <v>20</v>
-      </c>
-      <c r="F26" s="115"/>
-      <c r="G26" s="69"/>
-      <c r="H26" s="74" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="103"/>
-      <c r="B27" s="103" t="s">
-        <v>44</v>
-      </c>
-      <c r="C27" s="68"/>
-      <c r="D27" s="60" t="s">
-        <v>81</v>
-      </c>
-      <c r="E27" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F27" s="114"/>
-      <c r="G27" s="60">
-        <v>75</v>
-      </c>
-      <c r="H27" s="62" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="103"/>
-      <c r="B28" s="103" t="s">
-        <v>44</v>
-      </c>
-      <c r="C28" s="68"/>
-      <c r="D28" s="60" t="s">
-        <v>84</v>
-      </c>
-      <c r="E28" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F28" s="114"/>
-      <c r="G28" s="60">
-        <v>450</v>
-      </c>
-      <c r="H28" s="62" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="103"/>
-      <c r="B29" s="103" t="s">
-        <v>44</v>
-      </c>
-      <c r="C29" s="68"/>
-      <c r="D29" s="60" t="s">
-        <v>86</v>
-      </c>
-      <c r="E29" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F29" s="114"/>
-      <c r="G29" s="60">
-        <v>3600</v>
-      </c>
-      <c r="H29" s="62" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="103"/>
-      <c r="B30" s="103"/>
-      <c r="C30" s="68"/>
-      <c r="D30" s="60"/>
-      <c r="E30" s="61"/>
-      <c r="F30" s="114"/>
-      <c r="G30" s="60"/>
-      <c r="H30" s="62"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="104"/>
-      <c r="B31" s="104"/>
-      <c r="C31" s="68">
-        <v>3</v>
-      </c>
-      <c r="D31" s="60" t="s">
-        <v>88</v>
-      </c>
-      <c r="E31" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F31" s="115" t="s">
-        <v>275</v>
-      </c>
-      <c r="G31" s="69" t="s">
-        <v>89</v>
-      </c>
-      <c r="H31" s="62" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="104"/>
-      <c r="B32" s="104"/>
-      <c r="C32" s="68"/>
-      <c r="D32" s="60" t="s">
-        <v>91</v>
-      </c>
-      <c r="E32" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F32" s="114">
-        <v>2.06</v>
-      </c>
-      <c r="G32" s="60">
-        <v>1.234</v>
-      </c>
-      <c r="H32" s="62" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="104"/>
-      <c r="B33" s="104" t="s">
-        <v>44</v>
-      </c>
-      <c r="C33" s="68"/>
-      <c r="D33" s="60" t="s">
-        <v>93</v>
-      </c>
-      <c r="E33" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F33" s="114">
-        <v>1.33</v>
-      </c>
-      <c r="G33" s="60">
-        <v>5.6779999999999999</v>
-      </c>
-      <c r="H33" s="62" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="104"/>
-      <c r="B34" s="104" t="s">
-        <v>44</v>
-      </c>
-      <c r="C34" s="68"/>
-      <c r="D34" s="60" t="s">
-        <v>95</v>
-      </c>
-      <c r="E34" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F34" s="114">
-        <v>1.2</v>
-      </c>
-      <c r="G34" s="60">
-        <v>9.0120000000000005</v>
-      </c>
-      <c r="H34" s="62" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="104"/>
-      <c r="B35" s="104" t="s">
-        <v>44</v>
-      </c>
-      <c r="C35" s="72"/>
-      <c r="D35" s="60" t="s">
-        <v>97</v>
-      </c>
-      <c r="E35" s="73" t="s">
-        <v>20</v>
-      </c>
-      <c r="F35" s="115"/>
-      <c r="G35" s="69"/>
-      <c r="H35" s="74" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="104"/>
-      <c r="B36" s="104" t="s">
-        <v>44</v>
-      </c>
-      <c r="C36" s="68"/>
-      <c r="D36" s="60" t="s">
-        <v>100</v>
-      </c>
-      <c r="E36" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F36" s="114"/>
-      <c r="G36" s="60">
-        <v>75</v>
-      </c>
-      <c r="H36" s="62" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="104"/>
-      <c r="B37" s="104" t="s">
-        <v>44</v>
-      </c>
-      <c r="C37" s="68"/>
-      <c r="D37" s="60" t="s">
-        <v>102</v>
-      </c>
-      <c r="E37" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F37" s="114"/>
-      <c r="G37" s="60">
-        <v>450</v>
-      </c>
-      <c r="H37" s="62" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="104"/>
-      <c r="B38" s="104" t="s">
-        <v>44</v>
-      </c>
-      <c r="C38" s="68"/>
-      <c r="D38" s="60" t="s">
-        <v>104</v>
-      </c>
-      <c r="E38" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F38" s="114"/>
-      <c r="G38" s="60">
-        <v>3600</v>
-      </c>
-      <c r="H38" s="62" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="103"/>
-      <c r="B39" s="103"/>
-      <c r="C39" s="68"/>
-      <c r="D39" s="60"/>
-      <c r="E39" s="61"/>
-      <c r="F39" s="114"/>
-      <c r="G39" s="60"/>
-      <c r="H39" s="62"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="104"/>
-      <c r="B40" s="104"/>
-      <c r="C40" s="68">
-        <v>4</v>
-      </c>
-      <c r="D40" s="60" t="s">
-        <v>106</v>
-      </c>
-      <c r="E40" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F40" s="115" t="s">
-        <v>274</v>
-      </c>
-      <c r="G40" s="69" t="s">
-        <v>71</v>
-      </c>
-      <c r="H40" s="62" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="104"/>
-      <c r="B41" s="104"/>
-      <c r="C41" s="68"/>
-      <c r="D41" s="60" t="s">
-        <v>108</v>
-      </c>
-      <c r="E41" s="73" t="s">
-        <v>20</v>
-      </c>
-      <c r="F41" s="115">
-        <v>1.18</v>
-      </c>
-      <c r="G41" s="60">
-        <v>1.234</v>
-      </c>
-      <c r="H41" s="62" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42" s="104"/>
-      <c r="B42" s="104"/>
-      <c r="C42" s="68"/>
-      <c r="D42" s="60" t="s">
-        <v>110</v>
-      </c>
-      <c r="E42" s="73" t="s">
-        <v>20</v>
-      </c>
-      <c r="F42" s="115">
-        <v>0.74</v>
-      </c>
-      <c r="G42" s="60">
-        <v>5.6779999999999999</v>
-      </c>
-      <c r="H42" s="62" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43" s="104"/>
-      <c r="B43" s="104" t="s">
-        <v>44</v>
-      </c>
-      <c r="C43" s="68"/>
-      <c r="D43" s="60" t="s">
-        <v>112</v>
-      </c>
-      <c r="E43" s="73" t="s">
-        <v>20</v>
-      </c>
-      <c r="F43" s="114"/>
-      <c r="G43" s="60">
-        <v>9.0120000000000005</v>
-      </c>
-      <c r="H43" s="62"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44" s="104"/>
-      <c r="B44" s="104" t="s">
-        <v>44</v>
-      </c>
-      <c r="C44" s="72"/>
-      <c r="D44" s="60" t="s">
-        <v>113</v>
-      </c>
-      <c r="E44" s="73" t="s">
-        <v>20</v>
-      </c>
-      <c r="F44" s="115"/>
-      <c r="G44" s="69"/>
-      <c r="H44" s="74" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A45" s="104"/>
-      <c r="B45" s="104" t="s">
-        <v>44</v>
-      </c>
-      <c r="C45" s="68"/>
-      <c r="D45" s="60" t="s">
-        <v>115</v>
-      </c>
-      <c r="E45" s="73" t="s">
-        <v>20</v>
-      </c>
-      <c r="F45" s="114"/>
-      <c r="G45" s="60">
-        <v>75</v>
-      </c>
-      <c r="H45" s="62" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A46" s="104"/>
-      <c r="B46" s="104" t="s">
-        <v>44</v>
-      </c>
-      <c r="C46" s="68"/>
-      <c r="D46" s="60" t="s">
-        <v>116</v>
-      </c>
-      <c r="E46" s="73" t="s">
-        <v>20</v>
-      </c>
-      <c r="F46" s="114"/>
-      <c r="G46" s="60">
-        <v>450</v>
-      </c>
-      <c r="H46" s="62" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A47" s="104"/>
-      <c r="B47" s="104" t="s">
-        <v>44</v>
-      </c>
-      <c r="C47" s="68"/>
-      <c r="D47" s="60" t="s">
-        <v>117</v>
-      </c>
-      <c r="E47" s="73" t="s">
-        <v>20</v>
-      </c>
-      <c r="F47" s="114"/>
-      <c r="G47" s="60">
-        <v>3600</v>
-      </c>
-      <c r="H47" s="62" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A48" s="103"/>
-      <c r="B48" s="103"/>
-      <c r="C48" s="68"/>
-      <c r="D48" s="60"/>
-      <c r="E48" s="61"/>
-      <c r="F48" s="114"/>
-      <c r="G48" s="60"/>
-      <c r="H48" s="62"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" s="103"/>
-      <c r="B49" s="103"/>
-      <c r="C49" s="68">
-        <v>5</v>
-      </c>
-      <c r="D49" s="60" t="s">
-        <v>118</v>
-      </c>
-      <c r="E49" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F49" s="115" t="s">
-        <v>274</v>
-      </c>
-      <c r="G49" s="69" t="s">
-        <v>89</v>
-      </c>
-      <c r="H49" s="62" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A50" s="104"/>
-      <c r="B50" s="104"/>
-      <c r="C50" s="72"/>
-      <c r="D50" s="60" t="s">
-        <v>121</v>
-      </c>
-      <c r="E50" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F50" s="115">
-        <v>1.42</v>
-      </c>
-      <c r="G50" s="60">
-        <v>1.234</v>
-      </c>
-      <c r="H50" s="62" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A51" s="104"/>
-      <c r="B51" s="104"/>
-      <c r="C51" s="72"/>
-      <c r="D51" s="60" t="s">
-        <v>123</v>
-      </c>
-      <c r="E51" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F51" s="115">
-        <v>1.06</v>
-      </c>
-      <c r="G51" s="60">
-        <v>5.6779999999999999</v>
-      </c>
-      <c r="H51" s="62" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A52" s="104"/>
-      <c r="B52" s="104" t="s">
-        <v>44</v>
-      </c>
-      <c r="C52" s="72"/>
-      <c r="D52" s="60" t="s">
-        <v>125</v>
-      </c>
-      <c r="E52" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F52" s="115" t="s">
-        <v>274</v>
-      </c>
-      <c r="G52" s="60">
-        <v>9.0120000000000005</v>
-      </c>
-      <c r="H52" s="62" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A53" s="104"/>
-      <c r="B53" s="104" t="s">
-        <v>44</v>
-      </c>
-      <c r="C53" s="72"/>
-      <c r="D53" s="69" t="s">
-        <v>127</v>
-      </c>
-      <c r="E53" s="73" t="s">
-        <v>20</v>
-      </c>
-      <c r="F53" s="115">
-        <v>1.42</v>
-      </c>
-      <c r="G53" s="69"/>
-      <c r="H53" s="74" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="104"/>
-      <c r="B54" s="104" t="s">
-        <v>44</v>
-      </c>
-      <c r="C54" s="72"/>
-      <c r="D54" s="60" t="s">
-        <v>129</v>
-      </c>
-      <c r="E54" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F54" s="115">
-        <v>1.06</v>
-      </c>
-      <c r="G54" s="60">
-        <v>75</v>
-      </c>
-      <c r="H54" s="62" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A55" s="104"/>
-      <c r="B55" s="104" t="s">
-        <v>44</v>
-      </c>
-      <c r="C55" s="72"/>
-      <c r="D55" s="60" t="s">
-        <v>130</v>
-      </c>
-      <c r="E55" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F55" s="115" t="s">
-        <v>274</v>
-      </c>
-      <c r="G55" s="60">
-        <v>450</v>
-      </c>
-      <c r="H55" s="62" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56" s="104"/>
-      <c r="B56" s="104" t="s">
-        <v>44</v>
-      </c>
-      <c r="C56" s="72"/>
-      <c r="D56" s="60" t="s">
-        <v>131</v>
-      </c>
-      <c r="E56" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F56" s="115">
-        <v>1.42</v>
-      </c>
-      <c r="G56" s="60">
-        <v>3600</v>
-      </c>
-      <c r="H56" s="62" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A57" s="103"/>
-      <c r="B57" s="103"/>
-      <c r="C57" s="68"/>
-      <c r="D57" s="60"/>
-      <c r="E57" s="61"/>
-      <c r="F57" s="114"/>
-      <c r="G57" s="60"/>
-      <c r="H57" s="62"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A58" s="103"/>
-      <c r="B58" s="103" t="s">
-        <v>44</v>
-      </c>
-      <c r="C58" s="68">
-        <v>6</v>
-      </c>
-      <c r="D58" s="60" t="s">
-        <v>132</v>
-      </c>
-      <c r="E58" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F58" s="115" t="s">
-        <v>274</v>
-      </c>
-      <c r="G58" s="69" t="s">
-        <v>71</v>
-      </c>
-      <c r="H58" s="62" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A59" s="103"/>
-      <c r="B59" s="103" t="s">
-        <v>44</v>
-      </c>
-      <c r="C59" s="68"/>
-      <c r="D59" s="60" t="s">
-        <v>134</v>
-      </c>
-      <c r="E59" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F59" s="115">
-        <v>1.42</v>
-      </c>
-      <c r="G59" s="60">
-        <v>1.234</v>
-      </c>
-      <c r="H59" s="62" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" s="103"/>
-      <c r="B60" s="103" t="s">
-        <v>44</v>
-      </c>
-      <c r="C60" s="68"/>
-      <c r="D60" s="60" t="s">
-        <v>136</v>
-      </c>
-      <c r="E60" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F60" s="115">
-        <v>1.06</v>
-      </c>
-      <c r="G60" s="60">
-        <v>5.6779999999999999</v>
-      </c>
-      <c r="H60" s="62" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A61" s="103"/>
-      <c r="B61" s="103" t="s">
-        <v>44</v>
-      </c>
-      <c r="C61" s="68"/>
-      <c r="D61" s="60" t="s">
-        <v>138</v>
-      </c>
-      <c r="E61" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F61" s="114"/>
-      <c r="G61" s="60">
-        <v>9.0120000000000005</v>
-      </c>
-      <c r="H61" s="62"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A62" s="103"/>
-      <c r="B62" s="103" t="s">
-        <v>44</v>
-      </c>
-      <c r="C62" s="68"/>
-      <c r="D62" s="69" t="s">
-        <v>139</v>
-      </c>
-      <c r="E62" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F62" s="114"/>
-      <c r="G62" s="60"/>
-      <c r="H62" s="62"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" s="103"/>
-      <c r="B63" s="103" t="s">
-        <v>44</v>
-      </c>
-      <c r="C63" s="68"/>
-      <c r="D63" s="60" t="s">
-        <v>140</v>
-      </c>
-      <c r="E63" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F63" s="114"/>
-      <c r="G63" s="60">
-        <v>75</v>
-      </c>
-      <c r="H63" s="62"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A64" s="103"/>
-      <c r="B64" s="103" t="s">
-        <v>44</v>
-      </c>
-      <c r="C64" s="68"/>
-      <c r="D64" s="60" t="s">
-        <v>141</v>
-      </c>
-      <c r="E64" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F64" s="114"/>
-      <c r="G64" s="60">
-        <v>450</v>
-      </c>
-      <c r="H64" s="62"/>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A65" s="103"/>
-      <c r="B65" s="103" t="s">
-        <v>44</v>
-      </c>
-      <c r="C65" s="68"/>
-      <c r="D65" s="60" t="s">
-        <v>142</v>
-      </c>
-      <c r="E65" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F65" s="114"/>
-      <c r="G65" s="60">
-        <v>3600</v>
-      </c>
-      <c r="H65" s="62"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A66" s="103"/>
-      <c r="B66" s="103"/>
-      <c r="C66" s="68"/>
-      <c r="D66" s="60"/>
-      <c r="E66" s="61"/>
-      <c r="F66" s="114"/>
-      <c r="G66" s="60"/>
-      <c r="H66" s="62"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A67" s="103"/>
-      <c r="B67" s="103"/>
-      <c r="C67" s="68">
-        <v>7</v>
-      </c>
-      <c r="D67" s="60" t="s">
-        <v>143</v>
-      </c>
-      <c r="E67" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F67" s="115" t="s">
-        <v>144</v>
-      </c>
-      <c r="G67" s="69" t="s">
-        <v>71</v>
-      </c>
-      <c r="H67" s="62" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A68" s="103"/>
-      <c r="B68" s="103" t="s">
-        <v>44</v>
-      </c>
-      <c r="C68" s="68"/>
-      <c r="D68" s="60" t="s">
-        <v>146</v>
-      </c>
-      <c r="E68" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F68" s="115">
-        <v>1.5</v>
-      </c>
-      <c r="G68" s="60">
-        <v>1.234</v>
-      </c>
-      <c r="H68" s="62" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A69" s="103"/>
-      <c r="B69" s="103" t="s">
-        <v>44</v>
-      </c>
-      <c r="C69" s="68"/>
-      <c r="D69" s="60" t="s">
-        <v>148</v>
-      </c>
-      <c r="E69" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F69" s="115">
-        <v>7.63</v>
-      </c>
-      <c r="G69" s="60">
-        <v>5.6779999999999999</v>
-      </c>
-      <c r="H69" s="62" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A70" s="103"/>
-      <c r="B70" s="103" t="str">
-        <f>B69</f>
-        <v>#</v>
-      </c>
-      <c r="C70" s="68"/>
-      <c r="D70" s="60" t="s">
-        <v>150</v>
-      </c>
-      <c r="E70" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F70" s="114"/>
-      <c r="G70" s="60">
-        <v>9.0120000000000005</v>
-      </c>
-      <c r="H70" s="62"/>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A71" s="103"/>
-      <c r="B71" s="103" t="s">
-        <v>44</v>
-      </c>
-      <c r="C71" s="68"/>
-      <c r="D71" s="60" t="s">
-        <v>151</v>
-      </c>
-      <c r="E71" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F71" s="114"/>
-      <c r="G71" s="69"/>
-      <c r="H71" s="62"/>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A72" s="103"/>
-      <c r="B72" s="103" t="s">
-        <v>44</v>
-      </c>
-      <c r="C72" s="68"/>
-      <c r="D72" s="60" t="s">
-        <v>152</v>
-      </c>
-      <c r="E72" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F72" s="114"/>
-      <c r="G72" s="60">
-        <v>75</v>
-      </c>
-      <c r="H72" s="62"/>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A73" s="103"/>
-      <c r="B73" s="103" t="s">
-        <v>44</v>
-      </c>
-      <c r="C73" s="68"/>
-      <c r="D73" s="60" t="s">
-        <v>153</v>
-      </c>
-      <c r="E73" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F73" s="114"/>
-      <c r="G73" s="60">
-        <v>450</v>
-      </c>
-      <c r="H73" s="62"/>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="103"/>
-      <c r="B74" s="103" t="s">
-        <v>44</v>
-      </c>
-      <c r="C74" s="68"/>
-      <c r="D74" s="60" t="s">
-        <v>154</v>
-      </c>
-      <c r="E74" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="F74" s="114"/>
-      <c r="G74" s="60">
-        <v>3600</v>
-      </c>
-      <c r="H74" s="62"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -36668,8 +36675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1063"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B149" sqref="B149"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -40766,9 +40773,9 @@
       <c r="Z108" s="4"/>
     </row>
     <row r="109" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="64">
+      <c r="A109" s="64" t="str">
         <f>'Old Reagents'!B31</f>
-        <v>0</v>
+        <v>#</v>
       </c>
       <c r="B109" s="60" t="s">
         <v>298</v>
@@ -40806,9 +40813,9 @@
       <c r="Z109" s="4"/>
     </row>
     <row r="110" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="64">
+      <c r="A110" s="64" t="str">
         <f>'Old Reagents'!B32</f>
-        <v>0</v>
+        <v>#</v>
       </c>
       <c r="B110" s="99" t="s">
         <v>299</v>
@@ -41126,7 +41133,7 @@
       </c>
       <c r="D118" s="69" t="str">
         <f>'Old Reagents'!F40</f>
-        <v>['PbI2','PyrrolidiniumIodide','DMSO']</v>
+        <v>['PbI2','PyrrolidiniumIodide','CBz']</v>
       </c>
       <c r="E118" s="60" t="s">
         <v>196</v>

</xml_diff>

<commit_message>
change template to copy that works with multistock
</commit_message>
<xml_diff>
--- a/HC_LBL_SpecificationInterface.xlsx
+++ b/HC_LBL_SpecificationInterface.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="User Interface" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1032" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1032" uniqueCount="341">
   <si>
     <t>Manual Well Number</t>
   </si>
@@ -1465,9 +1465,6 @@
       <t xml:space="preserve"> multistock sampling is only supported for use with the Wolfram Mathematica sampler</t>
     </r>
   </si>
-  <si>
-    <t>['PbI2','PyrrolidiniumIodide','CBz']</t>
-  </si>
 </sst>
 </file>
 
@@ -8787,7 +8784,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
@@ -9460,7 +9457,7 @@
         <v>20</v>
       </c>
       <c r="F40" s="115" t="s">
-        <v>341</v>
+        <v>274</v>
       </c>
       <c r="G40" s="69" t="s">
         <v>71</v>
@@ -36675,7 +36672,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1063"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
@@ -41133,7 +41130,7 @@
       </c>
       <c r="D118" s="69" t="str">
         <f>'Old Reagents'!F40</f>
-        <v>['PbI2','PyrrolidiniumIodide','CBz']</v>
+        <v>['PbI2','PyrrolidiniumIodide','DMSO']</v>
       </c>
       <c r="E118" s="60" t="s">
         <v>196</v>

</xml_diff>

<commit_message>
updated version numbers, small fixes to excel defaults-presentation
</commit_message>
<xml_diff>
--- a/HC_LBL_SpecificationInterface.xlsx
+++ b/HC_LBL_SpecificationInterface.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27417"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaeltynes/repos/ESCALATE_Capture/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ipendleton/Dropbox/Desktop/ESCALATE/ESCALATE_Capture/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4E55749-F998-D44B-A2B1-7BCF492B2217}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" activeTab="1"/>
+    <workbookView xWindow="4820" yWindow="2080" windowWidth="35360" windowHeight="24200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User Interface" sheetId="1" r:id="rId1"/>
@@ -26,7 +27,7 @@
     <definedName name="wellcount" localSheetId="0">'User Interface'!$E$6</definedName>
     <definedName name="wellcount">'WF1'!$D$7</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1032" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1039" uniqueCount="342">
   <si>
     <t>Manual Well Number</t>
   </si>
@@ -286,6 +287,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">ECL model ID.  </t>
     </r>
@@ -296,6 +298,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Cannot be used in with `Reagent#_chemical_list`</t>
     </r>
@@ -357,6 +360,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">ECL model ID.  </t>
     </r>
@@ -367,6 +371,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Cannot be used in with `Reagent#_chemical_list`</t>
     </r>
@@ -422,6 +427,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">ECL model ID.  </t>
     </r>
@@ -432,6 +438,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Cannot be used in with `Reagent#_chemical_list`</t>
     </r>
@@ -481,6 +488,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">ECL model ID.  </t>
     </r>
@@ -491,6 +499,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Cannot be used in with `Reagent#_chemical_list`</t>
     </r>
@@ -737,6 +746,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Materials (</t>
     </r>
@@ -746,6 +756,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Chemicals</t>
     </r>
@@ -754,6 +765,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>)</t>
     </r>
@@ -766,6 +778,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>chem</t>
     </r>
@@ -774,6 +787,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>2_molarmin</t>
     </r>
@@ -786,6 +800,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>chem</t>
     </r>
@@ -794,6 +809,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>2_molarmax</t>
     </r>
@@ -804,6 +820,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Reagent1_</t>
     </r>
@@ -814,6 +831,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>chemical</t>
     </r>
@@ -822,6 +840,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>_list</t>
     </r>
@@ -853,6 +872,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Reagent2_</t>
     </r>
@@ -863,6 +883,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>chemical</t>
     </r>
@@ -871,6 +892,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>_list</t>
     </r>
@@ -902,6 +924,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Reagent3_</t>
     </r>
@@ -912,6 +935,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>chemical</t>
     </r>
@@ -920,6 +944,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>_list</t>
     </r>
@@ -951,6 +976,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Reagent4_</t>
     </r>
@@ -961,6 +987,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>chemical</t>
     </r>
@@ -969,6 +996,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>_list</t>
     </r>
@@ -1000,6 +1028,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Reagent5_</t>
     </r>
@@ -1010,6 +1039,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>chemical</t>
     </r>
@@ -1018,6 +1048,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>_list</t>
     </r>
@@ -1049,6 +1080,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Reagent6_</t>
     </r>
@@ -1059,6 +1091,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>chemical</t>
     </r>
@@ -1067,6 +1100,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>_list</t>
     </r>
@@ -1098,6 +1132,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Reagent7_</t>
     </r>
@@ -1108,6 +1143,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>chemical</t>
     </r>
@@ -1116,6 +1152,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>_list</t>
     </r>
@@ -1163,16 +1200,7 @@
     <t>LBL</t>
   </si>
   <si>
-    <t>['DMSO']</t>
-  </si>
-  <si>
     <t>['PbI2','PyrrolidiniumIodide','DMSO']</t>
-  </si>
-  <si>
-    <t>['PyrrolidiniumIodide','DMSO']</t>
-  </si>
-  <si>
-    <t>[[2,3,4,5,1,7]]</t>
   </si>
   <si>
     <t xml:space="preserve">This sheet is used for "Multi Stock Sampling". That is, if you have developed new reagents for reactions in the same chemical space, </t>
@@ -1187,6 +1215,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>H</t>
     </r>
@@ -1195,6 +1224,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> in chemical concentration space and your new reagents define a convex hull </t>
     </r>
@@ -1204,6 +1234,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>G</t>
     </r>
@@ -1212,6 +1243,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>,</t>
     </r>
@@ -1229,6 +1261,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">newly accessible </t>
     </r>
@@ -1237,6 +1270,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>by your new reagents.</t>
     </r>
@@ -1251,6 +1285,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>G</t>
     </r>
@@ -1259,6 +1294,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> but not in </t>
     </r>
@@ -1268,6 +1304,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>H.</t>
     </r>
@@ -1435,16 +1472,10 @@
     <t>OldReagent7_prep_duration</t>
   </si>
   <si>
-    <t>Multi Stock Sampling</t>
-  </si>
-  <si>
     <t>multi_stock_sampling</t>
   </si>
   <si>
     <t>Oldreagent3_ID</t>
-  </si>
-  <si>
-    <t>Yes</t>
   </si>
   <si>
     <r>
@@ -1453,6 +1484,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>NOTE:</t>
     </r>
@@ -1461,16 +1493,35 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> multistock sampling is only supported for use with the Wolfram Mathematica sampler</t>
     </r>
+  </si>
+  <si>
+    <t>Subtract Region of Previous Solutions?</t>
+  </si>
+  <si>
+    <t>['GBL']</t>
+  </si>
+  <si>
+    <t>['PbI2','EtNH3I','GBL']</t>
+  </si>
+  <si>
+    <t>['EtNH3I','GBL']</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>[[2,3,1,7]]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="23" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1480,11 +1531,13 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1492,6 +1545,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1499,6 +1553,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
@@ -1506,12 +1561,14 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
@@ -1519,12 +1576,14 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1532,30 +1591,35 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1563,6 +1627,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1570,6 +1635,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1577,42 +1643,55 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="24"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="11">
@@ -1841,7 +1920,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2197,6 +2276,28 @@
     <xf numFmtId="0" fontId="18" fillId="4" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2412,11 +2513,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" zoomScale="109" zoomScaleNormal="109" zoomScalePageLayoutView="109" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="109" zoomScalePageLayoutView="109" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -2615,7 +2716,7 @@
       <c r="D6" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="109">
+      <c r="E6" s="131">
         <f>SUM(E12,E17,E20)</f>
         <v>96</v>
       </c>
@@ -2691,7 +2792,7 @@
         <v>20</v>
       </c>
       <c r="E8" s="109" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="F8" s="28"/>
       <c r="G8" s="124"/>
@@ -2756,8 +2857,8 @@
       <c r="D10" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="111" t="s">
-        <v>276</v>
+      <c r="E10" s="132" t="s">
+        <v>341</v>
       </c>
       <c r="F10" s="41" t="s">
         <v>34</v>
@@ -3189,7 +3290,7 @@
         <v>20</v>
       </c>
       <c r="E23" s="115" t="s">
-        <v>273</v>
+        <v>337</v>
       </c>
       <c r="F23" s="69" t="s">
         <v>60</v>
@@ -3219,7 +3320,7 @@
       <c r="Y23" s="19"/>
       <c r="Z23" s="19"/>
     </row>
-    <row r="24" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A24" s="104" t="s">
         <v>44</v>
       </c>
@@ -3253,7 +3354,7 @@
       <c r="Y24" s="19"/>
       <c r="Z24" s="19"/>
     </row>
-    <row r="25" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A25" s="104" t="s">
         <v>44</v>
       </c>
@@ -3291,7 +3392,7 @@
       <c r="Y25" s="19"/>
       <c r="Z25" s="19"/>
     </row>
-    <row r="26" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A26" s="104" t="s">
         <v>44</v>
       </c>
@@ -3329,7 +3430,7 @@
       <c r="Y26" s="19"/>
       <c r="Z26" s="19"/>
     </row>
-    <row r="27" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A27" s="104" t="s">
         <v>44</v>
       </c>
@@ -3365,7 +3466,7 @@
       <c r="Y27" s="19"/>
       <c r="Z27" s="19"/>
     </row>
-    <row r="28" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A28" s="103" t="s">
         <v>44</v>
       </c>
@@ -3401,7 +3502,7 @@
       <c r="Y28" s="19"/>
       <c r="Z28" s="19"/>
     </row>
-    <row r="29" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A29" s="103" t="s">
         <v>44</v>
       </c>
@@ -3437,7 +3538,7 @@
       <c r="Y29" s="19"/>
       <c r="Z29" s="19"/>
     </row>
-    <row r="30" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A30" s="103" t="s">
         <v>44</v>
       </c>
@@ -3473,7 +3574,7 @@
       <c r="Y30" s="19"/>
       <c r="Z30" s="19"/>
     </row>
-    <row r="31" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:26" ht="18.75" customHeight="1" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A31" s="103"/>
       <c r="B31" s="68"/>
       <c r="C31" s="60"/>
@@ -3512,8 +3613,8 @@
       <c r="D32" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="E32" s="115" t="s">
-        <v>274</v>
+      <c r="E32" s="127" t="s">
+        <v>338</v>
       </c>
       <c r="F32" s="69" t="s">
         <v>71</v>
@@ -3553,7 +3654,7 @@
         <v>20</v>
       </c>
       <c r="E33" s="115">
-        <v>1.55</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F33" s="60">
         <v>1.234</v>
@@ -3591,7 +3692,7 @@
         <v>20</v>
       </c>
       <c r="E34" s="115">
-        <v>1.93</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F34" s="60">
         <v>5.6779999999999999</v>
@@ -3619,7 +3720,7 @@
       <c r="Y34" s="19"/>
       <c r="Z34" s="19"/>
     </row>
-    <row r="35" spans="1:26" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:26" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A35" s="104" t="s">
         <v>44</v>
       </c>
@@ -3655,7 +3756,7 @@
       <c r="Y35" s="19"/>
       <c r="Z35" s="19"/>
     </row>
-    <row r="36" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A36" s="104" t="s">
         <v>44</v>
       </c>
@@ -3693,7 +3794,7 @@
       <c r="Y36" s="19"/>
       <c r="Z36" s="19"/>
     </row>
-    <row r="37" spans="1:26" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:26" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A37" s="103" t="s">
         <v>44</v>
       </c>
@@ -3733,7 +3834,7 @@
       <c r="Y37" s="19"/>
       <c r="Z37" s="19"/>
     </row>
-    <row r="38" spans="1:26" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:26" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A38" s="103" t="s">
         <v>44</v>
       </c>
@@ -3773,7 +3874,7 @@
       <c r="Y38" s="19"/>
       <c r="Z38" s="19"/>
     </row>
-    <row r="39" spans="1:26" ht="15.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:26" ht="15.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A39" s="103" t="s">
         <v>44</v>
       </c>
@@ -3813,7 +3914,7 @@
       <c r="Y39" s="19"/>
       <c r="Z39" s="19"/>
     </row>
-    <row r="40" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:26" ht="18" customHeight="1" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A40" s="103"/>
       <c r="B40" s="68"/>
       <c r="C40" s="60"/>
@@ -3852,8 +3953,8 @@
       <c r="D41" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="E41" s="115" t="s">
-        <v>275</v>
+      <c r="E41" s="127" t="s">
+        <v>339</v>
       </c>
       <c r="F41" s="69" t="s">
         <v>89</v>
@@ -3891,7 +3992,7 @@
         <v>20</v>
       </c>
       <c r="E42" s="114">
-        <v>2.06</v>
+        <v>4</v>
       </c>
       <c r="F42" s="60">
         <v>1.234</v>
@@ -3919,7 +4020,7 @@
       <c r="Y42" s="19"/>
       <c r="Z42" s="19"/>
     </row>
-    <row r="43" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A43" s="104" t="s">
         <v>44</v>
       </c>
@@ -3930,9 +4031,7 @@
       <c r="D43" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="E43" s="114">
-        <v>1.33</v>
-      </c>
+      <c r="E43" s="114"/>
       <c r="F43" s="60">
         <v>5.6779999999999999</v>
       </c>
@@ -3959,7 +4058,7 @@
       <c r="Y43" s="19"/>
       <c r="Z43" s="19"/>
     </row>
-    <row r="44" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A44" s="104" t="s">
         <v>44</v>
       </c>
@@ -3970,9 +4069,7 @@
       <c r="D44" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="E44" s="114">
-        <v>1.2</v>
-      </c>
+      <c r="E44" s="114"/>
       <c r="F44" s="60">
         <v>9.0120000000000005</v>
       </c>
@@ -3999,7 +4096,7 @@
       <c r="Y44" s="19"/>
       <c r="Z44" s="19"/>
     </row>
-    <row r="45" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A45" s="104" t="s">
         <v>44</v>
       </c>
@@ -4037,7 +4134,7 @@
       <c r="Y45" s="19"/>
       <c r="Z45" s="19"/>
     </row>
-    <row r="46" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A46" s="104" t="s">
         <v>44</v>
       </c>
@@ -4077,7 +4174,7 @@
       <c r="Y46" s="19"/>
       <c r="Z46" s="19"/>
     </row>
-    <row r="47" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A47" s="104" t="s">
         <v>44</v>
       </c>
@@ -4117,7 +4214,7 @@
       <c r="Y47" s="19"/>
       <c r="Z47" s="19"/>
     </row>
-    <row r="48" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A48" s="104" t="s">
         <v>44</v>
       </c>
@@ -4157,7 +4254,7 @@
       <c r="Y48" s="19"/>
       <c r="Z48" s="19"/>
     </row>
-    <row r="49" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:26" ht="18.75" customHeight="1" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A49" s="103"/>
       <c r="B49" s="68"/>
       <c r="C49" s="60"/>
@@ -4186,7 +4283,9 @@
       <c r="Z49" s="19"/>
     </row>
     <row r="50" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="104"/>
+      <c r="A50" s="130" t="s">
+        <v>44</v>
+      </c>
       <c r="B50" s="68">
         <v>4</v>
       </c>
@@ -4196,8 +4295,8 @@
       <c r="D50" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="E50" s="115" t="s">
-        <v>274</v>
+      <c r="E50" s="127" t="s">
+        <v>338</v>
       </c>
       <c r="F50" s="69" t="s">
         <v>71</v>
@@ -4226,7 +4325,9 @@
       <c r="Z50" s="19"/>
     </row>
     <row r="51" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="104"/>
+      <c r="A51" s="130" t="s">
+        <v>44</v>
+      </c>
       <c r="B51" s="68"/>
       <c r="C51" s="60" t="s">
         <v>108</v>
@@ -4235,7 +4336,7 @@
         <v>20</v>
       </c>
       <c r="E51" s="115">
-        <v>1.18</v>
+        <v>1</v>
       </c>
       <c r="F51" s="60">
         <v>1.234</v>
@@ -4264,7 +4365,9 @@
       <c r="Z51" s="19"/>
     </row>
     <row r="52" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="104"/>
+      <c r="A52" s="130" t="s">
+        <v>44</v>
+      </c>
       <c r="B52" s="68"/>
       <c r="C52" s="60" t="s">
         <v>110</v>
@@ -4273,7 +4376,7 @@
         <v>20</v>
       </c>
       <c r="E52" s="115">
-        <v>0.74</v>
+        <v>1.3</v>
       </c>
       <c r="F52" s="60">
         <v>5.6779999999999999</v>
@@ -4301,7 +4404,7 @@
       <c r="Y52" s="19"/>
       <c r="Z52" s="19"/>
     </row>
-    <row r="53" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A53" s="104" t="s">
         <v>44</v>
       </c>
@@ -4337,7 +4440,7 @@
       <c r="Y53" s="19"/>
       <c r="Z53" s="19"/>
     </row>
-    <row r="54" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A54" s="104" t="s">
         <v>44</v>
       </c>
@@ -4375,7 +4478,7 @@
       <c r="Y54" s="19"/>
       <c r="Z54" s="19"/>
     </row>
-    <row r="55" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A55" s="104" t="s">
         <v>44</v>
       </c>
@@ -4415,7 +4518,7 @@
       <c r="Y55" s="19"/>
       <c r="Z55" s="19"/>
     </row>
-    <row r="56" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A56" s="104" t="s">
         <v>44</v>
       </c>
@@ -4455,7 +4558,7 @@
       <c r="Y56" s="19"/>
       <c r="Z56" s="19"/>
     </row>
-    <row r="57" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A57" s="104" t="s">
         <v>44</v>
       </c>
@@ -4495,7 +4598,7 @@
       <c r="Y57" s="19"/>
       <c r="Z57" s="19"/>
     </row>
-    <row r="58" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:26" ht="18.75" customHeight="1" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A58" s="103"/>
       <c r="B58" s="68"/>
       <c r="C58" s="60"/>
@@ -4524,7 +4627,9 @@
       <c r="Z58" s="19"/>
     </row>
     <row r="59" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="103"/>
+      <c r="A59" s="129" t="s">
+        <v>44</v>
+      </c>
       <c r="B59" s="68">
         <v>5</v>
       </c>
@@ -4534,8 +4639,8 @@
       <c r="D59" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="115" t="s">
-        <v>274</v>
+      <c r="E59" s="127" t="s">
+        <v>338</v>
       </c>
       <c r="F59" s="69" t="s">
         <v>89</v>
@@ -4566,7 +4671,9 @@
       <c r="Z59" s="19"/>
     </row>
     <row r="60" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="104"/>
+      <c r="A60" s="130" t="s">
+        <v>44</v>
+      </c>
       <c r="B60" s="72"/>
       <c r="C60" s="60" t="s">
         <v>121</v>
@@ -4575,7 +4682,7 @@
         <v>20</v>
       </c>
       <c r="E60" s="115">
-        <v>1.42</v>
+        <v>0.9</v>
       </c>
       <c r="F60" s="60">
         <v>1.234</v>
@@ -4604,7 +4711,9 @@
       <c r="Z60" s="19"/>
     </row>
     <row r="61" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="104"/>
+      <c r="A61" s="130" t="s">
+        <v>44</v>
+      </c>
       <c r="B61" s="72"/>
       <c r="C61" s="60" t="s">
         <v>123</v>
@@ -4613,7 +4722,7 @@
         <v>20</v>
       </c>
       <c r="E61" s="115">
-        <v>1.06</v>
+        <v>0.5</v>
       </c>
       <c r="F61" s="60">
         <v>5.6779999999999999</v>
@@ -4641,7 +4750,7 @@
       <c r="Y61" s="19"/>
       <c r="Z61" s="19"/>
     </row>
-    <row r="62" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A62" s="104" t="s">
         <v>44</v>
       </c>
@@ -4652,9 +4761,7 @@
       <c r="D62" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="E62" s="115" t="s">
-        <v>274</v>
-      </c>
+      <c r="E62" s="115"/>
       <c r="F62" s="60">
         <v>9.0120000000000005</v>
       </c>
@@ -4681,7 +4788,7 @@
       <c r="Y62" s="19"/>
       <c r="Z62" s="19"/>
     </row>
-    <row r="63" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A63" s="104" t="s">
         <v>44</v>
       </c>
@@ -4721,7 +4828,7 @@
       <c r="Y63" s="19"/>
       <c r="Z63" s="19"/>
     </row>
-    <row r="64" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A64" s="104" t="s">
         <v>44</v>
       </c>
@@ -4763,7 +4870,7 @@
       <c r="Y64" s="19"/>
       <c r="Z64" s="19"/>
     </row>
-    <row r="65" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A65" s="104" t="s">
         <v>44</v>
       </c>
@@ -4774,9 +4881,7 @@
       <c r="D65" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="E65" s="115" t="s">
-        <v>274</v>
-      </c>
+      <c r="E65" s="115"/>
       <c r="F65" s="60">
         <v>450</v>
       </c>
@@ -4805,7 +4910,7 @@
       <c r="Y65" s="19"/>
       <c r="Z65" s="19"/>
     </row>
-    <row r="66" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A66" s="104" t="s">
         <v>44</v>
       </c>
@@ -4847,7 +4952,7 @@
       <c r="Y66" s="19"/>
       <c r="Z66" s="19"/>
     </row>
-    <row r="67" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:26" ht="18.75" customHeight="1" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A67" s="103"/>
       <c r="B67" s="68"/>
       <c r="C67" s="60"/>
@@ -4876,7 +4981,7 @@
       <c r="Z67" s="19"/>
     </row>
     <row r="68" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="103" t="s">
+      <c r="A68" s="129" t="s">
         <v>44</v>
       </c>
       <c r="B68" s="68">
@@ -4888,9 +4993,7 @@
       <c r="D68" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="E68" s="115" t="s">
-        <v>274</v>
-      </c>
+      <c r="E68" s="127"/>
       <c r="F68" s="69" t="s">
         <v>71</v>
       </c>
@@ -4918,7 +5021,7 @@
       <c r="Z68" s="19"/>
     </row>
     <row r="69" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="103" t="s">
+      <c r="A69" s="129" t="s">
         <v>44</v>
       </c>
       <c r="B69" s="68"/>
@@ -4929,7 +5032,7 @@
         <v>20</v>
       </c>
       <c r="E69" s="115">
-        <v>1.42</v>
+        <v>1.5</v>
       </c>
       <c r="F69" s="60">
         <v>1.234</v>
@@ -4958,7 +5061,7 @@
       <c r="Z69" s="19"/>
     </row>
     <row r="70" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="103" t="s">
+      <c r="A70" s="129" t="s">
         <v>44</v>
       </c>
       <c r="B70" s="68"/>
@@ -4969,7 +5072,7 @@
         <v>20</v>
       </c>
       <c r="E70" s="115">
-        <v>1.06</v>
+        <v>6</v>
       </c>
       <c r="F70" s="60">
         <v>5.6779999999999999</v>
@@ -4997,7 +5100,7 @@
       <c r="Y70" s="19"/>
       <c r="Z70" s="19"/>
     </row>
-    <row r="71" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A71" s="103" t="s">
         <v>44</v>
       </c>
@@ -5033,7 +5136,7 @@
       <c r="Y71" s="19"/>
       <c r="Z71" s="19"/>
     </row>
-    <row r="72" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A72" s="103" t="s">
         <v>44</v>
       </c>
@@ -5069,7 +5172,7 @@
       <c r="Y72" s="19"/>
       <c r="Z72" s="19"/>
     </row>
-    <row r="73" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A73" s="103" t="s">
         <v>44</v>
       </c>
@@ -5107,7 +5210,7 @@
       <c r="Y73" s="19"/>
       <c r="Z73" s="19"/>
     </row>
-    <row r="74" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A74" s="103" t="s">
         <v>44</v>
       </c>
@@ -5145,7 +5248,7 @@
       <c r="Y74" s="19"/>
       <c r="Z74" s="19"/>
     </row>
-    <row r="75" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A75" s="103" t="s">
         <v>44</v>
       </c>
@@ -5183,7 +5286,7 @@
       <c r="Y75" s="19"/>
       <c r="Z75" s="19"/>
     </row>
-    <row r="76" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:26" ht="18.75" customHeight="1" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A76" s="103"/>
       <c r="B76" s="68"/>
       <c r="C76" s="60"/>
@@ -5251,7 +5354,7 @@
       <c r="Y77" s="19"/>
       <c r="Z77" s="19"/>
     </row>
-    <row r="78" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A78" s="103" t="s">
         <v>44</v>
       </c>
@@ -5262,9 +5365,7 @@
       <c r="D78" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="E78" s="115">
-        <v>1.5</v>
-      </c>
+      <c r="E78" s="115"/>
       <c r="F78" s="60">
         <v>1.234</v>
       </c>
@@ -5291,7 +5392,7 @@
       <c r="Y78" s="19"/>
       <c r="Z78" s="19"/>
     </row>
-    <row r="79" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A79" s="103" t="s">
         <v>44</v>
       </c>
@@ -5302,9 +5403,7 @@
       <c r="D79" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="E79" s="115">
-        <v>7.63</v>
-      </c>
+      <c r="E79" s="115"/>
       <c r="F79" s="60">
         <v>5.6779999999999999</v>
       </c>
@@ -5331,8 +5430,8 @@
       <c r="Y79" s="19"/>
       <c r="Z79" s="19"/>
     </row>
-    <row r="80" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="103" t="str">
+    <row r="80" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="128" t="str">
         <f>A79</f>
         <v>#</v>
       </c>
@@ -5368,7 +5467,7 @@
       <c r="Y80" s="19"/>
       <c r="Z80" s="19"/>
     </row>
-    <row r="81" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A81" s="103" t="s">
         <v>44</v>
       </c>
@@ -5404,7 +5503,7 @@
       <c r="Y81" s="19"/>
       <c r="Z81" s="19"/>
     </row>
-    <row r="82" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A82" s="103" t="s">
         <v>44</v>
       </c>
@@ -5442,7 +5541,7 @@
       <c r="Y82" s="19"/>
       <c r="Z82" s="19"/>
     </row>
-    <row r="83" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A83" s="103" t="s">
         <v>44</v>
       </c>
@@ -5480,7 +5579,7 @@
       <c r="Y83" s="19"/>
       <c r="Z83" s="19"/>
     </row>
-    <row r="84" spans="1:26" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:26" ht="18.75" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A84" s="103" t="s">
         <v>44</v>
       </c>
@@ -5518,7 +5617,7 @@
       <c r="Y84" s="19"/>
       <c r="Z84" s="19"/>
     </row>
-    <row r="85" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:26" ht="18.75" customHeight="1" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A85" s="77" t="s">
         <v>155</v>
       </c>
@@ -8756,24 +8855,24 @@
   </sheetData>
   <sheetProtection formatRows="0"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E4">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E4" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"MIT_PVLab,HC,LBL,dev"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E3">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E3" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"1.1,3.0"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E8" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="C20" location="Manual Experiment Interface!B2" display="Manual Experiments"/>
-    <hyperlink ref="H22" r:id="rId1"/>
-    <hyperlink ref="H23" r:id="rId2"/>
-    <hyperlink ref="H36" r:id="rId3"/>
-    <hyperlink ref="H45" r:id="rId4"/>
-    <hyperlink ref="H54" r:id="rId5"/>
-    <hyperlink ref="C8" location="'Old Reagents'!A1" display="Multi Stock Sampling"/>
+    <hyperlink ref="C20" location="Manual Experiment Interface!B2" display="Manual Experiments" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="H22" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="H23" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="H36" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="H45" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="H54" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C8" location="'Old Reagents'!A1" display="Multi Stock Sampling" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -8781,11 +8880,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38:E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8800,7 +8899,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="31" x14ac:dyDescent="0.35">
       <c r="A1" s="120" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B1" s="118"/>
       <c r="C1" s="118"/>
@@ -8822,7 +8921,7 @@
     </row>
     <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="119" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B3" s="118"/>
       <c r="C3" s="118"/>
@@ -8834,7 +8933,7 @@
     </row>
     <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="119" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B4" s="118"/>
       <c r="C4" s="118"/>
@@ -8856,7 +8955,7 @@
     </row>
     <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="119" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B6" s="118"/>
       <c r="C6" s="118"/>
@@ -8868,7 +8967,7 @@
     </row>
     <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="119" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B7" s="118"/>
       <c r="C7" s="118"/>
@@ -8890,7 +8989,7 @@
     </row>
     <row r="9" spans="1:8" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="119" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="B9" s="118"/>
       <c r="C9" s="118"/>
@@ -8922,7 +9021,7 @@
       <c r="G11" s="60"/>
       <c r="H11" s="62"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="103"/>
       <c r="B12" s="103" t="s">
         <v>44</v>
@@ -8951,7 +9050,7 @@
         <v>20</v>
       </c>
       <c r="F13" s="115" t="s">
-        <v>273</v>
+        <v>337</v>
       </c>
       <c r="G13" s="69" t="s">
         <v>60</v>
@@ -9110,8 +9209,8 @@
       <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="115" t="s">
-        <v>274</v>
+      <c r="F22" s="127" t="s">
+        <v>338</v>
       </c>
       <c r="G22" s="69" t="s">
         <v>71</v>
@@ -9131,7 +9230,7 @@
         <v>20</v>
       </c>
       <c r="F23" s="115">
-        <v>1.55</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G23" s="60">
         <v>1.234</v>
@@ -9151,7 +9250,7 @@
         <v>20</v>
       </c>
       <c r="F24" s="115">
-        <v>1.93</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="G24" s="60">
         <v>5.6779999999999999</v>
@@ -9268,9 +9367,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="104"/>
-      <c r="B31" s="104" t="s">
-        <v>44</v>
-      </c>
+      <c r="B31" s="104"/>
       <c r="C31" s="68">
         <v>3</v>
       </c>
@@ -9280,8 +9377,8 @@
       <c r="E31" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F31" s="115" t="s">
-        <v>275</v>
+      <c r="F31" s="127" t="s">
+        <v>339</v>
       </c>
       <c r="G31" s="69" t="s">
         <v>89</v>
@@ -9292,9 +9389,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="104"/>
-      <c r="B32" s="104" t="s">
-        <v>44</v>
-      </c>
+      <c r="B32" s="104"/>
       <c r="C32" s="68"/>
       <c r="D32" s="60" t="s">
         <v>91</v>
@@ -9303,7 +9398,7 @@
         <v>20</v>
       </c>
       <c r="F32" s="114">
-        <v>2.06</v>
+        <v>4</v>
       </c>
       <c r="G32" s="60">
         <v>1.234</v>
@@ -9314,7 +9409,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="104"/>
-      <c r="B33" s="104" t="s">
+      <c r="B33" s="130" t="s">
         <v>44</v>
       </c>
       <c r="C33" s="68"/>
@@ -9446,7 +9541,9 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="104"/>
-      <c r="B40" s="104"/>
+      <c r="B40" s="130" t="s">
+        <v>44</v>
+      </c>
       <c r="C40" s="68">
         <v>4</v>
       </c>
@@ -9457,7 +9554,7 @@
         <v>20</v>
       </c>
       <c r="F40" s="115" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G40" s="69" t="s">
         <v>71</v>
@@ -9468,7 +9565,9 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="104"/>
-      <c r="B41" s="104"/>
+      <c r="B41" s="130" t="s">
+        <v>44</v>
+      </c>
       <c r="C41" s="68"/>
       <c r="D41" s="60" t="s">
         <v>108</v>
@@ -9488,7 +9587,9 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="104"/>
-      <c r="B42" s="104"/>
+      <c r="B42" s="130" t="s">
+        <v>44</v>
+      </c>
       <c r="C42" s="68"/>
       <c r="D42" s="60" t="s">
         <v>110</v>
@@ -9614,7 +9715,9 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="103"/>
-      <c r="B49" s="103"/>
+      <c r="B49" s="129" t="s">
+        <v>44</v>
+      </c>
       <c r="C49" s="68">
         <v>5</v>
       </c>
@@ -9625,7 +9728,7 @@
         <v>20</v>
       </c>
       <c r="F49" s="115" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G49" s="69" t="s">
         <v>89</v>
@@ -9636,7 +9739,9 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="104"/>
-      <c r="B50" s="104"/>
+      <c r="B50" s="130" t="s">
+        <v>44</v>
+      </c>
       <c r="C50" s="72"/>
       <c r="D50" s="60" t="s">
         <v>121</v>
@@ -9656,7 +9761,9 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="104"/>
-      <c r="B51" s="104"/>
+      <c r="B51" s="130" t="s">
+        <v>44</v>
+      </c>
       <c r="C51" s="72"/>
       <c r="D51" s="60" t="s">
         <v>123</v>
@@ -9687,7 +9794,7 @@
         <v>20</v>
       </c>
       <c r="F52" s="115" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G52" s="60">
         <v>9.0120000000000005</v>
@@ -9751,7 +9858,7 @@
         <v>20</v>
       </c>
       <c r="F55" s="115" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G55" s="60">
         <v>450</v>
@@ -9807,7 +9914,7 @@
         <v>20</v>
       </c>
       <c r="F58" s="115" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G58" s="69" t="s">
         <v>71</v>
@@ -9960,7 +10067,7 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="103"/>
-      <c r="B67" s="103"/>
+      <c r="B67" s="129"/>
       <c r="C67" s="68">
         <v>7</v>
       </c>
@@ -10026,7 +10133,7 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" s="103"/>
-      <c r="B70" s="103" t="str">
+      <c r="B70" s="128" t="str">
         <f>B69</f>
         <v>#</v>
       </c>
@@ -10119,7 +10226,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -31250,7 +31357,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -36669,7 +36776,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Z1063"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -36972,14 +37079,14 @@
     <row r="9" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="32"/>
       <c r="B9" s="28" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="C9" s="29" t="s">
         <v>20</v>
       </c>
       <c r="D9" s="28">
         <f>IF(multi_stock_sampling="Yes", 1, 0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" s="28" t="s">
         <v>192</v>
@@ -37046,7 +37153,7 @@
       </c>
       <c r="D11" s="41" t="str">
         <f>'User Interface'!E10</f>
-        <v>[[2,3,4,5,1,7]]</v>
+        <v>[[2,3,1,7]]</v>
       </c>
       <c r="E11" s="41" t="s">
         <v>196</v>
@@ -37647,7 +37754,7 @@
       </c>
       <c r="D28" s="69" t="str">
         <f>'User Interface'!E23</f>
-        <v>['DMSO']</v>
+        <v>['GBL']</v>
       </c>
       <c r="E28" s="60" t="s">
         <v>196</v>
@@ -37995,7 +38102,7 @@
       </c>
       <c r="D37" s="60" t="str">
         <f>'User Interface'!E32</f>
-        <v>['PbI2','PyrrolidiniumIodide','DMSO']</v>
+        <v>['PbI2','EtNH3I','GBL']</v>
       </c>
       <c r="E37" s="60" t="s">
         <v>196</v>
@@ -38075,7 +38182,7 @@
       </c>
       <c r="D39" s="69">
         <f>'User Interface'!E33</f>
-        <v>1.55</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="E39" s="60" t="s">
         <v>190</v>
@@ -38115,7 +38222,7 @@
       </c>
       <c r="D40" s="69">
         <f>'User Interface'!E34</f>
-        <v>1.93</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E40" s="60" t="s">
         <v>190</v>
@@ -38343,7 +38450,7 @@
       </c>
       <c r="D46" s="60" t="str">
         <f>'User Interface'!E41</f>
-        <v>['PyrrolidiniumIodide','DMSO']</v>
+        <v>['EtNH3I','GBL']</v>
       </c>
       <c r="E46" s="60" t="s">
         <v>196</v>
@@ -38423,7 +38530,7 @@
       </c>
       <c r="D48" s="60">
         <f>'User Interface'!E42</f>
-        <v>2.06</v>
+        <v>4</v>
       </c>
       <c r="E48" s="60" t="s">
         <v>190</v>
@@ -38463,7 +38570,7 @@
       </c>
       <c r="D49" s="60">
         <f>'User Interface'!E43</f>
-        <v>1.33</v>
+        <v>0</v>
       </c>
       <c r="E49" s="60" t="s">
         <v>190</v>
@@ -38503,7 +38610,7 @@
       </c>
       <c r="D50" s="60">
         <f>'User Interface'!E44</f>
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="E50" s="60" t="s">
         <v>190</v>
@@ -38679,9 +38786,9 @@
       <c r="Z54" s="4"/>
     </row>
     <row r="55" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="64">
+      <c r="A55" s="64" t="str">
         <f>'User Interface'!A50</f>
-        <v>0</v>
+        <v>#</v>
       </c>
       <c r="B55" s="60" t="s">
         <v>234</v>
@@ -38691,7 +38798,7 @@
       </c>
       <c r="D55" s="60" t="str">
         <f>'User Interface'!E50</f>
-        <v>['PbI2','PyrrolidiniumIodide','DMSO']</v>
+        <v>['PbI2','EtNH3I','GBL']</v>
       </c>
       <c r="E55" s="60" t="s">
         <v>196</v>
@@ -38759,9 +38866,9 @@
       <c r="Z56" s="4"/>
     </row>
     <row r="57" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="64">
+      <c r="A57" s="64" t="str">
         <f>'User Interface'!A51</f>
-        <v>0</v>
+        <v>#</v>
       </c>
       <c r="B57" s="99" t="s">
         <v>236</v>
@@ -38771,7 +38878,7 @@
       </c>
       <c r="D57" s="60">
         <f>'User Interface'!E51</f>
-        <v>1.18</v>
+        <v>1</v>
       </c>
       <c r="E57" s="60" t="s">
         <v>190</v>
@@ -38799,9 +38906,9 @@
       <c r="Z57" s="4"/>
     </row>
     <row r="58" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="64">
+      <c r="A58" s="64" t="str">
         <f>'User Interface'!A52</f>
-        <v>0</v>
+        <v>#</v>
       </c>
       <c r="B58" s="99" t="s">
         <v>237</v>
@@ -38811,7 +38918,7 @@
       </c>
       <c r="D58" s="60">
         <f>'User Interface'!E52</f>
-        <v>0.74</v>
+        <v>1.3</v>
       </c>
       <c r="E58" s="60" t="s">
         <v>190</v>
@@ -39027,9 +39134,9 @@
       <c r="Z63" s="4"/>
     </row>
     <row r="64" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="64">
+      <c r="A64" s="64" t="str">
         <f>'User Interface'!A59</f>
-        <v>0</v>
+        <v>#</v>
       </c>
       <c r="B64" s="60" t="s">
         <v>242</v>
@@ -39039,7 +39146,7 @@
       </c>
       <c r="D64" s="60" t="str">
         <f>'User Interface'!E59</f>
-        <v>['PbI2','PyrrolidiniumIodide','DMSO']</v>
+        <v>['PbI2','EtNH3I','GBL']</v>
       </c>
       <c r="E64" s="60" t="s">
         <v>196</v>
@@ -39107,9 +39214,9 @@
       <c r="Z65" s="4"/>
     </row>
     <row r="66" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="64">
+      <c r="A66" s="64" t="str">
         <f>'User Interface'!A60</f>
-        <v>0</v>
+        <v>#</v>
       </c>
       <c r="B66" s="99" t="s">
         <v>244</v>
@@ -39119,7 +39226,7 @@
       </c>
       <c r="D66" s="60">
         <f>'User Interface'!E60</f>
-        <v>1.42</v>
+        <v>0.9</v>
       </c>
       <c r="E66" s="60" t="s">
         <v>190</v>
@@ -39147,9 +39254,9 @@
       <c r="Z66" s="4"/>
     </row>
     <row r="67" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="64">
+      <c r="A67" s="64" t="str">
         <f>'User Interface'!A61</f>
-        <v>0</v>
+        <v>#</v>
       </c>
       <c r="B67" s="99" t="s">
         <v>245</v>
@@ -39159,7 +39266,7 @@
       </c>
       <c r="D67" s="60">
         <f>'User Interface'!E61</f>
-        <v>1.06</v>
+        <v>0.5</v>
       </c>
       <c r="E67" s="60" t="s">
         <v>190</v>
@@ -39197,9 +39304,9 @@
       <c r="C68" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="D68" s="60" t="str">
+      <c r="D68" s="60">
         <f>'User Interface'!E62</f>
-        <v>['PbI2','PyrrolidiniumIodide','DMSO']</v>
+        <v>0</v>
       </c>
       <c r="E68" s="60" t="s">
         <v>190</v>
@@ -39277,9 +39384,9 @@
       <c r="C70" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="D70" s="60" t="str">
+      <c r="D70" s="60">
         <f>'User Interface'!E65</f>
-        <v>['PbI2','PyrrolidiniumIodide','DMSO']</v>
+        <v>0</v>
       </c>
       <c r="E70" s="60" t="s">
         <v>192</v>
@@ -39385,9 +39492,9 @@
       <c r="C73" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="D73" s="60" t="str">
+      <c r="D73" s="60">
         <f>'User Interface'!E68</f>
-        <v>['PbI2','PyrrolidiniumIodide','DMSO']</v>
+        <v>0</v>
       </c>
       <c r="E73" s="60" t="s">
         <v>196</v>
@@ -39467,7 +39574,7 @@
       </c>
       <c r="D75" s="60">
         <f>'User Interface'!E69</f>
-        <v>1.42</v>
+        <v>1.5</v>
       </c>
       <c r="E75" s="60" t="s">
         <v>190</v>
@@ -39507,7 +39614,7 @@
       </c>
       <c r="D76" s="60">
         <f>'User Interface'!E70</f>
-        <v>1.06</v>
+        <v>6</v>
       </c>
       <c r="E76" s="60" t="s">
         <v>190</v>
@@ -39815,7 +39922,7 @@
       </c>
       <c r="D84" s="60">
         <f>'User Interface'!E78</f>
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="E84" s="60" t="s">
         <v>190</v>
@@ -39855,7 +39962,7 @@
       </c>
       <c r="D85" s="60">
         <f>'User Interface'!E79</f>
-        <v>7.63</v>
+        <v>0</v>
       </c>
       <c r="E85" s="60" t="s">
         <v>190</v>
@@ -40076,14 +40183,14 @@
         <v>0</v>
       </c>
       <c r="B91" s="60" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C91" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D91" s="69" t="str">
         <f>'Old Reagents'!F13</f>
-        <v>['DMSO']</v>
+        <v>['GBL']</v>
       </c>
       <c r="E91" s="60" t="s">
         <v>196</v>
@@ -40116,7 +40223,7 @@
         <v>#</v>
       </c>
       <c r="B92" s="60" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C92" s="73" t="s">
         <v>20</v>
@@ -40156,7 +40263,7 @@
         <v>#</v>
       </c>
       <c r="B93" s="60" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C93" s="61" t="s">
         <v>20</v>
@@ -40196,7 +40303,7 @@
         <v>#</v>
       </c>
       <c r="B94" s="60" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C94" s="61" t="s">
         <v>20</v>
@@ -40236,7 +40343,7 @@
         <v>#</v>
       </c>
       <c r="B95" s="60" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C95" s="61" t="s">
         <v>20</v>
@@ -40276,7 +40383,7 @@
         <v>#</v>
       </c>
       <c r="B96" s="60" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C96" s="61" t="s">
         <v>20</v>
@@ -40316,7 +40423,7 @@
         <v>#</v>
       </c>
       <c r="B97" s="60" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C97" s="61" t="s">
         <v>20</v>
@@ -40356,7 +40463,7 @@
         <v>#</v>
       </c>
       <c r="B98" s="60" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C98" s="61" t="s">
         <v>20</v>
@@ -40424,14 +40531,14 @@
         <v>0</v>
       </c>
       <c r="B100" s="60" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C100" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D100" s="69" t="str">
         <f>'Old Reagents'!F22</f>
-        <v>['PbI2','PyrrolidiniumIodide','DMSO']</v>
+        <v>['PbI2','EtNH3I','GBL']</v>
       </c>
       <c r="E100" s="60" t="s">
         <v>196</v>
@@ -40464,14 +40571,14 @@
         <v>0</v>
       </c>
       <c r="B101" s="60" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C101" s="73" t="s">
         <v>20</v>
       </c>
       <c r="D101" s="69">
         <f>'Old Reagents'!F23</f>
-        <v>1.55</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="E101" s="69" t="s">
         <v>193</v>
@@ -40504,14 +40611,14 @@
         <v>0</v>
       </c>
       <c r="B102" s="60" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C102" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D102" s="69">
         <f>'Old Reagents'!F24</f>
-        <v>1.93</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E102" s="60" t="s">
         <v>190</v>
@@ -40544,7 +40651,7 @@
         <v>#</v>
       </c>
       <c r="B103" s="60" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C103" s="61" t="s">
         <v>20</v>
@@ -40584,7 +40691,7 @@
         <v>#</v>
       </c>
       <c r="B104" s="60" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C104" s="61" t="s">
         <v>20</v>
@@ -40624,7 +40731,7 @@
         <v>#</v>
       </c>
       <c r="B105" s="60" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C105" s="61" t="s">
         <v>20</v>
@@ -40664,7 +40771,7 @@
         <v>#</v>
       </c>
       <c r="B106" s="60" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C106" s="61" t="s">
         <v>20</v>
@@ -40704,7 +40811,7 @@
         <v>#</v>
       </c>
       <c r="B107" s="60" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C107" s="61" t="s">
         <v>20</v>
@@ -40770,19 +40877,19 @@
       <c r="Z108" s="4"/>
     </row>
     <row r="109" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="64" t="str">
+      <c r="A109" s="64">
         <f>'Old Reagents'!B31</f>
-        <v>#</v>
+        <v>0</v>
       </c>
       <c r="B109" s="60" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C109" s="61" t="s">
         <v>20</v>
       </c>
       <c r="D109" s="69" t="str">
         <f>'Old Reagents'!F31</f>
-        <v>['PyrrolidiniumIodide','DMSO']</v>
+        <v>['EtNH3I','GBL']</v>
       </c>
       <c r="E109" s="60" t="s">
         <v>196</v>
@@ -40810,19 +40917,19 @@
       <c r="Z109" s="4"/>
     </row>
     <row r="110" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="64" t="str">
+      <c r="A110" s="64">
         <f>'Old Reagents'!B32</f>
-        <v>#</v>
+        <v>0</v>
       </c>
       <c r="B110" s="99" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C110" s="73" t="s">
         <v>20</v>
       </c>
       <c r="D110" s="69">
         <f>'Old Reagents'!F32</f>
-        <v>2.06</v>
+        <v>4</v>
       </c>
       <c r="E110" s="69" t="s">
         <v>193</v>
@@ -40855,7 +40962,7 @@
         <v>#</v>
       </c>
       <c r="B111" s="60" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C111" s="61" t="s">
         <v>20</v>
@@ -40895,7 +41002,7 @@
         <v>#</v>
       </c>
       <c r="B112" s="60" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C112" s="61" t="s">
         <v>20</v>
@@ -40935,7 +41042,7 @@
         <v>#</v>
       </c>
       <c r="B113" s="60" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="C113" s="61" t="s">
         <v>20</v>
@@ -40975,7 +41082,7 @@
         <v>#</v>
       </c>
       <c r="B114" s="60" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C114" s="61" t="s">
         <v>20</v>
@@ -41015,7 +41122,7 @@
         <v>#</v>
       </c>
       <c r="B115" s="60" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C115" s="61" t="s">
         <v>20</v>
@@ -41055,7 +41162,7 @@
         <v>#</v>
       </c>
       <c r="B116" s="60" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C116" s="61" t="s">
         <v>20</v>
@@ -41118,12 +41225,12 @@
       <c r="Z117" s="4"/>
     </row>
     <row r="118" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="64">
+      <c r="A118" s="64" t="str">
         <f>'Old Reagents'!B40</f>
-        <v>0</v>
+        <v>#</v>
       </c>
       <c r="B118" s="60" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C118" s="61" t="s">
         <v>20</v>
@@ -41158,12 +41265,12 @@
       <c r="Z118" s="4"/>
     </row>
     <row r="119" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="64">
+      <c r="A119" s="64" t="str">
         <f>'Old Reagents'!B41</f>
-        <v>0</v>
+        <v>#</v>
       </c>
       <c r="B119" s="99" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C119" s="73" t="s">
         <v>20</v>
@@ -41198,12 +41305,12 @@
       <c r="Z119" s="4"/>
     </row>
     <row r="120" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="64">
+      <c r="A120" s="64" t="str">
         <f>'Old Reagents'!B42</f>
-        <v>0</v>
+        <v>#</v>
       </c>
       <c r="B120" s="99" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C120" s="61" t="s">
         <v>20</v>
@@ -41243,7 +41350,7 @@
         <v>#</v>
       </c>
       <c r="B121" s="60" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C121" s="61" t="s">
         <v>20</v>
@@ -41283,7 +41390,7 @@
         <v>#</v>
       </c>
       <c r="B122" s="60" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C122" s="61" t="s">
         <v>20</v>
@@ -41323,7 +41430,7 @@
         <v>#</v>
       </c>
       <c r="B123" s="60" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C123" s="61" t="s">
         <v>20</v>
@@ -41363,7 +41470,7 @@
         <v>#</v>
       </c>
       <c r="B124" s="60" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C124" s="61" t="s">
         <v>20</v>
@@ -41403,7 +41510,7 @@
         <v>#</v>
       </c>
       <c r="B125" s="60" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C125" s="61" t="s">
         <v>20</v>
@@ -41466,12 +41573,12 @@
       <c r="Z126" s="4"/>
     </row>
     <row r="127" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A127" s="64">
+      <c r="A127" s="64" t="str">
         <f>'Old Reagents'!B49</f>
-        <v>0</v>
+        <v>#</v>
       </c>
       <c r="B127" s="60" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C127" s="61" t="s">
         <v>20</v>
@@ -41506,12 +41613,12 @@
       <c r="Z127" s="4"/>
     </row>
     <row r="128" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A128" s="64">
+      <c r="A128" s="64" t="str">
         <f>'Old Reagents'!B50</f>
-        <v>0</v>
+        <v>#</v>
       </c>
       <c r="B128" s="99" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C128" s="73" t="s">
         <v>20</v>
@@ -41546,12 +41653,12 @@
       <c r="Z128" s="4"/>
     </row>
     <row r="129" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A129" s="64">
+      <c r="A129" s="64" t="str">
         <f>'Old Reagents'!B51</f>
-        <v>0</v>
+        <v>#</v>
       </c>
       <c r="B129" s="99" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C129" s="61" t="s">
         <v>20</v>
@@ -41591,7 +41698,7 @@
         <v>#</v>
       </c>
       <c r="B130" s="60" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C130" s="61" t="s">
         <v>20</v>
@@ -41631,7 +41738,7 @@
         <v>#</v>
       </c>
       <c r="B131" s="60" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C131" s="61" t="s">
         <v>20</v>
@@ -41671,7 +41778,7 @@
         <v>#</v>
       </c>
       <c r="B132" s="60" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C132" s="61" t="s">
         <v>20</v>
@@ -41711,7 +41818,7 @@
         <v>#</v>
       </c>
       <c r="B133" s="60" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C133" s="61" t="s">
         <v>20</v>
@@ -41751,7 +41858,7 @@
         <v>#</v>
       </c>
       <c r="B134" s="60" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C134" s="61" t="s">
         <v>20</v>
@@ -41819,7 +41926,7 @@
         <v>#</v>
       </c>
       <c r="B136" s="60" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C136" s="61" t="s">
         <v>20</v>
@@ -41859,7 +41966,7 @@
         <v>#</v>
       </c>
       <c r="B137" s="99" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C137" s="73" t="s">
         <v>20</v>
@@ -41899,7 +42006,7 @@
         <v>#</v>
       </c>
       <c r="B138" s="99" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C138" s="61" t="s">
         <v>20</v>
@@ -41939,7 +42046,7 @@
         <v>#</v>
       </c>
       <c r="B139" s="60" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C139" s="61" t="s">
         <v>20</v>
@@ -41979,7 +42086,7 @@
         <v>#</v>
       </c>
       <c r="B140" s="60" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C140" s="61" t="s">
         <v>20</v>
@@ -42019,7 +42126,7 @@
         <v>#</v>
       </c>
       <c r="B141" s="60" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C141" s="61" t="s">
         <v>20</v>
@@ -42059,7 +42166,7 @@
         <v>#</v>
       </c>
       <c r="B142" s="60" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C142" s="61" t="s">
         <v>20</v>
@@ -42099,7 +42206,7 @@
         <v>#</v>
       </c>
       <c r="B143" s="60" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C143" s="61" t="s">
         <v>20</v>
@@ -42167,7 +42274,7 @@
         <v>0</v>
       </c>
       <c r="B145" s="60" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C145" s="61" t="s">
         <v>20</v>
@@ -42207,7 +42314,7 @@
         <v>#</v>
       </c>
       <c r="B146" s="99" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C146" s="73" t="s">
         <v>20</v>
@@ -42247,7 +42354,7 @@
         <v>#</v>
       </c>
       <c r="B147" s="99" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C147" s="61" t="s">
         <v>20</v>
@@ -42287,7 +42394,7 @@
         <v>#</v>
       </c>
       <c r="B148" s="60" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C148" s="61" t="s">
         <v>20</v>
@@ -42327,7 +42434,7 @@
         <v>#</v>
       </c>
       <c r="B149" s="60" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C149" s="61" t="s">
         <v>20</v>
@@ -42367,7 +42474,7 @@
         <v>#</v>
       </c>
       <c r="B150" s="60" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C150" s="61" t="s">
         <v>20</v>
@@ -42407,7 +42514,7 @@
         <v>#</v>
       </c>
       <c r="B151" s="60" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C151" s="61" t="s">
         <v>20</v>
@@ -42447,7 +42554,7 @@
         <v>#</v>
       </c>
       <c r="B152" s="60" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C152" s="61" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
branch for generating reagent dictionary and associated state spaces for all dataset
</commit_message>
<xml_diff>
--- a/HC_LBL_SpecificationInterface.xlsx
+++ b/HC_LBL_SpecificationInterface.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27417"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaeltynes/repos/ESCALATE_Capture/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ipendleton/Dropbox/Desktop/ESCALATE/ESCALATE_Capture/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDC7A2A7-E07D-BB43-8A90-AE9620B34802}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="-16600" windowWidth="38400" windowHeight="21600" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User Interface" sheetId="1" r:id="rId1"/>
@@ -24,10 +25,15 @@
     <definedName name="wellcount" localSheetId="0">'User Interface'!$E$6</definedName>
     <definedName name="wellcount">'WF1'!$D$7</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -37,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="286">
   <si>
     <t>Manual Well Number</t>
   </si>
@@ -1194,13 +1200,16 @@
     <t>['PyrrolidiniumIodide','DMSO']</t>
   </si>
   <si>
-    <t>[[2,3,4,5,1,7]]</t>
+    <t>[[2,3,1,7]]</t>
+  </si>
+  <si>
+    <t>StateSet Generation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1526,7 +1535,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1865,6 +1874,9 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2079,11 +2091,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="109" zoomScaleNormal="109" zoomScalePageLayoutView="109" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+    <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="109" zoomScalePageLayoutView="109" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -2282,7 +2294,7 @@
       <c r="D6" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="109">
+      <c r="E6" s="118">
         <f>SUM(E11,E16,E19)</f>
         <v>96</v>
       </c>
@@ -2503,7 +2515,9 @@
       <c r="D12" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="111"/>
+      <c r="E12" s="111" t="s">
+        <v>285</v>
+      </c>
       <c r="F12" s="41" t="s">
         <v>43</v>
       </c>
@@ -3819,7 +3833,9 @@
       <c r="Z48" s="19"/>
     </row>
     <row r="49" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="104"/>
+      <c r="A49" s="104" t="s">
+        <v>44</v>
+      </c>
       <c r="B49" s="68">
         <v>4</v>
       </c>
@@ -3859,7 +3875,9 @@
       <c r="Z49" s="19"/>
     </row>
     <row r="50" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="104"/>
+      <c r="A50" s="104" t="s">
+        <v>44</v>
+      </c>
       <c r="B50" s="68"/>
       <c r="C50" s="60" t="s">
         <v>108</v>
@@ -3897,7 +3915,9 @@
       <c r="Z50" s="19"/>
     </row>
     <row r="51" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="104"/>
+      <c r="A51" s="104" t="s">
+        <v>44</v>
+      </c>
       <c r="B51" s="68"/>
       <c r="C51" s="60" t="s">
         <v>110</v>
@@ -4157,7 +4177,9 @@
       <c r="Z57" s="19"/>
     </row>
     <row r="58" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="103"/>
+      <c r="A58" s="103" t="s">
+        <v>44</v>
+      </c>
       <c r="B58" s="68">
         <v>5</v>
       </c>
@@ -4199,7 +4221,9 @@
       <c r="Z58" s="19"/>
     </row>
     <row r="59" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="104"/>
+      <c r="A59" s="104" t="s">
+        <v>44</v>
+      </c>
       <c r="B59" s="72"/>
       <c r="C59" s="60" t="s">
         <v>121</v>
@@ -4237,7 +4261,9 @@
       <c r="Z59" s="19"/>
     </row>
     <row r="60" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="104"/>
+      <c r="A60" s="104" t="s">
+        <v>44</v>
+      </c>
       <c r="B60" s="72"/>
       <c r="C60" s="60" t="s">
         <v>123</v>
@@ -8389,20 +8415,20 @@
   </sheetData>
   <sheetProtection formatRows="0"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E4">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E4" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"MIT_PVLab,HC,LBL,dev"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E3">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E3" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"1.1,3.0"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="C19" location="Manual Experiment Interface!B2" display="Manual Experiments"/>
-    <hyperlink ref="H21" r:id="rId1"/>
-    <hyperlink ref="H22" r:id="rId2"/>
-    <hyperlink ref="H35" r:id="rId3"/>
-    <hyperlink ref="H44" r:id="rId4"/>
-    <hyperlink ref="H53" r:id="rId5"/>
+    <hyperlink ref="C19" location="Manual Experiment Interface!B2" display="Manual Experiments" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="H21" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="H22" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="H35" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="H44" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="H53" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -8410,10 +8436,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B9"/>
     </sheetView>
   </sheetViews>
@@ -29621,7 +29647,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -35040,7 +35066,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView topLeftCell="A27" workbookViewId="0">
@@ -35383,7 +35409,7 @@
       </c>
       <c r="D10" s="41" t="str">
         <f>'User Interface'!E9</f>
-        <v>[[2,3,4,5,1,7]]</v>
+        <v>[[2,3,1,7]]</v>
       </c>
       <c r="E10" s="41" t="s">
         <v>196</v>
@@ -35501,9 +35527,9 @@
       <c r="C13" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="41">
+      <c r="D13" s="41" t="str">
         <f>'User Interface'!E12</f>
-        <v>0</v>
+        <v>StateSet Generation</v>
       </c>
       <c r="E13" s="41"/>
       <c r="F13" s="45"/>
@@ -37016,9 +37042,9 @@
       <c r="Z53" s="4"/>
     </row>
     <row r="54" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="64">
+      <c r="A54" s="64" t="str">
         <f>'User Interface'!A49</f>
-        <v>0</v>
+        <v>#</v>
       </c>
       <c r="B54" s="60" t="s">
         <v>234</v>
@@ -37096,9 +37122,9 @@
       <c r="Z55" s="4"/>
     </row>
     <row r="56" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="64">
+      <c r="A56" s="64" t="str">
         <f>'User Interface'!A50</f>
-        <v>0</v>
+        <v>#</v>
       </c>
       <c r="B56" s="99" t="s">
         <v>236</v>
@@ -37136,9 +37162,9 @@
       <c r="Z56" s="4"/>
     </row>
     <row r="57" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="64">
+      <c r="A57" s="64" t="str">
         <f>'User Interface'!A51</f>
-        <v>0</v>
+        <v>#</v>
       </c>
       <c r="B57" s="99" t="s">
         <v>237</v>
@@ -37364,9 +37390,9 @@
       <c r="Z62" s="4"/>
     </row>
     <row r="63" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="64">
+      <c r="A63" s="64" t="str">
         <f>'User Interface'!A58</f>
-        <v>0</v>
+        <v>#</v>
       </c>
       <c r="B63" s="60" t="s">
         <v>242</v>
@@ -37444,9 +37470,9 @@
       <c r="Z64" s="4"/>
     </row>
     <row r="65" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="64">
+      <c r="A65" s="64" t="str">
         <f>'User Interface'!A59</f>
-        <v>0</v>
+        <v>#</v>
       </c>
       <c r="B65" s="99" t="s">
         <v>244</v>
@@ -37484,9 +37510,9 @@
       <c r="Z65" s="4"/>
     </row>
     <row r="66" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="64">
+      <c r="A66" s="64" t="str">
         <f>'User Interface'!A60</f>
-        <v>0</v>
+        <v>#</v>
       </c>
       <c r="B66" s="99" t="s">
         <v>245</v>

</xml_diff>

<commit_message>
almost quickly generate state spaces for all failed runs
</commit_message>
<xml_diff>
--- a/HC_LBL_SpecificationInterface.xlsx
+++ b/HC_LBL_SpecificationInterface.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ipendleton/Dropbox/Desktop/ESCALATE/ESCALATE_Capture/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDC7A2A7-E07D-BB43-8A90-AE9620B34802}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F3C77E2-83E8-2748-BD68-D34D29B6279B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6060" yWindow="2360" windowWidth="36500" windowHeight="21920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User Interface" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="284">
   <si>
     <t>Manual Well Number</t>
   </si>
@@ -290,6 +290,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">ECL model ID.  </t>
     </r>
@@ -300,6 +301,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Cannot be used in with `Reagent#_chemical_list`</t>
     </r>
@@ -361,6 +363,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">ECL model ID.  </t>
     </r>
@@ -371,6 +374,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Cannot be used in with `Reagent#_chemical_list`</t>
     </r>
@@ -426,6 +430,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">ECL model ID.  </t>
     </r>
@@ -436,6 +441,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Cannot be used in with `Reagent#_chemical_list`</t>
     </r>
@@ -485,6 +491,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">ECL model ID.  </t>
     </r>
@@ -495,6 +502,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Cannot be used in with `Reagent#_chemical_list`</t>
     </r>
@@ -741,6 +749,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Materials (</t>
     </r>
@@ -750,6 +759,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Chemicals</t>
     </r>
@@ -758,6 +768,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>)</t>
     </r>
@@ -770,6 +781,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>chem</t>
     </r>
@@ -778,6 +790,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>2_molarmin</t>
     </r>
@@ -790,6 +803,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>chem</t>
     </r>
@@ -798,6 +812,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>2_molarmax</t>
     </r>
@@ -808,6 +823,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Reagent1_</t>
     </r>
@@ -818,6 +834,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>chemical</t>
     </r>
@@ -826,6 +843,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>_list</t>
     </r>
@@ -857,6 +875,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Reagent2_</t>
     </r>
@@ -867,6 +886,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>chemical</t>
     </r>
@@ -875,6 +895,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>_list</t>
     </r>
@@ -906,6 +927,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Reagent3_</t>
     </r>
@@ -916,6 +938,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>chemical</t>
     </r>
@@ -924,6 +947,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>_list</t>
     </r>
@@ -955,6 +979,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Reagent4_</t>
     </r>
@@ -965,6 +990,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>chemical</t>
     </r>
@@ -973,6 +999,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>_list</t>
     </r>
@@ -1004,6 +1031,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Reagent5_</t>
     </r>
@@ -1014,6 +1042,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>chemical</t>
     </r>
@@ -1022,6 +1051,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>_list</t>
     </r>
@@ -1053,6 +1083,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Reagent6_</t>
     </r>
@@ -1063,6 +1094,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>chemical</t>
     </r>
@@ -1071,6 +1103,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>_list</t>
     </r>
@@ -1102,6 +1135,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Reagent7_</t>
     </r>
@@ -1112,6 +1146,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>chemical</t>
     </r>
@@ -1120,6 +1155,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>_list</t>
     </r>
@@ -1164,30 +1200,6 @@
     <t>reagents_prep_duration</t>
   </si>
   <si>
-    <t>MAN 148.C1</t>
-  </si>
-  <si>
-    <t>MAN 148.C2</t>
-  </si>
-  <si>
-    <t>MAN 148.C3</t>
-  </si>
-  <si>
-    <t>MAN 148.C4</t>
-  </si>
-  <si>
-    <t>MAN 148.C5</t>
-  </si>
-  <si>
-    <t>MAN 148.C6</t>
-  </si>
-  <si>
-    <t>MAN 148.C7</t>
-  </si>
-  <si>
-    <t>MAN 148.C8</t>
-  </si>
-  <si>
     <t>LBL</t>
   </si>
   <si>
@@ -1205,12 +1217,30 @@
   <si>
     <t>StateSet Generation</t>
   </si>
+  <si>
+    <t>node1</t>
+  </si>
+  <si>
+    <t>node2</t>
+  </si>
+  <si>
+    <t>node3</t>
+  </si>
+  <si>
+    <t>node4</t>
+  </si>
+  <si>
+    <t>node5</t>
+  </si>
+  <si>
+    <t>node6</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1220,11 +1250,13 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1232,6 +1264,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1239,6 +1272,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
@@ -1246,12 +1280,14 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
@@ -1259,12 +1295,14 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1272,30 +1310,35 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1303,6 +1346,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1310,6 +1354,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1317,12 +1362,25 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="10">
@@ -2094,8 +2152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="109" zoomScalePageLayoutView="109" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="109" zoomScaleNormal="109" zoomScalePageLayoutView="109" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -2227,7 +2285,7 @@
         <v>20</v>
       </c>
       <c r="E4" s="108" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="F4" s="22"/>
       <c r="G4" s="24" t="s">
@@ -2296,7 +2354,7 @@
       </c>
       <c r="E6" s="118">
         <f>SUM(E11,E16,E19)</f>
-        <v>96</v>
+        <v>1</v>
       </c>
       <c r="F6" s="28"/>
       <c r="G6" s="30" t="s">
@@ -2402,7 +2460,7 @@
         <v>20</v>
       </c>
       <c r="E9" s="111" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="F9" s="41" t="s">
         <v>34</v>
@@ -2478,7 +2536,7 @@
         <v>20</v>
       </c>
       <c r="E11" s="111">
-        <v>96</v>
+        <v>1</v>
       </c>
       <c r="F11" s="41">
         <v>12</v>
@@ -2516,7 +2574,7 @@
         <v>20</v>
       </c>
       <c r="E12" s="111" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="F12" s="41" t="s">
         <v>43</v>
@@ -2836,7 +2894,7 @@
         <v>20</v>
       </c>
       <c r="E22" s="115" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="F22" s="69" t="s">
         <v>60</v>
@@ -3160,7 +3218,7 @@
         <v>20</v>
       </c>
       <c r="E31" s="115" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="F31" s="69" t="s">
         <v>71</v>
@@ -3500,7 +3558,7 @@
         <v>20</v>
       </c>
       <c r="E40" s="115" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="F40" s="69" t="s">
         <v>89</v>
@@ -3846,7 +3904,7 @@
         <v>20</v>
       </c>
       <c r="E49" s="115" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="F49" s="69" t="s">
         <v>71</v>
@@ -4190,7 +4248,7 @@
         <v>20</v>
       </c>
       <c r="E58" s="115" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="F58" s="69" t="s">
         <v>89</v>
@@ -4312,7 +4370,7 @@
         <v>20</v>
       </c>
       <c r="E61" s="115" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="F61" s="60">
         <v>9.0120000000000005</v>
@@ -4434,7 +4492,7 @@
         <v>20</v>
       </c>
       <c r="E64" s="115" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="F64" s="60">
         <v>450</v>
@@ -4548,7 +4606,7 @@
         <v>20</v>
       </c>
       <c r="E67" s="115" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="F67" s="69" t="s">
         <v>71</v>
@@ -8414,7 +8472,7 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <sheetProtection formatRows="0"/>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E4" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"MIT_PVLab,HC,LBL,dev"</formula1>
     </dataValidation>
@@ -8440,7 +8498,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B9"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8509,7 +8567,7 @@
         <v/>
       </c>
       <c r="B2" s="6" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="C2" s="3">
         <v>0</v>
@@ -8520,11 +8578,17 @@
       <c r="E2" s="3">
         <v>0</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
+      <c r="F2" s="3">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3">
+        <v>0</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0</v>
+      </c>
       <c r="I2" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="J2" s="3">
         <v>0</v>
@@ -8555,22 +8619,28 @@
         <v/>
       </c>
       <c r="B3" s="6" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="C3" s="3">
         <v>0</v>
       </c>
       <c r="D3" s="3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3">
         <v>500</v>
       </c>
-      <c r="E3" s="3">
-        <v>50</v>
-      </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="F3" s="3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0</v>
+      </c>
       <c r="I3" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="J3" s="3">
         <v>0</v>
@@ -8601,22 +8671,28 @@
         <v/>
       </c>
       <c r="B4" s="6" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="C4" s="3">
+        <v>500</v>
+      </c>
+      <c r="D4" s="3">
         <v>0</v>
       </c>
-      <c r="D4" s="3">
-        <v>500</v>
-      </c>
       <c r="E4" s="3">
-        <v>100</v>
-      </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
+        <v>0</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0</v>
+      </c>
       <c r="I4" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="J4" s="3">
         <v>0</v>
@@ -8647,22 +8723,28 @@
         <v/>
       </c>
       <c r="B5" s="6" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="C5" s="3">
         <v>0</v>
       </c>
       <c r="D5" s="3">
-        <v>500</v>
+        <v>218</v>
       </c>
       <c r="E5" s="3">
-        <v>150</v>
-      </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
+        <v>0</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0</v>
+      </c>
       <c r="I5" s="3">
-        <v>20</v>
+        <v>282</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3" t="str">
@@ -8691,22 +8773,28 @@
         <v/>
       </c>
       <c r="B6" s="6" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="C6" s="3">
         <v>0</v>
       </c>
       <c r="D6" s="3">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="E6" s="3">
-        <v>200</v>
-      </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
+        <v>218</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0</v>
+      </c>
       <c r="I6" s="3">
-        <v>20</v>
+        <v>282</v>
       </c>
       <c r="J6" s="3"/>
       <c r="K6" s="3" t="str">
@@ -8735,22 +8823,28 @@
         <v/>
       </c>
       <c r="B7" s="6" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="C7" s="3">
+        <v>218</v>
+      </c>
+      <c r="D7" s="3">
         <v>0</v>
       </c>
-      <c r="D7" s="3">
-        <v>500</v>
-      </c>
       <c r="E7" s="3">
-        <v>250</v>
-      </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
+        <v>0</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0</v>
+      </c>
       <c r="I7" s="3">
-        <v>20</v>
+        <v>282</v>
       </c>
       <c r="J7" s="3"/>
       <c r="K7" s="3" t="str">
@@ -8778,29 +8872,16 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>278</v>
-      </c>
-      <c r="C8" s="3">
-        <v>0</v>
-      </c>
-      <c r="D8" s="3">
-        <v>500</v>
-      </c>
-      <c r="E8" s="3">
-        <v>300</v>
-      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
-      <c r="I8" s="3">
-        <v>20</v>
-      </c>
+      <c r="I8" s="3"/>
       <c r="J8" s="3"/>
-      <c r="K8" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="K8" s="3"/>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
@@ -8822,29 +8903,16 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>279</v>
-      </c>
-      <c r="C9" s="3">
-        <v>0</v>
-      </c>
-      <c r="D9" s="3">
-        <v>500</v>
-      </c>
-      <c r="E9" s="3">
-        <v>350</v>
-      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
-      <c r="I9" s="3">
-        <v>20</v>
-      </c>
+      <c r="I9" s="3"/>
       <c r="J9" s="3"/>
-      <c r="K9" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="K9" s="3"/>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
@@ -29641,6 +29709,7 @@
       <c r="K1000" s="3"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
@@ -29702,7 +29771,7 @@
       </c>
       <c r="B2" s="5" t="str">
         <f>IF(NOT('Manual Experiment Interface'!B2=""),'Manual Experiment Interface'!B2,"")</f>
-        <v>MAN 148.C1</v>
+        <v>node1</v>
       </c>
       <c r="C2" s="5">
         <f>IF(NOT('Manual Experiment Interface'!C2=""),'Manual Experiment Interface'!C2,"")</f>
@@ -29716,21 +29785,21 @@
         <f>IF(NOT('Manual Experiment Interface'!E2=""),'Manual Experiment Interface'!E2,"")</f>
         <v>0</v>
       </c>
-      <c r="F2" s="5" t="str">
+      <c r="F2" s="5">
         <f>IF(NOT('Manual Experiment Interface'!F2=""),'Manual Experiment Interface'!F2,"")</f>
-        <v/>
-      </c>
-      <c r="G2" s="5" t="str">
+        <v>0</v>
+      </c>
+      <c r="G2" s="5">
         <f>IF(NOT('Manual Experiment Interface'!G2=""),'Manual Experiment Interface'!G2,"")</f>
-        <v/>
-      </c>
-      <c r="H2" s="5" t="str">
+        <v>0</v>
+      </c>
+      <c r="H2" s="5">
         <f>IF(NOT('Manual Experiment Interface'!H2=""),'Manual Experiment Interface'!H2,"")</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="I2" s="5">
         <f>IF(NOT('Manual Experiment Interface'!I2=""),'Manual Experiment Interface'!I2,"")</f>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="J2" s="5">
         <f>IF(NOT('Manual Experiment Interface'!J2=""),'Manual Experiment Interface'!J2,"")</f>
@@ -29748,7 +29817,7 @@
       </c>
       <c r="B3" s="5" t="str">
         <f>IF(NOT('Manual Experiment Interface'!B3=""),'Manual Experiment Interface'!B3,"")</f>
-        <v>MAN 148.C2</v>
+        <v>node2</v>
       </c>
       <c r="C3" s="5">
         <f>IF(NOT('Manual Experiment Interface'!C3=""),'Manual Experiment Interface'!C3,"")</f>
@@ -29756,27 +29825,27 @@
       </c>
       <c r="D3" s="5">
         <f>IF(NOT('Manual Experiment Interface'!D3=""),'Manual Experiment Interface'!D3,"")</f>
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="E3" s="5">
         <f>IF(NOT('Manual Experiment Interface'!E3=""),'Manual Experiment Interface'!E3,"")</f>
-        <v>50</v>
-      </c>
-      <c r="F3" s="5" t="str">
+        <v>500</v>
+      </c>
+      <c r="F3" s="5">
         <f>IF(NOT('Manual Experiment Interface'!F3=""),'Manual Experiment Interface'!F3,"")</f>
-        <v/>
-      </c>
-      <c r="G3" s="5" t="str">
+        <v>0</v>
+      </c>
+      <c r="G3" s="5">
         <f>IF(NOT('Manual Experiment Interface'!G3=""),'Manual Experiment Interface'!G3,"")</f>
-        <v/>
-      </c>
-      <c r="H3" s="5" t="str">
+        <v>0</v>
+      </c>
+      <c r="H3" s="5">
         <f>IF(NOT('Manual Experiment Interface'!H3=""),'Manual Experiment Interface'!H3,"")</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="I3" s="5">
         <f>IF(NOT('Manual Experiment Interface'!I3=""),'Manual Experiment Interface'!I3,"")</f>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="J3" s="5">
         <f>IF(NOT('Manual Experiment Interface'!J3=""),'Manual Experiment Interface'!J3,"")</f>
@@ -29794,35 +29863,35 @@
       </c>
       <c r="B4" s="5" t="str">
         <f>IF(NOT('Manual Experiment Interface'!B4=""),'Manual Experiment Interface'!B4,"")</f>
-        <v>MAN 148.C3</v>
+        <v>node3</v>
       </c>
       <c r="C4" s="5">
         <f>IF(NOT('Manual Experiment Interface'!C4=""),'Manual Experiment Interface'!C4,"")</f>
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="D4" s="5">
         <f>IF(NOT('Manual Experiment Interface'!D4=""),'Manual Experiment Interface'!D4,"")</f>
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="E4" s="5">
         <f>IF(NOT('Manual Experiment Interface'!E4=""),'Manual Experiment Interface'!E4,"")</f>
-        <v>100</v>
-      </c>
-      <c r="F4" s="5" t="str">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5">
         <f>IF(NOT('Manual Experiment Interface'!F4=""),'Manual Experiment Interface'!F4,"")</f>
-        <v/>
-      </c>
-      <c r="G4" s="5" t="str">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5">
         <f>IF(NOT('Manual Experiment Interface'!G4=""),'Manual Experiment Interface'!G4,"")</f>
-        <v/>
-      </c>
-      <c r="H4" s="5" t="str">
+        <v>0</v>
+      </c>
+      <c r="H4" s="5">
         <f>IF(NOT('Manual Experiment Interface'!H4=""),'Manual Experiment Interface'!H4,"")</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="I4" s="5">
         <f>IF(NOT('Manual Experiment Interface'!I4=""),'Manual Experiment Interface'!I4,"")</f>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="J4" s="5">
         <f>IF(NOT('Manual Experiment Interface'!J4=""),'Manual Experiment Interface'!J4,"")</f>
@@ -29840,7 +29909,7 @@
       </c>
       <c r="B5" s="5" t="str">
         <f>IF(NOT('Manual Experiment Interface'!B5=""),'Manual Experiment Interface'!B5,"")</f>
-        <v>MAN 148.C4</v>
+        <v>node4</v>
       </c>
       <c r="C5" s="5">
         <f>IF(NOT('Manual Experiment Interface'!C5=""),'Manual Experiment Interface'!C5,"")</f>
@@ -29848,27 +29917,27 @@
       </c>
       <c r="D5" s="5">
         <f>IF(NOT('Manual Experiment Interface'!D5=""),'Manual Experiment Interface'!D5,"")</f>
-        <v>500</v>
+        <v>218</v>
       </c>
       <c r="E5" s="5">
         <f>IF(NOT('Manual Experiment Interface'!E5=""),'Manual Experiment Interface'!E5,"")</f>
-        <v>150</v>
-      </c>
-      <c r="F5" s="5" t="str">
+        <v>0</v>
+      </c>
+      <c r="F5" s="5">
         <f>IF(NOT('Manual Experiment Interface'!F5=""),'Manual Experiment Interface'!F5,"")</f>
-        <v/>
-      </c>
-      <c r="G5" s="5" t="str">
+        <v>0</v>
+      </c>
+      <c r="G5" s="5">
         <f>IF(NOT('Manual Experiment Interface'!G5=""),'Manual Experiment Interface'!G5,"")</f>
-        <v/>
-      </c>
-      <c r="H5" s="5" t="str">
+        <v>0</v>
+      </c>
+      <c r="H5" s="5">
         <f>IF(NOT('Manual Experiment Interface'!H5=""),'Manual Experiment Interface'!H5,"")</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="I5" s="5">
         <f>IF(NOT('Manual Experiment Interface'!I5=""),'Manual Experiment Interface'!I5,"")</f>
-        <v>20</v>
+        <v>282</v>
       </c>
       <c r="J5" s="5" t="str">
         <f>IF(NOT('Manual Experiment Interface'!J5=""),'Manual Experiment Interface'!J5,"")</f>
@@ -29886,7 +29955,7 @@
       </c>
       <c r="B6" s="5" t="str">
         <f>IF(NOT('Manual Experiment Interface'!B6=""),'Manual Experiment Interface'!B6,"")</f>
-        <v>MAN 148.C5</v>
+        <v>node5</v>
       </c>
       <c r="C6" s="5">
         <f>IF(NOT('Manual Experiment Interface'!C6=""),'Manual Experiment Interface'!C6,"")</f>
@@ -29894,27 +29963,27 @@
       </c>
       <c r="D6" s="5">
         <f>IF(NOT('Manual Experiment Interface'!D6=""),'Manual Experiment Interface'!D6,"")</f>
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="E6" s="5">
         <f>IF(NOT('Manual Experiment Interface'!E6=""),'Manual Experiment Interface'!E6,"")</f>
-        <v>200</v>
-      </c>
-      <c r="F6" s="5" t="str">
+        <v>218</v>
+      </c>
+      <c r="F6" s="5">
         <f>IF(NOT('Manual Experiment Interface'!F6=""),'Manual Experiment Interface'!F6,"")</f>
-        <v/>
-      </c>
-      <c r="G6" s="5" t="str">
+        <v>0</v>
+      </c>
+      <c r="G6" s="5">
         <f>IF(NOT('Manual Experiment Interface'!G6=""),'Manual Experiment Interface'!G6,"")</f>
-        <v/>
-      </c>
-      <c r="H6" s="5" t="str">
+        <v>0</v>
+      </c>
+      <c r="H6" s="5">
         <f>IF(NOT('Manual Experiment Interface'!H6=""),'Manual Experiment Interface'!H6,"")</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="I6" s="5">
         <f>IF(NOT('Manual Experiment Interface'!I6=""),'Manual Experiment Interface'!I6,"")</f>
-        <v>20</v>
+        <v>282</v>
       </c>
       <c r="J6" s="5" t="str">
         <f>IF(NOT('Manual Experiment Interface'!J6=""),'Manual Experiment Interface'!J6,"")</f>
@@ -29932,35 +30001,35 @@
       </c>
       <c r="B7" s="5" t="str">
         <f>IF(NOT('Manual Experiment Interface'!B7=""),'Manual Experiment Interface'!B7,"")</f>
-        <v>MAN 148.C6</v>
+        <v>node6</v>
       </c>
       <c r="C7" s="5">
         <f>IF(NOT('Manual Experiment Interface'!C7=""),'Manual Experiment Interface'!C7,"")</f>
-        <v>0</v>
+        <v>218</v>
       </c>
       <c r="D7" s="5">
         <f>IF(NOT('Manual Experiment Interface'!D7=""),'Manual Experiment Interface'!D7,"")</f>
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="E7" s="5">
         <f>IF(NOT('Manual Experiment Interface'!E7=""),'Manual Experiment Interface'!E7,"")</f>
-        <v>250</v>
-      </c>
-      <c r="F7" s="5" t="str">
+        <v>0</v>
+      </c>
+      <c r="F7" s="5">
         <f>IF(NOT('Manual Experiment Interface'!F7=""),'Manual Experiment Interface'!F7,"")</f>
-        <v/>
-      </c>
-      <c r="G7" s="5" t="str">
+        <v>0</v>
+      </c>
+      <c r="G7" s="5">
         <f>IF(NOT('Manual Experiment Interface'!G7=""),'Manual Experiment Interface'!G7,"")</f>
-        <v/>
-      </c>
-      <c r="H7" s="5" t="str">
+        <v>0</v>
+      </c>
+      <c r="H7" s="5">
         <f>IF(NOT('Manual Experiment Interface'!H7=""),'Manual Experiment Interface'!H7,"")</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="I7" s="5">
         <f>IF(NOT('Manual Experiment Interface'!I7=""),'Manual Experiment Interface'!I7,"")</f>
-        <v>20</v>
+        <v>282</v>
       </c>
       <c r="J7" s="5" t="str">
         <f>IF(NOT('Manual Experiment Interface'!J7=""),'Manual Experiment Interface'!J7,"")</f>
@@ -29978,19 +30047,19 @@
       </c>
       <c r="B8" s="5" t="str">
         <f>IF(NOT('Manual Experiment Interface'!B8=""),'Manual Experiment Interface'!B8,"")</f>
-        <v>MAN 148.C7</v>
-      </c>
-      <c r="C8" s="5">
+        <v/>
+      </c>
+      <c r="C8" s="5" t="str">
         <f>IF(NOT('Manual Experiment Interface'!C8=""),'Manual Experiment Interface'!C8,"")</f>
-        <v>0</v>
-      </c>
-      <c r="D8" s="5">
+        <v/>
+      </c>
+      <c r="D8" s="5" t="str">
         <f>IF(NOT('Manual Experiment Interface'!D8=""),'Manual Experiment Interface'!D8,"")</f>
-        <v>500</v>
-      </c>
-      <c r="E8" s="5">
+        <v/>
+      </c>
+      <c r="E8" s="5" t="str">
         <f>IF(NOT('Manual Experiment Interface'!E8=""),'Manual Experiment Interface'!E8,"")</f>
-        <v>300</v>
+        <v/>
       </c>
       <c r="F8" s="5" t="str">
         <f>IF(NOT('Manual Experiment Interface'!F8=""),'Manual Experiment Interface'!F8,"")</f>
@@ -30004,9 +30073,9 @@
         <f>IF(NOT('Manual Experiment Interface'!H8=""),'Manual Experiment Interface'!H8,"")</f>
         <v/>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="5" t="str">
         <f>IF(NOT('Manual Experiment Interface'!I8=""),'Manual Experiment Interface'!I8,"")</f>
-        <v>20</v>
+        <v/>
       </c>
       <c r="J8" s="5" t="str">
         <f>IF(NOT('Manual Experiment Interface'!J8=""),'Manual Experiment Interface'!J8,"")</f>
@@ -30024,19 +30093,19 @@
       </c>
       <c r="B9" s="5" t="str">
         <f>IF(NOT('Manual Experiment Interface'!B9=""),'Manual Experiment Interface'!B9,"")</f>
-        <v>MAN 148.C8</v>
-      </c>
-      <c r="C9" s="5">
+        <v/>
+      </c>
+      <c r="C9" s="5" t="str">
         <f>IF(NOT('Manual Experiment Interface'!C9=""),'Manual Experiment Interface'!C9,"")</f>
-        <v>0</v>
-      </c>
-      <c r="D9" s="5">
+        <v/>
+      </c>
+      <c r="D9" s="5" t="str">
         <f>IF(NOT('Manual Experiment Interface'!D9=""),'Manual Experiment Interface'!D9,"")</f>
-        <v>500</v>
-      </c>
-      <c r="E9" s="5">
+        <v/>
+      </c>
+      <c r="E9" s="5" t="str">
         <f>IF(NOT('Manual Experiment Interface'!E9=""),'Manual Experiment Interface'!E9,"")</f>
-        <v>350</v>
+        <v/>
       </c>
       <c r="F9" s="5" t="str">
         <f>IF(NOT('Manual Experiment Interface'!F9=""),'Manual Experiment Interface'!F9,"")</f>
@@ -30050,9 +30119,9 @@
         <f>IF(NOT('Manual Experiment Interface'!H9=""),'Manual Experiment Interface'!H9,"")</f>
         <v/>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="5" t="str">
         <f>IF(NOT('Manual Experiment Interface'!I9=""),'Manual Experiment Interface'!I9,"")</f>
-        <v>20</v>
+        <v/>
       </c>
       <c r="J9" s="5" t="str">
         <f>IF(NOT('Manual Experiment Interface'!J9=""),'Manual Experiment Interface'!J9,"")</f>
@@ -35302,7 +35371,7 @@
       </c>
       <c r="D7" s="28">
         <f>'User Interface'!wellcount</f>
-        <v>96</v>
+        <v>1</v>
       </c>
       <c r="E7" s="28" t="s">
         <v>192</v>
@@ -35489,7 +35558,7 @@
       </c>
       <c r="D12" s="41">
         <f>'User Interface'!E11</f>
-        <v>96</v>
+        <v>1</v>
       </c>
       <c r="E12" s="41" t="s">
         <v>192</v>

</xml_diff>